<commit_message>
Capa 1 y 2 modelo OSI
</commit_message>
<xml_diff>
--- a/docs/protocol-suite.xlsx
+++ b/docs/protocol-suite.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EducacionIT\Documents\redes\saves\ccna-lx19\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE7A5A2A-7D6A-432B-909C-60ED1F345955}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4F76524-6F99-4D5D-92F0-0BE5658E553F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{3415D364-6D1D-489F-8C8D-BD784F513C31}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="125">
   <si>
     <t xml:space="preserve">TCP/IP </t>
   </si>
@@ -199,12 +199,6 @@
     <t>khz</t>
   </si>
   <si>
-    <t>TIA568A</t>
-  </si>
-  <si>
-    <t>TIA568B</t>
-  </si>
-  <si>
     <t>se envia y recibe en simultaneo</t>
   </si>
   <si>
@@ -220,15 +214,6 @@
     <t>Auto-MDIX</t>
   </si>
   <si>
-    <t>capacidad de un dispositivo de red para determinar que norma se utiliza en el otro extremo y adaptar los pines de envio y recepcion en base a esto</t>
-  </si>
-  <si>
-    <t>colision</t>
-  </si>
-  <si>
-    <t>crosstalk</t>
-  </si>
-  <si>
     <t>EMI</t>
   </si>
   <si>
@@ -244,15 +229,6 @@
     <t>FC (Ferrule Connector)</t>
   </si>
   <si>
-    <t>SMF (Fibra Optica Monomodo)</t>
-  </si>
-  <si>
-    <t>Utiliza un LED para el envio de datos, es mas economico y debido a esto es el mas utilizado para instalaciones hogareñas, su nucleo mide aprox. 60micrones y su alcance es de hasta 2km solamente.</t>
-  </si>
-  <si>
-    <t>MMF(Fibra Optica Multimodo)</t>
-  </si>
-  <si>
     <t>ST (Straight Connector)</t>
   </si>
   <si>
@@ -385,14 +361,62 @@
     <t>cruce de señales no intensionado dentro del mismo medio que producen interferencia</t>
   </si>
   <si>
-    <t>Utiliza laser para el envio de datos y posee un alcance de hasta 200km. Su nucleo mide aprox. 9 micrones y debido a sus costos se suele utilizar en grandes instalaciones como en el cableado submarino.</t>
+    <t>Colision</t>
+  </si>
+  <si>
+    <t>CrossTalk</t>
+  </si>
+  <si>
+    <t>Problematicas</t>
+  </si>
+  <si>
+    <t>Utiliza un LED para el envio de datos, es mas economico y debido a esto es el mas utilizado para instalaciones hogareñas, su nucleo mide aprox. 60micrones y su alcance es de hasta 2km.</t>
+  </si>
+  <si>
+    <t>Utiliza laser para el envio de datos y posee un alcance de 200km. Su nucleo mide aprox. 9 micrones y debido a sus costos se suele utilizar en  instalaciones grandes como cableado submarino.</t>
+  </si>
+  <si>
+    <t>TIA-568-A</t>
+  </si>
+  <si>
+    <t>TIA-568-B</t>
+  </si>
+  <si>
+    <t>Capacidad de un dispositivo de red para  adaptar los pines de envio y recepcion en base a la configuracion en el otro extremo del cable. Practico al momento de establecer una conexión FullDuplex.</t>
+  </si>
+  <si>
+    <t>UPC (Ultra Physical Contact)</t>
+  </si>
+  <si>
+    <t>APC (Angled Physical Contact)</t>
+  </si>
+  <si>
+    <t>TERMINACIONES</t>
+  </si>
+  <si>
+    <t>TIPOS DE CONECTORES</t>
+  </si>
+  <si>
+    <t>SMF (Monomodo)</t>
+  </si>
+  <si>
+    <t>MMF (Multimodo)</t>
+  </si>
+  <si>
+    <t>PC  (Physical Contact)</t>
+  </si>
+  <si>
+    <t>Fibra Optica</t>
+  </si>
+  <si>
+    <t>Par Trenzado</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -421,8 +445,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="19">
+  <fills count="26">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -528,6 +559,48 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor theme="4" tint="0.59999389629810485"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -841,10 +914,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="94">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -884,36 +958,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
@@ -929,72 +973,78 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="10" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
@@ -1008,19 +1058,98 @@
       <alignment horizontal="left" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="23" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="60% - Énfasis1" xfId="1" builtinId="32"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1047,13 +1176,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>541734</xdr:colOff>
-      <xdr:row>1</xdr:row>
+      <xdr:row>2</xdr:row>
       <xdr:rowOff>83344</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>83344</xdr:colOff>
-      <xdr:row>3</xdr:row>
+      <xdr:row>4</xdr:row>
       <xdr:rowOff>119063</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1069,8 +1198,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="732234" y="273844"/>
-          <a:ext cx="541735" cy="416719"/>
+          <a:off x="732234" y="464344"/>
+          <a:ext cx="582033" cy="416719"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -1105,13 +1234,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>559594</xdr:colOff>
-      <xdr:row>2</xdr:row>
+      <xdr:row>3</xdr:row>
       <xdr:rowOff>47625</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>29766</xdr:colOff>
-      <xdr:row>6</xdr:row>
+      <xdr:row>7</xdr:row>
       <xdr:rowOff>154781</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1127,8 +1256,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="750094" y="428625"/>
-          <a:ext cx="470297" cy="869156"/>
+          <a:off x="750094" y="619125"/>
+          <a:ext cx="510595" cy="869156"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -1160,13 +1289,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>553641</xdr:colOff>
-      <xdr:row>1</xdr:row>
+      <xdr:row>2</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>41672</xdr:colOff>
-      <xdr:row>3</xdr:row>
+      <xdr:row>4</xdr:row>
       <xdr:rowOff>130969</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1182,8 +1311,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="744141" y="285750"/>
-          <a:ext cx="488156" cy="416719"/>
+          <a:off x="744141" y="476250"/>
+          <a:ext cx="528454" cy="416719"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -1218,13 +1347,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>565547</xdr:colOff>
-      <xdr:row>2</xdr:row>
+      <xdr:row>3</xdr:row>
       <xdr:rowOff>47625</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>41672</xdr:colOff>
-      <xdr:row>6</xdr:row>
+      <xdr:row>7</xdr:row>
       <xdr:rowOff>130969</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1240,8 +1369,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="756047" y="428625"/>
-          <a:ext cx="476250" cy="845344"/>
+          <a:off x="756047" y="619125"/>
+          <a:ext cx="516548" cy="845344"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -1574,7 +1703,7 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="D8" sqref="D8:D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1603,13 +1732,13 @@
       <c r="A2" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="48" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="19" t="s">
+      <c r="C2" s="43" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="27" t="s">
+      <c r="D2" s="51" t="s">
         <v>23</v>
       </c>
     </row>
@@ -1617,17 +1746,17 @@
       <c r="A3" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="25"/>
-      <c r="C3" s="20"/>
-      <c r="D3" s="27"/>
+      <c r="B3" s="49"/>
+      <c r="C3" s="44"/>
+      <c r="D3" s="51"/>
     </row>
     <row r="4" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="26"/>
-      <c r="C4" s="21"/>
-      <c r="D4" s="27"/>
+      <c r="B4" s="50"/>
+      <c r="C4" s="45"/>
+      <c r="D4" s="51"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
@@ -1664,7 +1793,7 @@
       <c r="B7" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="22" t="s">
+      <c r="C7" s="46" t="s">
         <v>12</v>
       </c>
       <c r="D7" s="15" t="s">
@@ -1678,8 +1807,8 @@
       <c r="B8" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="23"/>
-      <c r="D8" s="27" t="s">
+      <c r="C8" s="47"/>
+      <c r="D8" s="51" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1693,7 +1822,7 @@
       <c r="C9" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D9" s="28"/>
+      <c r="D9" s="52"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -1710,228 +1839,273 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D6A4FC1-4453-4F66-8A6E-DB11164B3A80}">
-  <dimension ref="A1:H14"/>
+  <dimension ref="A1:I20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2.85546875" customWidth="1"/>
-    <col min="2" max="2" width="9" customWidth="1"/>
-    <col min="3" max="3" width="6" customWidth="1"/>
-    <col min="4" max="4" width="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="3.5703125" customWidth="1"/>
-    <col min="6" max="6" width="28.7109375" style="55" customWidth="1"/>
-    <col min="7" max="7" width="28.5703125" style="55" customWidth="1"/>
-    <col min="8" max="8" width="28.7109375" style="55" customWidth="1"/>
+    <col min="2" max="2" width="9.7109375" customWidth="1"/>
+    <col min="3" max="4" width="11" customWidth="1"/>
+    <col min="5" max="5" width="2.85546875" customWidth="1"/>
+    <col min="6" max="8" width="27.7109375" style="34" customWidth="1"/>
+    <col min="9" max="9" width="28.7109375" style="34" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B1" t="s">
-        <v>54</v>
-      </c>
-      <c r="D1" t="s">
+    <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="81" t="s">
+        <v>124</v>
+      </c>
+      <c r="C1" s="81"/>
+      <c r="D1" s="81"/>
+      <c r="F1" s="81" t="s">
+        <v>123</v>
+      </c>
+      <c r="G1" s="81"/>
+      <c r="H1" s="81"/>
+    </row>
+    <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="80" t="s">
+        <v>113</v>
+      </c>
+      <c r="D2" s="80" t="s">
+        <v>114</v>
+      </c>
+      <c r="F2" s="72" t="s">
+        <v>120</v>
+      </c>
+      <c r="G2" s="72" t="s">
+        <v>121</v>
+      </c>
+      <c r="H2" s="80" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" s="88" t="s">
         <v>55</v>
       </c>
-      <c r="F1" s="55" t="s">
+      <c r="D3" s="86" t="s">
+        <v>55</v>
+      </c>
+      <c r="F3" s="82" t="s">
+        <v>112</v>
+      </c>
+      <c r="G3" s="84" t="s">
+        <v>111</v>
+      </c>
+      <c r="H3" s="73" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" s="91" t="s">
+        <v>55</v>
+      </c>
+      <c r="D4" s="87" t="s">
+        <v>55</v>
+      </c>
+      <c r="F4" s="82"/>
+      <c r="G4" s="84"/>
+      <c r="H4" s="74" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" s="86" t="s">
+        <v>56</v>
+      </c>
+      <c r="D5" s="88" t="s">
+        <v>56</v>
+      </c>
+      <c r="F5" s="82"/>
+      <c r="G5" s="84"/>
+      <c r="H5" s="75" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" s="89" t="s">
+        <v>57</v>
+      </c>
+      <c r="D6" s="89" t="s">
+        <v>57</v>
+      </c>
+      <c r="F6" s="82"/>
+      <c r="G6" s="84"/>
+      <c r="H6" s="76" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" s="90" t="s">
+        <v>57</v>
+      </c>
+      <c r="D7" s="90" t="s">
+        <v>57</v>
+      </c>
+      <c r="F7" s="82"/>
+      <c r="G7" s="84"/>
+      <c r="H7" s="80" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8" s="87" t="s">
+        <v>56</v>
+      </c>
+      <c r="D8" s="91" t="s">
+        <v>56</v>
+      </c>
+      <c r="F8" s="82"/>
+      <c r="G8" s="84"/>
+      <c r="H8" s="77" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9" s="92" t="s">
+        <v>57</v>
+      </c>
+      <c r="D9" s="92" t="s">
+        <v>57</v>
+      </c>
+      <c r="F9" s="82"/>
+      <c r="G9" s="84"/>
+      <c r="H9" s="78" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10" s="93" t="s">
+        <v>57</v>
+      </c>
+      <c r="D10" s="93" t="s">
+        <v>57</v>
+      </c>
+      <c r="F10" s="83"/>
+      <c r="G10" s="85"/>
+      <c r="H10" s="79" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B12" s="65" t="s">
+        <v>110</v>
+      </c>
+      <c r="C12" s="65"/>
+      <c r="D12" s="65"/>
+      <c r="E12" s="65"/>
+      <c r="F12" s="65"/>
+      <c r="G12" s="68" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" s="41" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="70" t="s">
+        <v>108</v>
+      </c>
+      <c r="C13" s="66" t="s">
+        <v>107</v>
+      </c>
+      <c r="D13" s="66"/>
+      <c r="E13" s="66"/>
+      <c r="F13" s="66"/>
+      <c r="G13" s="69" t="s">
+        <v>115</v>
+      </c>
+      <c r="I13" s="42"/>
+    </row>
+    <row r="14" spans="1:9" s="41" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="71" t="s">
+        <v>59</v>
+      </c>
+      <c r="C14" s="67" t="s">
+        <v>104</v>
+      </c>
+      <c r="D14" s="67"/>
+      <c r="E14" s="67"/>
+      <c r="F14" s="67"/>
+      <c r="G14" s="69"/>
+      <c r="I14" s="42"/>
+    </row>
+    <row r="15" spans="1:9" s="41" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="70" t="s">
         <v>60</v>
       </c>
-      <c r="G1" s="55" t="s">
-        <v>69</v>
-      </c>
-      <c r="H1" s="55" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" s="46" t="s">
-        <v>57</v>
-      </c>
-      <c r="D2" s="48" t="s">
-        <v>57</v>
-      </c>
-      <c r="F2" s="56" t="s">
-        <v>61</v>
-      </c>
-      <c r="G2" s="56" t="s">
-        <v>116</v>
-      </c>
-      <c r="H2" s="56" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" s="47" t="s">
-        <v>57</v>
-      </c>
-      <c r="D3" s="51" t="s">
-        <v>57</v>
-      </c>
-      <c r="F3" s="56"/>
-      <c r="G3" s="56"/>
-      <c r="H3" s="56"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" s="48" t="s">
-        <v>58</v>
-      </c>
-      <c r="D4" s="46" t="s">
-        <v>58</v>
-      </c>
-      <c r="F4" s="56"/>
-      <c r="G4" s="56"/>
-      <c r="H4" s="56"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" s="49" t="s">
-        <v>59</v>
-      </c>
-      <c r="D5" s="49" t="s">
-        <v>59</v>
-      </c>
-      <c r="F5" s="56"/>
-      <c r="G5" s="56"/>
-      <c r="H5" s="56"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" s="50" t="s">
-        <v>59</v>
-      </c>
-      <c r="D6" s="50" t="s">
-        <v>59</v>
-      </c>
-      <c r="F6" s="56"/>
-      <c r="G6" s="56"/>
-      <c r="H6" s="56"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7" s="51" t="s">
-        <v>58</v>
-      </c>
-      <c r="D7" s="47" t="s">
-        <v>58</v>
-      </c>
-      <c r="F7" s="56"/>
-      <c r="G7" s="56"/>
-      <c r="H7" s="56"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8" s="52" t="s">
-        <v>59</v>
-      </c>
-      <c r="D8" s="52" t="s">
-        <v>59</v>
-      </c>
-      <c r="F8" s="56"/>
-      <c r="G8" s="56"/>
-      <c r="H8" s="56"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>8</v>
-      </c>
-      <c r="B9" s="53" t="s">
-        <v>59</v>
-      </c>
-      <c r="D9" s="53" t="s">
-        <v>59</v>
-      </c>
-      <c r="F9" s="56"/>
-      <c r="G9" s="56"/>
-      <c r="H9" s="56"/>
-    </row>
-    <row r="11" spans="1:8" s="72" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="75" t="s">
-        <v>62</v>
-      </c>
-      <c r="C11" s="54" t="s">
-        <v>115</v>
-      </c>
-      <c r="D11" s="54"/>
-      <c r="E11" s="54"/>
-      <c r="F11" s="54"/>
-      <c r="G11" s="73" t="s">
-        <v>66</v>
-      </c>
-      <c r="H11" s="73"/>
-    </row>
-    <row r="12" spans="1:8" s="72" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="75" t="s">
-        <v>64</v>
-      </c>
-      <c r="C12" s="74" t="s">
-        <v>112</v>
-      </c>
-      <c r="D12" s="74"/>
-      <c r="E12" s="74"/>
-      <c r="F12" s="74"/>
-      <c r="G12" s="73" t="s">
-        <v>67</v>
-      </c>
-      <c r="H12" s="73"/>
-    </row>
-    <row r="13" spans="1:8" s="72" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="75" t="s">
-        <v>65</v>
-      </c>
-      <c r="C13" s="54" t="s">
-        <v>113</v>
-      </c>
-      <c r="D13" s="54"/>
-      <c r="E13" s="54"/>
-      <c r="F13" s="54"/>
-      <c r="G13" s="73" t="s">
-        <v>68</v>
-      </c>
-      <c r="H13" s="73"/>
-    </row>
-    <row r="14" spans="1:8" s="72" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="75" t="s">
-        <v>63</v>
-      </c>
-      <c r="C14" s="54" t="s">
-        <v>114</v>
-      </c>
-      <c r="D14" s="54"/>
-      <c r="E14" s="54"/>
-      <c r="F14" s="54"/>
-      <c r="G14" s="73" t="s">
-        <v>72</v>
-      </c>
-      <c r="H14" s="73"/>
+      <c r="C15" s="66" t="s">
+        <v>105</v>
+      </c>
+      <c r="D15" s="66"/>
+      <c r="E15" s="66"/>
+      <c r="F15" s="66"/>
+      <c r="G15" s="69"/>
+      <c r="I15" s="42"/>
+    </row>
+    <row r="16" spans="1:9" s="41" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="71" t="s">
+        <v>109</v>
+      </c>
+      <c r="C16" s="67" t="s">
+        <v>106</v>
+      </c>
+      <c r="D16" s="67"/>
+      <c r="E16" s="67"/>
+      <c r="F16" s="67"/>
+      <c r="G16" s="69"/>
+      <c r="I16" s="42"/>
+    </row>
+    <row r="17" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G17" s="64"/>
+    </row>
+    <row r="18" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G18" s="64"/>
+    </row>
+    <row r="19" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G19" s="64"/>
+    </row>
+    <row r="20" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G20" s="64"/>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="10">
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="G13:G16"/>
+    <mergeCell ref="B12:F12"/>
+    <mergeCell ref="F1:H1"/>
+    <mergeCell ref="C16:F16"/>
+    <mergeCell ref="F3:F10"/>
+    <mergeCell ref="G3:G10"/>
+    <mergeCell ref="C13:F13"/>
     <mergeCell ref="C14:F14"/>
-    <mergeCell ref="F2:F9"/>
-    <mergeCell ref="G2:G9"/>
-    <mergeCell ref="H2:H9"/>
-    <mergeCell ref="C11:F11"/>
-    <mergeCell ref="C12:F12"/>
-    <mergeCell ref="C13:F13"/>
+    <mergeCell ref="C15:F15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -1962,290 +2136,290 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="44" t="s">
+      <c r="A2" s="58" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="45"/>
-      <c r="C2" s="37" t="s">
+      <c r="B2" s="59"/>
+      <c r="C2" s="27" t="s">
         <v>44</v>
       </c>
-      <c r="E2" s="44" t="s">
+      <c r="E2" s="58" t="s">
         <v>29</v>
       </c>
-      <c r="F2" s="45"/>
-      <c r="G2" s="37" t="s">
+      <c r="F2" s="59"/>
+      <c r="G2" s="27" t="s">
         <v>44</v>
       </c>
-      <c r="I2" s="44" t="s">
+      <c r="I2" s="58" t="s">
         <v>30</v>
       </c>
-      <c r="J2" s="45"/>
-      <c r="K2" s="37" t="s">
+      <c r="J2" s="59"/>
+      <c r="K2" s="27" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="66" t="s">
+      <c r="A3" s="39" t="s">
         <v>31</v>
       </c>
-      <c r="B3" s="67" t="s">
+      <c r="B3" s="40" t="s">
         <v>32</v>
       </c>
-      <c r="C3" s="40" t="s">
+      <c r="C3" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="E3" s="38" t="s">
+      <c r="E3" s="28" t="s">
+        <v>83</v>
+      </c>
+      <c r="F3" s="29" t="s">
+        <v>88</v>
+      </c>
+      <c r="G3" s="30" t="s">
+        <v>34</v>
+      </c>
+      <c r="I3" s="28" t="s">
+        <v>89</v>
+      </c>
+      <c r="J3" s="29" t="s">
+        <v>52</v>
+      </c>
+      <c r="K3" s="30" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="19" t="s">
+        <v>75</v>
+      </c>
+      <c r="B4" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4" s="23" t="s">
+        <v>35</v>
+      </c>
+      <c r="E4" s="31" t="s">
+        <v>45</v>
+      </c>
+      <c r="F4" s="32" t="s">
+        <v>87</v>
+      </c>
+      <c r="G4" s="23" t="s">
+        <v>35</v>
+      </c>
+      <c r="I4" s="31" t="s">
+        <v>53</v>
+      </c>
+      <c r="J4" s="32" t="s">
+        <v>92</v>
+      </c>
+      <c r="K4" s="23" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="39" t="s">
+        <v>76</v>
+      </c>
+      <c r="B5" s="40" t="s">
+        <v>96</v>
+      </c>
+      <c r="C5" s="30" t="s">
+        <v>36</v>
+      </c>
+      <c r="E5" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="F5" s="29" t="s">
+        <v>86</v>
+      </c>
+      <c r="G5" s="30" t="s">
+        <v>36</v>
+      </c>
+      <c r="I5" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="J5" s="29" t="s">
+        <v>93</v>
+      </c>
+      <c r="K5" s="30" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="19" t="s">
+        <v>77</v>
+      </c>
+      <c r="B6" s="20" t="s">
+        <v>97</v>
+      </c>
+      <c r="C6" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="E6" s="31" t="s">
+        <v>47</v>
+      </c>
+      <c r="F6" s="32" t="s">
+        <v>85</v>
+      </c>
+      <c r="G6" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="I6" s="31" t="s">
+        <v>50</v>
+      </c>
+      <c r="J6" s="32" t="s">
+        <v>94</v>
+      </c>
+      <c r="K6" s="23" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="39" t="s">
+        <v>78</v>
+      </c>
+      <c r="B7" s="40" t="s">
+        <v>98</v>
+      </c>
+      <c r="C7" s="30" t="s">
+        <v>38</v>
+      </c>
+      <c r="E7" s="25" t="s">
+        <v>48</v>
+      </c>
+      <c r="F7" s="26" t="s">
+        <v>84</v>
+      </c>
+      <c r="G7" s="33" t="s">
+        <v>38</v>
+      </c>
+      <c r="I7" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="J7" s="26" t="s">
+        <v>95</v>
+      </c>
+      <c r="K7" s="33" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="19" t="s">
+        <v>79</v>
+      </c>
+      <c r="B8" s="20" t="s">
+        <v>99</v>
+      </c>
+      <c r="C8" s="23" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="39" t="s">
+        <v>80</v>
+      </c>
+      <c r="B9" s="40" t="s">
+        <v>100</v>
+      </c>
+      <c r="C9" s="30" t="s">
+        <v>40</v>
+      </c>
+      <c r="E9" s="35" t="s">
+        <v>68</v>
+      </c>
+      <c r="F9" s="53" t="s">
+        <v>69</v>
+      </c>
+      <c r="G9" s="53"/>
+      <c r="I9" s="53" t="s">
         <v>91</v>
       </c>
-      <c r="F3" s="39" t="s">
-        <v>96</v>
-      </c>
-      <c r="G3" s="40" t="s">
-        <v>34</v>
-      </c>
-      <c r="I3" s="38" t="s">
-        <v>97</v>
-      </c>
-      <c r="J3" s="39" t="s">
-        <v>52</v>
-      </c>
-      <c r="K3" s="40" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="29" t="s">
-        <v>83</v>
-      </c>
-      <c r="B4" s="30" t="s">
-        <v>33</v>
-      </c>
-      <c r="C4" s="33" t="s">
-        <v>35</v>
-      </c>
-      <c r="E4" s="41" t="s">
-        <v>45</v>
-      </c>
-      <c r="F4" s="42" t="s">
-        <v>95</v>
-      </c>
-      <c r="G4" s="33" t="s">
-        <v>35</v>
-      </c>
-      <c r="I4" s="41" t="s">
-        <v>53</v>
-      </c>
-      <c r="J4" s="42" t="s">
-        <v>100</v>
-      </c>
-      <c r="K4" s="33" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="66" t="s">
-        <v>84</v>
-      </c>
-      <c r="B5" s="67" t="s">
-        <v>104</v>
-      </c>
-      <c r="C5" s="40" t="s">
-        <v>36</v>
-      </c>
-      <c r="E5" s="38" t="s">
-        <v>46</v>
-      </c>
-      <c r="F5" s="39" t="s">
-        <v>94</v>
-      </c>
-      <c r="G5" s="40" t="s">
-        <v>36</v>
-      </c>
-      <c r="I5" s="38" t="s">
-        <v>49</v>
-      </c>
-      <c r="J5" s="39" t="s">
+      <c r="J9" s="53"/>
+      <c r="K9" s="53"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="B10" s="20" t="s">
         <v>101</v>
       </c>
-      <c r="K5" s="40" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="29" t="s">
-        <v>85</v>
-      </c>
-      <c r="B6" s="30" t="s">
-        <v>105</v>
-      </c>
-      <c r="C6" s="33" t="s">
-        <v>37</v>
-      </c>
-      <c r="E6" s="41" t="s">
-        <v>47</v>
-      </c>
-      <c r="F6" s="42" t="s">
-        <v>93</v>
-      </c>
-      <c r="G6" s="33" t="s">
-        <v>37</v>
-      </c>
-      <c r="I6" s="41" t="s">
-        <v>50</v>
-      </c>
-      <c r="J6" s="42" t="s">
+      <c r="C10" s="23" t="s">
+        <v>41</v>
+      </c>
+      <c r="D10" s="36"/>
+      <c r="E10" s="37" t="s">
+        <v>70</v>
+      </c>
+      <c r="F10" s="54" t="s">
+        <v>72</v>
+      </c>
+      <c r="G10" s="55"/>
+      <c r="I10" s="60" t="s">
+        <v>65</v>
+      </c>
+      <c r="J10" s="54"/>
+      <c r="K10" s="55"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="39" t="s">
+        <v>82</v>
+      </c>
+      <c r="B11" s="40" t="s">
         <v>102</v>
       </c>
-      <c r="K6" s="33" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="66" t="s">
-        <v>86</v>
-      </c>
-      <c r="B7" s="67" t="s">
-        <v>106</v>
-      </c>
-      <c r="C7" s="40" t="s">
-        <v>38</v>
-      </c>
-      <c r="E7" s="35" t="s">
-        <v>48</v>
-      </c>
-      <c r="F7" s="36" t="s">
-        <v>92</v>
-      </c>
-      <c r="G7" s="43" t="s">
-        <v>38</v>
-      </c>
-      <c r="I7" s="35" t="s">
-        <v>51</v>
-      </c>
-      <c r="J7" s="36" t="s">
+      <c r="C11" s="30" t="s">
+        <v>42</v>
+      </c>
+      <c r="E11" s="38" t="s">
+        <v>71</v>
+      </c>
+      <c r="F11" s="56" t="s">
+        <v>54</v>
+      </c>
+      <c r="G11" s="57"/>
+      <c r="I11" s="61" t="s">
+        <v>66</v>
+      </c>
+      <c r="J11" s="62"/>
+      <c r="K11" s="63"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="21" t="s">
+        <v>90</v>
+      </c>
+      <c r="B12" s="22" t="s">
         <v>103</v>
       </c>
-      <c r="K7" s="43" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="29" t="s">
-        <v>87</v>
-      </c>
-      <c r="B8" s="30" t="s">
-        <v>107</v>
-      </c>
-      <c r="C8" s="33" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="66" t="s">
-        <v>88</v>
-      </c>
-      <c r="B9" s="67" t="s">
-        <v>108</v>
-      </c>
-      <c r="C9" s="40" t="s">
-        <v>40</v>
-      </c>
-      <c r="E9" s="57" t="s">
-        <v>76</v>
-      </c>
-      <c r="F9" s="65" t="s">
-        <v>77</v>
-      </c>
-      <c r="G9" s="65"/>
-      <c r="I9" s="65" t="s">
-        <v>99</v>
-      </c>
-      <c r="J9" s="65"/>
-      <c r="K9" s="65"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="29" t="s">
-        <v>89</v>
-      </c>
-      <c r="B10" s="30" t="s">
-        <v>109</v>
-      </c>
-      <c r="C10" s="33" t="s">
-        <v>41</v>
-      </c>
-      <c r="D10" s="60"/>
-      <c r="E10" s="61" t="s">
-        <v>78</v>
-      </c>
-      <c r="F10" s="62" t="s">
-        <v>80</v>
-      </c>
-      <c r="G10" s="63"/>
-      <c r="I10" s="68" t="s">
+      <c r="C12" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="E12" s="37" t="s">
         <v>73</v>
       </c>
-      <c r="J10" s="62"/>
-      <c r="K10" s="63"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="66" t="s">
-        <v>90</v>
-      </c>
-      <c r="B11" s="67" t="s">
-        <v>110</v>
-      </c>
-      <c r="C11" s="40" t="s">
-        <v>42</v>
-      </c>
-      <c r="E11" s="64" t="s">
-        <v>79</v>
-      </c>
-      <c r="F11" s="58" t="s">
-        <v>56</v>
-      </c>
-      <c r="G11" s="59"/>
-      <c r="I11" s="69" t="s">
+      <c r="F12" s="54" t="s">
         <v>74</v>
       </c>
-      <c r="J11" s="70"/>
-      <c r="K11" s="71"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="31" t="s">
-        <v>98</v>
-      </c>
-      <c r="B12" s="32" t="s">
-        <v>111</v>
-      </c>
-      <c r="C12" s="34" t="s">
-        <v>43</v>
-      </c>
-      <c r="E12" s="61" t="s">
-        <v>81</v>
-      </c>
-      <c r="F12" s="62" t="s">
-        <v>82</v>
-      </c>
-      <c r="G12" s="63"/>
-      <c r="I12" s="68" t="s">
-        <v>75</v>
-      </c>
-      <c r="J12" s="62"/>
-      <c r="K12" s="63"/>
+      <c r="G12" s="55"/>
+      <c r="I12" s="60" t="s">
+        <v>67</v>
+      </c>
+      <c r="J12" s="54"/>
+      <c r="K12" s="55"/>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="F9:G9"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="I9:K9"/>
     <mergeCell ref="I2:J2"/>
     <mergeCell ref="E2:F2"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="I12:K12"/>
     <mergeCell ref="I11:K11"/>
     <mergeCell ref="I10:K10"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="I9:K9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Caracteristicas TCP y UDP
</commit_message>
<xml_diff>
--- a/docs/protocol-suite.xlsx
+++ b/docs/protocol-suite.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EducacionIT\Documents\redes\saves\ccna-lx19\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33D06783-A92B-4722-BE09-A1E23C931976}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79F895D3-C35C-42F7-A197-48A7C61BFAA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="8" xr2:uid="{3415D364-6D1D-489F-8C8D-BD784F513C31}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="972" uniqueCount="651">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1004" uniqueCount="683">
   <si>
     <t xml:space="preserve">TCP/IP </t>
   </si>
@@ -7663,10 +7663,106 @@
     <t>reservados por la IANA</t>
   </si>
   <si>
-    <t>reservados para aplicaciones concretas</t>
-  </si>
-  <si>
     <t>puedes usarlos libremente</t>
+  </si>
+  <si>
+    <t>orientado a la conexión</t>
+  </si>
+  <si>
+    <t>sin conexión</t>
+  </si>
+  <si>
+    <t>reenvia datos perdidos</t>
+  </si>
+  <si>
+    <t>baja sobrecarga</t>
+  </si>
+  <si>
+    <t>tipo</t>
+  </si>
+  <si>
+    <t>aplicación</t>
+  </si>
+  <si>
+    <t>TCP</t>
+  </si>
+  <si>
+    <t>UDP</t>
+  </si>
+  <si>
+    <t>Protocolo</t>
+  </si>
+  <si>
+    <t>recepcion</t>
+  </si>
+  <si>
+    <t>acuses de recibo (ACK)</t>
+  </si>
+  <si>
+    <t>no reenvia datos (corrupto)</t>
+  </si>
+  <si>
+    <t>Puertos</t>
+  </si>
+  <si>
+    <t>Implementacion</t>
+  </si>
+  <si>
+    <t>reservados para aplicaciones</t>
+  </si>
+  <si>
+    <t>protocolos</t>
+  </si>
+  <si>
+    <t>Segmento</t>
+  </si>
+  <si>
+    <t>Datagrama</t>
+  </si>
+  <si>
+    <t>unidad</t>
+  </si>
+  <si>
+    <t>20 bytes</t>
+  </si>
+  <si>
+    <t>8 bytes</t>
+  </si>
+  <si>
+    <t>sentido</t>
+  </si>
+  <si>
+    <t>cabecera</t>
+  </si>
+  <si>
+    <t>confiable (lento)</t>
+  </si>
+  <si>
+    <t>rapido (no fidedigno)</t>
+  </si>
+  <si>
+    <t>significado</t>
+  </si>
+  <si>
+    <t>Transport Control Protocol</t>
+  </si>
+  <si>
+    <t>User Datagram Protocol</t>
+  </si>
+  <si>
+    <t>verificacion</t>
+  </si>
+  <si>
+    <t>Entrega en el orden enviado</t>
+  </si>
+  <si>
+    <t>Entrega en el orden recibido</t>
+  </si>
+  <si>
+    <t>http, ftp, pop, imap, smtp</t>
+  </si>
+  <si>
+    <t>dhcp, dns, snmp, tftp</t>
   </si>
 </sst>
 </file>
@@ -9130,7 +9226,7 @@
     <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="411">
+  <cellXfs count="417">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -9884,229 +9980,220 @@
     <xf numFmtId="49" fontId="0" fillId="38" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="1" fontId="0" fillId="10" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="30" borderId="0" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="30" borderId="65" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="31" borderId="0" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="31" borderId="65" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="65" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="31" borderId="67" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="31" borderId="68" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="61" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="31" borderId="62" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="31" borderId="63" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="32" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="52" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="53" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="59" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="54" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="56" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="32" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="52" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="53" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="10" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="30" borderId="0" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="30" borderId="65" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="31" borderId="0" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="31" borderId="65" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="65" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="31" borderId="67" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="31" borderId="68" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="61" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="31" borderId="62" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="31" borderId="63" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="15" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="32" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="52" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="53" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="59" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="54" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="56" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="32" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="52" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="53" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -10124,19 +10211,22 @@
     <xf numFmtId="0" fontId="3" fillId="26" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="15" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="15" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="29" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="30" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="31" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="28" borderId="43" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="24" borderId="54" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -10148,6 +10238,24 @@
     <xf numFmtId="49" fontId="0" fillId="24" borderId="55" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="36" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="36" borderId="59" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="36" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="59" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="60" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="28" borderId="30" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="25" borderId="54" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -10166,41 +10274,41 @@
     <xf numFmtId="49" fontId="0" fillId="24" borderId="57" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="36" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="36" borderId="59" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="36" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="59" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="60" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="28" borderId="30" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="15" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="29" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="30" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="31" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="28" borderId="43" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="91" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="76" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="87" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="91" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="76" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="87" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="92" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="82" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="88" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="92" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="82" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="88" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="10" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
@@ -10214,42 +10322,6 @@
     <xf numFmtId="49" fontId="3" fillId="9" borderId="77" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="37" borderId="92" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="37" borderId="82" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="37" borderId="88" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="37" borderId="91" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="37" borderId="76" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="37" borderId="87" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="91" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="76" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="87" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="92" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="82" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="88" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="40" borderId="80" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
@@ -10271,18 +10343,68 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="98" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="21" borderId="99" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="100" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="97" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="100" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="21" borderId="97" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="98" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="100" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="100" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="98" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="99" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="100" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="97" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="100" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="97" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
@@ -10845,7 +10967,7 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="D2" sqref="D2:D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10871,100 +10993,100 @@
       </c>
     </row>
     <row r="2" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="279" t="s">
+      <c r="A2" s="278" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="295" t="s">
+      <c r="B2" s="396" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="290" t="s">
+      <c r="C2" s="285" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="298" t="s">
+      <c r="D2" s="290" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="280" t="s">
+      <c r="A3" s="279" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="296"/>
-      <c r="C3" s="291"/>
-      <c r="D3" s="298"/>
+      <c r="B3" s="397"/>
+      <c r="C3" s="286"/>
+      <c r="D3" s="290"/>
     </row>
     <row r="4" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="281" t="s">
+      <c r="A4" s="280" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="297"/>
-      <c r="C4" s="292"/>
-      <c r="D4" s="298"/>
+      <c r="B4" s="398"/>
+      <c r="C4" s="287"/>
+      <c r="D4" s="290"/>
     </row>
     <row r="5" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="282" t="s">
+      <c r="A5" s="281" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="286" t="s">
+      <c r="B5" s="399" t="s">
         <v>16</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="277" t="s">
+      <c r="D5" s="276" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="283" t="s">
+      <c r="A6" s="282" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="287" t="s">
+      <c r="B6" s="400" t="s">
         <v>17</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="277" t="s">
+      <c r="D6" s="276" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="284" t="s">
+      <c r="A7" s="283" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="288" t="s">
+      <c r="B7" s="401" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="293" t="s">
+      <c r="C7" s="288" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="277" t="s">
+      <c r="D7" s="276" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="285" t="s">
+      <c r="A8" s="284" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="289" t="s">
+      <c r="B8" s="402" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="294"/>
-      <c r="D8" s="298" t="s">
+      <c r="C8" s="289"/>
+      <c r="D8" s="290" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="278" t="s">
+      <c r="A9" s="277" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="278" t="s">
+      <c r="B9" s="277" t="s">
         <v>25</v>
       </c>
-      <c r="C9" s="278" t="s">
+      <c r="C9" s="277" t="s">
         <v>14</v>
       </c>
-      <c r="D9" s="299"/>
+      <c r="D9" s="291"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -10983,8 +11105,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2546DD17-9723-4091-B9ED-D9677931F7C4}">
   <dimension ref="A2:K21"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:C3"/>
+    <sheetView topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H2" sqref="H1:H1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11003,24 +11125,24 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="300" t="s">
+      <c r="A2" s="305" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="301"/>
+      <c r="B2" s="306"/>
       <c r="C2" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="E2" s="300" t="s">
+      <c r="E2" s="305" t="s">
         <v>29</v>
       </c>
-      <c r="F2" s="301"/>
+      <c r="F2" s="306"/>
       <c r="G2" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="I2" s="300" t="s">
+      <c r="I2" s="305" t="s">
         <v>30</v>
       </c>
-      <c r="J2" s="301"/>
+      <c r="J2" s="306"/>
       <c r="K2" s="14" t="s">
         <v>42</v>
       </c>
@@ -11194,15 +11316,15 @@
       <c r="E9" s="22" t="s">
         <v>66</v>
       </c>
-      <c r="F9" s="308" t="s">
+      <c r="F9" s="313" t="s">
         <v>67</v>
       </c>
-      <c r="G9" s="308"/>
-      <c r="I9" s="308" t="s">
+      <c r="G9" s="313"/>
+      <c r="I9" s="313" t="s">
         <v>81</v>
       </c>
-      <c r="J9" s="308"/>
-      <c r="K9" s="308"/>
+      <c r="J9" s="313"/>
+      <c r="K9" s="313"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
@@ -11218,15 +11340,15 @@
       <c r="E10" s="24" t="s">
         <v>68</v>
       </c>
-      <c r="F10" s="303" t="s">
+      <c r="F10" s="308" t="s">
         <v>70</v>
       </c>
-      <c r="G10" s="304"/>
-      <c r="I10" s="302" t="s">
+      <c r="G10" s="309"/>
+      <c r="I10" s="307" t="s">
         <v>63</v>
       </c>
-      <c r="J10" s="303"/>
-      <c r="K10" s="304"/>
+      <c r="J10" s="308"/>
+      <c r="K10" s="309"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="26" t="s">
@@ -11241,15 +11363,15 @@
       <c r="E11" s="25" t="s">
         <v>69</v>
       </c>
-      <c r="F11" s="309" t="s">
+      <c r="F11" s="314" t="s">
         <v>52</v>
       </c>
-      <c r="G11" s="310"/>
-      <c r="I11" s="305" t="s">
+      <c r="G11" s="315"/>
+      <c r="I11" s="310" t="s">
         <v>64</v>
       </c>
-      <c r="J11" s="306"/>
-      <c r="K11" s="307"/>
+      <c r="J11" s="311"/>
+      <c r="K11" s="312"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
@@ -11264,15 +11386,15 @@
       <c r="E12" s="24" t="s">
         <v>71</v>
       </c>
-      <c r="F12" s="303" t="s">
+      <c r="F12" s="308" t="s">
         <v>72</v>
       </c>
-      <c r="G12" s="304"/>
-      <c r="I12" s="302" t="s">
+      <c r="G12" s="309"/>
+      <c r="I12" s="307" t="s">
         <v>65</v>
       </c>
-      <c r="J12" s="303"/>
-      <c r="K12" s="304"/>
+      <c r="J12" s="308"/>
+      <c r="K12" s="309"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="26" t="s">
@@ -11308,100 +11430,94 @@
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="319" t="s">
+      <c r="A17" s="300" t="s">
         <v>282</v>
       </c>
       <c r="B17" s="187" t="s">
         <v>272</v>
       </c>
-      <c r="C17" s="322" t="s">
+      <c r="C17" s="303" t="s">
         <v>273</v>
       </c>
-      <c r="D17" s="322"/>
-      <c r="E17" s="322"/>
-      <c r="F17" s="322"/>
-      <c r="G17" s="322"/>
-      <c r="H17" s="322"/>
-      <c r="I17" s="322"/>
-      <c r="J17" s="322"/>
-      <c r="K17" s="323"/>
+      <c r="D17" s="303"/>
+      <c r="E17" s="303"/>
+      <c r="F17" s="303"/>
+      <c r="G17" s="303"/>
+      <c r="H17" s="303"/>
+      <c r="I17" s="303"/>
+      <c r="J17" s="303"/>
+      <c r="K17" s="304"/>
     </row>
     <row r="18" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="320"/>
+      <c r="A18" s="301"/>
       <c r="B18" s="188" t="s">
         <v>274</v>
       </c>
-      <c r="C18" s="311" t="s">
+      <c r="C18" s="292" t="s">
         <v>275</v>
       </c>
-      <c r="D18" s="311"/>
-      <c r="E18" s="311"/>
-      <c r="F18" s="311"/>
-      <c r="G18" s="311"/>
-      <c r="H18" s="311"/>
-      <c r="I18" s="311"/>
-      <c r="J18" s="311"/>
-      <c r="K18" s="312"/>
+      <c r="D18" s="292"/>
+      <c r="E18" s="292"/>
+      <c r="F18" s="292"/>
+      <c r="G18" s="292"/>
+      <c r="H18" s="292"/>
+      <c r="I18" s="292"/>
+      <c r="J18" s="292"/>
+      <c r="K18" s="293"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="320"/>
+      <c r="A19" s="301"/>
       <c r="B19" s="189" t="s">
         <v>276</v>
       </c>
-      <c r="C19" s="313" t="s">
+      <c r="C19" s="294" t="s">
         <v>277</v>
       </c>
-      <c r="D19" s="313"/>
-      <c r="E19" s="313"/>
-      <c r="F19" s="313"/>
-      <c r="G19" s="313"/>
-      <c r="H19" s="313"/>
-      <c r="I19" s="313"/>
-      <c r="J19" s="313"/>
-      <c r="K19" s="314"/>
+      <c r="D19" s="294"/>
+      <c r="E19" s="294"/>
+      <c r="F19" s="294"/>
+      <c r="G19" s="294"/>
+      <c r="H19" s="294"/>
+      <c r="I19" s="294"/>
+      <c r="J19" s="294"/>
+      <c r="K19" s="295"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="320"/>
+      <c r="A20" s="301"/>
       <c r="B20" s="190" t="s">
         <v>278</v>
       </c>
-      <c r="C20" s="315" t="s">
+      <c r="C20" s="296" t="s">
         <v>279</v>
       </c>
-      <c r="D20" s="315"/>
-      <c r="E20" s="315"/>
-      <c r="F20" s="315"/>
-      <c r="G20" s="315"/>
-      <c r="H20" s="315"/>
-      <c r="I20" s="315"/>
-      <c r="J20" s="315"/>
-      <c r="K20" s="316"/>
+      <c r="D20" s="296"/>
+      <c r="E20" s="296"/>
+      <c r="F20" s="296"/>
+      <c r="G20" s="296"/>
+      <c r="H20" s="296"/>
+      <c r="I20" s="296"/>
+      <c r="J20" s="296"/>
+      <c r="K20" s="297"/>
     </row>
     <row r="21" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="321"/>
+      <c r="A21" s="302"/>
       <c r="B21" s="191" t="s">
         <v>280</v>
       </c>
-      <c r="C21" s="317" t="s">
+      <c r="C21" s="298" t="s">
         <v>281</v>
       </c>
-      <c r="D21" s="317"/>
-      <c r="E21" s="317"/>
-      <c r="F21" s="317"/>
-      <c r="G21" s="317"/>
-      <c r="H21" s="317"/>
-      <c r="I21" s="317"/>
-      <c r="J21" s="317"/>
-      <c r="K21" s="318"/>
+      <c r="D21" s="298"/>
+      <c r="E21" s="298"/>
+      <c r="F21" s="298"/>
+      <c r="G21" s="298"/>
+      <c r="H21" s="298"/>
+      <c r="I21" s="298"/>
+      <c r="J21" s="298"/>
+      <c r="K21" s="299"/>
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="C18:K18"/>
-    <mergeCell ref="C19:K19"/>
-    <mergeCell ref="C20:K20"/>
-    <mergeCell ref="C21:K21"/>
-    <mergeCell ref="A17:A21"/>
-    <mergeCell ref="C17:K17"/>
     <mergeCell ref="I2:J2"/>
     <mergeCell ref="E2:F2"/>
     <mergeCell ref="A2:B2"/>
@@ -11413,6 +11529,12 @@
     <mergeCell ref="F11:G11"/>
     <mergeCell ref="F12:G12"/>
     <mergeCell ref="I9:K9"/>
+    <mergeCell ref="C18:K18"/>
+    <mergeCell ref="C19:K19"/>
+    <mergeCell ref="C20:K20"/>
+    <mergeCell ref="C21:K21"/>
+    <mergeCell ref="A17:A21"/>
+    <mergeCell ref="C17:K17"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -11424,7 +11546,7 @@
   <dimension ref="A1:I20"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13:G16"/>
+      <selection activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11438,16 +11560,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="324" t="s">
+      <c r="B1" s="316" t="s">
         <v>105</v>
       </c>
-      <c r="C1" s="324"/>
-      <c r="D1" s="324"/>
-      <c r="F1" s="324" t="s">
+      <c r="C1" s="316"/>
+      <c r="D1" s="316"/>
+      <c r="F1" s="316" t="s">
         <v>104</v>
       </c>
-      <c r="G1" s="324"/>
-      <c r="H1" s="324"/>
+      <c r="G1" s="316"/>
+      <c r="H1" s="316"/>
     </row>
     <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="36" t="s">
@@ -11476,10 +11598,10 @@
       <c r="D3" s="166" t="s">
         <v>53</v>
       </c>
-      <c r="F3" s="333" t="s">
+      <c r="F3" s="325" t="s">
         <v>94</v>
       </c>
-      <c r="G3" s="335" t="s">
+      <c r="G3" s="327" t="s">
         <v>93</v>
       </c>
       <c r="H3" s="172" t="s">
@@ -11496,8 +11618,8 @@
       <c r="D4" s="169" t="s">
         <v>53</v>
       </c>
-      <c r="F4" s="333"/>
-      <c r="G4" s="336"/>
+      <c r="F4" s="325"/>
+      <c r="G4" s="328"/>
       <c r="H4" s="173" t="s">
         <v>60</v>
       </c>
@@ -11512,8 +11634,8 @@
       <c r="D5" s="164" t="s">
         <v>54</v>
       </c>
-      <c r="F5" s="333"/>
-      <c r="G5" s="336"/>
+      <c r="F5" s="325"/>
+      <c r="G5" s="328"/>
       <c r="H5" s="174" t="s">
         <v>61</v>
       </c>
@@ -11528,8 +11650,8 @@
       <c r="D6" s="167" t="s">
         <v>55</v>
       </c>
-      <c r="F6" s="333"/>
-      <c r="G6" s="336"/>
+      <c r="F6" s="325"/>
+      <c r="G6" s="328"/>
       <c r="H6" s="179" t="s">
         <v>62</v>
       </c>
@@ -11544,8 +11666,8 @@
       <c r="D7" s="168" t="s">
         <v>55</v>
       </c>
-      <c r="F7" s="333"/>
-      <c r="G7" s="336"/>
+      <c r="F7" s="325"/>
+      <c r="G7" s="328"/>
       <c r="H7" s="178" t="s">
         <v>99</v>
       </c>
@@ -11560,8 +11682,8 @@
       <c r="D8" s="165" t="s">
         <v>54</v>
       </c>
-      <c r="F8" s="333"/>
-      <c r="G8" s="336"/>
+      <c r="F8" s="325"/>
+      <c r="G8" s="328"/>
       <c r="H8" s="175" t="s">
         <v>103</v>
       </c>
@@ -11576,8 +11698,8 @@
       <c r="D9" s="170" t="s">
         <v>55</v>
       </c>
-      <c r="F9" s="333"/>
-      <c r="G9" s="336"/>
+      <c r="F9" s="325"/>
+      <c r="G9" s="328"/>
       <c r="H9" s="176" t="s">
         <v>97</v>
       </c>
@@ -11592,21 +11714,21 @@
       <c r="D10" s="171" t="s">
         <v>55</v>
       </c>
-      <c r="F10" s="334"/>
-      <c r="G10" s="337"/>
+      <c r="F10" s="326"/>
+      <c r="G10" s="329"/>
       <c r="H10" s="177" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="12" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="328" t="s">
+      <c r="B12" s="320" t="s">
         <v>92</v>
       </c>
-      <c r="C12" s="329"/>
-      <c r="D12" s="329"/>
-      <c r="E12" s="329"/>
-      <c r="F12" s="330"/>
+      <c r="C12" s="321"/>
+      <c r="D12" s="321"/>
+      <c r="E12" s="321"/>
+      <c r="F12" s="322"/>
       <c r="G12" s="180" t="s">
         <v>56</v>
       </c>
@@ -11615,13 +11737,13 @@
       <c r="B13" s="181" t="s">
         <v>90</v>
       </c>
-      <c r="C13" s="338" t="s">
+      <c r="C13" s="330" t="s">
         <v>89</v>
       </c>
-      <c r="D13" s="338"/>
-      <c r="E13" s="338"/>
-      <c r="F13" s="339"/>
-      <c r="G13" s="325" t="s">
+      <c r="D13" s="330"/>
+      <c r="E13" s="330"/>
+      <c r="F13" s="331"/>
+      <c r="G13" s="317" t="s">
         <v>219</v>
       </c>
       <c r="I13" s="29"/>
@@ -11630,39 +11752,39 @@
       <c r="B14" s="182" t="s">
         <v>57</v>
       </c>
-      <c r="C14" s="340" t="s">
+      <c r="C14" s="332" t="s">
         <v>86</v>
       </c>
-      <c r="D14" s="340"/>
-      <c r="E14" s="340"/>
-      <c r="F14" s="341"/>
-      <c r="G14" s="326"/>
+      <c r="D14" s="332"/>
+      <c r="E14" s="332"/>
+      <c r="F14" s="333"/>
+      <c r="G14" s="318"/>
       <c r="I14" s="29"/>
     </row>
     <row r="15" spans="1:9" s="28" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="181" t="s">
         <v>58</v>
       </c>
-      <c r="C15" s="338" t="s">
+      <c r="C15" s="330" t="s">
         <v>87</v>
       </c>
-      <c r="D15" s="338"/>
-      <c r="E15" s="338"/>
-      <c r="F15" s="339"/>
-      <c r="G15" s="326"/>
+      <c r="D15" s="330"/>
+      <c r="E15" s="330"/>
+      <c r="F15" s="331"/>
+      <c r="G15" s="318"/>
       <c r="I15" s="29"/>
     </row>
     <row r="16" spans="1:9" s="28" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="183" t="s">
         <v>91</v>
       </c>
-      <c r="C16" s="331" t="s">
+      <c r="C16" s="323" t="s">
         <v>88</v>
       </c>
-      <c r="D16" s="331"/>
-      <c r="E16" s="331"/>
-      <c r="F16" s="332"/>
-      <c r="G16" s="327"/>
+      <c r="D16" s="323"/>
+      <c r="E16" s="323"/>
+      <c r="F16" s="324"/>
+      <c r="G16" s="319"/>
       <c r="I16" s="29"/>
     </row>
     <row r="17" spans="7:7" x14ac:dyDescent="0.25">
@@ -11701,7 +11823,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="4" topLeftCell="E1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="R12" sqref="R12"/>
+      <selection pane="topRight" activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11718,76 +11840,76 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="342" t="s">
+      <c r="A1" s="334" t="s">
         <v>220</v>
       </c>
-      <c r="B1" s="343"/>
-      <c r="C1" s="343"/>
-      <c r="D1" s="343"/>
-      <c r="F1" s="342" t="s">
+      <c r="B1" s="335"/>
+      <c r="C1" s="335"/>
+      <c r="D1" s="335"/>
+      <c r="F1" s="334" t="s">
         <v>222</v>
       </c>
-      <c r="G1" s="343"/>
-      <c r="H1" s="343"/>
-      <c r="I1" s="343"/>
-      <c r="J1" s="343"/>
-      <c r="K1" s="343"/>
-      <c r="L1" s="343"/>
-      <c r="M1" s="343"/>
-      <c r="N1" s="343"/>
-      <c r="O1" s="343"/>
-      <c r="P1" s="344"/>
-      <c r="R1" s="342" t="s">
+      <c r="G1" s="335"/>
+      <c r="H1" s="335"/>
+      <c r="I1" s="335"/>
+      <c r="J1" s="335"/>
+      <c r="K1" s="335"/>
+      <c r="L1" s="335"/>
+      <c r="M1" s="335"/>
+      <c r="N1" s="335"/>
+      <c r="O1" s="335"/>
+      <c r="P1" s="336"/>
+      <c r="R1" s="334" t="s">
         <v>223</v>
       </c>
-      <c r="S1" s="343"/>
-      <c r="T1" s="343"/>
-      <c r="U1" s="343"/>
-      <c r="V1" s="343"/>
-      <c r="W1" s="343"/>
-      <c r="X1" s="343"/>
-      <c r="Y1" s="343"/>
-      <c r="Z1" s="343"/>
-      <c r="AA1" s="344"/>
+      <c r="S1" s="335"/>
+      <c r="T1" s="335"/>
+      <c r="U1" s="335"/>
+      <c r="V1" s="335"/>
+      <c r="W1" s="335"/>
+      <c r="X1" s="335"/>
+      <c r="Y1" s="335"/>
+      <c r="Z1" s="335"/>
+      <c r="AA1" s="336"/>
     </row>
     <row r="2" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="349" t="s">
+      <c r="A2" s="341" t="s">
         <v>119</v>
       </c>
-      <c r="B2" s="348"/>
-      <c r="C2" s="348"/>
-      <c r="D2" s="348"/>
-      <c r="F2" s="345" t="s">
+      <c r="B2" s="340"/>
+      <c r="C2" s="340"/>
+      <c r="D2" s="340"/>
+      <c r="F2" s="337" t="s">
         <v>130</v>
       </c>
-      <c r="G2" s="347"/>
-      <c r="H2" s="347"/>
-      <c r="I2" s="347"/>
-      <c r="J2" s="347"/>
-      <c r="K2" s="347"/>
-      <c r="L2" s="347"/>
-      <c r="M2" s="346"/>
+      <c r="G2" s="339"/>
+      <c r="H2" s="339"/>
+      <c r="I2" s="339"/>
+      <c r="J2" s="339"/>
+      <c r="K2" s="339"/>
+      <c r="L2" s="339"/>
+      <c r="M2" s="338"/>
       <c r="N2" s="91" t="s">
         <v>106</v>
       </c>
-      <c r="O2" s="345" t="s">
+      <c r="O2" s="337" t="s">
         <v>107</v>
       </c>
-      <c r="P2" s="346"/>
-      <c r="R2" s="345" t="s">
+      <c r="P2" s="338"/>
+      <c r="R2" s="337" t="s">
         <v>130</v>
       </c>
-      <c r="S2" s="347"/>
-      <c r="T2" s="347"/>
-      <c r="U2" s="347"/>
-      <c r="V2" s="347"/>
-      <c r="W2" s="347"/>
-      <c r="X2" s="347"/>
-      <c r="Y2" s="346"/>
-      <c r="Z2" s="345" t="s">
+      <c r="S2" s="339"/>
+      <c r="T2" s="339"/>
+      <c r="U2" s="339"/>
+      <c r="V2" s="339"/>
+      <c r="W2" s="339"/>
+      <c r="X2" s="339"/>
+      <c r="Y2" s="338"/>
+      <c r="Z2" s="337" t="s">
         <v>107</v>
       </c>
-      <c r="AA2" s="346"/>
+      <c r="AA2" s="338"/>
     </row>
     <row r="3" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="38" t="s">
@@ -12048,12 +12170,12 @@
       </c>
     </row>
     <row r="7" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="348" t="s">
+      <c r="A7" s="340" t="s">
         <v>120</v>
       </c>
-      <c r="B7" s="348"/>
-      <c r="C7" s="348"/>
-      <c r="D7" s="348"/>
+      <c r="B7" s="340"/>
+      <c r="C7" s="340"/>
+      <c r="D7" s="340"/>
       <c r="F7" s="59">
         <v>1</v>
       </c>
@@ -12347,12 +12469,12 @@
       </c>
     </row>
     <row r="12" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A12" s="348" t="s">
+      <c r="A12" s="340" t="s">
         <v>125</v>
       </c>
-      <c r="B12" s="348"/>
-      <c r="C12" s="348"/>
-      <c r="D12" s="348"/>
+      <c r="B12" s="340"/>
+      <c r="C12" s="340"/>
+      <c r="D12" s="340"/>
       <c r="F12" s="58">
         <v>0</v>
       </c>
@@ -12601,7 +12723,7 @@
   <dimension ref="A1:AG26"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="9" ySplit="8" topLeftCell="T9" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="9" ySplit="8" topLeftCell="J15" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="J1" sqref="J1"/>
       <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
       <selection pane="bottomRight" activeCell="F29" sqref="F29"/>
@@ -12631,28 +12753,28 @@
       <c r="A1" s="94" t="s">
         <v>238</v>
       </c>
-      <c r="B1" s="355" t="s">
+      <c r="B1" s="342" t="s">
         <v>230</v>
       </c>
-      <c r="C1" s="355"/>
-      <c r="D1" s="355"/>
-      <c r="E1" s="356"/>
-      <c r="F1" s="355" t="s">
+      <c r="C1" s="342"/>
+      <c r="D1" s="342"/>
+      <c r="E1" s="343"/>
+      <c r="F1" s="342" t="s">
         <v>231</v>
       </c>
-      <c r="G1" s="355"/>
-      <c r="H1" s="355"/>
-      <c r="I1" s="355"/>
-      <c r="J1" s="355"/>
-      <c r="K1" s="355"/>
-      <c r="L1" s="355"/>
-      <c r="M1" s="355"/>
-      <c r="N1" s="357">
+      <c r="G1" s="342"/>
+      <c r="H1" s="342"/>
+      <c r="I1" s="342"/>
+      <c r="J1" s="342"/>
+      <c r="K1" s="342"/>
+      <c r="L1" s="342"/>
+      <c r="M1" s="342"/>
+      <c r="N1" s="344">
         <f>2^32</f>
         <v>4294967296</v>
       </c>
-      <c r="O1" s="357"/>
-      <c r="P1" s="357"/>
+      <c r="O1" s="344"/>
+      <c r="P1" s="344"/>
       <c r="Q1" s="162" t="s">
         <v>239</v>
       </c>
@@ -12661,34 +12783,34 @@
       <c r="A2" s="94" t="s">
         <v>156</v>
       </c>
-      <c r="B2" s="358" t="s">
+      <c r="B2" s="345" t="s">
         <v>225</v>
       </c>
-      <c r="C2" s="358"/>
-      <c r="D2" s="358" t="s">
+      <c r="C2" s="345"/>
+      <c r="D2" s="345" t="s">
         <v>130</v>
       </c>
-      <c r="E2" s="359"/>
-      <c r="F2" s="358" t="s">
+      <c r="E2" s="346"/>
+      <c r="F2" s="345" t="s">
         <v>225</v>
       </c>
-      <c r="G2" s="358"/>
-      <c r="H2" s="358" t="s">
+      <c r="G2" s="345"/>
+      <c r="H2" s="345" t="s">
         <v>130</v>
       </c>
-      <c r="I2" s="358"/>
-      <c r="J2" s="358" t="s">
+      <c r="I2" s="345"/>
+      <c r="J2" s="345" t="s">
         <v>226</v>
       </c>
-      <c r="K2" s="358"/>
-      <c r="L2" s="358"/>
-      <c r="M2" s="358"/>
-      <c r="N2" s="354" t="s">
+      <c r="K2" s="345"/>
+      <c r="L2" s="345"/>
+      <c r="M2" s="345"/>
+      <c r="N2" s="351" t="s">
         <v>265</v>
       </c>
-      <c r="O2" s="354"/>
-      <c r="P2" s="354"/>
-      <c r="Q2" s="354"/>
+      <c r="O2" s="351"/>
+      <c r="P2" s="351"/>
+      <c r="Q2" s="351"/>
     </row>
     <row r="3" spans="1:33" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="161" t="s">
@@ -12915,18 +13037,18 @@
       <c r="E7" s="152" t="s">
         <v>143</v>
       </c>
-      <c r="F7" s="350" t="s">
+      <c r="F7" s="347" t="s">
         <v>148</v>
       </c>
-      <c r="G7" s="351"/>
-      <c r="H7" s="351"/>
-      <c r="I7" s="351"/>
-      <c r="J7" s="350" t="s">
+      <c r="G7" s="348"/>
+      <c r="H7" s="348"/>
+      <c r="I7" s="348"/>
+      <c r="J7" s="347" t="s">
         <v>148</v>
       </c>
-      <c r="K7" s="351"/>
-      <c r="L7" s="351"/>
-      <c r="M7" s="351"/>
+      <c r="K7" s="348"/>
+      <c r="L7" s="348"/>
+      <c r="M7" s="348"/>
       <c r="N7" s="199" t="s">
         <v>134</v>
       </c>
@@ -12956,18 +13078,18 @@
       <c r="E8" s="154" t="s">
         <v>145</v>
       </c>
-      <c r="F8" s="352" t="s">
+      <c r="F8" s="349" t="s">
         <v>149</v>
       </c>
-      <c r="G8" s="353"/>
-      <c r="H8" s="353"/>
-      <c r="I8" s="353"/>
-      <c r="J8" s="352" t="s">
+      <c r="G8" s="350"/>
+      <c r="H8" s="350"/>
+      <c r="I8" s="350"/>
+      <c r="J8" s="349" t="s">
         <v>149</v>
       </c>
-      <c r="K8" s="353"/>
-      <c r="L8" s="353"/>
-      <c r="M8" s="353"/>
+      <c r="K8" s="350"/>
+      <c r="L8" s="350"/>
+      <c r="M8" s="350"/>
       <c r="N8" s="202" t="s">
         <v>135</v>
       </c>
@@ -13682,6 +13804,11 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="F7:I7"/>
+    <mergeCell ref="F8:I8"/>
+    <mergeCell ref="J7:M7"/>
+    <mergeCell ref="J8:M8"/>
+    <mergeCell ref="N2:Q2"/>
     <mergeCell ref="B1:E1"/>
     <mergeCell ref="F1:M1"/>
     <mergeCell ref="N1:P1"/>
@@ -13690,11 +13817,6 @@
     <mergeCell ref="F2:G2"/>
     <mergeCell ref="H2:I2"/>
     <mergeCell ref="D2:E2"/>
-    <mergeCell ref="F7:I7"/>
-    <mergeCell ref="F8:I8"/>
-    <mergeCell ref="J7:M7"/>
-    <mergeCell ref="J8:M8"/>
-    <mergeCell ref="N2:Q2"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -13727,45 +13849,45 @@
       <c r="A1" s="97" t="s">
         <v>166</v>
       </c>
-      <c r="B1" s="375">
+      <c r="B1" s="352">
         <f>2^128</f>
         <v>3.4028236692093846E+38</v>
       </c>
-      <c r="C1" s="375"/>
-      <c r="D1" s="375"/>
-      <c r="E1" s="375"/>
-      <c r="F1" s="375"/>
-      <c r="G1" s="375"/>
-      <c r="H1" s="375"/>
-      <c r="I1" s="375"/>
+      <c r="C1" s="352"/>
+      <c r="D1" s="352"/>
+      <c r="E1" s="352"/>
+      <c r="F1" s="352"/>
+      <c r="G1" s="352"/>
+      <c r="H1" s="352"/>
+      <c r="I1" s="352"/>
       <c r="J1" s="97" t="s">
         <v>240</v>
       </c>
-      <c r="K1" s="376" t="s">
+      <c r="K1" s="353" t="s">
         <v>229</v>
       </c>
-      <c r="L1" s="376"/>
-      <c r="M1" s="376"/>
-      <c r="N1" s="376"/>
+      <c r="L1" s="353"/>
+      <c r="M1" s="353"/>
+      <c r="N1" s="353"/>
     </row>
     <row r="2" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="120" t="s">
         <v>177</v>
       </c>
-      <c r="B2" s="377" t="s">
+      <c r="B2" s="354" t="s">
         <v>173</v>
       </c>
-      <c r="C2" s="378"/>
-      <c r="D2" s="378"/>
+      <c r="C2" s="355"/>
+      <c r="D2" s="355"/>
       <c r="E2" s="98" t="s">
         <v>253</v>
       </c>
-      <c r="F2" s="378" t="s">
+      <c r="F2" s="355" t="s">
         <v>174</v>
       </c>
-      <c r="G2" s="378"/>
-      <c r="H2" s="378"/>
-      <c r="I2" s="379"/>
+      <c r="G2" s="355"/>
+      <c r="H2" s="355"/>
+      <c r="I2" s="356"/>
       <c r="J2" s="99" t="s">
         <v>175</v>
       </c>
@@ -13886,11 +14008,11 @@
       <c r="E5" s="118" t="s">
         <v>182</v>
       </c>
-      <c r="F5" s="380" t="s">
+      <c r="F5" s="357" t="s">
         <v>184</v>
       </c>
-      <c r="G5" s="380"/>
-      <c r="H5" s="380"/>
+      <c r="G5" s="357"/>
+      <c r="H5" s="357"/>
       <c r="I5" s="119">
         <v>1</v>
       </c>
@@ -13920,12 +14042,12 @@
       <c r="B7" s="103" t="s">
         <v>263</v>
       </c>
-      <c r="C7" s="372" t="s">
+      <c r="C7" s="364" t="s">
         <v>248</v>
       </c>
-      <c r="D7" s="372"/>
-      <c r="E7" s="372"/>
-      <c r="F7" s="373"/>
+      <c r="D7" s="364"/>
+      <c r="E7" s="364"/>
+      <c r="F7" s="365"/>
       <c r="G7" s="127" t="s">
         <v>261</v>
       </c>
@@ -13940,10 +14062,10 @@
       <c r="C8" s="123" t="s">
         <v>262</v>
       </c>
-      <c r="D8" s="374" t="s">
+      <c r="D8" s="366" t="s">
         <v>249</v>
       </c>
-      <c r="E8" s="374"/>
+      <c r="E8" s="366"/>
       <c r="F8" s="121" t="s">
         <v>250</v>
       </c>
@@ -14002,114 +14124,114 @@
       <c r="A12" s="130" t="s">
         <v>263</v>
       </c>
-      <c r="B12" s="369" t="s">
+      <c r="B12" s="361" t="s">
         <v>248</v>
       </c>
-      <c r="C12" s="370"/>
-      <c r="D12" s="371"/>
-      <c r="E12" s="369" t="s">
+      <c r="C12" s="362"/>
+      <c r="D12" s="363"/>
+      <c r="E12" s="361" t="s">
         <v>264</v>
       </c>
-      <c r="F12" s="370"/>
-      <c r="G12" s="371"/>
+      <c r="F12" s="362"/>
+      <c r="G12" s="363"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="128" t="s">
         <v>188</v>
       </c>
-      <c r="B13" s="360" t="s">
+      <c r="B13" s="358" t="s">
         <v>190</v>
       </c>
-      <c r="C13" s="361"/>
-      <c r="D13" s="362"/>
-      <c r="E13" s="361" t="s">
+      <c r="C13" s="359"/>
+      <c r="D13" s="360"/>
+      <c r="E13" s="359" t="s">
         <v>191</v>
       </c>
-      <c r="F13" s="361"/>
-      <c r="G13" s="362"/>
+      <c r="F13" s="359"/>
+      <c r="G13" s="360"/>
       <c r="H13" s="37"/>
       <c r="I13" s="37"/>
       <c r="J13" s="37"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="129"/>
-      <c r="B14" s="363"/>
-      <c r="C14" s="364"/>
-      <c r="D14" s="365"/>
-      <c r="E14" s="364"/>
-      <c r="F14" s="364"/>
-      <c r="G14" s="365"/>
+      <c r="B14" s="367"/>
+      <c r="C14" s="368"/>
+      <c r="D14" s="369"/>
+      <c r="E14" s="368"/>
+      <c r="F14" s="368"/>
+      <c r="G14" s="369"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="128"/>
-      <c r="B15" s="360"/>
-      <c r="C15" s="361"/>
-      <c r="D15" s="362"/>
-      <c r="E15" s="361"/>
-      <c r="F15" s="361"/>
-      <c r="G15" s="362"/>
+      <c r="B15" s="358"/>
+      <c r="C15" s="359"/>
+      <c r="D15" s="360"/>
+      <c r="E15" s="359"/>
+      <c r="F15" s="359"/>
+      <c r="G15" s="360"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="129"/>
-      <c r="B16" s="363"/>
-      <c r="C16" s="364"/>
-      <c r="D16" s="365"/>
-      <c r="E16" s="364"/>
-      <c r="F16" s="364"/>
-      <c r="G16" s="365"/>
+      <c r="B16" s="367"/>
+      <c r="C16" s="368"/>
+      <c r="D16" s="369"/>
+      <c r="E16" s="368"/>
+      <c r="F16" s="368"/>
+      <c r="G16" s="369"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="128"/>
-      <c r="B17" s="360"/>
-      <c r="C17" s="361"/>
-      <c r="D17" s="362"/>
-      <c r="E17" s="361"/>
-      <c r="F17" s="361"/>
-      <c r="G17" s="362"/>
+      <c r="B17" s="358"/>
+      <c r="C17" s="359"/>
+      <c r="D17" s="360"/>
+      <c r="E17" s="359"/>
+      <c r="F17" s="359"/>
+      <c r="G17" s="360"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="129"/>
-      <c r="B18" s="363"/>
-      <c r="C18" s="364"/>
-      <c r="D18" s="365"/>
-      <c r="E18" s="364"/>
-      <c r="F18" s="364"/>
-      <c r="G18" s="365"/>
+      <c r="B18" s="367"/>
+      <c r="C18" s="368"/>
+      <c r="D18" s="369"/>
+      <c r="E18" s="368"/>
+      <c r="F18" s="368"/>
+      <c r="G18" s="369"/>
     </row>
     <row r="19" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="116"/>
-      <c r="B19" s="366"/>
-      <c r="C19" s="367"/>
-      <c r="D19" s="368"/>
-      <c r="E19" s="367"/>
-      <c r="F19" s="367"/>
-      <c r="G19" s="368"/>
+      <c r="B19" s="370"/>
+      <c r="C19" s="371"/>
+      <c r="D19" s="372"/>
+      <c r="E19" s="371"/>
+      <c r="F19" s="371"/>
+      <c r="G19" s="372"/>
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="B1:I1"/>
-    <mergeCell ref="K1:N1"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="F2:I2"/>
-    <mergeCell ref="F5:H5"/>
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="E17:G17"/>
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="E18:G18"/>
+    <mergeCell ref="B19:D19"/>
+    <mergeCell ref="E19:G19"/>
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="E14:G14"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="E15:G15"/>
+    <mergeCell ref="B16:D16"/>
+    <mergeCell ref="E16:G16"/>
     <mergeCell ref="B13:D13"/>
     <mergeCell ref="E13:G13"/>
     <mergeCell ref="B12:D12"/>
     <mergeCell ref="E12:G12"/>
     <mergeCell ref="C7:F7"/>
     <mergeCell ref="D8:E8"/>
-    <mergeCell ref="B14:D14"/>
-    <mergeCell ref="E14:G14"/>
-    <mergeCell ref="B15:D15"/>
-    <mergeCell ref="E15:G15"/>
-    <mergeCell ref="B16:D16"/>
-    <mergeCell ref="E16:G16"/>
-    <mergeCell ref="B17:D17"/>
-    <mergeCell ref="E17:G17"/>
-    <mergeCell ref="B18:D18"/>
-    <mergeCell ref="E18:G18"/>
-    <mergeCell ref="B19:D19"/>
-    <mergeCell ref="E19:G19"/>
+    <mergeCell ref="B1:I1"/>
+    <mergeCell ref="K1:N1"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="F2:I2"/>
+    <mergeCell ref="F5:H5"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -14124,7 +14246,7 @@
   <dimension ref="A1:P53"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="6" ySplit="3" topLeftCell="G4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="3" topLeftCell="G45" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
       <selection pane="bottomRight" activeCell="K2" sqref="K2"/>
@@ -14144,11 +14266,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="384" t="s">
+      <c r="A1" s="388" t="s">
         <v>320</v>
       </c>
-      <c r="B1" s="384"/>
-      <c r="C1" s="384"/>
+      <c r="B1" s="388"/>
+      <c r="C1" s="388"/>
       <c r="D1" s="226" t="s">
         <v>471</v>
       </c>
@@ -14176,11 +14298,11 @@
       <c r="P1" s="34"/>
     </row>
     <row r="2" spans="1:16" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="381" t="s">
+      <c r="A2" s="385" t="s">
         <v>470</v>
       </c>
-      <c r="B2" s="382"/>
-      <c r="C2" s="383"/>
+      <c r="B2" s="386"/>
+      <c r="C2" s="387"/>
       <c r="D2" s="230" t="s">
         <v>321</v>
       </c>
@@ -14193,7 +14315,7 @@
       <c r="G2" s="231" t="s">
         <v>111</v>
       </c>
-      <c r="H2" s="276">
+      <c r="H2" s="275">
         <v>20</v>
       </c>
       <c r="I2" s="231">
@@ -14264,21 +14386,21 @@
       <c r="F4" s="244" t="s">
         <v>326</v>
       </c>
-      <c r="G4" s="388" t="s">
+      <c r="G4" s="376" t="s">
         <v>108</v>
       </c>
-      <c r="H4" s="388">
+      <c r="H4" s="376">
         <v>3</v>
       </c>
-      <c r="I4" s="388">
+      <c r="I4" s="376">
         <f>IF(H4="","",IF(H4&lt;=2,1,IF(H4&lt;=4,2,IF(H4&lt;=8,3,IF(H4&lt;=16,4,IF(H4&lt;=32,5,IF(H4&lt;=64,6,IF(H4&lt;=128,7,8))))))))</f>
         <v>2</v>
       </c>
-      <c r="J4" s="388">
+      <c r="J4" s="376">
         <f>IF(G4="","",IF(G4="A",8+I4,IF(G4="B",16+I4,IF(G4="C",24+I4,"invalid"))))</f>
         <v>10</v>
       </c>
-      <c r="K4" s="385">
+      <c r="K4" s="379">
         <f>IF(J4="","",2^(32-J4))</f>
         <v>4194304</v>
       </c>
@@ -14302,11 +14424,11 @@
       <c r="F5" s="214" t="s">
         <v>326</v>
       </c>
-      <c r="G5" s="389"/>
-      <c r="H5" s="389"/>
-      <c r="I5" s="389"/>
-      <c r="J5" s="389"/>
-      <c r="K5" s="386"/>
+      <c r="G5" s="377"/>
+      <c r="H5" s="377"/>
+      <c r="I5" s="377"/>
+      <c r="J5" s="377"/>
+      <c r="K5" s="380"/>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="237" t="s">
@@ -14327,11 +14449,11 @@
       <c r="F6" s="212" t="s">
         <v>326</v>
       </c>
-      <c r="G6" s="389"/>
-      <c r="H6" s="389"/>
-      <c r="I6" s="389"/>
-      <c r="J6" s="389"/>
-      <c r="K6" s="386"/>
+      <c r="G6" s="377"/>
+      <c r="H6" s="377"/>
+      <c r="I6" s="377"/>
+      <c r="J6" s="377"/>
+      <c r="K6" s="380"/>
     </row>
     <row r="7" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="239" t="s">
@@ -14352,11 +14474,11 @@
       <c r="F7" s="241" t="s">
         <v>326</v>
       </c>
-      <c r="G7" s="390"/>
-      <c r="H7" s="390"/>
-      <c r="I7" s="390"/>
-      <c r="J7" s="390"/>
-      <c r="K7" s="387"/>
+      <c r="G7" s="378"/>
+      <c r="H7" s="378"/>
+      <c r="I7" s="378"/>
+      <c r="J7" s="378"/>
+      <c r="K7" s="381"/>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="242" t="s">
@@ -14377,21 +14499,21 @@
       <c r="F8" s="244" t="s">
         <v>389</v>
       </c>
-      <c r="G8" s="391" t="s">
+      <c r="G8" s="373" t="s">
         <v>109</v>
       </c>
-      <c r="H8" s="391">
+      <c r="H8" s="373">
         <v>5</v>
       </c>
-      <c r="I8" s="391">
+      <c r="I8" s="373">
         <f t="shared" ref="I8:I44" si="0">IF(H8="","",IF(H8&lt;=2,1,IF(H8&lt;=4,2,IF(H8&lt;=8,3,IF(H8&lt;=16,4,IF(H8&lt;=32,5,IF(H8&lt;=64,6,IF(H8&lt;=128,7,8))))))))</f>
         <v>3</v>
       </c>
-      <c r="J8" s="391">
+      <c r="J8" s="373">
         <f t="shared" ref="J8:J20" si="1">IF(G8="","",IF(G8="A",8+I8,IF(G8="B",16+I8,IF(G8="C",24+I8,"invalid"))))</f>
         <v>19</v>
       </c>
-      <c r="K8" s="394">
+      <c r="K8" s="382">
         <f t="shared" ref="K8:K44" si="2">IF(J8="","",2^(32-J8))</f>
         <v>8192</v>
       </c>
@@ -14415,11 +14537,11 @@
       <c r="F9" s="214" t="s">
         <v>389</v>
       </c>
-      <c r="G9" s="392"/>
-      <c r="H9" s="392"/>
-      <c r="I9" s="392"/>
-      <c r="J9" s="392"/>
-      <c r="K9" s="395"/>
+      <c r="G9" s="374"/>
+      <c r="H9" s="374"/>
+      <c r="I9" s="374"/>
+      <c r="J9" s="374"/>
+      <c r="K9" s="383"/>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="237" t="s">
@@ -14440,11 +14562,11 @@
       <c r="F10" s="212" t="s">
         <v>389</v>
       </c>
-      <c r="G10" s="392"/>
-      <c r="H10" s="392"/>
-      <c r="I10" s="392"/>
-      <c r="J10" s="392"/>
-      <c r="K10" s="395"/>
+      <c r="G10" s="374"/>
+      <c r="H10" s="374"/>
+      <c r="I10" s="374"/>
+      <c r="J10" s="374"/>
+      <c r="K10" s="383"/>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="238" t="s">
@@ -14465,11 +14587,11 @@
       <c r="F11" s="216" t="s">
         <v>389</v>
       </c>
-      <c r="G11" s="392"/>
-      <c r="H11" s="392"/>
-      <c r="I11" s="392"/>
-      <c r="J11" s="392"/>
-      <c r="K11" s="395"/>
+      <c r="G11" s="374"/>
+      <c r="H11" s="374"/>
+      <c r="I11" s="374"/>
+      <c r="J11" s="374"/>
+      <c r="K11" s="383"/>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="237" t="s">
@@ -14490,11 +14612,11 @@
       <c r="F12" s="212" t="s">
         <v>389</v>
       </c>
-      <c r="G12" s="392"/>
-      <c r="H12" s="392"/>
-      <c r="I12" s="392"/>
-      <c r="J12" s="392"/>
-      <c r="K12" s="395"/>
+      <c r="G12" s="374"/>
+      <c r="H12" s="374"/>
+      <c r="I12" s="374"/>
+      <c r="J12" s="374"/>
+      <c r="K12" s="383"/>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="236" t="s">
@@ -14515,11 +14637,11 @@
       <c r="F13" s="214" t="s">
         <v>389</v>
       </c>
-      <c r="G13" s="392"/>
-      <c r="H13" s="392"/>
-      <c r="I13" s="392"/>
-      <c r="J13" s="392"/>
-      <c r="K13" s="395"/>
+      <c r="G13" s="374"/>
+      <c r="H13" s="374"/>
+      <c r="I13" s="374"/>
+      <c r="J13" s="374"/>
+      <c r="K13" s="383"/>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="237" t="s">
@@ -14540,11 +14662,11 @@
       <c r="F14" s="212" t="s">
         <v>389</v>
       </c>
-      <c r="G14" s="392"/>
-      <c r="H14" s="392"/>
-      <c r="I14" s="392"/>
-      <c r="J14" s="392"/>
-      <c r="K14" s="395"/>
+      <c r="G14" s="374"/>
+      <c r="H14" s="374"/>
+      <c r="I14" s="374"/>
+      <c r="J14" s="374"/>
+      <c r="K14" s="383"/>
     </row>
     <row r="15" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="239" t="s">
@@ -14565,11 +14687,11 @@
       <c r="F15" s="241" t="s">
         <v>389</v>
       </c>
-      <c r="G15" s="393"/>
-      <c r="H15" s="393"/>
-      <c r="I15" s="393"/>
-      <c r="J15" s="393"/>
-      <c r="K15" s="396"/>
+      <c r="G15" s="375"/>
+      <c r="H15" s="375"/>
+      <c r="I15" s="375"/>
+      <c r="J15" s="375"/>
+      <c r="K15" s="384"/>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="242" t="s">
@@ -14590,21 +14712,21 @@
       <c r="F16" s="245">
         <v>255255255192</v>
       </c>
-      <c r="G16" s="388" t="s">
+      <c r="G16" s="376" t="s">
         <v>111</v>
       </c>
-      <c r="H16" s="388">
+      <c r="H16" s="376">
         <v>4</v>
       </c>
-      <c r="I16" s="388">
+      <c r="I16" s="376">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="J16" s="388">
+      <c r="J16" s="376">
         <f t="shared" si="1"/>
         <v>26</v>
       </c>
-      <c r="K16" s="385">
+      <c r="K16" s="379">
         <f t="shared" si="2"/>
         <v>64</v>
       </c>
@@ -14628,11 +14750,11 @@
       <c r="F17" s="225">
         <v>255255255192</v>
       </c>
-      <c r="G17" s="389"/>
-      <c r="H17" s="389"/>
-      <c r="I17" s="389"/>
-      <c r="J17" s="389"/>
-      <c r="K17" s="386"/>
+      <c r="G17" s="377"/>
+      <c r="H17" s="377"/>
+      <c r="I17" s="377"/>
+      <c r="J17" s="377"/>
+      <c r="K17" s="380"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="237" t="s">
@@ -14653,11 +14775,11 @@
       <c r="F18" s="224">
         <v>255255255192</v>
       </c>
-      <c r="G18" s="389"/>
-      <c r="H18" s="389"/>
-      <c r="I18" s="389"/>
-      <c r="J18" s="389"/>
-      <c r="K18" s="386"/>
+      <c r="G18" s="377"/>
+      <c r="H18" s="377"/>
+      <c r="I18" s="377"/>
+      <c r="J18" s="377"/>
+      <c r="K18" s="380"/>
     </row>
     <row r="19" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="239" t="s">
@@ -14678,11 +14800,11 @@
       <c r="F19" s="246">
         <v>255255255192</v>
       </c>
-      <c r="G19" s="390"/>
-      <c r="H19" s="390"/>
-      <c r="I19" s="390"/>
-      <c r="J19" s="390"/>
-      <c r="K19" s="387"/>
+      <c r="G19" s="378"/>
+      <c r="H19" s="378"/>
+      <c r="I19" s="378"/>
+      <c r="J19" s="378"/>
+      <c r="K19" s="381"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="242" t="s">
@@ -14703,21 +14825,21 @@
       <c r="F20" s="244" t="s">
         <v>440</v>
       </c>
-      <c r="G20" s="391" t="s">
+      <c r="G20" s="373" t="s">
         <v>108</v>
       </c>
-      <c r="H20" s="391">
+      <c r="H20" s="373">
         <v>20</v>
       </c>
-      <c r="I20" s="391">
+      <c r="I20" s="373">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="J20" s="391">
+      <c r="J20" s="373">
         <f t="shared" si="1"/>
         <v>13</v>
       </c>
-      <c r="K20" s="394">
+      <c r="K20" s="382">
         <f t="shared" si="2"/>
         <v>524288</v>
       </c>
@@ -14741,11 +14863,11 @@
       <c r="F21" s="214" t="s">
         <v>440</v>
       </c>
-      <c r="G21" s="392"/>
-      <c r="H21" s="392"/>
-      <c r="I21" s="392"/>
-      <c r="J21" s="392"/>
-      <c r="K21" s="395"/>
+      <c r="G21" s="374"/>
+      <c r="H21" s="374"/>
+      <c r="I21" s="374"/>
+      <c r="J21" s="374"/>
+      <c r="K21" s="383"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="237" t="s">
@@ -14766,11 +14888,11 @@
       <c r="F22" s="212" t="s">
         <v>440</v>
       </c>
-      <c r="G22" s="392"/>
-      <c r="H22" s="392"/>
-      <c r="I22" s="392"/>
-      <c r="J22" s="392"/>
-      <c r="K22" s="395"/>
+      <c r="G22" s="374"/>
+      <c r="H22" s="374"/>
+      <c r="I22" s="374"/>
+      <c r="J22" s="374"/>
+      <c r="K22" s="383"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="238" t="s">
@@ -14791,11 +14913,11 @@
       <c r="F23" s="216" t="s">
         <v>440</v>
       </c>
-      <c r="G23" s="392"/>
-      <c r="H23" s="392"/>
-      <c r="I23" s="392"/>
-      <c r="J23" s="392"/>
-      <c r="K23" s="395"/>
+      <c r="G23" s="374"/>
+      <c r="H23" s="374"/>
+      <c r="I23" s="374"/>
+      <c r="J23" s="374"/>
+      <c r="K23" s="383"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="237" t="s">
@@ -14816,11 +14938,11 @@
       <c r="F24" s="212" t="s">
         <v>440</v>
       </c>
-      <c r="G24" s="392"/>
-      <c r="H24" s="392"/>
-      <c r="I24" s="392"/>
-      <c r="J24" s="392"/>
-      <c r="K24" s="395"/>
+      <c r="G24" s="374"/>
+      <c r="H24" s="374"/>
+      <c r="I24" s="374"/>
+      <c r="J24" s="374"/>
+      <c r="K24" s="383"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="236" t="s">
@@ -14841,11 +14963,11 @@
       <c r="F25" s="214" t="s">
         <v>440</v>
       </c>
-      <c r="G25" s="392"/>
-      <c r="H25" s="392"/>
-      <c r="I25" s="392"/>
-      <c r="J25" s="392"/>
-      <c r="K25" s="395"/>
+      <c r="G25" s="374"/>
+      <c r="H25" s="374"/>
+      <c r="I25" s="374"/>
+      <c r="J25" s="374"/>
+      <c r="K25" s="383"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="237" t="s">
@@ -14866,11 +14988,11 @@
       <c r="F26" s="212" t="s">
         <v>440</v>
       </c>
-      <c r="G26" s="392"/>
-      <c r="H26" s="392"/>
-      <c r="I26" s="392"/>
-      <c r="J26" s="392"/>
-      <c r="K26" s="395"/>
+      <c r="G26" s="374"/>
+      <c r="H26" s="374"/>
+      <c r="I26" s="374"/>
+      <c r="J26" s="374"/>
+      <c r="K26" s="383"/>
     </row>
     <row r="27" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="239" t="s">
@@ -14891,11 +15013,11 @@
       <c r="F27" s="241" t="s">
         <v>440</v>
       </c>
-      <c r="G27" s="393"/>
-      <c r="H27" s="393"/>
-      <c r="I27" s="393"/>
-      <c r="J27" s="393"/>
-      <c r="K27" s="396"/>
+      <c r="G27" s="375"/>
+      <c r="H27" s="375"/>
+      <c r="I27" s="375"/>
+      <c r="J27" s="375"/>
+      <c r="K27" s="384"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="242" t="s">
@@ -14916,21 +15038,21 @@
       <c r="F28" s="244" t="s">
         <v>440</v>
       </c>
-      <c r="G28" s="388" t="s">
+      <c r="G28" s="376" t="s">
         <v>108</v>
       </c>
-      <c r="H28" s="388">
+      <c r="H28" s="376">
         <v>20</v>
       </c>
-      <c r="I28" s="388">
+      <c r="I28" s="376">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="J28" s="388">
+      <c r="J28" s="376">
         <f t="shared" ref="J28" si="3">IF(G28="","",IF(G28="A",8+I28,IF(G28="B",16+I28,IF(G28="C",24+I28,"invalid"))))</f>
         <v>13</v>
       </c>
-      <c r="K28" s="385">
+      <c r="K28" s="379">
         <f t="shared" si="2"/>
         <v>524288</v>
       </c>
@@ -14954,11 +15076,11 @@
       <c r="F29" s="214" t="s">
         <v>440</v>
       </c>
-      <c r="G29" s="389"/>
-      <c r="H29" s="389"/>
-      <c r="I29" s="389"/>
-      <c r="J29" s="389"/>
-      <c r="K29" s="386"/>
+      <c r="G29" s="377"/>
+      <c r="H29" s="377"/>
+      <c r="I29" s="377"/>
+      <c r="J29" s="377"/>
+      <c r="K29" s="380"/>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="237" t="s">
@@ -14979,11 +15101,11 @@
       <c r="F30" s="212" t="s">
         <v>440</v>
       </c>
-      <c r="G30" s="389"/>
-      <c r="H30" s="389"/>
-      <c r="I30" s="389"/>
-      <c r="J30" s="389"/>
-      <c r="K30" s="386"/>
+      <c r="G30" s="377"/>
+      <c r="H30" s="377"/>
+      <c r="I30" s="377"/>
+      <c r="J30" s="377"/>
+      <c r="K30" s="380"/>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="238" t="s">
@@ -15004,11 +15126,11 @@
       <c r="F31" s="216" t="s">
         <v>440</v>
       </c>
-      <c r="G31" s="389"/>
-      <c r="H31" s="389"/>
-      <c r="I31" s="389"/>
-      <c r="J31" s="389"/>
-      <c r="K31" s="386"/>
+      <c r="G31" s="377"/>
+      <c r="H31" s="377"/>
+      <c r="I31" s="377"/>
+      <c r="J31" s="377"/>
+      <c r="K31" s="380"/>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="237" t="s">
@@ -15029,11 +15151,11 @@
       <c r="F32" s="212" t="s">
         <v>440</v>
       </c>
-      <c r="G32" s="389"/>
-      <c r="H32" s="389"/>
-      <c r="I32" s="389"/>
-      <c r="J32" s="389"/>
-      <c r="K32" s="386"/>
+      <c r="G32" s="377"/>
+      <c r="H32" s="377"/>
+      <c r="I32" s="377"/>
+      <c r="J32" s="377"/>
+      <c r="K32" s="380"/>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="236" t="s">
@@ -15054,11 +15176,11 @@
       <c r="F33" s="214" t="s">
         <v>440</v>
       </c>
-      <c r="G33" s="389"/>
-      <c r="H33" s="389"/>
-      <c r="I33" s="389"/>
-      <c r="J33" s="389"/>
-      <c r="K33" s="386"/>
+      <c r="G33" s="377"/>
+      <c r="H33" s="377"/>
+      <c r="I33" s="377"/>
+      <c r="J33" s="377"/>
+      <c r="K33" s="380"/>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="237" t="s">
@@ -15079,11 +15201,11 @@
       <c r="F34" s="212" t="s">
         <v>440</v>
       </c>
-      <c r="G34" s="389"/>
-      <c r="H34" s="389"/>
-      <c r="I34" s="389"/>
-      <c r="J34" s="389"/>
-      <c r="K34" s="386"/>
+      <c r="G34" s="377"/>
+      <c r="H34" s="377"/>
+      <c r="I34" s="377"/>
+      <c r="J34" s="377"/>
+      <c r="K34" s="380"/>
     </row>
     <row r="35" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="239" t="s">
@@ -15104,11 +15226,11 @@
       <c r="F35" s="241" t="s">
         <v>440</v>
       </c>
-      <c r="G35" s="390"/>
-      <c r="H35" s="390"/>
-      <c r="I35" s="390"/>
-      <c r="J35" s="390"/>
-      <c r="K35" s="387"/>
+      <c r="G35" s="378"/>
+      <c r="H35" s="378"/>
+      <c r="I35" s="378"/>
+      <c r="J35" s="378"/>
+      <c r="K35" s="381"/>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="242" t="s">
@@ -15129,21 +15251,21 @@
       <c r="F36" s="244" t="s">
         <v>440</v>
       </c>
-      <c r="G36" s="391" t="s">
+      <c r="G36" s="373" t="s">
         <v>108</v>
       </c>
-      <c r="H36" s="391">
+      <c r="H36" s="373">
         <v>20</v>
       </c>
-      <c r="I36" s="391">
+      <c r="I36" s="373">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="J36" s="391">
+      <c r="J36" s="373">
         <f t="shared" ref="J36" si="4">IF(G36="","",IF(G36="A",8+I36,IF(G36="B",16+I36,IF(G36="C",24+I36,"invalid"))))</f>
         <v>13</v>
       </c>
-      <c r="K36" s="394">
+      <c r="K36" s="382">
         <f t="shared" si="2"/>
         <v>524288</v>
       </c>
@@ -15167,11 +15289,11 @@
       <c r="F37" s="214" t="s">
         <v>440</v>
       </c>
-      <c r="G37" s="392"/>
-      <c r="H37" s="392"/>
-      <c r="I37" s="392"/>
-      <c r="J37" s="392"/>
-      <c r="K37" s="395"/>
+      <c r="G37" s="374"/>
+      <c r="H37" s="374"/>
+      <c r="I37" s="374"/>
+      <c r="J37" s="374"/>
+      <c r="K37" s="383"/>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="237" t="s">
@@ -15192,11 +15314,11 @@
       <c r="F38" s="212" t="s">
         <v>440</v>
       </c>
-      <c r="G38" s="392"/>
-      <c r="H38" s="392"/>
-      <c r="I38" s="392"/>
-      <c r="J38" s="392"/>
-      <c r="K38" s="395"/>
+      <c r="G38" s="374"/>
+      <c r="H38" s="374"/>
+      <c r="I38" s="374"/>
+      <c r="J38" s="374"/>
+      <c r="K38" s="383"/>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="238" t="s">
@@ -15217,11 +15339,11 @@
       <c r="F39" s="216" t="s">
         <v>440</v>
       </c>
-      <c r="G39" s="392"/>
-      <c r="H39" s="392"/>
-      <c r="I39" s="392"/>
-      <c r="J39" s="392"/>
-      <c r="K39" s="395"/>
+      <c r="G39" s="374"/>
+      <c r="H39" s="374"/>
+      <c r="I39" s="374"/>
+      <c r="J39" s="374"/>
+      <c r="K39" s="383"/>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" s="237" t="s">
@@ -15242,11 +15364,11 @@
       <c r="F40" s="212" t="s">
         <v>440</v>
       </c>
-      <c r="G40" s="392"/>
-      <c r="H40" s="392"/>
-      <c r="I40" s="392"/>
-      <c r="J40" s="392"/>
-      <c r="K40" s="395"/>
+      <c r="G40" s="374"/>
+      <c r="H40" s="374"/>
+      <c r="I40" s="374"/>
+      <c r="J40" s="374"/>
+      <c r="K40" s="383"/>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" s="236" t="s">
@@ -15267,11 +15389,11 @@
       <c r="F41" s="214" t="s">
         <v>440</v>
       </c>
-      <c r="G41" s="392"/>
-      <c r="H41" s="392"/>
-      <c r="I41" s="392"/>
-      <c r="J41" s="392"/>
-      <c r="K41" s="395"/>
+      <c r="G41" s="374"/>
+      <c r="H41" s="374"/>
+      <c r="I41" s="374"/>
+      <c r="J41" s="374"/>
+      <c r="K41" s="383"/>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" s="237" t="s">
@@ -15292,11 +15414,11 @@
       <c r="F42" s="212" t="s">
         <v>440</v>
       </c>
-      <c r="G42" s="392"/>
-      <c r="H42" s="392"/>
-      <c r="I42" s="392"/>
-      <c r="J42" s="392"/>
-      <c r="K42" s="395"/>
+      <c r="G42" s="374"/>
+      <c r="H42" s="374"/>
+      <c r="I42" s="374"/>
+      <c r="J42" s="374"/>
+      <c r="K42" s="383"/>
     </row>
     <row r="43" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="239" t="s">
@@ -15317,11 +15439,11 @@
       <c r="F43" s="241" t="s">
         <v>440</v>
       </c>
-      <c r="G43" s="393"/>
-      <c r="H43" s="393"/>
-      <c r="I43" s="393"/>
-      <c r="J43" s="393"/>
-      <c r="K43" s="396"/>
+      <c r="G43" s="375"/>
+      <c r="H43" s="375"/>
+      <c r="I43" s="375"/>
+      <c r="J43" s="375"/>
+      <c r="K43" s="384"/>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="242" t="s">
@@ -15342,21 +15464,21 @@
       <c r="F44" s="244" t="s">
         <v>440</v>
       </c>
-      <c r="G44" s="388" t="s">
+      <c r="G44" s="376" t="s">
         <v>108</v>
       </c>
-      <c r="H44" s="388">
+      <c r="H44" s="376">
         <v>20</v>
       </c>
-      <c r="I44" s="388">
+      <c r="I44" s="376">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="J44" s="388">
+      <c r="J44" s="376">
         <f t="shared" ref="J44" si="5">IF(G44="","",IF(G44="A",8+I44,IF(G44="B",16+I44,IF(G44="C",24+I44,"invalid"))))</f>
         <v>13</v>
       </c>
-      <c r="K44" s="385">
+      <c r="K44" s="379">
         <f t="shared" si="2"/>
         <v>524288</v>
       </c>
@@ -15380,11 +15502,11 @@
       <c r="F45" s="214" t="s">
         <v>440</v>
       </c>
-      <c r="G45" s="389"/>
-      <c r="H45" s="389"/>
-      <c r="I45" s="389"/>
-      <c r="J45" s="389"/>
-      <c r="K45" s="386"/>
+      <c r="G45" s="377"/>
+      <c r="H45" s="377"/>
+      <c r="I45" s="377"/>
+      <c r="J45" s="377"/>
+      <c r="K45" s="380"/>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" s="237" t="s">
@@ -15405,11 +15527,11 @@
       <c r="F46" s="212" t="s">
         <v>440</v>
       </c>
-      <c r="G46" s="389"/>
-      <c r="H46" s="389"/>
-      <c r="I46" s="389"/>
-      <c r="J46" s="389"/>
-      <c r="K46" s="386"/>
+      <c r="G46" s="377"/>
+      <c r="H46" s="377"/>
+      <c r="I46" s="377"/>
+      <c r="J46" s="377"/>
+      <c r="K46" s="380"/>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" s="238" t="s">
@@ -15430,11 +15552,11 @@
       <c r="F47" s="216" t="s">
         <v>440</v>
       </c>
-      <c r="G47" s="389"/>
-      <c r="H47" s="389"/>
-      <c r="I47" s="389"/>
-      <c r="J47" s="389"/>
-      <c r="K47" s="386"/>
+      <c r="G47" s="377"/>
+      <c r="H47" s="377"/>
+      <c r="I47" s="377"/>
+      <c r="J47" s="377"/>
+      <c r="K47" s="380"/>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" s="237" t="s">
@@ -15455,11 +15577,11 @@
       <c r="F48" s="212" t="s">
         <v>440</v>
       </c>
-      <c r="G48" s="389"/>
-      <c r="H48" s="389"/>
-      <c r="I48" s="389"/>
-      <c r="J48" s="389"/>
-      <c r="K48" s="386"/>
+      <c r="G48" s="377"/>
+      <c r="H48" s="377"/>
+      <c r="I48" s="377"/>
+      <c r="J48" s="377"/>
+      <c r="K48" s="380"/>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" s="236" t="s">
@@ -15480,11 +15602,11 @@
       <c r="F49" s="214" t="s">
         <v>440</v>
       </c>
-      <c r="G49" s="389"/>
-      <c r="H49" s="389"/>
-      <c r="I49" s="389"/>
-      <c r="J49" s="389"/>
-      <c r="K49" s="386"/>
+      <c r="G49" s="377"/>
+      <c r="H49" s="377"/>
+      <c r="I49" s="377"/>
+      <c r="J49" s="377"/>
+      <c r="K49" s="380"/>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" s="237" t="s">
@@ -15505,11 +15627,11 @@
       <c r="F50" s="212" t="s">
         <v>440</v>
       </c>
-      <c r="G50" s="389"/>
-      <c r="H50" s="389"/>
-      <c r="I50" s="389"/>
-      <c r="J50" s="389"/>
-      <c r="K50" s="386"/>
+      <c r="G50" s="377"/>
+      <c r="H50" s="377"/>
+      <c r="I50" s="377"/>
+      <c r="J50" s="377"/>
+      <c r="K50" s="380"/>
     </row>
     <row r="51" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="239" t="s">
@@ -15530,11 +15652,11 @@
       <c r="F51" s="241" t="s">
         <v>440</v>
       </c>
-      <c r="G51" s="390"/>
-      <c r="H51" s="390"/>
-      <c r="I51" s="390"/>
-      <c r="J51" s="390"/>
-      <c r="K51" s="387"/>
+      <c r="G51" s="378"/>
+      <c r="H51" s="378"/>
+      <c r="I51" s="378"/>
+      <c r="J51" s="378"/>
+      <c r="K51" s="381"/>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="G52" s="229"/>
@@ -15544,27 +15666,13 @@
     </row>
   </sheetData>
   <mergeCells count="37">
-    <mergeCell ref="H36:H43"/>
-    <mergeCell ref="H44:H51"/>
-    <mergeCell ref="I44:I51"/>
-    <mergeCell ref="J44:J51"/>
-    <mergeCell ref="K44:K51"/>
-    <mergeCell ref="K36:K43"/>
-    <mergeCell ref="J36:J43"/>
-    <mergeCell ref="I36:I43"/>
-    <mergeCell ref="H20:H27"/>
-    <mergeCell ref="I20:I27"/>
-    <mergeCell ref="J20:J27"/>
-    <mergeCell ref="K20:K27"/>
-    <mergeCell ref="H28:H35"/>
-    <mergeCell ref="I28:I35"/>
-    <mergeCell ref="J28:J35"/>
-    <mergeCell ref="K28:K35"/>
-    <mergeCell ref="G20:G27"/>
-    <mergeCell ref="G28:G35"/>
-    <mergeCell ref="G36:G43"/>
-    <mergeCell ref="G44:G51"/>
-    <mergeCell ref="G16:G19"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="K4:K7"/>
+    <mergeCell ref="J4:J7"/>
+    <mergeCell ref="I4:I7"/>
+    <mergeCell ref="H4:H7"/>
+    <mergeCell ref="G4:G7"/>
     <mergeCell ref="H16:H19"/>
     <mergeCell ref="I16:I19"/>
     <mergeCell ref="J16:J19"/>
@@ -15574,13 +15682,27 @@
     <mergeCell ref="I8:I15"/>
     <mergeCell ref="J8:J15"/>
     <mergeCell ref="K8:K15"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="K4:K7"/>
-    <mergeCell ref="J4:J7"/>
-    <mergeCell ref="I4:I7"/>
-    <mergeCell ref="H4:H7"/>
-    <mergeCell ref="G4:G7"/>
+    <mergeCell ref="G20:G27"/>
+    <mergeCell ref="G28:G35"/>
+    <mergeCell ref="G36:G43"/>
+    <mergeCell ref="G44:G51"/>
+    <mergeCell ref="G16:G19"/>
+    <mergeCell ref="H20:H27"/>
+    <mergeCell ref="I20:I27"/>
+    <mergeCell ref="J20:J27"/>
+    <mergeCell ref="K20:K27"/>
+    <mergeCell ref="H28:H35"/>
+    <mergeCell ref="I28:I35"/>
+    <mergeCell ref="J28:J35"/>
+    <mergeCell ref="K28:K35"/>
+    <mergeCell ref="H36:H43"/>
+    <mergeCell ref="H44:H51"/>
+    <mergeCell ref="I44:I51"/>
+    <mergeCell ref="J44:J51"/>
+    <mergeCell ref="K44:K51"/>
+    <mergeCell ref="K36:K43"/>
+    <mergeCell ref="J36:J43"/>
+    <mergeCell ref="I36:I43"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -15629,11 +15751,11 @@
       <c r="A1" t="s">
         <v>392</v>
       </c>
-      <c r="G1" s="384" t="s">
+      <c r="G1" s="388" t="s">
         <v>574</v>
       </c>
-      <c r="H1" s="384"/>
-      <c r="I1" s="384"/>
+      <c r="H1" s="388"/>
+      <c r="I1" s="388"/>
       <c r="J1" s="226" t="s">
         <v>471</v>
       </c>
@@ -15663,17 +15785,17 @@
       </c>
     </row>
     <row r="2" spans="1:29" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="403"/>
-      <c r="B2" s="403"/>
-      <c r="C2" s="403"/>
-      <c r="D2" s="403"/>
-      <c r="E2" s="403"/>
-      <c r="F2" s="403"/>
-      <c r="G2" s="381" t="s">
+      <c r="A2" s="395"/>
+      <c r="B2" s="395"/>
+      <c r="C2" s="395"/>
+      <c r="D2" s="395"/>
+      <c r="E2" s="395"/>
+      <c r="F2" s="395"/>
+      <c r="G2" s="385" t="s">
         <v>575</v>
       </c>
-      <c r="H2" s="382"/>
-      <c r="I2" s="383"/>
+      <c r="H2" s="386"/>
+      <c r="I2" s="387"/>
       <c r="J2" s="230" t="s">
         <v>445</v>
       </c>
@@ -15810,7 +15932,7 @@
         <f>IF(O4="","",32-O4)</f>
         <v>25</v>
       </c>
-      <c r="R4" s="400" t="s">
+      <c r="R4" s="392" t="s">
         <v>612</v>
       </c>
     </row>
@@ -15863,7 +15985,7 @@
         <f t="shared" ref="Q5:Q8" si="2">IF(O5="","",32-O5)</f>
         <v>26</v>
       </c>
-      <c r="R5" s="401"/>
+      <c r="R5" s="393"/>
     </row>
     <row r="6" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -15914,7 +16036,7 @@
         <f t="shared" si="2"/>
         <v>26</v>
       </c>
-      <c r="R6" s="401"/>
+      <c r="R6" s="393"/>
       <c r="AC6" s="33"/>
     </row>
     <row r="7" spans="1:29" x14ac:dyDescent="0.25">
@@ -15966,7 +16088,7 @@
         <f t="shared" si="2"/>
         <v>27</v>
       </c>
-      <c r="R7" s="401"/>
+      <c r="R7" s="393"/>
       <c r="AC7" s="33"/>
     </row>
     <row r="8" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -16018,7 +16140,7 @@
         <f t="shared" si="2"/>
         <v>29</v>
       </c>
-      <c r="R8" s="402"/>
+      <c r="R8" s="394"/>
       <c r="AC8" s="33"/>
     </row>
     <row r="9" spans="1:29" x14ac:dyDescent="0.25">
@@ -16061,7 +16183,7 @@
         <f>IF(O9="","",32-O9)</f>
         <v>25</v>
       </c>
-      <c r="R9" s="397" t="s">
+      <c r="R9" s="389" t="s">
         <v>613</v>
       </c>
       <c r="AC9" s="33"/>
@@ -16103,7 +16225,7 @@
         <f>IF(O10="","",32-O10)</f>
         <v>26</v>
       </c>
-      <c r="R10" s="398"/>
+      <c r="R10" s="390"/>
       <c r="AC10" s="33"/>
     </row>
     <row r="11" spans="1:29" x14ac:dyDescent="0.25">
@@ -16161,7 +16283,7 @@
         <f>IF(O11="","",32-O11)</f>
         <v>27</v>
       </c>
-      <c r="R11" s="398"/>
+      <c r="R11" s="390"/>
     </row>
     <row r="12" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
@@ -16218,7 +16340,7 @@
         <f>IF(O12="","",32-O12)</f>
         <v>29</v>
       </c>
-      <c r="R12" s="398"/>
+      <c r="R12" s="390"/>
     </row>
     <row r="13" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
@@ -16275,7 +16397,7 @@
         <f>IF(O13="","",32-O13)</f>
         <v>26</v>
       </c>
-      <c r="R13" s="399"/>
+      <c r="R13" s="391"/>
     </row>
     <row r="14" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
@@ -16353,72 +16475,196 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCF9BCDD-FD43-410A-9645-E36DC57C747A}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="3" width="6.28515625" style="222" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="35.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.140625" style="222" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.42578125" style="222" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="2.7109375" customWidth="1"/>
+    <col min="5" max="5" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="26.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="404" t="s">
+    <row r="1" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="403" t="s">
+        <v>658</v>
+      </c>
+      <c r="B1" s="404" t="s">
+        <v>656</v>
+      </c>
+      <c r="C1" s="404" t="s">
+        <v>657</v>
+      </c>
+      <c r="E1" s="316" t="s">
+        <v>662</v>
+      </c>
+      <c r="F1" s="316"/>
+      <c r="G1" s="316"/>
+      <c r="H1" s="316"/>
+    </row>
+    <row r="2" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="411" t="s">
+        <v>675</v>
+      </c>
+      <c r="B2" s="412" t="s">
+        <v>676</v>
+      </c>
+      <c r="C2" s="412" t="s">
+        <v>677</v>
+      </c>
+      <c r="E2" s="403" t="s">
         <v>646</v>
       </c>
-      <c r="B1" s="275" t="s">
+      <c r="F2" s="404" t="s">
         <v>647</v>
       </c>
-      <c r="C1" s="275" t="s">
+      <c r="G2" s="404" t="s">
         <v>228</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="405" t="s">
+      <c r="H2" s="403" t="s">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="413" t="s">
+        <v>668</v>
+      </c>
+      <c r="B3" s="414" t="s">
+        <v>666</v>
+      </c>
+      <c r="C3" s="414" t="s">
+        <v>667</v>
+      </c>
+      <c r="E3" s="408" t="s">
         <v>644</v>
       </c>
-      <c r="B2" s="406">
+      <c r="F3" s="405">
         <v>0</v>
       </c>
-      <c r="C2" s="406">
+      <c r="G3" s="405">
         <v>1023</v>
       </c>
-      <c r="D2" t="s">
+      <c r="H3" s="408" t="s">
         <v>648</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="407" t="s">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="415" t="s">
+        <v>672</v>
+      </c>
+      <c r="B4" s="416" t="s">
+        <v>669</v>
+      </c>
+      <c r="C4" s="416" t="s">
+        <v>670</v>
+      </c>
+      <c r="E4" s="409" t="s">
         <v>643</v>
       </c>
-      <c r="B3" s="408">
+      <c r="F4" s="406">
         <v>1024</v>
       </c>
-      <c r="C3" s="408">
+      <c r="G4" s="406">
         <v>49151</v>
       </c>
-      <c r="D3" t="s">
+      <c r="H4" s="409" t="s">
+        <v>664</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="413" t="s">
+        <v>654</v>
+      </c>
+      <c r="B5" s="414" t="s">
+        <v>673</v>
+      </c>
+      <c r="C5" s="414" t="s">
+        <v>674</v>
+      </c>
+      <c r="E5" s="410" t="s">
+        <v>645</v>
+      </c>
+      <c r="F5" s="407">
+        <v>49152</v>
+      </c>
+      <c r="G5" s="407">
+        <v>65535</v>
+      </c>
+      <c r="H5" s="410" t="s">
         <v>649</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="409" t="s">
-        <v>645</v>
-      </c>
-      <c r="B4" s="410">
-        <v>49152</v>
-      </c>
-      <c r="C4" s="410">
-        <v>65535</v>
-      </c>
-      <c r="D4" t="s">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="415" t="s">
+        <v>671</v>
+      </c>
+      <c r="B6" s="416" t="s">
         <v>650</v>
       </c>
+      <c r="C6" s="416" t="s">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="413" t="s">
+        <v>659</v>
+      </c>
+      <c r="B7" s="414" t="s">
+        <v>660</v>
+      </c>
+      <c r="C7" s="414" t="s">
+        <v>653</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="415" t="s">
+        <v>678</v>
+      </c>
+      <c r="B8" s="416" t="s">
+        <v>652</v>
+      </c>
+      <c r="C8" s="416" t="s">
+        <v>661</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="413" t="s">
+        <v>655</v>
+      </c>
+      <c r="B9" s="414" t="s">
+        <v>679</v>
+      </c>
+      <c r="C9" s="414" t="s">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="415" t="s">
+        <v>665</v>
+      </c>
+      <c r="B10" s="416" t="s">
+        <v>681</v>
+      </c>
+      <c r="C10" s="416" t="s">
+        <v>682</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="413"/>
+      <c r="B11" s="414"/>
+      <c r="C11" s="414"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="E1:H1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Configuracion DHCP y VLAN
</commit_message>
<xml_diff>
--- a/docs/protocol-suite.xlsx
+++ b/docs/protocol-suite.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EducacionIT\Documents\redes\saves\ccna-lx19\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79F895D3-C35C-42F7-A197-48A7C61BFAA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02E698E0-E3E7-4B9F-A29B-4DFEF3D1EAAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="8" xr2:uid="{3415D364-6D1D-489F-8C8D-BD784F513C31}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="8" xr2:uid="{3415D364-6D1D-489F-8C8D-BD784F513C31}"/>
   </bookViews>
   <sheets>
     <sheet name="modelos" sheetId="1" r:id="rId1"/>
@@ -10010,6 +10010,60 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="99" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="97" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="97" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="98" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="100" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="100" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="98" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="99" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="100" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="97" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="100" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="97" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -10023,6 +10077,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
@@ -10031,6 +10094,39 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="30" borderId="0" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
@@ -10070,39 +10166,6 @@
     <xf numFmtId="0" fontId="0" fillId="31" borderId="63" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -10181,6 +10244,21 @@
     <xf numFmtId="0" fontId="3" fillId="9" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="15" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -10196,19 +10274,49 @@
     <xf numFmtId="0" fontId="3" fillId="26" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="24" borderId="54" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="24" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="24" borderId="55" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="25" borderId="54" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="25" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="25" borderId="55" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="24" borderId="56" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="24" borderId="43" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="24" borderId="57" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="36" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="36" borderId="59" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="36" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="59" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="60" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="28" borderId="30" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="3" fillId="15" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -10229,87 +10337,6 @@
     <xf numFmtId="49" fontId="0" fillId="28" borderId="43" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="24" borderId="54" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="24" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="24" borderId="55" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="36" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="36" borderId="59" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="36" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="59" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="60" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="28" borderId="30" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="25" borderId="54" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="25" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="25" borderId="55" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="24" borderId="56" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="24" borderId="43" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="24" borderId="57" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="91" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="76" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="87" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="37" borderId="91" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="37" borderId="76" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="37" borderId="87" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="37" borderId="92" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="37" borderId="82" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="37" borderId="88" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="92" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="82" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="88" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="10" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
@@ -10322,6 +10349,42 @@
     <xf numFmtId="49" fontId="3" fillId="9" borderId="77" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="92" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="82" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="88" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="91" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="76" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="87" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="91" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="76" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="87" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="92" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="82" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="88" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="40" borderId="80" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
@@ -10342,69 +10405,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="99" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="97" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="97" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="98" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="100" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="100" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="98" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="99" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="100" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="97" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="100" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="97" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
@@ -10996,13 +10996,13 @@
       <c r="A2" s="278" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="396" t="s">
+      <c r="B2" s="308" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="285" t="s">
+      <c r="C2" s="303" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="290" t="s">
+      <c r="D2" s="311" t="s">
         <v>23</v>
       </c>
     </row>
@@ -11010,23 +11010,23 @@
       <c r="A3" s="279" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="397"/>
-      <c r="C3" s="286"/>
-      <c r="D3" s="290"/>
+      <c r="B3" s="309"/>
+      <c r="C3" s="304"/>
+      <c r="D3" s="311"/>
     </row>
     <row r="4" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="280" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="398"/>
-      <c r="C4" s="287"/>
-      <c r="D4" s="290"/>
+      <c r="B4" s="310"/>
+      <c r="C4" s="305"/>
+      <c r="D4" s="311"/>
     </row>
     <row r="5" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="281" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="399" t="s">
+      <c r="B5" s="285" t="s">
         <v>16</v>
       </c>
       <c r="C5" s="2" t="s">
@@ -11040,7 +11040,7 @@
       <c r="A6" s="282" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="400" t="s">
+      <c r="B6" s="286" t="s">
         <v>17</v>
       </c>
       <c r="C6" s="3" t="s">
@@ -11054,10 +11054,10 @@
       <c r="A7" s="283" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="401" t="s">
+      <c r="B7" s="287" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="288" t="s">
+      <c r="C7" s="306" t="s">
         <v>12</v>
       </c>
       <c r="D7" s="276" t="s">
@@ -11068,11 +11068,11 @@
       <c r="A8" s="284" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="402" t="s">
+      <c r="B8" s="288" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="289"/>
-      <c r="D8" s="290" t="s">
+      <c r="C8" s="307"/>
+      <c r="D8" s="311" t="s">
         <v>20</v>
       </c>
     </row>
@@ -11086,7 +11086,7 @@
       <c r="C9" s="277" t="s">
         <v>14</v>
       </c>
-      <c r="D9" s="291"/>
+      <c r="D9" s="312"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -11105,8 +11105,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2546DD17-9723-4091-B9ED-D9677931F7C4}">
   <dimension ref="A2:K21"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H2" sqref="H1:H1048576"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19:K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11125,24 +11125,24 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="305" t="s">
+      <c r="A2" s="313" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="306"/>
+      <c r="B2" s="314"/>
       <c r="C2" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="E2" s="305" t="s">
+      <c r="E2" s="313" t="s">
         <v>29</v>
       </c>
-      <c r="F2" s="306"/>
+      <c r="F2" s="314"/>
       <c r="G2" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="I2" s="305" t="s">
+      <c r="I2" s="313" t="s">
         <v>30</v>
       </c>
-      <c r="J2" s="306"/>
+      <c r="J2" s="314"/>
       <c r="K2" s="14" t="s">
         <v>42</v>
       </c>
@@ -11316,15 +11316,15 @@
       <c r="E9" s="22" t="s">
         <v>66</v>
       </c>
-      <c r="F9" s="313" t="s">
+      <c r="F9" s="321" t="s">
         <v>67</v>
       </c>
-      <c r="G9" s="313"/>
-      <c r="I9" s="313" t="s">
+      <c r="G9" s="321"/>
+      <c r="I9" s="321" t="s">
         <v>81</v>
       </c>
-      <c r="J9" s="313"/>
-      <c r="K9" s="313"/>
+      <c r="J9" s="321"/>
+      <c r="K9" s="321"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
@@ -11340,15 +11340,15 @@
       <c r="E10" s="24" t="s">
         <v>68</v>
       </c>
-      <c r="F10" s="308" t="s">
+      <c r="F10" s="316" t="s">
         <v>70</v>
       </c>
-      <c r="G10" s="309"/>
-      <c r="I10" s="307" t="s">
+      <c r="G10" s="317"/>
+      <c r="I10" s="315" t="s">
         <v>63</v>
       </c>
-      <c r="J10" s="308"/>
-      <c r="K10" s="309"/>
+      <c r="J10" s="316"/>
+      <c r="K10" s="317"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="26" t="s">
@@ -11363,15 +11363,15 @@
       <c r="E11" s="25" t="s">
         <v>69</v>
       </c>
-      <c r="F11" s="314" t="s">
+      <c r="F11" s="322" t="s">
         <v>52</v>
       </c>
-      <c r="G11" s="315"/>
-      <c r="I11" s="310" t="s">
+      <c r="G11" s="323"/>
+      <c r="I11" s="318" t="s">
         <v>64</v>
       </c>
-      <c r="J11" s="311"/>
-      <c r="K11" s="312"/>
+      <c r="J11" s="319"/>
+      <c r="K11" s="320"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
@@ -11386,15 +11386,15 @@
       <c r="E12" s="24" t="s">
         <v>71</v>
       </c>
-      <c r="F12" s="308" t="s">
+      <c r="F12" s="316" t="s">
         <v>72</v>
       </c>
-      <c r="G12" s="309"/>
-      <c r="I12" s="307" t="s">
+      <c r="G12" s="317"/>
+      <c r="I12" s="315" t="s">
         <v>65</v>
       </c>
-      <c r="J12" s="308"/>
-      <c r="K12" s="309"/>
+      <c r="J12" s="316"/>
+      <c r="K12" s="317"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="26" t="s">
@@ -11430,94 +11430,100 @@
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="300" t="s">
+      <c r="A17" s="332" t="s">
         <v>282</v>
       </c>
       <c r="B17" s="187" t="s">
         <v>272</v>
       </c>
-      <c r="C17" s="303" t="s">
+      <c r="C17" s="335" t="s">
         <v>273</v>
       </c>
-      <c r="D17" s="303"/>
-      <c r="E17" s="303"/>
-      <c r="F17" s="303"/>
-      <c r="G17" s="303"/>
-      <c r="H17" s="303"/>
-      <c r="I17" s="303"/>
-      <c r="J17" s="303"/>
-      <c r="K17" s="304"/>
+      <c r="D17" s="335"/>
+      <c r="E17" s="335"/>
+      <c r="F17" s="335"/>
+      <c r="G17" s="335"/>
+      <c r="H17" s="335"/>
+      <c r="I17" s="335"/>
+      <c r="J17" s="335"/>
+      <c r="K17" s="336"/>
     </row>
     <row r="18" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="301"/>
+      <c r="A18" s="333"/>
       <c r="B18" s="188" t="s">
         <v>274</v>
       </c>
-      <c r="C18" s="292" t="s">
+      <c r="C18" s="324" t="s">
         <v>275</v>
       </c>
-      <c r="D18" s="292"/>
-      <c r="E18" s="292"/>
-      <c r="F18" s="292"/>
-      <c r="G18" s="292"/>
-      <c r="H18" s="292"/>
-      <c r="I18" s="292"/>
-      <c r="J18" s="292"/>
-      <c r="K18" s="293"/>
+      <c r="D18" s="324"/>
+      <c r="E18" s="324"/>
+      <c r="F18" s="324"/>
+      <c r="G18" s="324"/>
+      <c r="H18" s="324"/>
+      <c r="I18" s="324"/>
+      <c r="J18" s="324"/>
+      <c r="K18" s="325"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="301"/>
+      <c r="A19" s="333"/>
       <c r="B19" s="189" t="s">
         <v>276</v>
       </c>
-      <c r="C19" s="294" t="s">
+      <c r="C19" s="326" t="s">
         <v>277</v>
       </c>
-      <c r="D19" s="294"/>
-      <c r="E19" s="294"/>
-      <c r="F19" s="294"/>
-      <c r="G19" s="294"/>
-      <c r="H19" s="294"/>
-      <c r="I19" s="294"/>
-      <c r="J19" s="294"/>
-      <c r="K19" s="295"/>
+      <c r="D19" s="326"/>
+      <c r="E19" s="326"/>
+      <c r="F19" s="326"/>
+      <c r="G19" s="326"/>
+      <c r="H19" s="326"/>
+      <c r="I19" s="326"/>
+      <c r="J19" s="326"/>
+      <c r="K19" s="327"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="301"/>
+      <c r="A20" s="333"/>
       <c r="B20" s="190" t="s">
         <v>278</v>
       </c>
-      <c r="C20" s="296" t="s">
+      <c r="C20" s="328" t="s">
         <v>279</v>
       </c>
-      <c r="D20" s="296"/>
-      <c r="E20" s="296"/>
-      <c r="F20" s="296"/>
-      <c r="G20" s="296"/>
-      <c r="H20" s="296"/>
-      <c r="I20" s="296"/>
-      <c r="J20" s="296"/>
-      <c r="K20" s="297"/>
+      <c r="D20" s="328"/>
+      <c r="E20" s="328"/>
+      <c r="F20" s="328"/>
+      <c r="G20" s="328"/>
+      <c r="H20" s="328"/>
+      <c r="I20" s="328"/>
+      <c r="J20" s="328"/>
+      <c r="K20" s="329"/>
     </row>
     <row r="21" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="302"/>
+      <c r="A21" s="334"/>
       <c r="B21" s="191" t="s">
         <v>280</v>
       </c>
-      <c r="C21" s="298" t="s">
+      <c r="C21" s="330" t="s">
         <v>281</v>
       </c>
-      <c r="D21" s="298"/>
-      <c r="E21" s="298"/>
-      <c r="F21" s="298"/>
-      <c r="G21" s="298"/>
-      <c r="H21" s="298"/>
-      <c r="I21" s="298"/>
-      <c r="J21" s="298"/>
-      <c r="K21" s="299"/>
+      <c r="D21" s="330"/>
+      <c r="E21" s="330"/>
+      <c r="F21" s="330"/>
+      <c r="G21" s="330"/>
+      <c r="H21" s="330"/>
+      <c r="I21" s="330"/>
+      <c r="J21" s="330"/>
+      <c r="K21" s="331"/>
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="C18:K18"/>
+    <mergeCell ref="C19:K19"/>
+    <mergeCell ref="C20:K20"/>
+    <mergeCell ref="C21:K21"/>
+    <mergeCell ref="A17:A21"/>
+    <mergeCell ref="C17:K17"/>
     <mergeCell ref="I2:J2"/>
     <mergeCell ref="E2:F2"/>
     <mergeCell ref="A2:B2"/>
@@ -11529,12 +11535,6 @@
     <mergeCell ref="F11:G11"/>
     <mergeCell ref="F12:G12"/>
     <mergeCell ref="I9:K9"/>
-    <mergeCell ref="C18:K18"/>
-    <mergeCell ref="C19:K19"/>
-    <mergeCell ref="C20:K20"/>
-    <mergeCell ref="C21:K21"/>
-    <mergeCell ref="A17:A21"/>
-    <mergeCell ref="C17:K17"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -11546,7 +11546,7 @@
   <dimension ref="A1:I20"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
+      <selection activeCell="H2" sqref="H1:H1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11555,21 +11555,22 @@
     <col min="2" max="2" width="9.7109375" customWidth="1"/>
     <col min="3" max="4" width="11" customWidth="1"/>
     <col min="5" max="5" width="2.85546875" customWidth="1"/>
-    <col min="6" max="8" width="27.7109375" style="21" customWidth="1"/>
+    <col min="6" max="7" width="27.7109375" style="21" customWidth="1"/>
+    <col min="8" max="8" width="29.140625" style="21" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="28.7109375" style="21" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="316" t="s">
+      <c r="B1" s="337" t="s">
         <v>105</v>
       </c>
-      <c r="C1" s="316"/>
-      <c r="D1" s="316"/>
-      <c r="F1" s="316" t="s">
+      <c r="C1" s="337"/>
+      <c r="D1" s="337"/>
+      <c r="F1" s="337" t="s">
         <v>104</v>
       </c>
-      <c r="G1" s="316"/>
-      <c r="H1" s="316"/>
+      <c r="G1" s="337"/>
+      <c r="H1" s="337"/>
     </row>
     <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="36" t="s">
@@ -11598,10 +11599,10 @@
       <c r="D3" s="166" t="s">
         <v>53</v>
       </c>
-      <c r="F3" s="325" t="s">
+      <c r="F3" s="346" t="s">
         <v>94</v>
       </c>
-      <c r="G3" s="327" t="s">
+      <c r="G3" s="348" t="s">
         <v>93</v>
       </c>
       <c r="H3" s="172" t="s">
@@ -11618,8 +11619,8 @@
       <c r="D4" s="169" t="s">
         <v>53</v>
       </c>
-      <c r="F4" s="325"/>
-      <c r="G4" s="328"/>
+      <c r="F4" s="346"/>
+      <c r="G4" s="349"/>
       <c r="H4" s="173" t="s">
         <v>60</v>
       </c>
@@ -11634,8 +11635,8 @@
       <c r="D5" s="164" t="s">
         <v>54</v>
       </c>
-      <c r="F5" s="325"/>
-      <c r="G5" s="328"/>
+      <c r="F5" s="346"/>
+      <c r="G5" s="349"/>
       <c r="H5" s="174" t="s">
         <v>61</v>
       </c>
@@ -11650,8 +11651,8 @@
       <c r="D6" s="167" t="s">
         <v>55</v>
       </c>
-      <c r="F6" s="325"/>
-      <c r="G6" s="328"/>
+      <c r="F6" s="346"/>
+      <c r="G6" s="349"/>
       <c r="H6" s="179" t="s">
         <v>62</v>
       </c>
@@ -11666,8 +11667,8 @@
       <c r="D7" s="168" t="s">
         <v>55</v>
       </c>
-      <c r="F7" s="325"/>
-      <c r="G7" s="328"/>
+      <c r="F7" s="346"/>
+      <c r="G7" s="349"/>
       <c r="H7" s="178" t="s">
         <v>99</v>
       </c>
@@ -11682,8 +11683,8 @@
       <c r="D8" s="165" t="s">
         <v>54</v>
       </c>
-      <c r="F8" s="325"/>
-      <c r="G8" s="328"/>
+      <c r="F8" s="346"/>
+      <c r="G8" s="349"/>
       <c r="H8" s="175" t="s">
         <v>103</v>
       </c>
@@ -11698,8 +11699,8 @@
       <c r="D9" s="170" t="s">
         <v>55</v>
       </c>
-      <c r="F9" s="325"/>
-      <c r="G9" s="328"/>
+      <c r="F9" s="346"/>
+      <c r="G9" s="349"/>
       <c r="H9" s="176" t="s">
         <v>97</v>
       </c>
@@ -11714,21 +11715,21 @@
       <c r="D10" s="171" t="s">
         <v>55</v>
       </c>
-      <c r="F10" s="326"/>
-      <c r="G10" s="329"/>
+      <c r="F10" s="347"/>
+      <c r="G10" s="350"/>
       <c r="H10" s="177" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="12" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="320" t="s">
+      <c r="B12" s="341" t="s">
         <v>92</v>
       </c>
-      <c r="C12" s="321"/>
-      <c r="D12" s="321"/>
-      <c r="E12" s="321"/>
-      <c r="F12" s="322"/>
+      <c r="C12" s="342"/>
+      <c r="D12" s="342"/>
+      <c r="E12" s="342"/>
+      <c r="F12" s="343"/>
       <c r="G12" s="180" t="s">
         <v>56</v>
       </c>
@@ -11737,13 +11738,13 @@
       <c r="B13" s="181" t="s">
         <v>90</v>
       </c>
-      <c r="C13" s="330" t="s">
+      <c r="C13" s="351" t="s">
         <v>89</v>
       </c>
-      <c r="D13" s="330"/>
-      <c r="E13" s="330"/>
-      <c r="F13" s="331"/>
-      <c r="G13" s="317" t="s">
+      <c r="D13" s="351"/>
+      <c r="E13" s="351"/>
+      <c r="F13" s="352"/>
+      <c r="G13" s="338" t="s">
         <v>219</v>
       </c>
       <c r="I13" s="29"/>
@@ -11752,39 +11753,39 @@
       <c r="B14" s="182" t="s">
         <v>57</v>
       </c>
-      <c r="C14" s="332" t="s">
+      <c r="C14" s="353" t="s">
         <v>86</v>
       </c>
-      <c r="D14" s="332"/>
-      <c r="E14" s="332"/>
-      <c r="F14" s="333"/>
-      <c r="G14" s="318"/>
+      <c r="D14" s="353"/>
+      <c r="E14" s="353"/>
+      <c r="F14" s="354"/>
+      <c r="G14" s="339"/>
       <c r="I14" s="29"/>
     </row>
     <row r="15" spans="1:9" s="28" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="181" t="s">
         <v>58</v>
       </c>
-      <c r="C15" s="330" t="s">
+      <c r="C15" s="351" t="s">
         <v>87</v>
       </c>
-      <c r="D15" s="330"/>
-      <c r="E15" s="330"/>
-      <c r="F15" s="331"/>
-      <c r="G15" s="318"/>
+      <c r="D15" s="351"/>
+      <c r="E15" s="351"/>
+      <c r="F15" s="352"/>
+      <c r="G15" s="339"/>
       <c r="I15" s="29"/>
     </row>
     <row r="16" spans="1:9" s="28" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="183" t="s">
         <v>91</v>
       </c>
-      <c r="C16" s="323" t="s">
+      <c r="C16" s="344" t="s">
         <v>88</v>
       </c>
-      <c r="D16" s="323"/>
-      <c r="E16" s="323"/>
-      <c r="F16" s="324"/>
-      <c r="G16" s="319"/>
+      <c r="D16" s="344"/>
+      <c r="E16" s="344"/>
+      <c r="F16" s="345"/>
+      <c r="G16" s="340"/>
       <c r="I16" s="29"/>
     </row>
     <row r="17" spans="7:7" x14ac:dyDescent="0.25">
@@ -11840,76 +11841,76 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="334" t="s">
+      <c r="A1" s="355" t="s">
         <v>220</v>
       </c>
-      <c r="B1" s="335"/>
-      <c r="C1" s="335"/>
-      <c r="D1" s="335"/>
-      <c r="F1" s="334" t="s">
+      <c r="B1" s="356"/>
+      <c r="C1" s="356"/>
+      <c r="D1" s="356"/>
+      <c r="F1" s="355" t="s">
         <v>222</v>
       </c>
-      <c r="G1" s="335"/>
-      <c r="H1" s="335"/>
-      <c r="I1" s="335"/>
-      <c r="J1" s="335"/>
-      <c r="K1" s="335"/>
-      <c r="L1" s="335"/>
-      <c r="M1" s="335"/>
-      <c r="N1" s="335"/>
-      <c r="O1" s="335"/>
-      <c r="P1" s="336"/>
-      <c r="R1" s="334" t="s">
+      <c r="G1" s="356"/>
+      <c r="H1" s="356"/>
+      <c r="I1" s="356"/>
+      <c r="J1" s="356"/>
+      <c r="K1" s="356"/>
+      <c r="L1" s="356"/>
+      <c r="M1" s="356"/>
+      <c r="N1" s="356"/>
+      <c r="O1" s="356"/>
+      <c r="P1" s="357"/>
+      <c r="R1" s="355" t="s">
         <v>223</v>
       </c>
-      <c r="S1" s="335"/>
-      <c r="T1" s="335"/>
-      <c r="U1" s="335"/>
-      <c r="V1" s="335"/>
-      <c r="W1" s="335"/>
-      <c r="X1" s="335"/>
-      <c r="Y1" s="335"/>
-      <c r="Z1" s="335"/>
-      <c r="AA1" s="336"/>
+      <c r="S1" s="356"/>
+      <c r="T1" s="356"/>
+      <c r="U1" s="356"/>
+      <c r="V1" s="356"/>
+      <c r="W1" s="356"/>
+      <c r="X1" s="356"/>
+      <c r="Y1" s="356"/>
+      <c r="Z1" s="356"/>
+      <c r="AA1" s="357"/>
     </row>
     <row r="2" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="341" t="s">
+      <c r="A2" s="362" t="s">
         <v>119</v>
       </c>
-      <c r="B2" s="340"/>
-      <c r="C2" s="340"/>
-      <c r="D2" s="340"/>
-      <c r="F2" s="337" t="s">
+      <c r="B2" s="361"/>
+      <c r="C2" s="361"/>
+      <c r="D2" s="361"/>
+      <c r="F2" s="358" t="s">
         <v>130</v>
       </c>
-      <c r="G2" s="339"/>
-      <c r="H2" s="339"/>
-      <c r="I2" s="339"/>
-      <c r="J2" s="339"/>
-      <c r="K2" s="339"/>
-      <c r="L2" s="339"/>
-      <c r="M2" s="338"/>
+      <c r="G2" s="360"/>
+      <c r="H2" s="360"/>
+      <c r="I2" s="360"/>
+      <c r="J2" s="360"/>
+      <c r="K2" s="360"/>
+      <c r="L2" s="360"/>
+      <c r="M2" s="359"/>
       <c r="N2" s="91" t="s">
         <v>106</v>
       </c>
-      <c r="O2" s="337" t="s">
+      <c r="O2" s="358" t="s">
         <v>107</v>
       </c>
-      <c r="P2" s="338"/>
-      <c r="R2" s="337" t="s">
+      <c r="P2" s="359"/>
+      <c r="R2" s="358" t="s">
         <v>130</v>
       </c>
-      <c r="S2" s="339"/>
-      <c r="T2" s="339"/>
-      <c r="U2" s="339"/>
-      <c r="V2" s="339"/>
-      <c r="W2" s="339"/>
-      <c r="X2" s="339"/>
-      <c r="Y2" s="338"/>
-      <c r="Z2" s="337" t="s">
+      <c r="S2" s="360"/>
+      <c r="T2" s="360"/>
+      <c r="U2" s="360"/>
+      <c r="V2" s="360"/>
+      <c r="W2" s="360"/>
+      <c r="X2" s="360"/>
+      <c r="Y2" s="359"/>
+      <c r="Z2" s="358" t="s">
         <v>107</v>
       </c>
-      <c r="AA2" s="338"/>
+      <c r="AA2" s="359"/>
     </row>
     <row r="3" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="38" t="s">
@@ -12170,12 +12171,12 @@
       </c>
     </row>
     <row r="7" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="340" t="s">
+      <c r="A7" s="361" t="s">
         <v>120</v>
       </c>
-      <c r="B7" s="340"/>
-      <c r="C7" s="340"/>
-      <c r="D7" s="340"/>
+      <c r="B7" s="361"/>
+      <c r="C7" s="361"/>
+      <c r="D7" s="361"/>
       <c r="F7" s="59">
         <v>1</v>
       </c>
@@ -12469,12 +12470,12 @@
       </c>
     </row>
     <row r="12" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A12" s="340" t="s">
+      <c r="A12" s="361" t="s">
         <v>125</v>
       </c>
-      <c r="B12" s="340"/>
-      <c r="C12" s="340"/>
-      <c r="D12" s="340"/>
+      <c r="B12" s="361"/>
+      <c r="C12" s="361"/>
+      <c r="D12" s="361"/>
       <c r="F12" s="58">
         <v>0</v>
       </c>
@@ -12753,28 +12754,28 @@
       <c r="A1" s="94" t="s">
         <v>238</v>
       </c>
-      <c r="B1" s="342" t="s">
+      <c r="B1" s="368" t="s">
         <v>230</v>
       </c>
-      <c r="C1" s="342"/>
-      <c r="D1" s="342"/>
-      <c r="E1" s="343"/>
-      <c r="F1" s="342" t="s">
+      <c r="C1" s="368"/>
+      <c r="D1" s="368"/>
+      <c r="E1" s="369"/>
+      <c r="F1" s="368" t="s">
         <v>231</v>
       </c>
-      <c r="G1" s="342"/>
-      <c r="H1" s="342"/>
-      <c r="I1" s="342"/>
-      <c r="J1" s="342"/>
-      <c r="K1" s="342"/>
-      <c r="L1" s="342"/>
-      <c r="M1" s="342"/>
-      <c r="N1" s="344">
+      <c r="G1" s="368"/>
+      <c r="H1" s="368"/>
+      <c r="I1" s="368"/>
+      <c r="J1" s="368"/>
+      <c r="K1" s="368"/>
+      <c r="L1" s="368"/>
+      <c r="M1" s="368"/>
+      <c r="N1" s="370">
         <f>2^32</f>
         <v>4294967296</v>
       </c>
-      <c r="O1" s="344"/>
-      <c r="P1" s="344"/>
+      <c r="O1" s="370"/>
+      <c r="P1" s="370"/>
       <c r="Q1" s="162" t="s">
         <v>239</v>
       </c>
@@ -12783,34 +12784,34 @@
       <c r="A2" s="94" t="s">
         <v>156</v>
       </c>
-      <c r="B2" s="345" t="s">
+      <c r="B2" s="371" t="s">
         <v>225</v>
       </c>
-      <c r="C2" s="345"/>
-      <c r="D2" s="345" t="s">
+      <c r="C2" s="371"/>
+      <c r="D2" s="371" t="s">
         <v>130</v>
       </c>
-      <c r="E2" s="346"/>
-      <c r="F2" s="345" t="s">
+      <c r="E2" s="372"/>
+      <c r="F2" s="371" t="s">
         <v>225</v>
       </c>
-      <c r="G2" s="345"/>
-      <c r="H2" s="345" t="s">
+      <c r="G2" s="371"/>
+      <c r="H2" s="371" t="s">
         <v>130</v>
       </c>
-      <c r="I2" s="345"/>
-      <c r="J2" s="345" t="s">
+      <c r="I2" s="371"/>
+      <c r="J2" s="371" t="s">
         <v>226</v>
       </c>
-      <c r="K2" s="345"/>
-      <c r="L2" s="345"/>
-      <c r="M2" s="345"/>
-      <c r="N2" s="351" t="s">
+      <c r="K2" s="371"/>
+      <c r="L2" s="371"/>
+      <c r="M2" s="371"/>
+      <c r="N2" s="367" t="s">
         <v>265</v>
       </c>
-      <c r="O2" s="351"/>
-      <c r="P2" s="351"/>
-      <c r="Q2" s="351"/>
+      <c r="O2" s="367"/>
+      <c r="P2" s="367"/>
+      <c r="Q2" s="367"/>
     </row>
     <row r="3" spans="1:33" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="161" t="s">
@@ -13037,18 +13038,18 @@
       <c r="E7" s="152" t="s">
         <v>143</v>
       </c>
-      <c r="F7" s="347" t="s">
+      <c r="F7" s="363" t="s">
         <v>148</v>
       </c>
-      <c r="G7" s="348"/>
-      <c r="H7" s="348"/>
-      <c r="I7" s="348"/>
-      <c r="J7" s="347" t="s">
+      <c r="G7" s="364"/>
+      <c r="H7" s="364"/>
+      <c r="I7" s="364"/>
+      <c r="J7" s="363" t="s">
         <v>148</v>
       </c>
-      <c r="K7" s="348"/>
-      <c r="L7" s="348"/>
-      <c r="M7" s="348"/>
+      <c r="K7" s="364"/>
+      <c r="L7" s="364"/>
+      <c r="M7" s="364"/>
       <c r="N7" s="199" t="s">
         <v>134</v>
       </c>
@@ -13078,18 +13079,18 @@
       <c r="E8" s="154" t="s">
         <v>145</v>
       </c>
-      <c r="F8" s="349" t="s">
+      <c r="F8" s="365" t="s">
         <v>149</v>
       </c>
-      <c r="G8" s="350"/>
-      <c r="H8" s="350"/>
-      <c r="I8" s="350"/>
-      <c r="J8" s="349" t="s">
+      <c r="G8" s="366"/>
+      <c r="H8" s="366"/>
+      <c r="I8" s="366"/>
+      <c r="J8" s="365" t="s">
         <v>149</v>
       </c>
-      <c r="K8" s="350"/>
-      <c r="L8" s="350"/>
-      <c r="M8" s="350"/>
+      <c r="K8" s="366"/>
+      <c r="L8" s="366"/>
+      <c r="M8" s="366"/>
       <c r="N8" s="202" t="s">
         <v>135</v>
       </c>
@@ -13804,11 +13805,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="F7:I7"/>
-    <mergeCell ref="F8:I8"/>
-    <mergeCell ref="J7:M7"/>
-    <mergeCell ref="J8:M8"/>
-    <mergeCell ref="N2:Q2"/>
     <mergeCell ref="B1:E1"/>
     <mergeCell ref="F1:M1"/>
     <mergeCell ref="N1:P1"/>
@@ -13817,6 +13813,11 @@
     <mergeCell ref="F2:G2"/>
     <mergeCell ref="H2:I2"/>
     <mergeCell ref="D2:E2"/>
+    <mergeCell ref="F7:I7"/>
+    <mergeCell ref="F8:I8"/>
+    <mergeCell ref="J7:M7"/>
+    <mergeCell ref="J8:M8"/>
+    <mergeCell ref="N2:Q2"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -13849,45 +13850,45 @@
       <c r="A1" s="97" t="s">
         <v>166</v>
       </c>
-      <c r="B1" s="352">
+      <c r="B1" s="388">
         <f>2^128</f>
         <v>3.4028236692093846E+38</v>
       </c>
-      <c r="C1" s="352"/>
-      <c r="D1" s="352"/>
-      <c r="E1" s="352"/>
-      <c r="F1" s="352"/>
-      <c r="G1" s="352"/>
-      <c r="H1" s="352"/>
-      <c r="I1" s="352"/>
+      <c r="C1" s="388"/>
+      <c r="D1" s="388"/>
+      <c r="E1" s="388"/>
+      <c r="F1" s="388"/>
+      <c r="G1" s="388"/>
+      <c r="H1" s="388"/>
+      <c r="I1" s="388"/>
       <c r="J1" s="97" t="s">
         <v>240</v>
       </c>
-      <c r="K1" s="353" t="s">
+      <c r="K1" s="389" t="s">
         <v>229</v>
       </c>
-      <c r="L1" s="353"/>
-      <c r="M1" s="353"/>
-      <c r="N1" s="353"/>
+      <c r="L1" s="389"/>
+      <c r="M1" s="389"/>
+      <c r="N1" s="389"/>
     </row>
     <row r="2" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="120" t="s">
         <v>177</v>
       </c>
-      <c r="B2" s="354" t="s">
+      <c r="B2" s="390" t="s">
         <v>173</v>
       </c>
-      <c r="C2" s="355"/>
-      <c r="D2" s="355"/>
+      <c r="C2" s="391"/>
+      <c r="D2" s="391"/>
       <c r="E2" s="98" t="s">
         <v>253</v>
       </c>
-      <c r="F2" s="355" t="s">
+      <c r="F2" s="391" t="s">
         <v>174</v>
       </c>
-      <c r="G2" s="355"/>
-      <c r="H2" s="355"/>
-      <c r="I2" s="356"/>
+      <c r="G2" s="391"/>
+      <c r="H2" s="391"/>
+      <c r="I2" s="392"/>
       <c r="J2" s="99" t="s">
         <v>175</v>
       </c>
@@ -14008,11 +14009,11 @@
       <c r="E5" s="118" t="s">
         <v>182</v>
       </c>
-      <c r="F5" s="357" t="s">
+      <c r="F5" s="393" t="s">
         <v>184</v>
       </c>
-      <c r="G5" s="357"/>
-      <c r="H5" s="357"/>
+      <c r="G5" s="393"/>
+      <c r="H5" s="393"/>
       <c r="I5" s="119">
         <v>1</v>
       </c>
@@ -14042,12 +14043,12 @@
       <c r="B7" s="103" t="s">
         <v>263</v>
       </c>
-      <c r="C7" s="364" t="s">
+      <c r="C7" s="385" t="s">
         <v>248</v>
       </c>
-      <c r="D7" s="364"/>
-      <c r="E7" s="364"/>
-      <c r="F7" s="365"/>
+      <c r="D7" s="385"/>
+      <c r="E7" s="385"/>
+      <c r="F7" s="386"/>
       <c r="G7" s="127" t="s">
         <v>261</v>
       </c>
@@ -14062,10 +14063,10 @@
       <c r="C8" s="123" t="s">
         <v>262</v>
       </c>
-      <c r="D8" s="366" t="s">
+      <c r="D8" s="387" t="s">
         <v>249</v>
       </c>
-      <c r="E8" s="366"/>
+      <c r="E8" s="387"/>
       <c r="F8" s="121" t="s">
         <v>250</v>
       </c>
@@ -14124,114 +14125,114 @@
       <c r="A12" s="130" t="s">
         <v>263</v>
       </c>
-      <c r="B12" s="361" t="s">
+      <c r="B12" s="382" t="s">
         <v>248</v>
       </c>
-      <c r="C12" s="362"/>
-      <c r="D12" s="363"/>
-      <c r="E12" s="361" t="s">
+      <c r="C12" s="383"/>
+      <c r="D12" s="384"/>
+      <c r="E12" s="382" t="s">
         <v>264</v>
       </c>
-      <c r="F12" s="362"/>
-      <c r="G12" s="363"/>
+      <c r="F12" s="383"/>
+      <c r="G12" s="384"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="128" t="s">
         <v>188</v>
       </c>
-      <c r="B13" s="358" t="s">
+      <c r="B13" s="373" t="s">
         <v>190</v>
       </c>
-      <c r="C13" s="359"/>
-      <c r="D13" s="360"/>
-      <c r="E13" s="359" t="s">
+      <c r="C13" s="374"/>
+      <c r="D13" s="375"/>
+      <c r="E13" s="374" t="s">
         <v>191</v>
       </c>
-      <c r="F13" s="359"/>
-      <c r="G13" s="360"/>
+      <c r="F13" s="374"/>
+      <c r="G13" s="375"/>
       <c r="H13" s="37"/>
       <c r="I13" s="37"/>
       <c r="J13" s="37"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="129"/>
-      <c r="B14" s="367"/>
-      <c r="C14" s="368"/>
-      <c r="D14" s="369"/>
-      <c r="E14" s="368"/>
-      <c r="F14" s="368"/>
-      <c r="G14" s="369"/>
+      <c r="B14" s="376"/>
+      <c r="C14" s="377"/>
+      <c r="D14" s="378"/>
+      <c r="E14" s="377"/>
+      <c r="F14" s="377"/>
+      <c r="G14" s="378"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="128"/>
-      <c r="B15" s="358"/>
-      <c r="C15" s="359"/>
-      <c r="D15" s="360"/>
-      <c r="E15" s="359"/>
-      <c r="F15" s="359"/>
-      <c r="G15" s="360"/>
+      <c r="B15" s="373"/>
+      <c r="C15" s="374"/>
+      <c r="D15" s="375"/>
+      <c r="E15" s="374"/>
+      <c r="F15" s="374"/>
+      <c r="G15" s="375"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="129"/>
-      <c r="B16" s="367"/>
-      <c r="C16" s="368"/>
-      <c r="D16" s="369"/>
-      <c r="E16" s="368"/>
-      <c r="F16" s="368"/>
-      <c r="G16" s="369"/>
+      <c r="B16" s="376"/>
+      <c r="C16" s="377"/>
+      <c r="D16" s="378"/>
+      <c r="E16" s="377"/>
+      <c r="F16" s="377"/>
+      <c r="G16" s="378"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="128"/>
-      <c r="B17" s="358"/>
-      <c r="C17" s="359"/>
-      <c r="D17" s="360"/>
-      <c r="E17" s="359"/>
-      <c r="F17" s="359"/>
-      <c r="G17" s="360"/>
+      <c r="B17" s="373"/>
+      <c r="C17" s="374"/>
+      <c r="D17" s="375"/>
+      <c r="E17" s="374"/>
+      <c r="F17" s="374"/>
+      <c r="G17" s="375"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="129"/>
-      <c r="B18" s="367"/>
-      <c r="C18" s="368"/>
-      <c r="D18" s="369"/>
-      <c r="E18" s="368"/>
-      <c r="F18" s="368"/>
-      <c r="G18" s="369"/>
+      <c r="B18" s="376"/>
+      <c r="C18" s="377"/>
+      <c r="D18" s="378"/>
+      <c r="E18" s="377"/>
+      <c r="F18" s="377"/>
+      <c r="G18" s="378"/>
     </row>
     <row r="19" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="116"/>
-      <c r="B19" s="370"/>
-      <c r="C19" s="371"/>
-      <c r="D19" s="372"/>
-      <c r="E19" s="371"/>
-      <c r="F19" s="371"/>
-      <c r="G19" s="372"/>
+      <c r="B19" s="379"/>
+      <c r="C19" s="380"/>
+      <c r="D19" s="381"/>
+      <c r="E19" s="380"/>
+      <c r="F19" s="380"/>
+      <c r="G19" s="381"/>
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="B1:I1"/>
+    <mergeCell ref="K1:N1"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="F2:I2"/>
+    <mergeCell ref="F5:H5"/>
+    <mergeCell ref="B13:D13"/>
+    <mergeCell ref="E13:G13"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="E12:G12"/>
+    <mergeCell ref="C7:F7"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="E14:G14"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="E15:G15"/>
+    <mergeCell ref="B16:D16"/>
+    <mergeCell ref="E16:G16"/>
     <mergeCell ref="B17:D17"/>
     <mergeCell ref="E17:G17"/>
     <mergeCell ref="B18:D18"/>
     <mergeCell ref="E18:G18"/>
     <mergeCell ref="B19:D19"/>
     <mergeCell ref="E19:G19"/>
-    <mergeCell ref="B14:D14"/>
-    <mergeCell ref="E14:G14"/>
-    <mergeCell ref="B15:D15"/>
-    <mergeCell ref="E15:G15"/>
-    <mergeCell ref="B16:D16"/>
-    <mergeCell ref="E16:G16"/>
-    <mergeCell ref="B13:D13"/>
-    <mergeCell ref="E13:G13"/>
-    <mergeCell ref="B12:D12"/>
-    <mergeCell ref="E12:G12"/>
-    <mergeCell ref="C7:F7"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="B1:I1"/>
-    <mergeCell ref="K1:N1"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="F2:I2"/>
-    <mergeCell ref="F5:H5"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -14266,11 +14267,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="388" t="s">
+      <c r="A1" s="397" t="s">
         <v>320</v>
       </c>
-      <c r="B1" s="388"/>
-      <c r="C1" s="388"/>
+      <c r="B1" s="397"/>
+      <c r="C1" s="397"/>
       <c r="D1" s="226" t="s">
         <v>471</v>
       </c>
@@ -14298,11 +14299,11 @@
       <c r="P1" s="34"/>
     </row>
     <row r="2" spans="1:16" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="385" t="s">
+      <c r="A2" s="394" t="s">
         <v>470</v>
       </c>
-      <c r="B2" s="386"/>
-      <c r="C2" s="387"/>
+      <c r="B2" s="395"/>
+      <c r="C2" s="396"/>
       <c r="D2" s="230" t="s">
         <v>321</v>
       </c>
@@ -14386,21 +14387,21 @@
       <c r="F4" s="244" t="s">
         <v>326</v>
       </c>
-      <c r="G4" s="376" t="s">
+      <c r="G4" s="401" t="s">
         <v>108</v>
       </c>
-      <c r="H4" s="376">
+      <c r="H4" s="401">
         <v>3</v>
       </c>
-      <c r="I4" s="376">
+      <c r="I4" s="401">
         <f>IF(H4="","",IF(H4&lt;=2,1,IF(H4&lt;=4,2,IF(H4&lt;=8,3,IF(H4&lt;=16,4,IF(H4&lt;=32,5,IF(H4&lt;=64,6,IF(H4&lt;=128,7,8))))))))</f>
         <v>2</v>
       </c>
-      <c r="J4" s="376">
+      <c r="J4" s="401">
         <f>IF(G4="","",IF(G4="A",8+I4,IF(G4="B",16+I4,IF(G4="C",24+I4,"invalid"))))</f>
         <v>10</v>
       </c>
-      <c r="K4" s="379">
+      <c r="K4" s="398">
         <f>IF(J4="","",2^(32-J4))</f>
         <v>4194304</v>
       </c>
@@ -14424,11 +14425,11 @@
       <c r="F5" s="214" t="s">
         <v>326</v>
       </c>
-      <c r="G5" s="377"/>
-      <c r="H5" s="377"/>
-      <c r="I5" s="377"/>
-      <c r="J5" s="377"/>
-      <c r="K5" s="380"/>
+      <c r="G5" s="402"/>
+      <c r="H5" s="402"/>
+      <c r="I5" s="402"/>
+      <c r="J5" s="402"/>
+      <c r="K5" s="399"/>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="237" t="s">
@@ -14449,11 +14450,11 @@
       <c r="F6" s="212" t="s">
         <v>326</v>
       </c>
-      <c r="G6" s="377"/>
-      <c r="H6" s="377"/>
-      <c r="I6" s="377"/>
-      <c r="J6" s="377"/>
-      <c r="K6" s="380"/>
+      <c r="G6" s="402"/>
+      <c r="H6" s="402"/>
+      <c r="I6" s="402"/>
+      <c r="J6" s="402"/>
+      <c r="K6" s="399"/>
     </row>
     <row r="7" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="239" t="s">
@@ -14474,11 +14475,11 @@
       <c r="F7" s="241" t="s">
         <v>326</v>
       </c>
-      <c r="G7" s="378"/>
-      <c r="H7" s="378"/>
-      <c r="I7" s="378"/>
-      <c r="J7" s="378"/>
-      <c r="K7" s="381"/>
+      <c r="G7" s="403"/>
+      <c r="H7" s="403"/>
+      <c r="I7" s="403"/>
+      <c r="J7" s="403"/>
+      <c r="K7" s="400"/>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="242" t="s">
@@ -14499,21 +14500,21 @@
       <c r="F8" s="244" t="s">
         <v>389</v>
       </c>
-      <c r="G8" s="373" t="s">
+      <c r="G8" s="404" t="s">
         <v>109</v>
       </c>
-      <c r="H8" s="373">
+      <c r="H8" s="404">
         <v>5</v>
       </c>
-      <c r="I8" s="373">
+      <c r="I8" s="404">
         <f t="shared" ref="I8:I44" si="0">IF(H8="","",IF(H8&lt;=2,1,IF(H8&lt;=4,2,IF(H8&lt;=8,3,IF(H8&lt;=16,4,IF(H8&lt;=32,5,IF(H8&lt;=64,6,IF(H8&lt;=128,7,8))))))))</f>
         <v>3</v>
       </c>
-      <c r="J8" s="373">
+      <c r="J8" s="404">
         <f t="shared" ref="J8:J20" si="1">IF(G8="","",IF(G8="A",8+I8,IF(G8="B",16+I8,IF(G8="C",24+I8,"invalid"))))</f>
         <v>19</v>
       </c>
-      <c r="K8" s="382">
+      <c r="K8" s="407">
         <f t="shared" ref="K8:K44" si="2">IF(J8="","",2^(32-J8))</f>
         <v>8192</v>
       </c>
@@ -14537,11 +14538,11 @@
       <c r="F9" s="214" t="s">
         <v>389</v>
       </c>
-      <c r="G9" s="374"/>
-      <c r="H9" s="374"/>
-      <c r="I9" s="374"/>
-      <c r="J9" s="374"/>
-      <c r="K9" s="383"/>
+      <c r="G9" s="405"/>
+      <c r="H9" s="405"/>
+      <c r="I9" s="405"/>
+      <c r="J9" s="405"/>
+      <c r="K9" s="408"/>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="237" t="s">
@@ -14562,11 +14563,11 @@
       <c r="F10" s="212" t="s">
         <v>389</v>
       </c>
-      <c r="G10" s="374"/>
-      <c r="H10" s="374"/>
-      <c r="I10" s="374"/>
-      <c r="J10" s="374"/>
-      <c r="K10" s="383"/>
+      <c r="G10" s="405"/>
+      <c r="H10" s="405"/>
+      <c r="I10" s="405"/>
+      <c r="J10" s="405"/>
+      <c r="K10" s="408"/>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="238" t="s">
@@ -14587,11 +14588,11 @@
       <c r="F11" s="216" t="s">
         <v>389</v>
       </c>
-      <c r="G11" s="374"/>
-      <c r="H11" s="374"/>
-      <c r="I11" s="374"/>
-      <c r="J11" s="374"/>
-      <c r="K11" s="383"/>
+      <c r="G11" s="405"/>
+      <c r="H11" s="405"/>
+      <c r="I11" s="405"/>
+      <c r="J11" s="405"/>
+      <c r="K11" s="408"/>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="237" t="s">
@@ -14612,11 +14613,11 @@
       <c r="F12" s="212" t="s">
         <v>389</v>
       </c>
-      <c r="G12" s="374"/>
-      <c r="H12" s="374"/>
-      <c r="I12" s="374"/>
-      <c r="J12" s="374"/>
-      <c r="K12" s="383"/>
+      <c r="G12" s="405"/>
+      <c r="H12" s="405"/>
+      <c r="I12" s="405"/>
+      <c r="J12" s="405"/>
+      <c r="K12" s="408"/>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="236" t="s">
@@ -14637,11 +14638,11 @@
       <c r="F13" s="214" t="s">
         <v>389</v>
       </c>
-      <c r="G13" s="374"/>
-      <c r="H13" s="374"/>
-      <c r="I13" s="374"/>
-      <c r="J13" s="374"/>
-      <c r="K13" s="383"/>
+      <c r="G13" s="405"/>
+      <c r="H13" s="405"/>
+      <c r="I13" s="405"/>
+      <c r="J13" s="405"/>
+      <c r="K13" s="408"/>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="237" t="s">
@@ -14662,11 +14663,11 @@
       <c r="F14" s="212" t="s">
         <v>389</v>
       </c>
-      <c r="G14" s="374"/>
-      <c r="H14" s="374"/>
-      <c r="I14" s="374"/>
-      <c r="J14" s="374"/>
-      <c r="K14" s="383"/>
+      <c r="G14" s="405"/>
+      <c r="H14" s="405"/>
+      <c r="I14" s="405"/>
+      <c r="J14" s="405"/>
+      <c r="K14" s="408"/>
     </row>
     <row r="15" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="239" t="s">
@@ -14687,11 +14688,11 @@
       <c r="F15" s="241" t="s">
         <v>389</v>
       </c>
-      <c r="G15" s="375"/>
-      <c r="H15" s="375"/>
-      <c r="I15" s="375"/>
-      <c r="J15" s="375"/>
-      <c r="K15" s="384"/>
+      <c r="G15" s="406"/>
+      <c r="H15" s="406"/>
+      <c r="I15" s="406"/>
+      <c r="J15" s="406"/>
+      <c r="K15" s="409"/>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="242" t="s">
@@ -14712,21 +14713,21 @@
       <c r="F16" s="245">
         <v>255255255192</v>
       </c>
-      <c r="G16" s="376" t="s">
+      <c r="G16" s="401" t="s">
         <v>111</v>
       </c>
-      <c r="H16" s="376">
+      <c r="H16" s="401">
         <v>4</v>
       </c>
-      <c r="I16" s="376">
+      <c r="I16" s="401">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="J16" s="376">
+      <c r="J16" s="401">
         <f t="shared" si="1"/>
         <v>26</v>
       </c>
-      <c r="K16" s="379">
+      <c r="K16" s="398">
         <f t="shared" si="2"/>
         <v>64</v>
       </c>
@@ -14750,11 +14751,11 @@
       <c r="F17" s="225">
         <v>255255255192</v>
       </c>
-      <c r="G17" s="377"/>
-      <c r="H17" s="377"/>
-      <c r="I17" s="377"/>
-      <c r="J17" s="377"/>
-      <c r="K17" s="380"/>
+      <c r="G17" s="402"/>
+      <c r="H17" s="402"/>
+      <c r="I17" s="402"/>
+      <c r="J17" s="402"/>
+      <c r="K17" s="399"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="237" t="s">
@@ -14775,11 +14776,11 @@
       <c r="F18" s="224">
         <v>255255255192</v>
       </c>
-      <c r="G18" s="377"/>
-      <c r="H18" s="377"/>
-      <c r="I18" s="377"/>
-      <c r="J18" s="377"/>
-      <c r="K18" s="380"/>
+      <c r="G18" s="402"/>
+      <c r="H18" s="402"/>
+      <c r="I18" s="402"/>
+      <c r="J18" s="402"/>
+      <c r="K18" s="399"/>
     </row>
     <row r="19" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="239" t="s">
@@ -14800,11 +14801,11 @@
       <c r="F19" s="246">
         <v>255255255192</v>
       </c>
-      <c r="G19" s="378"/>
-      <c r="H19" s="378"/>
-      <c r="I19" s="378"/>
-      <c r="J19" s="378"/>
-      <c r="K19" s="381"/>
+      <c r="G19" s="403"/>
+      <c r="H19" s="403"/>
+      <c r="I19" s="403"/>
+      <c r="J19" s="403"/>
+      <c r="K19" s="400"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="242" t="s">
@@ -14825,21 +14826,21 @@
       <c r="F20" s="244" t="s">
         <v>440</v>
       </c>
-      <c r="G20" s="373" t="s">
+      <c r="G20" s="404" t="s">
         <v>108</v>
       </c>
-      <c r="H20" s="373">
+      <c r="H20" s="404">
         <v>20</v>
       </c>
-      <c r="I20" s="373">
+      <c r="I20" s="404">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="J20" s="373">
+      <c r="J20" s="404">
         <f t="shared" si="1"/>
         <v>13</v>
       </c>
-      <c r="K20" s="382">
+      <c r="K20" s="407">
         <f t="shared" si="2"/>
         <v>524288</v>
       </c>
@@ -14863,11 +14864,11 @@
       <c r="F21" s="214" t="s">
         <v>440</v>
       </c>
-      <c r="G21" s="374"/>
-      <c r="H21" s="374"/>
-      <c r="I21" s="374"/>
-      <c r="J21" s="374"/>
-      <c r="K21" s="383"/>
+      <c r="G21" s="405"/>
+      <c r="H21" s="405"/>
+      <c r="I21" s="405"/>
+      <c r="J21" s="405"/>
+      <c r="K21" s="408"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="237" t="s">
@@ -14888,11 +14889,11 @@
       <c r="F22" s="212" t="s">
         <v>440</v>
       </c>
-      <c r="G22" s="374"/>
-      <c r="H22" s="374"/>
-      <c r="I22" s="374"/>
-      <c r="J22" s="374"/>
-      <c r="K22" s="383"/>
+      <c r="G22" s="405"/>
+      <c r="H22" s="405"/>
+      <c r="I22" s="405"/>
+      <c r="J22" s="405"/>
+      <c r="K22" s="408"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="238" t="s">
@@ -14913,11 +14914,11 @@
       <c r="F23" s="216" t="s">
         <v>440</v>
       </c>
-      <c r="G23" s="374"/>
-      <c r="H23" s="374"/>
-      <c r="I23" s="374"/>
-      <c r="J23" s="374"/>
-      <c r="K23" s="383"/>
+      <c r="G23" s="405"/>
+      <c r="H23" s="405"/>
+      <c r="I23" s="405"/>
+      <c r="J23" s="405"/>
+      <c r="K23" s="408"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="237" t="s">
@@ -14938,11 +14939,11 @@
       <c r="F24" s="212" t="s">
         <v>440</v>
       </c>
-      <c r="G24" s="374"/>
-      <c r="H24" s="374"/>
-      <c r="I24" s="374"/>
-      <c r="J24" s="374"/>
-      <c r="K24" s="383"/>
+      <c r="G24" s="405"/>
+      <c r="H24" s="405"/>
+      <c r="I24" s="405"/>
+      <c r="J24" s="405"/>
+      <c r="K24" s="408"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="236" t="s">
@@ -14963,11 +14964,11 @@
       <c r="F25" s="214" t="s">
         <v>440</v>
       </c>
-      <c r="G25" s="374"/>
-      <c r="H25" s="374"/>
-      <c r="I25" s="374"/>
-      <c r="J25" s="374"/>
-      <c r="K25" s="383"/>
+      <c r="G25" s="405"/>
+      <c r="H25" s="405"/>
+      <c r="I25" s="405"/>
+      <c r="J25" s="405"/>
+      <c r="K25" s="408"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="237" t="s">
@@ -14988,11 +14989,11 @@
       <c r="F26" s="212" t="s">
         <v>440</v>
       </c>
-      <c r="G26" s="374"/>
-      <c r="H26" s="374"/>
-      <c r="I26" s="374"/>
-      <c r="J26" s="374"/>
-      <c r="K26" s="383"/>
+      <c r="G26" s="405"/>
+      <c r="H26" s="405"/>
+      <c r="I26" s="405"/>
+      <c r="J26" s="405"/>
+      <c r="K26" s="408"/>
     </row>
     <row r="27" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="239" t="s">
@@ -15013,11 +15014,11 @@
       <c r="F27" s="241" t="s">
         <v>440</v>
       </c>
-      <c r="G27" s="375"/>
-      <c r="H27" s="375"/>
-      <c r="I27" s="375"/>
-      <c r="J27" s="375"/>
-      <c r="K27" s="384"/>
+      <c r="G27" s="406"/>
+      <c r="H27" s="406"/>
+      <c r="I27" s="406"/>
+      <c r="J27" s="406"/>
+      <c r="K27" s="409"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="242" t="s">
@@ -15038,21 +15039,21 @@
       <c r="F28" s="244" t="s">
         <v>440</v>
       </c>
-      <c r="G28" s="376" t="s">
+      <c r="G28" s="401" t="s">
         <v>108</v>
       </c>
-      <c r="H28" s="376">
+      <c r="H28" s="401">
         <v>20</v>
       </c>
-      <c r="I28" s="376">
+      <c r="I28" s="401">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="J28" s="376">
+      <c r="J28" s="401">
         <f t="shared" ref="J28" si="3">IF(G28="","",IF(G28="A",8+I28,IF(G28="B",16+I28,IF(G28="C",24+I28,"invalid"))))</f>
         <v>13</v>
       </c>
-      <c r="K28" s="379">
+      <c r="K28" s="398">
         <f t="shared" si="2"/>
         <v>524288</v>
       </c>
@@ -15076,11 +15077,11 @@
       <c r="F29" s="214" t="s">
         <v>440</v>
       </c>
-      <c r="G29" s="377"/>
-      <c r="H29" s="377"/>
-      <c r="I29" s="377"/>
-      <c r="J29" s="377"/>
-      <c r="K29" s="380"/>
+      <c r="G29" s="402"/>
+      <c r="H29" s="402"/>
+      <c r="I29" s="402"/>
+      <c r="J29" s="402"/>
+      <c r="K29" s="399"/>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="237" t="s">
@@ -15101,11 +15102,11 @@
       <c r="F30" s="212" t="s">
         <v>440</v>
       </c>
-      <c r="G30" s="377"/>
-      <c r="H30" s="377"/>
-      <c r="I30" s="377"/>
-      <c r="J30" s="377"/>
-      <c r="K30" s="380"/>
+      <c r="G30" s="402"/>
+      <c r="H30" s="402"/>
+      <c r="I30" s="402"/>
+      <c r="J30" s="402"/>
+      <c r="K30" s="399"/>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="238" t="s">
@@ -15126,11 +15127,11 @@
       <c r="F31" s="216" t="s">
         <v>440</v>
       </c>
-      <c r="G31" s="377"/>
-      <c r="H31" s="377"/>
-      <c r="I31" s="377"/>
-      <c r="J31" s="377"/>
-      <c r="K31" s="380"/>
+      <c r="G31" s="402"/>
+      <c r="H31" s="402"/>
+      <c r="I31" s="402"/>
+      <c r="J31" s="402"/>
+      <c r="K31" s="399"/>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="237" t="s">
@@ -15151,11 +15152,11 @@
       <c r="F32" s="212" t="s">
         <v>440</v>
       </c>
-      <c r="G32" s="377"/>
-      <c r="H32" s="377"/>
-      <c r="I32" s="377"/>
-      <c r="J32" s="377"/>
-      <c r="K32" s="380"/>
+      <c r="G32" s="402"/>
+      <c r="H32" s="402"/>
+      <c r="I32" s="402"/>
+      <c r="J32" s="402"/>
+      <c r="K32" s="399"/>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="236" t="s">
@@ -15176,11 +15177,11 @@
       <c r="F33" s="214" t="s">
         <v>440</v>
       </c>
-      <c r="G33" s="377"/>
-      <c r="H33" s="377"/>
-      <c r="I33" s="377"/>
-      <c r="J33" s="377"/>
-      <c r="K33" s="380"/>
+      <c r="G33" s="402"/>
+      <c r="H33" s="402"/>
+      <c r="I33" s="402"/>
+      <c r="J33" s="402"/>
+      <c r="K33" s="399"/>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="237" t="s">
@@ -15201,11 +15202,11 @@
       <c r="F34" s="212" t="s">
         <v>440</v>
       </c>
-      <c r="G34" s="377"/>
-      <c r="H34" s="377"/>
-      <c r="I34" s="377"/>
-      <c r="J34" s="377"/>
-      <c r="K34" s="380"/>
+      <c r="G34" s="402"/>
+      <c r="H34" s="402"/>
+      <c r="I34" s="402"/>
+      <c r="J34" s="402"/>
+      <c r="K34" s="399"/>
     </row>
     <row r="35" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="239" t="s">
@@ -15226,11 +15227,11 @@
       <c r="F35" s="241" t="s">
         <v>440</v>
       </c>
-      <c r="G35" s="378"/>
-      <c r="H35" s="378"/>
-      <c r="I35" s="378"/>
-      <c r="J35" s="378"/>
-      <c r="K35" s="381"/>
+      <c r="G35" s="403"/>
+      <c r="H35" s="403"/>
+      <c r="I35" s="403"/>
+      <c r="J35" s="403"/>
+      <c r="K35" s="400"/>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="242" t="s">
@@ -15251,21 +15252,21 @@
       <c r="F36" s="244" t="s">
         <v>440</v>
       </c>
-      <c r="G36" s="373" t="s">
+      <c r="G36" s="404" t="s">
         <v>108</v>
       </c>
-      <c r="H36" s="373">
+      <c r="H36" s="404">
         <v>20</v>
       </c>
-      <c r="I36" s="373">
+      <c r="I36" s="404">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="J36" s="373">
+      <c r="J36" s="404">
         <f t="shared" ref="J36" si="4">IF(G36="","",IF(G36="A",8+I36,IF(G36="B",16+I36,IF(G36="C",24+I36,"invalid"))))</f>
         <v>13</v>
       </c>
-      <c r="K36" s="382">
+      <c r="K36" s="407">
         <f t="shared" si="2"/>
         <v>524288</v>
       </c>
@@ -15289,11 +15290,11 @@
       <c r="F37" s="214" t="s">
         <v>440</v>
       </c>
-      <c r="G37" s="374"/>
-      <c r="H37" s="374"/>
-      <c r="I37" s="374"/>
-      <c r="J37" s="374"/>
-      <c r="K37" s="383"/>
+      <c r="G37" s="405"/>
+      <c r="H37" s="405"/>
+      <c r="I37" s="405"/>
+      <c r="J37" s="405"/>
+      <c r="K37" s="408"/>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="237" t="s">
@@ -15314,11 +15315,11 @@
       <c r="F38" s="212" t="s">
         <v>440</v>
       </c>
-      <c r="G38" s="374"/>
-      <c r="H38" s="374"/>
-      <c r="I38" s="374"/>
-      <c r="J38" s="374"/>
-      <c r="K38" s="383"/>
+      <c r="G38" s="405"/>
+      <c r="H38" s="405"/>
+      <c r="I38" s="405"/>
+      <c r="J38" s="405"/>
+      <c r="K38" s="408"/>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="238" t="s">
@@ -15339,11 +15340,11 @@
       <c r="F39" s="216" t="s">
         <v>440</v>
       </c>
-      <c r="G39" s="374"/>
-      <c r="H39" s="374"/>
-      <c r="I39" s="374"/>
-      <c r="J39" s="374"/>
-      <c r="K39" s="383"/>
+      <c r="G39" s="405"/>
+      <c r="H39" s="405"/>
+      <c r="I39" s="405"/>
+      <c r="J39" s="405"/>
+      <c r="K39" s="408"/>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" s="237" t="s">
@@ -15364,11 +15365,11 @@
       <c r="F40" s="212" t="s">
         <v>440</v>
       </c>
-      <c r="G40" s="374"/>
-      <c r="H40" s="374"/>
-      <c r="I40" s="374"/>
-      <c r="J40" s="374"/>
-      <c r="K40" s="383"/>
+      <c r="G40" s="405"/>
+      <c r="H40" s="405"/>
+      <c r="I40" s="405"/>
+      <c r="J40" s="405"/>
+      <c r="K40" s="408"/>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" s="236" t="s">
@@ -15389,11 +15390,11 @@
       <c r="F41" s="214" t="s">
         <v>440</v>
       </c>
-      <c r="G41" s="374"/>
-      <c r="H41" s="374"/>
-      <c r="I41" s="374"/>
-      <c r="J41" s="374"/>
-      <c r="K41" s="383"/>
+      <c r="G41" s="405"/>
+      <c r="H41" s="405"/>
+      <c r="I41" s="405"/>
+      <c r="J41" s="405"/>
+      <c r="K41" s="408"/>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" s="237" t="s">
@@ -15414,11 +15415,11 @@
       <c r="F42" s="212" t="s">
         <v>440</v>
       </c>
-      <c r="G42" s="374"/>
-      <c r="H42" s="374"/>
-      <c r="I42" s="374"/>
-      <c r="J42" s="374"/>
-      <c r="K42" s="383"/>
+      <c r="G42" s="405"/>
+      <c r="H42" s="405"/>
+      <c r="I42" s="405"/>
+      <c r="J42" s="405"/>
+      <c r="K42" s="408"/>
     </row>
     <row r="43" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="239" t="s">
@@ -15439,11 +15440,11 @@
       <c r="F43" s="241" t="s">
         <v>440</v>
       </c>
-      <c r="G43" s="375"/>
-      <c r="H43" s="375"/>
-      <c r="I43" s="375"/>
-      <c r="J43" s="375"/>
-      <c r="K43" s="384"/>
+      <c r="G43" s="406"/>
+      <c r="H43" s="406"/>
+      <c r="I43" s="406"/>
+      <c r="J43" s="406"/>
+      <c r="K43" s="409"/>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="242" t="s">
@@ -15464,21 +15465,21 @@
       <c r="F44" s="244" t="s">
         <v>440</v>
       </c>
-      <c r="G44" s="376" t="s">
+      <c r="G44" s="401" t="s">
         <v>108</v>
       </c>
-      <c r="H44" s="376">
+      <c r="H44" s="401">
         <v>20</v>
       </c>
-      <c r="I44" s="376">
+      <c r="I44" s="401">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="J44" s="376">
+      <c r="J44" s="401">
         <f t="shared" ref="J44" si="5">IF(G44="","",IF(G44="A",8+I44,IF(G44="B",16+I44,IF(G44="C",24+I44,"invalid"))))</f>
         <v>13</v>
       </c>
-      <c r="K44" s="379">
+      <c r="K44" s="398">
         <f t="shared" si="2"/>
         <v>524288</v>
       </c>
@@ -15502,11 +15503,11 @@
       <c r="F45" s="214" t="s">
         <v>440</v>
       </c>
-      <c r="G45" s="377"/>
-      <c r="H45" s="377"/>
-      <c r="I45" s="377"/>
-      <c r="J45" s="377"/>
-      <c r="K45" s="380"/>
+      <c r="G45" s="402"/>
+      <c r="H45" s="402"/>
+      <c r="I45" s="402"/>
+      <c r="J45" s="402"/>
+      <c r="K45" s="399"/>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" s="237" t="s">
@@ -15527,11 +15528,11 @@
       <c r="F46" s="212" t="s">
         <v>440</v>
       </c>
-      <c r="G46" s="377"/>
-      <c r="H46" s="377"/>
-      <c r="I46" s="377"/>
-      <c r="J46" s="377"/>
-      <c r="K46" s="380"/>
+      <c r="G46" s="402"/>
+      <c r="H46" s="402"/>
+      <c r="I46" s="402"/>
+      <c r="J46" s="402"/>
+      <c r="K46" s="399"/>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" s="238" t="s">
@@ -15552,11 +15553,11 @@
       <c r="F47" s="216" t="s">
         <v>440</v>
       </c>
-      <c r="G47" s="377"/>
-      <c r="H47" s="377"/>
-      <c r="I47" s="377"/>
-      <c r="J47" s="377"/>
-      <c r="K47" s="380"/>
+      <c r="G47" s="402"/>
+      <c r="H47" s="402"/>
+      <c r="I47" s="402"/>
+      <c r="J47" s="402"/>
+      <c r="K47" s="399"/>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" s="237" t="s">
@@ -15577,11 +15578,11 @@
       <c r="F48" s="212" t="s">
         <v>440</v>
       </c>
-      <c r="G48" s="377"/>
-      <c r="H48" s="377"/>
-      <c r="I48" s="377"/>
-      <c r="J48" s="377"/>
-      <c r="K48" s="380"/>
+      <c r="G48" s="402"/>
+      <c r="H48" s="402"/>
+      <c r="I48" s="402"/>
+      <c r="J48" s="402"/>
+      <c r="K48" s="399"/>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" s="236" t="s">
@@ -15602,11 +15603,11 @@
       <c r="F49" s="214" t="s">
         <v>440</v>
       </c>
-      <c r="G49" s="377"/>
-      <c r="H49" s="377"/>
-      <c r="I49" s="377"/>
-      <c r="J49" s="377"/>
-      <c r="K49" s="380"/>
+      <c r="G49" s="402"/>
+      <c r="H49" s="402"/>
+      <c r="I49" s="402"/>
+      <c r="J49" s="402"/>
+      <c r="K49" s="399"/>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" s="237" t="s">
@@ -15627,11 +15628,11 @@
       <c r="F50" s="212" t="s">
         <v>440</v>
       </c>
-      <c r="G50" s="377"/>
-      <c r="H50" s="377"/>
-      <c r="I50" s="377"/>
-      <c r="J50" s="377"/>
-      <c r="K50" s="380"/>
+      <c r="G50" s="402"/>
+      <c r="H50" s="402"/>
+      <c r="I50" s="402"/>
+      <c r="J50" s="402"/>
+      <c r="K50" s="399"/>
     </row>
     <row r="51" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="239" t="s">
@@ -15652,11 +15653,11 @@
       <c r="F51" s="241" t="s">
         <v>440</v>
       </c>
-      <c r="G51" s="378"/>
-      <c r="H51" s="378"/>
-      <c r="I51" s="378"/>
-      <c r="J51" s="378"/>
-      <c r="K51" s="381"/>
+      <c r="G51" s="403"/>
+      <c r="H51" s="403"/>
+      <c r="I51" s="403"/>
+      <c r="J51" s="403"/>
+      <c r="K51" s="400"/>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="G52" s="229"/>
@@ -15666,13 +15667,27 @@
     </row>
   </sheetData>
   <mergeCells count="37">
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="K4:K7"/>
-    <mergeCell ref="J4:J7"/>
-    <mergeCell ref="I4:I7"/>
-    <mergeCell ref="H4:H7"/>
-    <mergeCell ref="G4:G7"/>
+    <mergeCell ref="H36:H43"/>
+    <mergeCell ref="H44:H51"/>
+    <mergeCell ref="I44:I51"/>
+    <mergeCell ref="J44:J51"/>
+    <mergeCell ref="K44:K51"/>
+    <mergeCell ref="K36:K43"/>
+    <mergeCell ref="J36:J43"/>
+    <mergeCell ref="I36:I43"/>
+    <mergeCell ref="H20:H27"/>
+    <mergeCell ref="I20:I27"/>
+    <mergeCell ref="J20:J27"/>
+    <mergeCell ref="K20:K27"/>
+    <mergeCell ref="H28:H35"/>
+    <mergeCell ref="I28:I35"/>
+    <mergeCell ref="J28:J35"/>
+    <mergeCell ref="K28:K35"/>
+    <mergeCell ref="G20:G27"/>
+    <mergeCell ref="G28:G35"/>
+    <mergeCell ref="G36:G43"/>
+    <mergeCell ref="G44:G51"/>
+    <mergeCell ref="G16:G19"/>
     <mergeCell ref="H16:H19"/>
     <mergeCell ref="I16:I19"/>
     <mergeCell ref="J16:J19"/>
@@ -15682,27 +15697,13 @@
     <mergeCell ref="I8:I15"/>
     <mergeCell ref="J8:J15"/>
     <mergeCell ref="K8:K15"/>
-    <mergeCell ref="G20:G27"/>
-    <mergeCell ref="G28:G35"/>
-    <mergeCell ref="G36:G43"/>
-    <mergeCell ref="G44:G51"/>
-    <mergeCell ref="G16:G19"/>
-    <mergeCell ref="H20:H27"/>
-    <mergeCell ref="I20:I27"/>
-    <mergeCell ref="J20:J27"/>
-    <mergeCell ref="K20:K27"/>
-    <mergeCell ref="H28:H35"/>
-    <mergeCell ref="I28:I35"/>
-    <mergeCell ref="J28:J35"/>
-    <mergeCell ref="K28:K35"/>
-    <mergeCell ref="H36:H43"/>
-    <mergeCell ref="H44:H51"/>
-    <mergeCell ref="I44:I51"/>
-    <mergeCell ref="J44:J51"/>
-    <mergeCell ref="K44:K51"/>
-    <mergeCell ref="K36:K43"/>
-    <mergeCell ref="J36:J43"/>
-    <mergeCell ref="I36:I43"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="K4:K7"/>
+    <mergeCell ref="J4:J7"/>
+    <mergeCell ref="I4:I7"/>
+    <mergeCell ref="H4:H7"/>
+    <mergeCell ref="G4:G7"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -15751,11 +15752,11 @@
       <c r="A1" t="s">
         <v>392</v>
       </c>
-      <c r="G1" s="388" t="s">
+      <c r="G1" s="397" t="s">
         <v>574</v>
       </c>
-      <c r="H1" s="388"/>
-      <c r="I1" s="388"/>
+      <c r="H1" s="397"/>
+      <c r="I1" s="397"/>
       <c r="J1" s="226" t="s">
         <v>471</v>
       </c>
@@ -15785,17 +15786,17 @@
       </c>
     </row>
     <row r="2" spans="1:29" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="395"/>
-      <c r="B2" s="395"/>
-      <c r="C2" s="395"/>
-      <c r="D2" s="395"/>
-      <c r="E2" s="395"/>
-      <c r="F2" s="395"/>
-      <c r="G2" s="385" t="s">
+      <c r="A2" s="416"/>
+      <c r="B2" s="416"/>
+      <c r="C2" s="416"/>
+      <c r="D2" s="416"/>
+      <c r="E2" s="416"/>
+      <c r="F2" s="416"/>
+      <c r="G2" s="394" t="s">
         <v>575</v>
       </c>
-      <c r="H2" s="386"/>
-      <c r="I2" s="387"/>
+      <c r="H2" s="395"/>
+      <c r="I2" s="396"/>
       <c r="J2" s="230" t="s">
         <v>445</v>
       </c>
@@ -15932,7 +15933,7 @@
         <f>IF(O4="","",32-O4)</f>
         <v>25</v>
       </c>
-      <c r="R4" s="392" t="s">
+      <c r="R4" s="413" t="s">
         <v>612</v>
       </c>
     </row>
@@ -15985,7 +15986,7 @@
         <f t="shared" ref="Q5:Q8" si="2">IF(O5="","",32-O5)</f>
         <v>26</v>
       </c>
-      <c r="R5" s="393"/>
+      <c r="R5" s="414"/>
     </row>
     <row r="6" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -16036,7 +16037,7 @@
         <f t="shared" si="2"/>
         <v>26</v>
       </c>
-      <c r="R6" s="393"/>
+      <c r="R6" s="414"/>
       <c r="AC6" s="33"/>
     </row>
     <row r="7" spans="1:29" x14ac:dyDescent="0.25">
@@ -16088,7 +16089,7 @@
         <f t="shared" si="2"/>
         <v>27</v>
       </c>
-      <c r="R7" s="393"/>
+      <c r="R7" s="414"/>
       <c r="AC7" s="33"/>
     </row>
     <row r="8" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -16140,7 +16141,7 @@
         <f t="shared" si="2"/>
         <v>29</v>
       </c>
-      <c r="R8" s="394"/>
+      <c r="R8" s="415"/>
       <c r="AC8" s="33"/>
     </row>
     <row r="9" spans="1:29" x14ac:dyDescent="0.25">
@@ -16183,7 +16184,7 @@
         <f>IF(O9="","",32-O9)</f>
         <v>25</v>
       </c>
-      <c r="R9" s="389" t="s">
+      <c r="R9" s="410" t="s">
         <v>613</v>
       </c>
       <c r="AC9" s="33"/>
@@ -16225,7 +16226,7 @@
         <f>IF(O10="","",32-O10)</f>
         <v>26</v>
       </c>
-      <c r="R10" s="390"/>
+      <c r="R10" s="411"/>
       <c r="AC10" s="33"/>
     </row>
     <row r="11" spans="1:29" x14ac:dyDescent="0.25">
@@ -16283,7 +16284,7 @@
         <f>IF(O11="","",32-O11)</f>
         <v>27</v>
       </c>
-      <c r="R11" s="390"/>
+      <c r="R11" s="411"/>
     </row>
     <row r="12" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
@@ -16340,7 +16341,7 @@
         <f>IF(O12="","",32-O12)</f>
         <v>29</v>
       </c>
-      <c r="R12" s="390"/>
+      <c r="R12" s="411"/>
     </row>
     <row r="13" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
@@ -16397,7 +16398,7 @@
         <f>IF(O13="","",32-O13)</f>
         <v>26</v>
       </c>
-      <c r="R13" s="391"/>
+      <c r="R13" s="412"/>
     </row>
     <row r="14" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
@@ -16478,7 +16479,7 @@
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16493,173 +16494,173 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="403" t="s">
+      <c r="A1" s="289" t="s">
         <v>658</v>
       </c>
-      <c r="B1" s="404" t="s">
+      <c r="B1" s="290" t="s">
         <v>656</v>
       </c>
-      <c r="C1" s="404" t="s">
+      <c r="C1" s="290" t="s">
         <v>657</v>
       </c>
-      <c r="E1" s="316" t="s">
+      <c r="E1" s="337" t="s">
         <v>662</v>
       </c>
-      <c r="F1" s="316"/>
-      <c r="G1" s="316"/>
-      <c r="H1" s="316"/>
+      <c r="F1" s="337"/>
+      <c r="G1" s="337"/>
+      <c r="H1" s="337"/>
     </row>
     <row r="2" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="411" t="s">
+      <c r="A2" s="297" t="s">
         <v>675</v>
       </c>
-      <c r="B2" s="412" t="s">
+      <c r="B2" s="298" t="s">
         <v>676</v>
       </c>
-      <c r="C2" s="412" t="s">
+      <c r="C2" s="298" t="s">
         <v>677</v>
       </c>
-      <c r="E2" s="403" t="s">
+      <c r="E2" s="289" t="s">
         <v>646</v>
       </c>
-      <c r="F2" s="404" t="s">
+      <c r="F2" s="290" t="s">
         <v>647</v>
       </c>
-      <c r="G2" s="404" t="s">
+      <c r="G2" s="290" t="s">
         <v>228</v>
       </c>
-      <c r="H2" s="403" t="s">
+      <c r="H2" s="289" t="s">
         <v>663</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="413" t="s">
+      <c r="A3" s="299" t="s">
         <v>668</v>
       </c>
-      <c r="B3" s="414" t="s">
+      <c r="B3" s="300" t="s">
         <v>666</v>
       </c>
-      <c r="C3" s="414" t="s">
+      <c r="C3" s="300" t="s">
         <v>667</v>
       </c>
-      <c r="E3" s="408" t="s">
+      <c r="E3" s="294" t="s">
         <v>644</v>
       </c>
-      <c r="F3" s="405">
+      <c r="F3" s="291">
         <v>0</v>
       </c>
-      <c r="G3" s="405">
+      <c r="G3" s="291">
         <v>1023</v>
       </c>
-      <c r="H3" s="408" t="s">
+      <c r="H3" s="294" t="s">
         <v>648</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="415" t="s">
+      <c r="A4" s="301" t="s">
         <v>672</v>
       </c>
-      <c r="B4" s="416" t="s">
+      <c r="B4" s="302" t="s">
         <v>669</v>
       </c>
-      <c r="C4" s="416" t="s">
+      <c r="C4" s="302" t="s">
         <v>670</v>
       </c>
-      <c r="E4" s="409" t="s">
+      <c r="E4" s="295" t="s">
         <v>643</v>
       </c>
-      <c r="F4" s="406">
+      <c r="F4" s="292">
         <v>1024</v>
       </c>
-      <c r="G4" s="406">
+      <c r="G4" s="292">
         <v>49151</v>
       </c>
-      <c r="H4" s="409" t="s">
+      <c r="H4" s="295" t="s">
         <v>664</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="413" t="s">
+      <c r="A5" s="299" t="s">
         <v>654</v>
       </c>
-      <c r="B5" s="414" t="s">
+      <c r="B5" s="300" t="s">
         <v>673</v>
       </c>
-      <c r="C5" s="414" t="s">
+      <c r="C5" s="300" t="s">
         <v>674</v>
       </c>
-      <c r="E5" s="410" t="s">
+      <c r="E5" s="296" t="s">
         <v>645</v>
       </c>
-      <c r="F5" s="407">
+      <c r="F5" s="293">
         <v>49152</v>
       </c>
-      <c r="G5" s="407">
+      <c r="G5" s="293">
         <v>65535</v>
       </c>
-      <c r="H5" s="410" t="s">
+      <c r="H5" s="296" t="s">
         <v>649</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="415" t="s">
+      <c r="A6" s="301" t="s">
         <v>671</v>
       </c>
-      <c r="B6" s="416" t="s">
+      <c r="B6" s="302" t="s">
         <v>650</v>
       </c>
-      <c r="C6" s="416" t="s">
+      <c r="C6" s="302" t="s">
         <v>651</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="413" t="s">
+      <c r="A7" s="299" t="s">
         <v>659</v>
       </c>
-      <c r="B7" s="414" t="s">
+      <c r="B7" s="300" t="s">
         <v>660</v>
       </c>
-      <c r="C7" s="414" t="s">
+      <c r="C7" s="300" t="s">
         <v>653</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="415" t="s">
+      <c r="A8" s="301" t="s">
         <v>678</v>
       </c>
-      <c r="B8" s="416" t="s">
+      <c r="B8" s="302" t="s">
         <v>652</v>
       </c>
-      <c r="C8" s="416" t="s">
+      <c r="C8" s="302" t="s">
         <v>661</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="413" t="s">
+      <c r="A9" s="299" t="s">
         <v>655</v>
       </c>
-      <c r="B9" s="414" t="s">
+      <c r="B9" s="300" t="s">
         <v>679</v>
       </c>
-      <c r="C9" s="414" t="s">
+      <c r="C9" s="300" t="s">
         <v>680</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="415" t="s">
+      <c r="A10" s="301" t="s">
         <v>665</v>
       </c>
-      <c r="B10" s="416" t="s">
+      <c r="B10" s="302" t="s">
         <v>681</v>
       </c>
-      <c r="C10" s="416" t="s">
+      <c r="C10" s="302" t="s">
         <v>682</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="413"/>
-      <c r="B11" s="414"/>
-      <c r="C11" s="414"/>
+      <c r="A11" s="299"/>
+      <c r="B11" s="300"/>
+      <c r="C11" s="300"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Documentacion Capa de Red
</commit_message>
<xml_diff>
--- a/docs/protocol-suite.xlsx
+++ b/docs/protocol-suite.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EducacionIT\Documents\networks\CISCO\saves\ccna1-lx20\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{122B050A-430D-485F-96BA-004DB9BFF1B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE61336A-2EAA-4DC7-951F-8E891ABF4314}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="5" xr2:uid="{A284E486-C6D6-48E7-9614-2E5470B19042}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="6" xr2:uid="{A284E486-C6D6-48E7-9614-2E5470B19042}"/>
   </bookViews>
   <sheets>
     <sheet name="Modelos" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="Sist." sheetId="4" r:id="rId4"/>
     <sheet name="IPv4" sheetId="5" r:id="rId5"/>
     <sheet name="classic" sheetId="6" r:id="rId6"/>
+    <sheet name="VLSM" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="670" uniqueCount="445">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="719" uniqueCount="482">
   <si>
     <t>osi de iso</t>
   </si>
@@ -2263,6 +2264,117 @@
       </rPr>
       <t>192</t>
     </r>
+  </si>
+  <si>
+    <t>VLSM</t>
+  </si>
+  <si>
+    <t>Practica de subnetting que prioriza la cantidad de hosts por encima de la porcion de subred</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>Bits Host</t>
+  </si>
+  <si>
+    <t>2^h - 2 &gt;= H</t>
+  </si>
+  <si>
+    <t>Depto</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>e</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>32 - h</t>
+  </si>
+  <si>
+    <t>Last Bit 1</t>
+  </si>
+  <si>
+    <t>RED</t>
+  </si>
+  <si>
+    <t>Mask</t>
+  </si>
+  <si>
+    <t>10.0.0.1</t>
+  </si>
+  <si>
+    <t>10.0.0.128</t>
+  </si>
+  <si>
+    <t>10.0.0.129</t>
+  </si>
+  <si>
+    <t>10.0.0.126</t>
+  </si>
+  <si>
+    <t>10.0.0.127</t>
+  </si>
+  <si>
+    <t>10.0.0.254</t>
+  </si>
+  <si>
+    <t>10.0.0.255</t>
+  </si>
+  <si>
+    <t>10.0.1.0</t>
+  </si>
+  <si>
+    <t>par</t>
+  </si>
+  <si>
+    <t>impar</t>
+  </si>
+  <si>
+    <t>10.0.1.1</t>
+  </si>
+  <si>
+    <t>10.0.1.64</t>
+  </si>
+  <si>
+    <t>10.0.1.63</t>
+  </si>
+  <si>
+    <t>10.0.1.62</t>
+  </si>
+  <si>
+    <t>10.0.1.96</t>
+  </si>
+  <si>
+    <t>10.0.1.97</t>
+  </si>
+  <si>
+    <t>10.0.1.95</t>
+  </si>
+  <si>
+    <t>10.0.1.112</t>
+  </si>
+  <si>
+    <t>10.0.1.110</t>
+  </si>
+  <si>
+    <t>10.0.1.111</t>
+  </si>
+  <si>
+    <t>10.0.1.94</t>
+  </si>
+  <si>
+    <t>Hosts2</t>
   </si>
 </sst>
 </file>
@@ -2273,14 +2385,7 @@
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2789,36 +2894,36 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="181">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -2830,14 +2935,14 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2875,13 +2980,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2905,10 +3010,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2923,7 +3028,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2996,9 +3101,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -3009,13 +3114,13 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="17" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3057,7 +3162,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -3069,8 +3174,8 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3130,85 +3235,16 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="10" borderId="17" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="8" fillId="10" borderId="17" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="17" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="17" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="10" borderId="16" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="8" fillId="10" borderId="16" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="20" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="10" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3229,10 +3265,10 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3242,25 +3278,97 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="3" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="3" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="20" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Énfasis1" xfId="1" builtinId="29"/>
     <cellStyle name="Millares" xfId="2" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="29">
+  <dxfs count="30">
+    <dxf>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -3833,13 +3941,13 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{0ADCD326-5B10-43FB-9AA2-AB768BBDBA9C}" name="Tabla1012" displayName="Tabla1012" ref="A19:G23" totalsRowShown="0">
   <autoFilter ref="A19:G23" xr:uid="{0ADCD326-5B10-43FB-9AA2-AB768BBDBA9C}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{DF50FB73-0BE7-4854-956E-C7023988D229}" name="Binario" dataDxfId="11"/>
+    <tableColumn id="1" xr3:uid="{DF50FB73-0BE7-4854-956E-C7023988D229}" name="Binario" dataDxfId="12"/>
     <tableColumn id="2" xr3:uid="{DE8352F4-3AF3-43A0-BB45-D5F5668CBB76}" name="Red"/>
-    <tableColumn id="3" xr3:uid="{20D54671-9004-432E-B6D6-FBA66370BAC2}" name="Primer IP" dataDxfId="10"/>
-    <tableColumn id="4" xr3:uid="{C9E4837C-B0D1-45D4-AC3A-2CB87026E30C}" name="Ultima IP" dataDxfId="9"/>
-    <tableColumn id="5" xr3:uid="{603009AB-2856-4410-B873-FC6522515A52}" name="Broadcast" dataDxfId="8"/>
-    <tableColumn id="6" xr3:uid="{EE8CE6EA-DB26-400E-B7DF-187FD3044ABA}" name="Mascara" dataDxfId="7"/>
-    <tableColumn id="7" xr3:uid="{64A7D0E0-5029-4FB2-8EAF-08BA13AC6510}" name="Hosts" dataDxfId="6" dataCellStyle="Millares"/>
+    <tableColumn id="3" xr3:uid="{20D54671-9004-432E-B6D6-FBA66370BAC2}" name="Primer IP" dataDxfId="11"/>
+    <tableColumn id="4" xr3:uid="{C9E4837C-B0D1-45D4-AC3A-2CB87026E30C}" name="Ultima IP" dataDxfId="10"/>
+    <tableColumn id="5" xr3:uid="{603009AB-2856-4410-B873-FC6522515A52}" name="Broadcast" dataDxfId="9"/>
+    <tableColumn id="6" xr3:uid="{EE8CE6EA-DB26-400E-B7DF-187FD3044ABA}" name="Mascara" dataDxfId="8"/>
+    <tableColumn id="7" xr3:uid="{64A7D0E0-5029-4FB2-8EAF-08BA13AC6510}" name="Hosts" dataDxfId="7" dataCellStyle="Millares"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3849,13 +3957,31 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{F4D1F3F3-C3A7-4A41-B3DE-DF427F97D09A}" name="Tabla101213" displayName="Tabla101213" ref="A27:G31" totalsRowShown="0">
   <autoFilter ref="A27:G31" xr:uid="{F4D1F3F3-C3A7-4A41-B3DE-DF427F97D09A}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{D1B2423F-C86A-4B39-AB38-96F9DD9BEF71}" name="Binario" dataDxfId="5"/>
+    <tableColumn id="1" xr3:uid="{D1B2423F-C86A-4B39-AB38-96F9DD9BEF71}" name="Binario" dataDxfId="6"/>
     <tableColumn id="2" xr3:uid="{16DB9FDF-15F8-4AF6-A562-7BAF42370F83}" name="Red"/>
-    <tableColumn id="3" xr3:uid="{E4368E94-D5DB-4EC6-9525-32C54F17D759}" name="Primer IP" dataDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{E3B008EB-2EC2-453A-A957-6DE3704D4332}" name="Ultima IP" dataDxfId="3"/>
-    <tableColumn id="5" xr3:uid="{406FF1E2-D54D-437E-A099-5D7101698894}" name="Broadcast" dataDxfId="2"/>
-    <tableColumn id="6" xr3:uid="{3633FA0A-4FF6-4978-B548-F7218383F997}" name="Mascara" dataDxfId="1"/>
-    <tableColumn id="7" xr3:uid="{C552E1B7-4D5D-4720-9190-356180982A87}" name="Hosts" dataDxfId="0" dataCellStyle="Millares"/>
+    <tableColumn id="3" xr3:uid="{E4368E94-D5DB-4EC6-9525-32C54F17D759}" name="Primer IP" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{E3B008EB-2EC2-453A-A957-6DE3704D4332}" name="Ultima IP" dataDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{406FF1E2-D54D-437E-A099-5D7101698894}" name="Broadcast" dataDxfId="3"/>
+    <tableColumn id="6" xr3:uid="{3633FA0A-4FF6-4978-B548-F7218383F997}" name="Mascara" dataDxfId="2"/>
+    <tableColumn id="7" xr3:uid="{C552E1B7-4D5D-4720-9190-356180982A87}" name="Hosts" dataDxfId="1" dataCellStyle="Millares"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{B2F2D2BB-D473-4C7E-8F49-EFFA8697289E}" name="Tabla9" displayName="Tabla9" ref="A6:I11" totalsRowShown="0">
+  <autoFilter ref="A6:I11" xr:uid="{B2F2D2BB-D473-4C7E-8F49-EFFA8697289E}"/>
+  <tableColumns count="9">
+    <tableColumn id="1" xr3:uid="{D9906D0F-3946-4551-80EF-E794B6763060}" name="Depto"/>
+    <tableColumn id="2" xr3:uid="{B76BD207-564D-4A40-B5DA-7BF31D94DFB2}" name="Hosts"/>
+    <tableColumn id="3" xr3:uid="{8C0C9E86-C925-46E4-B1BC-29615F12D011}" name="CIDR"/>
+    <tableColumn id="4" xr3:uid="{CF7ABD0A-6D10-4595-BDAC-7BA73453ABAF}" name="RED"/>
+    <tableColumn id="5" xr3:uid="{7BF44CD3-59C1-477F-879E-BC30F033B13B}" name="Primer IP"/>
+    <tableColumn id="6" xr3:uid="{DD6AB662-A048-4664-92D6-345C97C445DC}" name="Ultima IP"/>
+    <tableColumn id="7" xr3:uid="{017E9AD7-B745-43B5-81F0-79C3975FB105}" name="Broadcast"/>
+    <tableColumn id="8" xr3:uid="{462988E0-4B36-40BC-A6DB-50D0502BF978}" name="Mask" dataDxfId="0"/>
+    <tableColumn id="9" xr3:uid="{C576A661-4DDB-4C17-9D73-FAECEDEB0934}" name="Hosts2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3874,12 +4000,12 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{EEE4898D-F2C9-4799-9B27-1047E0B389B5}" name="Tabla3" displayName="Tabla3" ref="E11:G16" totalsRowShown="0" tableBorderDxfId="28">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{EEE4898D-F2C9-4799-9B27-1047E0B389B5}" name="Tabla3" displayName="Tabla3" ref="E11:G16" totalsRowShown="0" tableBorderDxfId="29">
   <autoFilter ref="E11:G16" xr:uid="{EEE4898D-F2C9-4799-9B27-1047E0B389B5}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{2CD52E63-0CF7-448F-AFB9-E1222BA3751A}" name="Unidad" dataDxfId="27"/>
-    <tableColumn id="2" xr3:uid="{7C167E46-06D4-494C-BDD1-BE076BFED87B}" name="Equivalencia" dataDxfId="26"/>
-    <tableColumn id="3" xr3:uid="{718EF86A-E60E-4E44-AA6E-6B9F80923B2B}" name="Decimal" dataDxfId="25"/>
+    <tableColumn id="1" xr3:uid="{2CD52E63-0CF7-448F-AFB9-E1222BA3751A}" name="Unidad" dataDxfId="28"/>
+    <tableColumn id="2" xr3:uid="{7C167E46-06D4-494C-BDD1-BE076BFED87B}" name="Equivalencia" dataDxfId="27"/>
+    <tableColumn id="3" xr3:uid="{718EF86A-E60E-4E44-AA6E-6B9F80923B2B}" name="Decimal" dataDxfId="26"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3924,7 +4050,7 @@
   <autoFilter ref="A2:C10" xr:uid="{45E7EA22-C177-4276-8B26-DDBEF03C3978}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{FC122938-914F-4524-8BC2-A2AB7E9EFA2F}" name="TIA-568A"/>
-    <tableColumn id="2" xr3:uid="{01E34A6D-5A3D-4AB9-978D-1A0E98329F04}" name="Funcion" dataDxfId="24"/>
+    <tableColumn id="2" xr3:uid="{01E34A6D-5A3D-4AB9-978D-1A0E98329F04}" name="Funcion" dataDxfId="25"/>
     <tableColumn id="3" xr3:uid="{DB624384-12B4-4D70-9C0C-F257659F54DB}" name="TIA-568B"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -3932,12 +4058,12 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{211AC8E5-0F06-469C-8451-8834EF93985D}" name="Tabla8" displayName="Tabla8" ref="A1:C21" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22" tableBorderDxfId="21">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{211AC8E5-0F06-469C-8451-8834EF93985D}" name="Tabla8" displayName="Tabla8" ref="A1:C21" totalsRowShown="0" headerRowDxfId="24" dataDxfId="23" tableBorderDxfId="22">
   <autoFilter ref="A1:C21" xr:uid="{211AC8E5-0F06-469C-8451-8834EF93985D}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{4876463E-FEC9-444A-9168-CF595FD609F6}" name="DEC" dataDxfId="20"/>
-    <tableColumn id="2" xr3:uid="{E4D07485-93E2-4F97-8FBE-604048C0DAF6}" name="BIN" dataDxfId="19"/>
-    <tableColumn id="3" xr3:uid="{49B333D7-98AB-40FA-A1DC-C5B4EFE941BE}" name="HEX" dataDxfId="18"/>
+    <tableColumn id="1" xr3:uid="{4876463E-FEC9-444A-9168-CF595FD609F6}" name="DEC" dataDxfId="21"/>
+    <tableColumn id="2" xr3:uid="{E4D07485-93E2-4F97-8FBE-604048C0DAF6}" name="BIN" dataDxfId="20"/>
+    <tableColumn id="3" xr3:uid="{49B333D7-98AB-40FA-A1DC-C5B4EFE941BE}" name="HEX" dataDxfId="19"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3947,13 +4073,13 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{4B54C147-9701-4C87-AAD9-57684EED0442}" name="Tabla10" displayName="Tabla10" ref="A7:G15" totalsRowShown="0">
   <autoFilter ref="A7:G15" xr:uid="{4B54C147-9701-4C87-AAD9-57684EED0442}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{3AE09342-9692-421C-A55C-FE1B0A7ECF19}" name="Binario" dataDxfId="17"/>
+    <tableColumn id="1" xr3:uid="{3AE09342-9692-421C-A55C-FE1B0A7ECF19}" name="Binario" dataDxfId="18"/>
     <tableColumn id="2" xr3:uid="{A8621E02-BA5A-45D8-9E8A-122B44769B98}" name="Red"/>
-    <tableColumn id="3" xr3:uid="{A1D38B69-7051-4F73-96BF-58502BFC45A2}" name="Primer IP" dataDxfId="16"/>
-    <tableColumn id="4" xr3:uid="{0EFB3B67-7DD6-485A-85F5-F023F312738D}" name="Ultima IP" dataDxfId="15"/>
-    <tableColumn id="5" xr3:uid="{80083827-B95B-41F1-A7D4-107398248A1B}" name="Broadcast" dataDxfId="14"/>
-    <tableColumn id="6" xr3:uid="{26BF6E67-CEB6-439B-A22A-E945E36678FB}" name="Mascara" dataDxfId="13"/>
-    <tableColumn id="7" xr3:uid="{EF991478-7589-40D7-B551-973071858FAD}" name="Hosts" dataDxfId="12" dataCellStyle="Millares"/>
+    <tableColumn id="3" xr3:uid="{A1D38B69-7051-4F73-96BF-58502BFC45A2}" name="Primer IP" dataDxfId="17"/>
+    <tableColumn id="4" xr3:uid="{0EFB3B67-7DD6-485A-85F5-F023F312738D}" name="Ultima IP" dataDxfId="16"/>
+    <tableColumn id="5" xr3:uid="{80083827-B95B-41F1-A7D4-107398248A1B}" name="Broadcast" dataDxfId="15"/>
+    <tableColumn id="6" xr3:uid="{26BF6E67-CEB6-439B-A22A-E945E36678FB}" name="Mascara" dataDxfId="14"/>
+    <tableColumn id="7" xr3:uid="{EF991478-7589-40D7-B551-973071858FAD}" name="Hosts" dataDxfId="13" dataCellStyle="Millares"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4288,13 +4414,13 @@
       <c r="A2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="138" t="s">
+      <c r="B2" s="157" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="140" t="s">
+      <c r="C2" s="159" t="s">
         <v>23</v>
       </c>
-      <c r="D2" s="138" t="s">
+      <c r="D2" s="157" t="s">
         <v>12</v>
       </c>
     </row>
@@ -4302,17 +4428,17 @@
       <c r="A3" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="138"/>
-      <c r="C3" s="140"/>
-      <c r="D3" s="138"/>
+      <c r="B3" s="157"/>
+      <c r="C3" s="159"/>
+      <c r="D3" s="157"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="138"/>
-      <c r="C4" s="140"/>
-      <c r="D4" s="138"/>
+      <c r="B4" s="157"/>
+      <c r="C4" s="159"/>
+      <c r="D4" s="157"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
@@ -4352,7 +4478,7 @@
       <c r="C7" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="D7" s="139" t="s">
+      <c r="D7" s="158" t="s">
         <v>9</v>
       </c>
     </row>
@@ -4366,7 +4492,7 @@
       <c r="C8" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="D8" s="139"/>
+      <c r="D8" s="158"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
@@ -4439,7 +4565,7 @@
     <mergeCell ref="B2:B4"/>
     <mergeCell ref="C2:C4"/>
   </mergeCells>
-  <phoneticPr fontId="3" type="noConversion"/>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -4474,16 +4600,16 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="141" t="s">
+      <c r="A3" s="160" t="s">
         <v>44</v>
       </c>
-      <c r="B3" s="141"/>
-      <c r="C3" s="141"/>
-      <c r="E3" s="141" t="s">
+      <c r="B3" s="160"/>
+      <c r="C3" s="160"/>
+      <c r="E3" s="160" t="s">
         <v>84</v>
       </c>
-      <c r="F3" s="141"/>
-      <c r="G3" s="141"/>
+      <c r="F3" s="160"/>
+      <c r="G3" s="160"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -4615,11 +4741,11 @@
       <c r="C10" t="s">
         <v>59</v>
       </c>
-      <c r="E10" s="141" t="s">
+      <c r="E10" s="160" t="s">
         <v>95</v>
       </c>
-      <c r="F10" s="141"/>
-      <c r="G10" s="141"/>
+      <c r="F10" s="160"/>
+      <c r="G10" s="160"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
@@ -4747,7 +4873,7 @@
     <mergeCell ref="E3:G3"/>
     <mergeCell ref="E10:G10"/>
   </mergeCells>
-  <phoneticPr fontId="3" type="noConversion"/>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
   <tableParts count="3">
@@ -4777,18 +4903,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="142" t="s">
+      <c r="A1" s="161" t="s">
         <v>117</v>
       </c>
-      <c r="B1" s="142"/>
-      <c r="C1" s="142"/>
-      <c r="D1" s="142"/>
-      <c r="E1" s="142"/>
-      <c r="F1" s="142"/>
-      <c r="G1" s="142"/>
-      <c r="H1" s="142"/>
-      <c r="I1" s="142"/>
-      <c r="J1" s="142"/>
+      <c r="B1" s="161"/>
+      <c r="C1" s="161"/>
+      <c r="D1" s="161"/>
+      <c r="E1" s="161"/>
+      <c r="F1" s="161"/>
+      <c r="G1" s="161"/>
+      <c r="H1" s="161"/>
+      <c r="I1" s="161"/>
+      <c r="J1" s="161"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -5376,32 +5502,32 @@
       <c r="E6" s="42" t="s">
         <v>180</v>
       </c>
-      <c r="F6" s="143" t="s">
+      <c r="F6" s="162" t="s">
         <v>243</v>
       </c>
-      <c r="G6" s="143"/>
-      <c r="H6" s="143"/>
-      <c r="I6" s="143"/>
-      <c r="J6" s="143"/>
-      <c r="K6" s="143"/>
-      <c r="L6" s="143"/>
-      <c r="M6" s="143"/>
+      <c r="G6" s="162"/>
+      <c r="H6" s="162"/>
+      <c r="I6" s="162"/>
+      <c r="J6" s="162"/>
+      <c r="K6" s="162"/>
+      <c r="L6" s="162"/>
+      <c r="M6" s="162"/>
       <c r="N6" s="50" t="s">
         <v>204</v>
       </c>
       <c r="O6" s="51"/>
-      <c r="P6" s="144" t="s">
+      <c r="P6" s="163" t="s">
         <v>246</v>
       </c>
-      <c r="Q6" s="145"/>
-      <c r="R6" s="145"/>
-      <c r="S6" s="145"/>
-      <c r="T6" s="145"/>
-      <c r="U6" s="145"/>
-      <c r="V6" s="145"/>
-      <c r="W6" s="145"/>
-      <c r="X6" s="145"/>
-      <c r="Y6" s="146"/>
+      <c r="Q6" s="164"/>
+      <c r="R6" s="164"/>
+      <c r="S6" s="164"/>
+      <c r="T6" s="164"/>
+      <c r="U6" s="164"/>
+      <c r="V6" s="164"/>
+      <c r="W6" s="164"/>
+      <c r="X6" s="164"/>
+      <c r="Y6" s="165"/>
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A7" s="32">
@@ -6347,7 +6473,7 @@
     <mergeCell ref="F6:M6"/>
     <mergeCell ref="P6:Y6"/>
   </mergeCells>
-  <phoneticPr fontId="3" type="noConversion"/>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
@@ -6387,53 +6513,53 @@
       <c r="A1" s="85" t="s">
         <v>264</v>
       </c>
-      <c r="B1" s="147" t="s">
+      <c r="B1" s="172" t="s">
         <v>293</v>
       </c>
-      <c r="C1" s="147"/>
-      <c r="D1" s="147"/>
-      <c r="E1" s="148"/>
-      <c r="F1" s="147" t="s">
+      <c r="C1" s="172"/>
+      <c r="D1" s="172"/>
+      <c r="E1" s="173"/>
+      <c r="F1" s="172" t="s">
         <v>292</v>
       </c>
-      <c r="G1" s="147"/>
-      <c r="H1" s="147"/>
-      <c r="I1" s="148"/>
-      <c r="J1" s="147" t="s">
+      <c r="G1" s="172"/>
+      <c r="H1" s="172"/>
+      <c r="I1" s="173"/>
+      <c r="J1" s="172" t="s">
         <v>298</v>
       </c>
-      <c r="K1" s="147"/>
-      <c r="L1" s="147"/>
-      <c r="M1" s="148"/>
+      <c r="K1" s="172"/>
+      <c r="L1" s="172"/>
+      <c r="M1" s="173"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="86" t="s">
         <v>290</v>
       </c>
-      <c r="B2" s="149" t="s">
+      <c r="B2" s="170" t="s">
         <v>289</v>
       </c>
-      <c r="C2" s="149"/>
-      <c r="D2" s="149" t="s">
+      <c r="C2" s="170"/>
+      <c r="D2" s="170" t="s">
         <v>288</v>
       </c>
-      <c r="E2" s="150"/>
-      <c r="F2" s="149" t="s">
+      <c r="E2" s="171"/>
+      <c r="F2" s="170" t="s">
         <v>289</v>
       </c>
-      <c r="G2" s="149"/>
-      <c r="H2" s="149" t="s">
+      <c r="G2" s="170"/>
+      <c r="H2" s="170" t="s">
         <v>288</v>
       </c>
-      <c r="I2" s="150"/>
-      <c r="J2" s="149" t="s">
+      <c r="I2" s="171"/>
+      <c r="J2" s="170" t="s">
         <v>299</v>
       </c>
-      <c r="K2" s="150"/>
-      <c r="L2" s="149" t="s">
+      <c r="K2" s="171"/>
+      <c r="L2" s="170" t="s">
         <v>310</v>
       </c>
-      <c r="M2" s="150"/>
+      <c r="M2" s="171"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="87" t="s">
@@ -6618,16 +6744,16 @@
       <c r="E7" s="103" t="s">
         <v>279</v>
       </c>
-      <c r="F7" s="151" t="s">
+      <c r="F7" s="174" t="s">
         <v>16</v>
       </c>
-      <c r="G7" s="152"/>
-      <c r="H7" s="152"/>
-      <c r="I7" s="153"/>
-      <c r="J7" s="151"/>
-      <c r="K7" s="152"/>
-      <c r="L7" s="152"/>
-      <c r="M7" s="153"/>
+      <c r="G7" s="175"/>
+      <c r="H7" s="175"/>
+      <c r="I7" s="176"/>
+      <c r="J7" s="174"/>
+      <c r="K7" s="175"/>
+      <c r="L7" s="175"/>
+      <c r="M7" s="176"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="90" t="s">
@@ -6645,32 +6771,32 @@
       <c r="E8" s="108" t="s">
         <v>281</v>
       </c>
-      <c r="F8" s="154" t="s">
+      <c r="F8" s="177" t="s">
         <v>282</v>
       </c>
-      <c r="G8" s="155"/>
-      <c r="H8" s="155"/>
-      <c r="I8" s="156"/>
-      <c r="J8" s="154"/>
-      <c r="K8" s="155"/>
-      <c r="L8" s="155"/>
-      <c r="M8" s="156"/>
+      <c r="G8" s="178"/>
+      <c r="H8" s="178"/>
+      <c r="I8" s="179"/>
+      <c r="J8" s="177"/>
+      <c r="K8" s="178"/>
+      <c r="L8" s="178"/>
+      <c r="M8" s="179"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="91" t="s">
         <v>291</v>
       </c>
-      <c r="B9" s="157">
+      <c r="B9" s="166">
         <f>2^32</f>
         <v>4294967296</v>
       </c>
-      <c r="C9" s="157"/>
-      <c r="D9" s="157"/>
-      <c r="E9" s="158"/>
-      <c r="F9" s="159"/>
-      <c r="G9" s="159"/>
-      <c r="H9" s="159"/>
-      <c r="I9" s="160"/>
+      <c r="C9" s="166"/>
+      <c r="D9" s="166"/>
+      <c r="E9" s="167"/>
+      <c r="F9" s="168"/>
+      <c r="G9" s="168"/>
+      <c r="H9" s="168"/>
+      <c r="I9" s="169"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="114" t="s">
@@ -6688,7 +6814,7 @@
       <c r="E11" s="115" t="s">
         <v>319</v>
       </c>
-      <c r="F11" s="161" t="s">
+      <c r="F11" s="138" t="s">
         <v>320</v>
       </c>
       <c r="G11" s="115" t="s">
@@ -6723,7 +6849,7 @@
       <c r="E12" s="117" t="s">
         <v>322</v>
       </c>
-      <c r="F12" s="162" t="s">
+      <c r="F12" s="139" t="s">
         <v>323</v>
       </c>
       <c r="G12" s="59" t="s">
@@ -6758,7 +6884,7 @@
       <c r="E13" s="121" t="s">
         <v>184</v>
       </c>
-      <c r="F13" s="163" t="s">
+      <c r="F13" s="140" t="s">
         <v>184</v>
       </c>
       <c r="G13" s="61" t="s">
@@ -6793,7 +6919,7 @@
       <c r="E14" s="117" t="s">
         <v>184</v>
       </c>
-      <c r="F14" s="162" t="s">
+      <c r="F14" s="139" t="s">
         <v>184</v>
       </c>
       <c r="G14" s="59" t="s">
@@ -6828,7 +6954,7 @@
       <c r="E15" s="131" t="s">
         <v>187</v>
       </c>
-      <c r="F15" s="164" t="s">
+      <c r="F15" s="141" t="s">
         <v>187</v>
       </c>
       <c r="G15" s="134">
@@ -6848,7 +6974,7 @@
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="F16" s="165"/>
+      <c r="F16" s="142"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="114" t="s">
@@ -6866,7 +6992,7 @@
       <c r="E17" s="115" t="s">
         <v>319</v>
       </c>
-      <c r="F17" s="161" t="s">
+      <c r="F17" s="138" t="s">
         <v>320</v>
       </c>
       <c r="G17" s="115" t="s">
@@ -6901,7 +7027,7 @@
       <c r="E18" s="117" t="s">
         <v>330</v>
       </c>
-      <c r="F18" s="162" t="s">
+      <c r="F18" s="139" t="s">
         <v>331</v>
       </c>
       <c r="G18" s="59" t="s">
@@ -6936,7 +7062,7 @@
       <c r="E19" s="121" t="s">
         <v>184</v>
       </c>
-      <c r="F19" s="163" t="s">
+      <c r="F19" s="140" t="s">
         <v>327</v>
       </c>
       <c r="G19" s="61" t="s">
@@ -6971,7 +7097,7 @@
       <c r="E20" s="117" t="s">
         <v>184</v>
       </c>
-      <c r="F20" s="162" t="s">
+      <c r="F20" s="139" t="s">
         <v>327</v>
       </c>
       <c r="G20" s="59" t="s">
@@ -7006,7 +7132,7 @@
       <c r="E21" s="131" t="s">
         <v>187</v>
       </c>
-      <c r="F21" s="164" t="s">
+      <c r="F21" s="141" t="s">
         <v>187</v>
       </c>
       <c r="G21" s="80" t="s">
@@ -7026,7 +7152,7 @@
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="F22" s="165"/>
+      <c r="F22" s="142"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="114" t="s">
@@ -7044,7 +7170,7 @@
       <c r="E23" s="115" t="s">
         <v>319</v>
       </c>
-      <c r="F23" s="161" t="s">
+      <c r="F23" s="138" t="s">
         <v>320</v>
       </c>
       <c r="G23" s="115" t="s">
@@ -7079,7 +7205,7 @@
       <c r="E24" s="117" t="s">
         <v>337</v>
       </c>
-      <c r="F24" s="162" t="s">
+      <c r="F24" s="139" t="s">
         <v>338</v>
       </c>
       <c r="G24" s="118">
@@ -7114,7 +7240,7 @@
       <c r="E25" s="121" t="s">
         <v>187</v>
       </c>
-      <c r="F25" s="163" t="s">
+      <c r="F25" s="140" t="s">
         <v>184</v>
       </c>
       <c r="G25" s="48" t="s">
@@ -7149,7 +7275,7 @@
       <c r="E26" s="124" t="s">
         <v>337</v>
       </c>
-      <c r="F26" s="166" t="s">
+      <c r="F26" s="143" t="s">
         <v>184</v>
       </c>
       <c r="G26" s="125" t="s">
@@ -7184,7 +7310,7 @@
       <c r="E27" s="111" t="s">
         <v>337</v>
       </c>
-      <c r="F27" s="167" t="s">
+      <c r="F27" s="144" t="s">
         <v>187</v>
       </c>
       <c r="G27" s="112">
@@ -7205,6 +7331,11 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="J1:M1"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="L2:M2"/>
+    <mergeCell ref="J7:M7"/>
+    <mergeCell ref="J8:M8"/>
     <mergeCell ref="B9:E9"/>
     <mergeCell ref="F9:I9"/>
     <mergeCell ref="B2:C2"/>
@@ -7215,11 +7346,6 @@
     <mergeCell ref="F1:I1"/>
     <mergeCell ref="F7:I7"/>
     <mergeCell ref="F8:I8"/>
-    <mergeCell ref="J1:M1"/>
-    <mergeCell ref="J2:K2"/>
-    <mergeCell ref="L2:M2"/>
-    <mergeCell ref="J7:M7"/>
-    <mergeCell ref="J8:M8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -7230,9 +7356,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE1C5EB1-FF6C-4B6C-B630-875CA3ECA979}">
   <dimension ref="A1:K37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D8" sqref="D8"/>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A7" sqref="A7:B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7245,42 +7371,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="173" t="s">
+      <c r="A1" s="180" t="s">
         <v>350</v>
       </c>
-      <c r="B1" s="173"/>
-      <c r="C1" s="142" t="s">
+      <c r="B1" s="180"/>
+      <c r="C1" s="161" t="s">
         <v>351</v>
       </c>
-      <c r="D1" s="142"/>
-      <c r="E1" s="142"/>
-      <c r="F1" s="142"/>
-      <c r="G1" s="142"/>
-      <c r="H1" s="142"/>
-      <c r="I1" s="142"/>
-      <c r="J1" s="142"/>
-      <c r="K1" s="142"/>
+      <c r="D1" s="161"/>
+      <c r="E1" s="161"/>
+      <c r="F1" s="161"/>
+      <c r="G1" s="161"/>
+      <c r="H1" s="161"/>
+      <c r="I1" s="161"/>
+      <c r="J1" s="161"/>
+      <c r="K1" s="161"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="42" t="s">
         <v>361</v>
       </c>
-      <c r="B2" s="168" t="s">
+      <c r="B2" s="145" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="168" t="s">
+      <c r="C2" s="145" t="s">
         <v>298</v>
       </c>
-      <c r="D2" s="168" t="s">
+      <c r="D2" s="145" t="s">
         <v>300</v>
       </c>
-      <c r="E2" s="168" t="s">
+      <c r="E2" s="145" t="s">
         <v>355</v>
       </c>
-      <c r="F2" s="168" t="s">
+      <c r="F2" s="145" t="s">
         <v>357</v>
       </c>
-      <c r="G2" s="169" t="s">
+      <c r="G2" s="146" t="s">
         <v>358</v>
       </c>
       <c r="H2" s="27"/>
@@ -7288,25 +7414,25 @@
       <c r="J2" s="27"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="170" t="s">
+      <c r="A3" s="147" t="s">
         <v>352</v>
       </c>
-      <c r="B3" s="171" t="s">
+      <c r="B3" s="148" t="s">
         <v>353</v>
       </c>
-      <c r="C3" s="171" t="s">
+      <c r="C3" s="148" t="s">
         <v>363</v>
       </c>
-      <c r="D3" s="171" t="s">
+      <c r="D3" s="148" t="s">
         <v>359</v>
       </c>
-      <c r="E3" s="171" t="s">
+      <c r="E3" s="148" t="s">
         <v>356</v>
       </c>
-      <c r="F3" s="171" t="s">
+      <c r="F3" s="148" t="s">
         <v>362</v>
       </c>
-      <c r="G3" s="172" t="s">
+      <c r="G3" s="149" t="s">
         <v>360</v>
       </c>
       <c r="H3" s="27"/>
@@ -7335,7 +7461,7 @@
         <f>32-D5</f>
         <v>21</v>
       </c>
-      <c r="G5" s="174">
+      <c r="G5" s="150">
         <f>2^F5-2</f>
         <v>2097150</v>
       </c>
@@ -7364,191 +7490,191 @@
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="175" t="s">
+      <c r="A8" s="151" t="s">
         <v>379</v>
       </c>
       <c r="B8" t="s">
         <v>365</v>
       </c>
-      <c r="C8" s="177" t="s">
+      <c r="C8" s="153" t="s">
         <v>390</v>
       </c>
-      <c r="D8" s="177" t="s">
+      <c r="D8" s="153" t="s">
         <v>372</v>
       </c>
-      <c r="E8" s="177" t="s">
+      <c r="E8" s="153" t="s">
         <v>371</v>
       </c>
-      <c r="F8" s="177" t="s">
+      <c r="F8" s="153" t="s">
         <v>398</v>
       </c>
-      <c r="G8" s="174">
+      <c r="G8" s="150">
         <v>2097150</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="175" t="s">
+      <c r="A9" s="151" t="s">
         <v>380</v>
       </c>
       <c r="B9" t="s">
         <v>370</v>
       </c>
-      <c r="C9" s="177" t="s">
+      <c r="C9" s="153" t="s">
         <v>391</v>
       </c>
-      <c r="D9" s="177" t="s">
+      <c r="D9" s="153" t="s">
         <v>387</v>
       </c>
-      <c r="E9" s="177" t="s">
+      <c r="E9" s="153" t="s">
         <v>386</v>
       </c>
-      <c r="F9" s="177" t="s">
+      <c r="F9" s="153" t="s">
         <v>398</v>
       </c>
-      <c r="G9" s="174">
+      <c r="G9" s="150">
         <v>2097150</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="175" t="s">
+      <c r="A10" s="151" t="s">
         <v>381</v>
       </c>
       <c r="B10" t="s">
         <v>373</v>
       </c>
-      <c r="C10" s="177" t="s">
+      <c r="C10" s="153" t="s">
         <v>392</v>
       </c>
-      <c r="D10" s="177" t="s">
+      <c r="D10" s="153" t="s">
         <v>389</v>
       </c>
-      <c r="E10" s="177" t="s">
+      <c r="E10" s="153" t="s">
         <v>388</v>
       </c>
-      <c r="F10" s="177" t="s">
+      <c r="F10" s="153" t="s">
         <v>398</v>
       </c>
-      <c r="G10" s="174">
+      <c r="G10" s="150">
         <v>2097150</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="175" t="s">
+      <c r="A11" s="151" t="s">
         <v>382</v>
       </c>
       <c r="B11" t="s">
         <v>374</v>
       </c>
-      <c r="C11" s="177" t="s">
+      <c r="C11" s="153" t="s">
         <v>393</v>
       </c>
-      <c r="D11" s="178">
+      <c r="D11" s="154">
         <v>10127255255</v>
       </c>
-      <c r="E11" s="178">
+      <c r="E11" s="154">
         <v>10127255255</v>
       </c>
-      <c r="F11" s="177" t="s">
+      <c r="F11" s="153" t="s">
         <v>398</v>
       </c>
-      <c r="G11" s="174">
+      <c r="G11" s="150">
         <v>2097150</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="175" t="s">
+      <c r="A12" s="151" t="s">
         <v>383</v>
       </c>
       <c r="B12" t="s">
         <v>375</v>
       </c>
-      <c r="C12" s="177" t="s">
+      <c r="C12" s="153" t="s">
         <v>394</v>
       </c>
-      <c r="D12" s="178">
+      <c r="D12" s="154">
         <v>10159255255</v>
       </c>
-      <c r="E12" s="178">
+      <c r="E12" s="154">
         <v>10159255255</v>
       </c>
-      <c r="F12" s="177" t="s">
+      <c r="F12" s="153" t="s">
         <v>398</v>
       </c>
-      <c r="G12" s="174">
+      <c r="G12" s="150">
         <v>2097150</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="175" t="s">
+      <c r="A13" s="151" t="s">
         <v>384</v>
       </c>
       <c r="B13" t="s">
         <v>376</v>
       </c>
-      <c r="C13" s="177" t="s">
+      <c r="C13" s="153" t="s">
         <v>395</v>
       </c>
-      <c r="D13" s="178">
+      <c r="D13" s="154">
         <v>10191255255</v>
       </c>
-      <c r="E13" s="178">
+      <c r="E13" s="154">
         <v>10191255255</v>
       </c>
-      <c r="F13" s="177" t="s">
+      <c r="F13" s="153" t="s">
         <v>398</v>
       </c>
-      <c r="G13" s="174">
+      <c r="G13" s="150">
         <v>2097150</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="175" t="s">
+      <c r="A14" s="151" t="s">
         <v>276</v>
       </c>
       <c r="B14" t="s">
         <v>377</v>
       </c>
-      <c r="C14" s="177" t="s">
+      <c r="C14" s="153" t="s">
         <v>396</v>
       </c>
-      <c r="D14" s="178">
+      <c r="D14" s="154">
         <v>10223255255</v>
       </c>
-      <c r="E14" s="178">
+      <c r="E14" s="154">
         <v>10223255255</v>
       </c>
-      <c r="F14" s="177" t="s">
+      <c r="F14" s="153" t="s">
         <v>398</v>
       </c>
-      <c r="G14" s="174">
+      <c r="G14" s="150">
         <v>2097150</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="175" t="s">
+      <c r="A15" s="151" t="s">
         <v>385</v>
       </c>
       <c r="B15" t="s">
         <v>378</v>
       </c>
-      <c r="C15" s="177" t="s">
+      <c r="C15" s="153" t="s">
         <v>397</v>
       </c>
-      <c r="D15" s="178">
+      <c r="D15" s="154">
         <v>10255255255</v>
       </c>
-      <c r="E15" s="178">
+      <c r="E15" s="154">
         <v>10255255255</v>
       </c>
-      <c r="F15" s="177" t="s">
+      <c r="F15" s="153" t="s">
         <v>398</v>
       </c>
-      <c r="G15" s="174">
+      <c r="G15" s="150">
         <v>2097150</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="G16" s="179"/>
+      <c r="G16" s="155"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17">
@@ -7598,7 +7724,7 @@
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="175" t="s">
+      <c r="A20" s="151" t="s">
         <v>400</v>
       </c>
       <c r="B20" t="s">
@@ -7607,21 +7733,21 @@
       <c r="C20" t="s">
         <v>399</v>
       </c>
-      <c r="D20" s="177" t="s">
+      <c r="D20" s="153" t="s">
         <v>407</v>
       </c>
-      <c r="E20" s="177" t="s">
+      <c r="E20" s="153" t="s">
         <v>406</v>
       </c>
-      <c r="F20" s="177" t="s">
+      <c r="F20" s="153" t="s">
         <v>414</v>
       </c>
-      <c r="G20" s="174">
+      <c r="G20" s="150">
         <v>4094</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="175" t="s">
+      <c r="A21" s="151" t="s">
         <v>401</v>
       </c>
       <c r="B21" t="s">
@@ -7630,21 +7756,21 @@
       <c r="C21" t="s">
         <v>403</v>
       </c>
-      <c r="D21" s="177" t="s">
+      <c r="D21" s="153" t="s">
         <v>411</v>
       </c>
-      <c r="E21" s="177" t="s">
+      <c r="E21" s="153" t="s">
         <v>408</v>
       </c>
-      <c r="F21" s="177" t="s">
+      <c r="F21" s="153" t="s">
         <v>415</v>
       </c>
-      <c r="G21" s="174">
+      <c r="G21" s="150">
         <v>4094</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="175" t="s">
+      <c r="A22" s="151" t="s">
         <v>274</v>
       </c>
       <c r="B22" t="s">
@@ -7653,21 +7779,21 @@
       <c r="C22" t="s">
         <v>404</v>
       </c>
-      <c r="D22" s="177" t="s">
+      <c r="D22" s="153" t="s">
         <v>412</v>
       </c>
-      <c r="E22" s="177" t="s">
+      <c r="E22" s="153" t="s">
         <v>409</v>
       </c>
-      <c r="F22" s="177" t="s">
+      <c r="F22" s="153" t="s">
         <v>416</v>
       </c>
-      <c r="G22" s="174">
+      <c r="G22" s="150">
         <v>4094</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="175" t="s">
+      <c r="A23" s="151" t="s">
         <v>402</v>
       </c>
       <c r="B23" t="s">
@@ -7676,16 +7802,16 @@
       <c r="C23" t="s">
         <v>405</v>
       </c>
-      <c r="D23" s="178" t="s">
+      <c r="D23" s="154" t="s">
         <v>413</v>
       </c>
-      <c r="E23" s="178" t="s">
+      <c r="E23" s="154" t="s">
         <v>410</v>
       </c>
-      <c r="F23" s="177" t="s">
+      <c r="F23" s="153" t="s">
         <v>417</v>
       </c>
-      <c r="G23" s="174">
+      <c r="G23" s="150">
         <v>4094</v>
       </c>
     </row>
@@ -7736,7 +7862,7 @@
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="175" t="s">
+      <c r="A28" s="151" t="s">
         <v>400</v>
       </c>
       <c r="B28" t="s">
@@ -7745,21 +7871,21 @@
       <c r="C28" t="s">
         <v>422</v>
       </c>
-      <c r="D28" s="177" t="s">
+      <c r="D28" s="153" t="s">
         <v>426</v>
       </c>
-      <c r="E28" s="177" t="s">
+      <c r="E28" s="153" t="s">
         <v>427</v>
       </c>
-      <c r="F28" s="178">
+      <c r="F28" s="154">
         <v>255255255192</v>
       </c>
-      <c r="G28" s="174">
+      <c r="G28" s="150">
         <v>62</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="175" t="s">
+      <c r="A29" s="151" t="s">
         <v>401</v>
       </c>
       <c r="B29" t="s">
@@ -7768,21 +7894,21 @@
       <c r="C29" t="s">
         <v>423</v>
       </c>
-      <c r="D29" s="177" t="s">
+      <c r="D29" s="153" t="s">
         <v>436</v>
       </c>
-      <c r="E29" s="178" t="s">
+      <c r="E29" s="154" t="s">
         <v>435</v>
       </c>
-      <c r="F29" s="178">
+      <c r="F29" s="154">
         <v>255255255192</v>
       </c>
-      <c r="G29" s="174">
+      <c r="G29" s="150">
         <v>62</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="175" t="s">
+      <c r="A30" s="151" t="s">
         <v>274</v>
       </c>
       <c r="B30" t="s">
@@ -7797,15 +7923,15 @@
       <c r="E30" t="s">
         <v>439</v>
       </c>
-      <c r="F30" s="178">
+      <c r="F30" s="154">
         <v>255255255192</v>
       </c>
-      <c r="G30" s="174">
+      <c r="G30" s="150">
         <v>62</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="175" t="s">
+      <c r="A31" s="151" t="s">
         <v>402</v>
       </c>
       <c r="B31" t="s">
@@ -7820,10 +7946,10 @@
       <c r="E31" t="s">
         <v>440</v>
       </c>
-      <c r="F31" s="178">
+      <c r="F31" s="154">
         <v>255255255192</v>
       </c>
-      <c r="G31" s="174">
+      <c r="G31" s="150">
         <v>62</v>
       </c>
     </row>
@@ -7836,19 +7962,19 @@
       <c r="A34" t="s">
         <v>428</v>
       </c>
-      <c r="B34" s="175" t="s">
+      <c r="B34" s="151" t="s">
         <v>335</v>
       </c>
-      <c r="C34" s="175" t="s">
+      <c r="C34" s="151" t="s">
         <v>336</v>
       </c>
-      <c r="D34" s="175" t="s">
+      <c r="D34" s="151" t="s">
         <v>184</v>
       </c>
-      <c r="E34" s="175" t="s">
+      <c r="E34" s="151" t="s">
         <v>432</v>
       </c>
-      <c r="F34" s="180" t="s">
+      <c r="F34" s="156" t="s">
         <v>433</v>
       </c>
     </row>
@@ -7856,19 +7982,19 @@
       <c r="A35" t="s">
         <v>429</v>
       </c>
-      <c r="B35" s="175" t="s">
+      <c r="B35" s="151" t="s">
         <v>187</v>
       </c>
-      <c r="C35" s="175" t="s">
+      <c r="C35" s="151" t="s">
         <v>187</v>
       </c>
-      <c r="D35" s="175" t="s">
+      <c r="D35" s="151" t="s">
         <v>187</v>
       </c>
-      <c r="E35" s="175" t="s">
+      <c r="E35" s="151" t="s">
         <v>335</v>
       </c>
-      <c r="F35" s="176">
+      <c r="F35" s="152">
         <v>255255255192</v>
       </c>
     </row>
@@ -7876,19 +8002,19 @@
       <c r="A36" t="s">
         <v>430</v>
       </c>
-      <c r="B36" s="175" t="s">
+      <c r="B36" s="151" t="s">
         <v>335</v>
       </c>
-      <c r="C36" s="175" t="s">
+      <c r="C36" s="151" t="s">
         <v>336</v>
       </c>
-      <c r="D36" s="175" t="s">
+      <c r="D36" s="151" t="s">
         <v>184</v>
       </c>
-      <c r="E36" s="175" t="s">
+      <c r="E36" s="151" t="s">
         <v>342</v>
       </c>
-      <c r="F36" s="175" t="s">
+      <c r="F36" s="151" t="s">
         <v>423</v>
       </c>
     </row>
@@ -7896,19 +8022,19 @@
       <c r="A37" t="s">
         <v>431</v>
       </c>
-      <c r="B37" s="175" t="s">
+      <c r="B37" s="151" t="s">
         <v>335</v>
       </c>
-      <c r="C37" s="175" t="s">
+      <c r="C37" s="151" t="s">
         <v>336</v>
       </c>
-      <c r="D37" s="175" t="s">
+      <c r="D37" s="151" t="s">
         <v>184</v>
       </c>
-      <c r="E37" s="175" t="s">
+      <c r="E37" s="151" t="s">
         <v>434</v>
       </c>
-      <c r="F37" s="175" t="s">
+      <c r="F37" s="151" t="s">
         <v>435</v>
       </c>
     </row>
@@ -7917,7 +8043,7 @@
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="C1:K1"/>
   </mergeCells>
-  <phoneticPr fontId="3" type="noConversion"/>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="3">
@@ -7926,4 +8052,278 @@
     <tablePart r:id="rId4"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E5C05F7-1048-457F-9AB9-1A7675D27262}">
+  <dimension ref="A1:I12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:I1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="7.28515625" customWidth="1"/>
+    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.140625" customWidth="1"/>
+    <col min="4" max="6" width="10" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.42578125" customWidth="1"/>
+    <col min="8" max="8" width="15.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>445</v>
+      </c>
+      <c r="B1" s="161" t="s">
+        <v>446</v>
+      </c>
+      <c r="C1" s="161"/>
+      <c r="D1" s="161"/>
+      <c r="E1" s="161"/>
+      <c r="F1" s="161"/>
+      <c r="G1" s="161"/>
+      <c r="H1" s="161"/>
+      <c r="I1" s="161"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="42" t="s">
+        <v>455</v>
+      </c>
+      <c r="B3" s="145" t="s">
+        <v>448</v>
+      </c>
+      <c r="C3" s="145" t="s">
+        <v>300</v>
+      </c>
+      <c r="D3" s="145" t="s">
+        <v>355</v>
+      </c>
+      <c r="E3" s="145"/>
+      <c r="F3" s="145"/>
+      <c r="G3" s="146"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="147" t="s">
+        <v>447</v>
+      </c>
+      <c r="B4" s="148" t="s">
+        <v>449</v>
+      </c>
+      <c r="C4" s="148" t="s">
+        <v>456</v>
+      </c>
+      <c r="D4" s="148" t="s">
+        <v>457</v>
+      </c>
+      <c r="E4" s="148"/>
+      <c r="F4" s="148"/>
+      <c r="G4" s="149"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D5" t="s">
+        <v>468</v>
+      </c>
+      <c r="E5" t="s">
+        <v>469</v>
+      </c>
+      <c r="F5" t="s">
+        <v>468</v>
+      </c>
+      <c r="G5" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>450</v>
+      </c>
+      <c r="B6" t="s">
+        <v>369</v>
+      </c>
+      <c r="C6" t="s">
+        <v>300</v>
+      </c>
+      <c r="D6" t="s">
+        <v>458</v>
+      </c>
+      <c r="E6" t="s">
+        <v>366</v>
+      </c>
+      <c r="F6" t="s">
+        <v>367</v>
+      </c>
+      <c r="G6" t="s">
+        <v>17</v>
+      </c>
+      <c r="H6" t="s">
+        <v>459</v>
+      </c>
+      <c r="I6" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>43</v>
+      </c>
+      <c r="B7">
+        <v>100</v>
+      </c>
+      <c r="C7">
+        <v>25</v>
+      </c>
+      <c r="D7" t="s">
+        <v>283</v>
+      </c>
+      <c r="E7" t="s">
+        <v>460</v>
+      </c>
+      <c r="F7" t="s">
+        <v>463</v>
+      </c>
+      <c r="G7" t="s">
+        <v>464</v>
+      </c>
+      <c r="H7" s="152">
+        <v>255255255128</v>
+      </c>
+      <c r="I7">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>452</v>
+      </c>
+      <c r="B8">
+        <v>80</v>
+      </c>
+      <c r="C8">
+        <v>25</v>
+      </c>
+      <c r="D8" t="s">
+        <v>461</v>
+      </c>
+      <c r="E8" t="s">
+        <v>462</v>
+      </c>
+      <c r="F8" t="s">
+        <v>465</v>
+      </c>
+      <c r="G8" t="s">
+        <v>466</v>
+      </c>
+      <c r="H8" s="152">
+        <v>255255255128</v>
+      </c>
+      <c r="I8">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>451</v>
+      </c>
+      <c r="B9">
+        <v>40</v>
+      </c>
+      <c r="C9">
+        <v>26</v>
+      </c>
+      <c r="D9" t="s">
+        <v>467</v>
+      </c>
+      <c r="E9" t="s">
+        <v>470</v>
+      </c>
+      <c r="F9" t="s">
+        <v>473</v>
+      </c>
+      <c r="G9" t="s">
+        <v>472</v>
+      </c>
+      <c r="H9" s="152">
+        <v>255255255192</v>
+      </c>
+      <c r="I9">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>453</v>
+      </c>
+      <c r="B10">
+        <v>20</v>
+      </c>
+      <c r="C10">
+        <v>27</v>
+      </c>
+      <c r="D10" t="s">
+        <v>471</v>
+      </c>
+      <c r="E10" t="s">
+        <v>471</v>
+      </c>
+      <c r="F10" t="s">
+        <v>480</v>
+      </c>
+      <c r="G10" t="s">
+        <v>476</v>
+      </c>
+      <c r="H10" s="152">
+        <v>255255255224</v>
+      </c>
+      <c r="I10">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>454</v>
+      </c>
+      <c r="B11">
+        <v>10</v>
+      </c>
+      <c r="C11">
+        <v>28</v>
+      </c>
+      <c r="D11" t="s">
+        <v>474</v>
+      </c>
+      <c r="E11" t="s">
+        <v>475</v>
+      </c>
+      <c r="F11" t="s">
+        <v>478</v>
+      </c>
+      <c r="G11" t="s">
+        <v>479</v>
+      </c>
+      <c r="H11" s="152">
+        <v>255255255240</v>
+      </c>
+      <c r="I11">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D12" t="s">
+        <v>477</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A7:B11">
+    <sortCondition descending="1" ref="B7:B11"/>
+  </sortState>
+  <mergeCells count="1">
+    <mergeCell ref="B1:I1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Enrutamiento IPv4 y VLSM
</commit_message>
<xml_diff>
--- a/docs/protocol-suite.xlsx
+++ b/docs/protocol-suite.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EducacionIT\Documents\networks\CISCO\saves\ccna1-lx20\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE61336A-2EAA-4DC7-951F-8E891ABF4314}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BBE9F91-5681-4685-A010-6150BC8CDD8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="6" xr2:uid="{A284E486-C6D6-48E7-9614-2E5470B19042}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="719" uniqueCount="482">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="851" uniqueCount="533">
   <si>
     <t>osi de iso</t>
   </si>
@@ -2374,7 +2374,160 @@
     <t>10.0.1.94</t>
   </si>
   <si>
-    <t>Hosts2</t>
+    <t>f</t>
+  </si>
+  <si>
+    <t>10.0.1.113</t>
+  </si>
+  <si>
+    <t>10.0.1.114</t>
+  </si>
+  <si>
+    <t>10.0.1.115</t>
+  </si>
+  <si>
+    <t>Max</t>
+  </si>
+  <si>
+    <t>10.0.0.62</t>
+  </si>
+  <si>
+    <t>10.0.0.63</t>
+  </si>
+  <si>
+    <t>10.0.0.64</t>
+  </si>
+  <si>
+    <t>10.0.0.192</t>
+  </si>
+  <si>
+    <t>10.0.0.65</t>
+  </si>
+  <si>
+    <t>10.0.0.190</t>
+  </si>
+  <si>
+    <t>10.0.0.191</t>
+  </si>
+  <si>
+    <t>10.0.0.193</t>
+  </si>
+  <si>
+    <t>10.0.1.65</t>
+  </si>
+  <si>
+    <t>10.0.1.78</t>
+  </si>
+  <si>
+    <t>10.0.1.79</t>
+  </si>
+  <si>
+    <t>10.0.1.80</t>
+  </si>
+  <si>
+    <t>10.0.1.81</t>
+  </si>
+  <si>
+    <t>BYTE 1</t>
+  </si>
+  <si>
+    <t>BYTE 2</t>
+  </si>
+  <si>
+    <t>BYTE 3</t>
+  </si>
+  <si>
+    <t>BYTE 4</t>
+  </si>
+  <si>
+    <t>10.0.0.0/26</t>
+  </si>
+  <si>
+    <t>10.0.1.64/28</t>
+  </si>
+  <si>
+    <t>10.0.1.112/30</t>
+  </si>
+  <si>
+    <t>10.0.0.0/25</t>
+  </si>
+  <si>
+    <t>10.0.0.128/25</t>
+  </si>
+  <si>
+    <t>Revision</t>
+  </si>
+  <si>
+    <t>11100000</t>
+  </si>
+  <si>
+    <t>10.0.1.64/27</t>
+  </si>
+  <si>
+    <t>10.0.1.128</t>
+  </si>
+  <si>
+    <t>10.0.1.126</t>
+  </si>
+  <si>
+    <t>10.0.1.127</t>
+  </si>
+  <si>
+    <t>10.0.1.129</t>
+  </si>
+  <si>
+    <t>10.0.1.142</t>
+  </si>
+  <si>
+    <t>10.0.1.143</t>
+  </si>
+  <si>
+    <t>10.0.1.160</t>
+  </si>
+  <si>
+    <t>10.0.1.161</t>
+  </si>
+  <si>
+    <t>10.0.1.192</t>
+  </si>
+  <si>
+    <t>10.0.1.190</t>
+  </si>
+  <si>
+    <t>10.0.1.191</t>
+  </si>
+  <si>
+    <t>10.0.1.193</t>
+  </si>
+  <si>
+    <t>10.0.1.194</t>
+  </si>
+  <si>
+    <t>10.0.1.195</t>
+  </si>
+  <si>
+    <t>10.0.1.255</t>
+  </si>
+  <si>
+    <t>192.168.30.0</t>
+  </si>
+  <si>
+    <t>NET 1</t>
+  </si>
+  <si>
+    <t>NET 2</t>
+  </si>
+  <si>
+    <t>00011110</t>
+  </si>
+  <si>
+    <t>255.255.224.0</t>
+  </si>
+  <si>
+    <t>00011111</t>
+  </si>
+  <si>
+    <t>192.168.31.255</t>
   </si>
 </sst>
 </file>
@@ -2897,7 +3050,7 @@
     <xf numFmtId="0" fontId="1" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="181">
+  <cellXfs count="183">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -3314,6 +3467,36 @@
     <xf numFmtId="0" fontId="3" fillId="18" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3326,46 +3509,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="3" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Énfasis1" xfId="1" builtinId="29"/>
     <cellStyle name="Millares" xfId="2" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="30">
+  <dxfs count="32">
+    <dxf>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="3" formatCode="#,##0"/>
     </dxf>
@@ -3941,13 +4102,13 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{0ADCD326-5B10-43FB-9AA2-AB768BBDBA9C}" name="Tabla1012" displayName="Tabla1012" ref="A19:G23" totalsRowShown="0">
   <autoFilter ref="A19:G23" xr:uid="{0ADCD326-5B10-43FB-9AA2-AB768BBDBA9C}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{DF50FB73-0BE7-4854-956E-C7023988D229}" name="Binario" dataDxfId="12"/>
+    <tableColumn id="1" xr3:uid="{DF50FB73-0BE7-4854-956E-C7023988D229}" name="Binario" dataDxfId="14"/>
     <tableColumn id="2" xr3:uid="{DE8352F4-3AF3-43A0-BB45-D5F5668CBB76}" name="Red"/>
-    <tableColumn id="3" xr3:uid="{20D54671-9004-432E-B6D6-FBA66370BAC2}" name="Primer IP" dataDxfId="11"/>
-    <tableColumn id="4" xr3:uid="{C9E4837C-B0D1-45D4-AC3A-2CB87026E30C}" name="Ultima IP" dataDxfId="10"/>
-    <tableColumn id="5" xr3:uid="{603009AB-2856-4410-B873-FC6522515A52}" name="Broadcast" dataDxfId="9"/>
-    <tableColumn id="6" xr3:uid="{EE8CE6EA-DB26-400E-B7DF-187FD3044ABA}" name="Mascara" dataDxfId="8"/>
-    <tableColumn id="7" xr3:uid="{64A7D0E0-5029-4FB2-8EAF-08BA13AC6510}" name="Hosts" dataDxfId="7" dataCellStyle="Millares"/>
+    <tableColumn id="3" xr3:uid="{20D54671-9004-432E-B6D6-FBA66370BAC2}" name="Primer IP" dataDxfId="13"/>
+    <tableColumn id="4" xr3:uid="{C9E4837C-B0D1-45D4-AC3A-2CB87026E30C}" name="Ultima IP" dataDxfId="12"/>
+    <tableColumn id="5" xr3:uid="{603009AB-2856-4410-B873-FC6522515A52}" name="Broadcast" dataDxfId="11"/>
+    <tableColumn id="6" xr3:uid="{EE8CE6EA-DB26-400E-B7DF-187FD3044ABA}" name="Mascara" dataDxfId="10"/>
+    <tableColumn id="7" xr3:uid="{64A7D0E0-5029-4FB2-8EAF-08BA13AC6510}" name="Hosts" dataDxfId="9" dataCellStyle="Millares"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3957,21 +4118,24 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{F4D1F3F3-C3A7-4A41-B3DE-DF427F97D09A}" name="Tabla101213" displayName="Tabla101213" ref="A27:G31" totalsRowShown="0">
   <autoFilter ref="A27:G31" xr:uid="{F4D1F3F3-C3A7-4A41-B3DE-DF427F97D09A}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{D1B2423F-C86A-4B39-AB38-96F9DD9BEF71}" name="Binario" dataDxfId="6"/>
+    <tableColumn id="1" xr3:uid="{D1B2423F-C86A-4B39-AB38-96F9DD9BEF71}" name="Binario" dataDxfId="8"/>
     <tableColumn id="2" xr3:uid="{16DB9FDF-15F8-4AF6-A562-7BAF42370F83}" name="Red"/>
-    <tableColumn id="3" xr3:uid="{E4368E94-D5DB-4EC6-9525-32C54F17D759}" name="Primer IP" dataDxfId="5"/>
-    <tableColumn id="4" xr3:uid="{E3B008EB-2EC2-453A-A957-6DE3704D4332}" name="Ultima IP" dataDxfId="4"/>
-    <tableColumn id="5" xr3:uid="{406FF1E2-D54D-437E-A099-5D7101698894}" name="Broadcast" dataDxfId="3"/>
-    <tableColumn id="6" xr3:uid="{3633FA0A-4FF6-4978-B548-F7218383F997}" name="Mascara" dataDxfId="2"/>
-    <tableColumn id="7" xr3:uid="{C552E1B7-4D5D-4720-9190-356180982A87}" name="Hosts" dataDxfId="1" dataCellStyle="Millares"/>
+    <tableColumn id="3" xr3:uid="{E4368E94-D5DB-4EC6-9525-32C54F17D759}" name="Primer IP" dataDxfId="7"/>
+    <tableColumn id="4" xr3:uid="{E3B008EB-2EC2-453A-A957-6DE3704D4332}" name="Ultima IP" dataDxfId="6"/>
+    <tableColumn id="5" xr3:uid="{406FF1E2-D54D-437E-A099-5D7101698894}" name="Broadcast" dataDxfId="5"/>
+    <tableColumn id="6" xr3:uid="{3633FA0A-4FF6-4978-B548-F7218383F997}" name="Mascara" dataDxfId="4"/>
+    <tableColumn id="7" xr3:uid="{C552E1B7-4D5D-4720-9190-356180982A87}" name="Hosts" dataDxfId="3" dataCellStyle="Millares"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{B2F2D2BB-D473-4C7E-8F49-EFFA8697289E}" name="Tabla9" displayName="Tabla9" ref="A6:I11" totalsRowShown="0">
-  <autoFilter ref="A6:I11" xr:uid="{B2F2D2BB-D473-4C7E-8F49-EFFA8697289E}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{B2F2D2BB-D473-4C7E-8F49-EFFA8697289E}" name="Tabla9" displayName="Tabla9" ref="A6:I12" totalsRowShown="0">
+  <autoFilter ref="A6:I12" xr:uid="{B2F2D2BB-D473-4C7E-8F49-EFFA8697289E}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A7:I12">
+    <sortCondition descending="1" ref="B6:B12"/>
+  </sortState>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{D9906D0F-3946-4551-80EF-E794B6763060}" name="Depto"/>
     <tableColumn id="2" xr3:uid="{B76BD207-564D-4A40-B5DA-7BF31D94DFB2}" name="Hosts"/>
@@ -3980,10 +4144,53 @@
     <tableColumn id="5" xr3:uid="{7BF44CD3-59C1-477F-879E-BC30F033B13B}" name="Primer IP"/>
     <tableColumn id="6" xr3:uid="{DD6AB662-A048-4664-92D6-345C97C445DC}" name="Ultima IP"/>
     <tableColumn id="7" xr3:uid="{017E9AD7-B745-43B5-81F0-79C3975FB105}" name="Broadcast"/>
-    <tableColumn id="8" xr3:uid="{462988E0-4B36-40BC-A6DB-50D0502BF978}" name="Mask" dataDxfId="0"/>
-    <tableColumn id="9" xr3:uid="{C576A661-4DDB-4C17-9D73-FAECEDEB0934}" name="Hosts2"/>
+    <tableColumn id="8" xr3:uid="{462988E0-4B36-40BC-A6DB-50D0502BF978}" name="Mask" dataDxfId="2"/>
+    <tableColumn id="9" xr3:uid="{C576A661-4DDB-4C17-9D73-FAECEDEB0934}" name="Max"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{367C717A-65F1-46E7-8FDF-51DF27BFA891}" name="Tabla914" displayName="Tabla914" ref="A14:J20" totalsRowShown="0">
+  <autoFilter ref="A14:J20" xr:uid="{367C717A-65F1-46E7-8FDF-51DF27BFA891}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A15:I19">
+    <sortCondition ref="A7:A11"/>
+  </sortState>
+  <tableColumns count="10">
+    <tableColumn id="1" xr3:uid="{43FA649F-8A2E-435E-BE55-0F00E2C4E160}" name="Depto"/>
+    <tableColumn id="2" xr3:uid="{10CE8206-BAAA-4328-93A7-A4CC28834759}" name="Hosts"/>
+    <tableColumn id="3" xr3:uid="{4EF1EC2B-3EBA-4A5C-B063-E10AEF3E4D7B}" name="CIDR"/>
+    <tableColumn id="4" xr3:uid="{7BCAF0C4-A9E6-4752-A7E0-4A812F7D12D6}" name="RED"/>
+    <tableColumn id="5" xr3:uid="{2DE9B59C-A72A-42B0-B4DE-B00E3329E24E}" name="Primer IP"/>
+    <tableColumn id="6" xr3:uid="{E3B32BD5-A011-4074-9135-1D78A1D8D0A1}" name="Ultima IP"/>
+    <tableColumn id="7" xr3:uid="{EB8B7B11-882C-451E-8AE5-57CE5C74B7D2}" name="Broadcast"/>
+    <tableColumn id="8" xr3:uid="{CC654A28-A3D2-4157-92DD-1C6F330A2B20}" name="Mask" dataDxfId="1"/>
+    <tableColumn id="9" xr3:uid="{0627D91B-B04A-4845-AF26-CD7DC6A9C4F1}" name="Max"/>
+    <tableColumn id="10" xr3:uid="{40EBC305-F66C-458C-8A36-77260382BE6F}" name="Revision"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{BA564455-EE43-48C5-AB99-BA35B3C65474}" name="Tabla91415" displayName="Tabla91415" ref="A22:I28" totalsRowShown="0">
+  <autoFilter ref="A22:I28" xr:uid="{BA564455-EE43-48C5-AB99-BA35B3C65474}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A23:I27">
+    <sortCondition ref="A7:A11"/>
+  </sortState>
+  <tableColumns count="9">
+    <tableColumn id="1" xr3:uid="{B7018CE9-2CFA-4E0C-8E42-A011F8E485E3}" name="Depto"/>
+    <tableColumn id="2" xr3:uid="{AAB55690-CCD9-451A-9201-A021790E8348}" name="Hosts"/>
+    <tableColumn id="3" xr3:uid="{8E5DCC83-2F14-48D9-A9B9-26A32C73F620}" name="CIDR"/>
+    <tableColumn id="4" xr3:uid="{DFB74CF1-3CA1-4EDD-9045-071FC68ED657}" name="RED"/>
+    <tableColumn id="5" xr3:uid="{11EC91F0-F85E-4796-9D17-09C11D045938}" name="Primer IP"/>
+    <tableColumn id="6" xr3:uid="{C31AD560-C54A-4A84-997F-4A16C99758BB}" name="Ultima IP"/>
+    <tableColumn id="7" xr3:uid="{EB8D2EAC-2D7C-4332-B521-B4ED39D49F0C}" name="Broadcast"/>
+    <tableColumn id="8" xr3:uid="{4B8CFE69-4C9C-4A04-96D7-C3977051BF3C}" name="Mask" dataDxfId="0"/>
+    <tableColumn id="9" xr3:uid="{31C59E22-0F85-4BB1-A3DB-0A0F675C76CE}" name="Max"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium25" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -4000,12 +4207,12 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{EEE4898D-F2C9-4799-9B27-1047E0B389B5}" name="Tabla3" displayName="Tabla3" ref="E11:G16" totalsRowShown="0" tableBorderDxfId="29">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{EEE4898D-F2C9-4799-9B27-1047E0B389B5}" name="Tabla3" displayName="Tabla3" ref="E11:G16" totalsRowShown="0" tableBorderDxfId="31">
   <autoFilter ref="E11:G16" xr:uid="{EEE4898D-F2C9-4799-9B27-1047E0B389B5}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{2CD52E63-0CF7-448F-AFB9-E1222BA3751A}" name="Unidad" dataDxfId="28"/>
-    <tableColumn id="2" xr3:uid="{7C167E46-06D4-494C-BDD1-BE076BFED87B}" name="Equivalencia" dataDxfId="27"/>
-    <tableColumn id="3" xr3:uid="{718EF86A-E60E-4E44-AA6E-6B9F80923B2B}" name="Decimal" dataDxfId="26"/>
+    <tableColumn id="1" xr3:uid="{2CD52E63-0CF7-448F-AFB9-E1222BA3751A}" name="Unidad" dataDxfId="30"/>
+    <tableColumn id="2" xr3:uid="{7C167E46-06D4-494C-BDD1-BE076BFED87B}" name="Equivalencia" dataDxfId="29"/>
+    <tableColumn id="3" xr3:uid="{718EF86A-E60E-4E44-AA6E-6B9F80923B2B}" name="Decimal" dataDxfId="28"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4050,7 +4257,7 @@
   <autoFilter ref="A2:C10" xr:uid="{45E7EA22-C177-4276-8B26-DDBEF03C3978}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{FC122938-914F-4524-8BC2-A2AB7E9EFA2F}" name="TIA-568A"/>
-    <tableColumn id="2" xr3:uid="{01E34A6D-5A3D-4AB9-978D-1A0E98329F04}" name="Funcion" dataDxfId="25"/>
+    <tableColumn id="2" xr3:uid="{01E34A6D-5A3D-4AB9-978D-1A0E98329F04}" name="Funcion" dataDxfId="27"/>
     <tableColumn id="3" xr3:uid="{DB624384-12B4-4D70-9C0C-F257659F54DB}" name="TIA-568B"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -4058,12 +4265,12 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{211AC8E5-0F06-469C-8451-8834EF93985D}" name="Tabla8" displayName="Tabla8" ref="A1:C21" totalsRowShown="0" headerRowDxfId="24" dataDxfId="23" tableBorderDxfId="22">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{211AC8E5-0F06-469C-8451-8834EF93985D}" name="Tabla8" displayName="Tabla8" ref="A1:C21" totalsRowShown="0" headerRowDxfId="26" dataDxfId="25" tableBorderDxfId="24">
   <autoFilter ref="A1:C21" xr:uid="{211AC8E5-0F06-469C-8451-8834EF93985D}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{4876463E-FEC9-444A-9168-CF595FD609F6}" name="DEC" dataDxfId="21"/>
-    <tableColumn id="2" xr3:uid="{E4D07485-93E2-4F97-8FBE-604048C0DAF6}" name="BIN" dataDxfId="20"/>
-    <tableColumn id="3" xr3:uid="{49B333D7-98AB-40FA-A1DC-C5B4EFE941BE}" name="HEX" dataDxfId="19"/>
+    <tableColumn id="1" xr3:uid="{4876463E-FEC9-444A-9168-CF595FD609F6}" name="DEC" dataDxfId="23"/>
+    <tableColumn id="2" xr3:uid="{E4D07485-93E2-4F97-8FBE-604048C0DAF6}" name="BIN" dataDxfId="22"/>
+    <tableColumn id="3" xr3:uid="{49B333D7-98AB-40FA-A1DC-C5B4EFE941BE}" name="HEX" dataDxfId="21"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4073,13 +4280,13 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{4B54C147-9701-4C87-AAD9-57684EED0442}" name="Tabla10" displayName="Tabla10" ref="A7:G15" totalsRowShown="0">
   <autoFilter ref="A7:G15" xr:uid="{4B54C147-9701-4C87-AAD9-57684EED0442}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{3AE09342-9692-421C-A55C-FE1B0A7ECF19}" name="Binario" dataDxfId="18"/>
+    <tableColumn id="1" xr3:uid="{3AE09342-9692-421C-A55C-FE1B0A7ECF19}" name="Binario" dataDxfId="20"/>
     <tableColumn id="2" xr3:uid="{A8621E02-BA5A-45D8-9E8A-122B44769B98}" name="Red"/>
-    <tableColumn id="3" xr3:uid="{A1D38B69-7051-4F73-96BF-58502BFC45A2}" name="Primer IP" dataDxfId="17"/>
-    <tableColumn id="4" xr3:uid="{0EFB3B67-7DD6-485A-85F5-F023F312738D}" name="Ultima IP" dataDxfId="16"/>
-    <tableColumn id="5" xr3:uid="{80083827-B95B-41F1-A7D4-107398248A1B}" name="Broadcast" dataDxfId="15"/>
-    <tableColumn id="6" xr3:uid="{26BF6E67-CEB6-439B-A22A-E945E36678FB}" name="Mascara" dataDxfId="14"/>
-    <tableColumn id="7" xr3:uid="{EF991478-7589-40D7-B551-973071858FAD}" name="Hosts" dataDxfId="13" dataCellStyle="Millares"/>
+    <tableColumn id="3" xr3:uid="{A1D38B69-7051-4F73-96BF-58502BFC45A2}" name="Primer IP" dataDxfId="19"/>
+    <tableColumn id="4" xr3:uid="{0EFB3B67-7DD6-485A-85F5-F023F312738D}" name="Ultima IP" dataDxfId="18"/>
+    <tableColumn id="5" xr3:uid="{80083827-B95B-41F1-A7D4-107398248A1B}" name="Broadcast" dataDxfId="17"/>
+    <tableColumn id="6" xr3:uid="{26BF6E67-CEB6-439B-A22A-E945E36678FB}" name="Mascara" dataDxfId="16"/>
+    <tableColumn id="7" xr3:uid="{EF991478-7589-40D7-B551-973071858FAD}" name="Hosts" dataDxfId="15" dataCellStyle="Millares"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -6513,53 +6720,53 @@
       <c r="A1" s="85" t="s">
         <v>264</v>
       </c>
-      <c r="B1" s="172" t="s">
+      <c r="B1" s="166" t="s">
         <v>293</v>
       </c>
-      <c r="C1" s="172"/>
-      <c r="D1" s="172"/>
-      <c r="E1" s="173"/>
-      <c r="F1" s="172" t="s">
+      <c r="C1" s="166"/>
+      <c r="D1" s="166"/>
+      <c r="E1" s="167"/>
+      <c r="F1" s="166" t="s">
         <v>292</v>
       </c>
-      <c r="G1" s="172"/>
-      <c r="H1" s="172"/>
-      <c r="I1" s="173"/>
-      <c r="J1" s="172" t="s">
+      <c r="G1" s="166"/>
+      <c r="H1" s="166"/>
+      <c r="I1" s="167"/>
+      <c r="J1" s="166" t="s">
         <v>298</v>
       </c>
-      <c r="K1" s="172"/>
-      <c r="L1" s="172"/>
-      <c r="M1" s="173"/>
+      <c r="K1" s="166"/>
+      <c r="L1" s="166"/>
+      <c r="M1" s="167"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="86" t="s">
         <v>290</v>
       </c>
-      <c r="B2" s="170" t="s">
+      <c r="B2" s="168" t="s">
         <v>289</v>
       </c>
-      <c r="C2" s="170"/>
-      <c r="D2" s="170" t="s">
+      <c r="C2" s="168"/>
+      <c r="D2" s="168" t="s">
         <v>288</v>
       </c>
-      <c r="E2" s="171"/>
-      <c r="F2" s="170" t="s">
+      <c r="E2" s="169"/>
+      <c r="F2" s="168" t="s">
         <v>289</v>
       </c>
-      <c r="G2" s="170"/>
-      <c r="H2" s="170" t="s">
+      <c r="G2" s="168"/>
+      <c r="H2" s="168" t="s">
         <v>288</v>
       </c>
-      <c r="I2" s="171"/>
-      <c r="J2" s="170" t="s">
+      <c r="I2" s="169"/>
+      <c r="J2" s="168" t="s">
         <v>299</v>
       </c>
-      <c r="K2" s="171"/>
-      <c r="L2" s="170" t="s">
+      <c r="K2" s="169"/>
+      <c r="L2" s="168" t="s">
         <v>310</v>
       </c>
-      <c r="M2" s="171"/>
+      <c r="M2" s="169"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="87" t="s">
@@ -6744,16 +6951,16 @@
       <c r="E7" s="103" t="s">
         <v>279</v>
       </c>
-      <c r="F7" s="174" t="s">
+      <c r="F7" s="170" t="s">
         <v>16</v>
       </c>
-      <c r="G7" s="175"/>
-      <c r="H7" s="175"/>
-      <c r="I7" s="176"/>
-      <c r="J7" s="174"/>
-      <c r="K7" s="175"/>
-      <c r="L7" s="175"/>
-      <c r="M7" s="176"/>
+      <c r="G7" s="171"/>
+      <c r="H7" s="171"/>
+      <c r="I7" s="172"/>
+      <c r="J7" s="170"/>
+      <c r="K7" s="171"/>
+      <c r="L7" s="171"/>
+      <c r="M7" s="172"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="90" t="s">
@@ -6771,32 +6978,32 @@
       <c r="E8" s="108" t="s">
         <v>281</v>
       </c>
-      <c r="F8" s="177" t="s">
+      <c r="F8" s="173" t="s">
         <v>282</v>
       </c>
-      <c r="G8" s="178"/>
-      <c r="H8" s="178"/>
-      <c r="I8" s="179"/>
-      <c r="J8" s="177"/>
-      <c r="K8" s="178"/>
-      <c r="L8" s="178"/>
-      <c r="M8" s="179"/>
+      <c r="G8" s="174"/>
+      <c r="H8" s="174"/>
+      <c r="I8" s="175"/>
+      <c r="J8" s="173"/>
+      <c r="K8" s="174"/>
+      <c r="L8" s="174"/>
+      <c r="M8" s="175"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="91" t="s">
         <v>291</v>
       </c>
-      <c r="B9" s="166">
+      <c r="B9" s="176">
         <f>2^32</f>
         <v>4294967296</v>
       </c>
-      <c r="C9" s="166"/>
-      <c r="D9" s="166"/>
-      <c r="E9" s="167"/>
-      <c r="F9" s="168"/>
-      <c r="G9" s="168"/>
-      <c r="H9" s="168"/>
-      <c r="I9" s="169"/>
+      <c r="C9" s="176"/>
+      <c r="D9" s="176"/>
+      <c r="E9" s="177"/>
+      <c r="F9" s="178"/>
+      <c r="G9" s="178"/>
+      <c r="H9" s="178"/>
+      <c r="I9" s="179"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="114" t="s">
@@ -7331,11 +7538,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="J1:M1"/>
-    <mergeCell ref="J2:K2"/>
-    <mergeCell ref="L2:M2"/>
-    <mergeCell ref="J7:M7"/>
-    <mergeCell ref="J8:M8"/>
     <mergeCell ref="B9:E9"/>
     <mergeCell ref="F9:I9"/>
     <mergeCell ref="B2:C2"/>
@@ -7346,6 +7548,11 @@
     <mergeCell ref="F1:I1"/>
     <mergeCell ref="F7:I7"/>
     <mergeCell ref="F8:I8"/>
+    <mergeCell ref="J1:M1"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="L2:M2"/>
+    <mergeCell ref="J7:M7"/>
+    <mergeCell ref="J8:M8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -8056,23 +8263,30 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E5C05F7-1048-457F-9AB9-1A7675D27262}">
-  <dimension ref="A1:I12"/>
+  <dimension ref="A1:T28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:I1"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="Q14" sqref="Q14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.28515625" customWidth="1"/>
-    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.140625" customWidth="1"/>
-    <col min="4" max="6" width="10" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.42578125" customWidth="1"/>
+    <col min="1" max="1" width="4" customWidth="1"/>
+    <col min="2" max="2" width="8" customWidth="1"/>
+    <col min="3" max="3" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="16" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>445</v>
       </c>
@@ -8087,7 +8301,7 @@
       <c r="H1" s="161"/>
       <c r="I1" s="161"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="42" t="s">
         <v>455</v>
       </c>
@@ -8104,7 +8318,7 @@
       <c r="F3" s="145"/>
       <c r="G3" s="146"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="147" t="s">
         <v>447</v>
       </c>
@@ -8121,7 +8335,7 @@
       <c r="F4" s="148"/>
       <c r="G4" s="149"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="D5" t="s">
         <v>468</v>
       </c>
@@ -8135,7 +8349,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>450</v>
       </c>
@@ -8161,10 +8375,10 @@
         <v>459</v>
       </c>
       <c r="I6" t="s">
-        <v>481</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>43</v>
       </c>
@@ -8193,7 +8407,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>452</v>
       </c>
@@ -8222,7 +8436,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>451</v>
       </c>
@@ -8251,7 +8465,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>453</v>
       </c>
@@ -8265,7 +8479,7 @@
         <v>471</v>
       </c>
       <c r="E10" t="s">
-        <v>471</v>
+        <v>494</v>
       </c>
       <c r="F10" t="s">
         <v>480</v>
@@ -8280,7 +8494,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>454</v>
       </c>
@@ -8308,10 +8522,598 @@
       <c r="I11">
         <v>14</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="R11" t="s">
+        <v>283</v>
+      </c>
+      <c r="S11" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>481</v>
+      </c>
+      <c r="B12">
+        <v>2</v>
+      </c>
+      <c r="C12">
+        <v>30</v>
+      </c>
       <c r="D12" t="s">
         <v>477</v>
+      </c>
+      <c r="E12" t="s">
+        <v>482</v>
+      </c>
+      <c r="F12" t="s">
+        <v>483</v>
+      </c>
+      <c r="G12" t="s">
+        <v>484</v>
+      </c>
+      <c r="H12" s="152">
+        <v>255255255252</v>
+      </c>
+      <c r="I12">
+        <v>2</v>
+      </c>
+      <c r="R12" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="L13" t="s">
+        <v>311</v>
+      </c>
+      <c r="M13" t="s">
+        <v>499</v>
+      </c>
+      <c r="N13" t="s">
+        <v>500</v>
+      </c>
+      <c r="O13" t="s">
+        <v>501</v>
+      </c>
+      <c r="P13" t="s">
+        <v>502</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>262</v>
+      </c>
+      <c r="R13" t="s">
+        <v>474</v>
+      </c>
+      <c r="S13" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>450</v>
+      </c>
+      <c r="B14" t="s">
+        <v>369</v>
+      </c>
+      <c r="C14" t="s">
+        <v>300</v>
+      </c>
+      <c r="D14" t="s">
+        <v>458</v>
+      </c>
+      <c r="E14" t="s">
+        <v>366</v>
+      </c>
+      <c r="F14" t="s">
+        <v>367</v>
+      </c>
+      <c r="G14" t="s">
+        <v>17</v>
+      </c>
+      <c r="H14" t="s">
+        <v>459</v>
+      </c>
+      <c r="I14" t="s">
+        <v>485</v>
+      </c>
+      <c r="J14" t="s">
+        <v>508</v>
+      </c>
+      <c r="L14" t="s">
+        <v>527</v>
+      </c>
+      <c r="M14" s="151" t="s">
+        <v>335</v>
+      </c>
+      <c r="N14" s="151" t="s">
+        <v>336</v>
+      </c>
+      <c r="O14" s="151" t="s">
+        <v>184</v>
+      </c>
+      <c r="P14" s="151" t="s">
+        <v>184</v>
+      </c>
+      <c r="Q14" s="151" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>451</v>
+      </c>
+      <c r="B15">
+        <v>40</v>
+      </c>
+      <c r="C15">
+        <v>26</v>
+      </c>
+      <c r="D15" t="s">
+        <v>283</v>
+      </c>
+      <c r="E15" t="s">
+        <v>460</v>
+      </c>
+      <c r="F15" t="s">
+        <v>486</v>
+      </c>
+      <c r="G15" t="s">
+        <v>487</v>
+      </c>
+      <c r="H15" s="152">
+        <v>255255255192</v>
+      </c>
+      <c r="I15">
+        <v>62</v>
+      </c>
+      <c r="J15" t="s">
+        <v>503</v>
+      </c>
+      <c r="L15" t="s">
+        <v>528</v>
+      </c>
+      <c r="M15" s="151" t="s">
+        <v>335</v>
+      </c>
+      <c r="N15" s="151" t="s">
+        <v>336</v>
+      </c>
+      <c r="O15" s="151" t="s">
+        <v>529</v>
+      </c>
+      <c r="P15" s="151" t="s">
+        <v>184</v>
+      </c>
+      <c r="Q15" s="152" t="s">
+        <v>526</v>
+      </c>
+      <c r="S15" s="151" t="s">
+        <v>286</v>
+      </c>
+      <c r="T15">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>43</v>
+      </c>
+      <c r="B16">
+        <v>100</v>
+      </c>
+      <c r="C16">
+        <v>25</v>
+      </c>
+      <c r="D16" s="181" t="s">
+        <v>488</v>
+      </c>
+      <c r="E16" s="181" t="s">
+        <v>490</v>
+      </c>
+      <c r="F16" s="181" t="s">
+        <v>491</v>
+      </c>
+      <c r="G16" s="181" t="s">
+        <v>492</v>
+      </c>
+      <c r="H16" s="182">
+        <v>255255255128</v>
+      </c>
+      <c r="I16">
+        <v>126</v>
+      </c>
+      <c r="J16" t="s">
+        <v>506</v>
+      </c>
+      <c r="L16" t="s">
+        <v>313</v>
+      </c>
+      <c r="M16" s="151" t="s">
+        <v>187</v>
+      </c>
+      <c r="N16" s="151" t="s">
+        <v>187</v>
+      </c>
+      <c r="O16" s="151" t="s">
+        <v>509</v>
+      </c>
+      <c r="P16" s="151" t="s">
+        <v>184</v>
+      </c>
+      <c r="Q16" s="151" t="s">
+        <v>530</v>
+      </c>
+      <c r="S16" s="151" t="s">
+        <v>526</v>
+      </c>
+      <c r="T16">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>452</v>
+      </c>
+      <c r="B17">
+        <v>80</v>
+      </c>
+      <c r="C17">
+        <v>25</v>
+      </c>
+      <c r="D17" s="181" t="s">
+        <v>489</v>
+      </c>
+      <c r="E17" s="181" t="s">
+        <v>493</v>
+      </c>
+      <c r="F17" s="181" t="s">
+        <v>473</v>
+      </c>
+      <c r="G17" s="181" t="s">
+        <v>472</v>
+      </c>
+      <c r="H17" s="182">
+        <v>255255255128</v>
+      </c>
+      <c r="I17">
+        <v>126</v>
+      </c>
+      <c r="J17" t="s">
+        <v>507</v>
+      </c>
+      <c r="L17" t="s">
+        <v>315</v>
+      </c>
+      <c r="M17" s="151" t="s">
+        <v>335</v>
+      </c>
+      <c r="N17" s="151" t="s">
+        <v>336</v>
+      </c>
+      <c r="O17" s="151" t="s">
+        <v>184</v>
+      </c>
+      <c r="P17" s="151" t="s">
+        <v>184</v>
+      </c>
+      <c r="Q17" s="151" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>454</v>
+      </c>
+      <c r="B18">
+        <v>10</v>
+      </c>
+      <c r="C18">
+        <v>28</v>
+      </c>
+      <c r="D18" t="s">
+        <v>471</v>
+      </c>
+      <c r="E18" t="s">
+        <v>494</v>
+      </c>
+      <c r="F18" t="s">
+        <v>495</v>
+      </c>
+      <c r="G18" t="s">
+        <v>496</v>
+      </c>
+      <c r="H18" s="152">
+        <v>255255255240</v>
+      </c>
+      <c r="I18">
+        <v>14</v>
+      </c>
+      <c r="J18" t="s">
+        <v>504</v>
+      </c>
+      <c r="L18" t="s">
+        <v>314</v>
+      </c>
+      <c r="M18" s="151" t="s">
+        <v>335</v>
+      </c>
+      <c r="N18" s="151" t="s">
+        <v>336</v>
+      </c>
+      <c r="O18" s="151" t="s">
+        <v>531</v>
+      </c>
+      <c r="P18" s="151" t="s">
+        <v>187</v>
+      </c>
+      <c r="Q18" s="151" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>453</v>
+      </c>
+      <c r="B19">
+        <v>20</v>
+      </c>
+      <c r="C19">
+        <v>27</v>
+      </c>
+      <c r="D19" s="181" t="s">
+        <v>497</v>
+      </c>
+      <c r="E19" s="181" t="s">
+        <v>498</v>
+      </c>
+      <c r="F19" s="181" t="s">
+        <v>478</v>
+      </c>
+      <c r="G19" s="181" t="s">
+        <v>479</v>
+      </c>
+      <c r="H19" s="182">
+        <v>255255255224</v>
+      </c>
+      <c r="I19">
+        <v>30</v>
+      </c>
+      <c r="J19" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>481</v>
+      </c>
+      <c r="B20">
+        <v>2</v>
+      </c>
+      <c r="C20">
+        <v>30</v>
+      </c>
+      <c r="D20" t="s">
+        <v>477</v>
+      </c>
+      <c r="E20" t="s">
+        <v>482</v>
+      </c>
+      <c r="F20" t="s">
+        <v>483</v>
+      </c>
+      <c r="G20" t="s">
+        <v>484</v>
+      </c>
+      <c r="H20" s="152">
+        <v>255255255252</v>
+      </c>
+      <c r="I20">
+        <v>2</v>
+      </c>
+      <c r="J20" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>450</v>
+      </c>
+      <c r="B22" t="s">
+        <v>369</v>
+      </c>
+      <c r="C22" t="s">
+        <v>300</v>
+      </c>
+      <c r="D22" t="s">
+        <v>458</v>
+      </c>
+      <c r="E22" t="s">
+        <v>366</v>
+      </c>
+      <c r="F22" t="s">
+        <v>367</v>
+      </c>
+      <c r="G22" t="s">
+        <v>17</v>
+      </c>
+      <c r="H22" t="s">
+        <v>459</v>
+      </c>
+      <c r="I22" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>451</v>
+      </c>
+      <c r="B23">
+        <v>40</v>
+      </c>
+      <c r="C23">
+        <v>26</v>
+      </c>
+      <c r="D23" t="s">
+        <v>283</v>
+      </c>
+      <c r="E23" t="s">
+        <v>460</v>
+      </c>
+      <c r="F23" t="s">
+        <v>486</v>
+      </c>
+      <c r="G23" t="s">
+        <v>487</v>
+      </c>
+      <c r="H23" s="152">
+        <v>255255255192</v>
+      </c>
+      <c r="I23">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>43</v>
+      </c>
+      <c r="B24">
+        <v>100</v>
+      </c>
+      <c r="C24">
+        <v>25</v>
+      </c>
+      <c r="D24" s="181" t="s">
+        <v>461</v>
+      </c>
+      <c r="E24" s="181" t="s">
+        <v>462</v>
+      </c>
+      <c r="F24" s="181" t="s">
+        <v>465</v>
+      </c>
+      <c r="G24" s="181" t="s">
+        <v>466</v>
+      </c>
+      <c r="H24" s="182">
+        <v>255255255128</v>
+      </c>
+      <c r="I24">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>452</v>
+      </c>
+      <c r="B25">
+        <v>80</v>
+      </c>
+      <c r="C25">
+        <v>25</v>
+      </c>
+      <c r="D25" s="153" t="s">
+        <v>467</v>
+      </c>
+      <c r="E25" s="153" t="s">
+        <v>470</v>
+      </c>
+      <c r="F25" s="153" t="s">
+        <v>512</v>
+      </c>
+      <c r="G25" s="153" t="s">
+        <v>513</v>
+      </c>
+      <c r="H25" s="154">
+        <v>255255255128</v>
+      </c>
+      <c r="I25">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>454</v>
+      </c>
+      <c r="B26">
+        <v>10</v>
+      </c>
+      <c r="C26">
+        <v>28</v>
+      </c>
+      <c r="D26" t="s">
+        <v>511</v>
+      </c>
+      <c r="E26" t="s">
+        <v>514</v>
+      </c>
+      <c r="F26" t="s">
+        <v>515</v>
+      </c>
+      <c r="G26" t="s">
+        <v>516</v>
+      </c>
+      <c r="H26" s="152">
+        <v>255255255240</v>
+      </c>
+      <c r="I26">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>453</v>
+      </c>
+      <c r="B27">
+        <v>20</v>
+      </c>
+      <c r="C27">
+        <v>27</v>
+      </c>
+      <c r="D27" s="181" t="s">
+        <v>517</v>
+      </c>
+      <c r="E27" s="181" t="s">
+        <v>518</v>
+      </c>
+      <c r="F27" s="181" t="s">
+        <v>520</v>
+      </c>
+      <c r="G27" s="181" t="s">
+        <v>521</v>
+      </c>
+      <c r="H27" s="182">
+        <v>255255255224</v>
+      </c>
+      <c r="I27">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>481</v>
+      </c>
+      <c r="B28">
+        <v>2</v>
+      </c>
+      <c r="C28">
+        <v>30</v>
+      </c>
+      <c r="D28" t="s">
+        <v>519</v>
+      </c>
+      <c r="E28" t="s">
+        <v>522</v>
+      </c>
+      <c r="F28" t="s">
+        <v>523</v>
+      </c>
+      <c r="G28" t="s">
+        <v>524</v>
+      </c>
+      <c r="H28" s="152">
+        <v>255255255252</v>
+      </c>
+      <c r="I28">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -8321,9 +9123,12 @@
   <mergeCells count="1">
     <mergeCell ref="B1:I1"/>
   </mergeCells>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
+  <tableParts count="3">
     <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
comunicacion de segmentos de red
</commit_message>
<xml_diff>
--- a/docs/protocol-suite.xlsx
+++ b/docs/protocol-suite.xlsx
@@ -5,15 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EducacionIT\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EducacionIT\Documents\networks\CISCO\saves\ccna-lx08\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77C74F3E-3298-4E99-8FBC-A0709374D12A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75149EF9-4786-4EF7-A5F9-383C66927E61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{5C0FE7F9-9F0A-47A7-8741-1649DE5ACCD4}"/>
+    <workbookView xWindow="30" yWindow="30" windowWidth="20460" windowHeight="10770" activeTab="1" xr2:uid="{5C0FE7F9-9F0A-47A7-8741-1649DE5ACCD4}"/>
   </bookViews>
   <sheets>
     <sheet name="models" sheetId="1" r:id="rId1"/>
+    <sheet name="unidades" sheetId="2" r:id="rId2"/>
+    <sheet name="fisica" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="140">
   <si>
     <t>OSI de ISO</t>
   </si>
@@ -115,13 +117,352 @@
   </si>
   <si>
     <t>1000BaseTx - 1000BaseLx</t>
+  </si>
+  <si>
+    <t>Bit</t>
+  </si>
+  <si>
+    <t>unidad minima</t>
+  </si>
+  <si>
+    <t>Almacenamiento</t>
+  </si>
+  <si>
+    <t>Ancho de Banda</t>
+  </si>
+  <si>
+    <t>Byte</t>
+  </si>
+  <si>
+    <t>Unidad</t>
+  </si>
+  <si>
+    <t>Equivalencia</t>
+  </si>
+  <si>
+    <t>Representacion</t>
+  </si>
+  <si>
+    <t>10^0</t>
+  </si>
+  <si>
+    <t>8 bits</t>
+  </si>
+  <si>
+    <t>Binary Digit</t>
+  </si>
+  <si>
+    <t>KiloByte</t>
+  </si>
+  <si>
+    <t>1000 B</t>
+  </si>
+  <si>
+    <t>10^3</t>
+  </si>
+  <si>
+    <t>10^6</t>
+  </si>
+  <si>
+    <t>10^9</t>
+  </si>
+  <si>
+    <t>10^12</t>
+  </si>
+  <si>
+    <t>10^15</t>
+  </si>
+  <si>
+    <t>10^18</t>
+  </si>
+  <si>
+    <t>10^21</t>
+  </si>
+  <si>
+    <t>10^24</t>
+  </si>
+  <si>
+    <t>10^27</t>
+  </si>
+  <si>
+    <t>10^30</t>
+  </si>
+  <si>
+    <t>10^33</t>
+  </si>
+  <si>
+    <t>MegaByte</t>
+  </si>
+  <si>
+    <t>1000 KB</t>
+  </si>
+  <si>
+    <t>GigaByte</t>
+  </si>
+  <si>
+    <t>1000 MB</t>
+  </si>
+  <si>
+    <t>TeraByte</t>
+  </si>
+  <si>
+    <t>1000 GB</t>
+  </si>
+  <si>
+    <t>PetaByte</t>
+  </si>
+  <si>
+    <t>ExaByte</t>
+  </si>
+  <si>
+    <t>ZettaByte</t>
+  </si>
+  <si>
+    <t>YotaByte</t>
+  </si>
+  <si>
+    <t>BrontoByte</t>
+  </si>
+  <si>
+    <t>GeopByte</t>
+  </si>
+  <si>
+    <t>SaganByte</t>
+  </si>
+  <si>
+    <t>1000 TB</t>
+  </si>
+  <si>
+    <t>1000 PB</t>
+  </si>
+  <si>
+    <t>1000 XB</t>
+  </si>
+  <si>
+    <t>1000 ZB</t>
+  </si>
+  <si>
+    <t>1000 YB</t>
+  </si>
+  <si>
+    <t>1000 BB</t>
+  </si>
+  <si>
+    <t>1000 GeB</t>
+  </si>
+  <si>
+    <t>Kilobit /sec</t>
+  </si>
+  <si>
+    <t>Megabit /Sec</t>
+  </si>
+  <si>
+    <t>Gigabit /Sec</t>
+  </si>
+  <si>
+    <t>Terabit /Sec</t>
+  </si>
+  <si>
+    <t>Bits por segundo</t>
+  </si>
+  <si>
+    <t>bit/sec</t>
+  </si>
+  <si>
+    <t>1000 bps</t>
+  </si>
+  <si>
+    <t>1000 Kbps</t>
+  </si>
+  <si>
+    <t>1000 Mbps</t>
+  </si>
+  <si>
+    <t>1000 Gbps</t>
+  </si>
+  <si>
+    <t>Frecuencia</t>
+  </si>
+  <si>
+    <t>Hertz</t>
+  </si>
+  <si>
+    <t>KiloHertz</t>
+  </si>
+  <si>
+    <t>MegaHertz</t>
+  </si>
+  <si>
+    <t>GigaHertz</t>
+  </si>
+  <si>
+    <t>1 ciclo por segundo</t>
+  </si>
+  <si>
+    <t>1000Hz</t>
+  </si>
+  <si>
+    <t>1000KHz</t>
+  </si>
+  <si>
+    <t>1000MHz</t>
+  </si>
+  <si>
+    <t>AM</t>
+  </si>
+  <si>
+    <t>FM</t>
+  </si>
+  <si>
+    <t>PM</t>
+  </si>
+  <si>
+    <t>EMI</t>
+  </si>
+  <si>
+    <t>RFI</t>
+  </si>
+  <si>
+    <t>CrossTalk</t>
+  </si>
+  <si>
+    <t>Colision</t>
+  </si>
+  <si>
+    <t>Carrier</t>
+  </si>
+  <si>
+    <t>Concepto</t>
+  </si>
+  <si>
+    <t>Definicion</t>
+  </si>
+  <si>
+    <t>Interferencia ElectroMagnetica</t>
+  </si>
+  <si>
+    <t>Interferencia por RadioFrecuencia</t>
+  </si>
+  <si>
+    <t>Diafonia (Cruce de Señales)</t>
+  </si>
+  <si>
+    <t>Choque de Tramas (Señales)</t>
+  </si>
+  <si>
+    <t>TIA-568A</t>
+  </si>
+  <si>
+    <t>TIA-568B</t>
+  </si>
+  <si>
+    <t>B.verde</t>
+  </si>
+  <si>
+    <t>Verde</t>
+  </si>
+  <si>
+    <t>B.Naranja</t>
+  </si>
+  <si>
+    <t>Azul</t>
+  </si>
+  <si>
+    <t>B.Azul</t>
+  </si>
+  <si>
+    <t>Naranja</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B.Marron </t>
+  </si>
+  <si>
+    <t>Marron</t>
+  </si>
+  <si>
+    <t>Tx</t>
+  </si>
+  <si>
+    <t>Rx</t>
+  </si>
+  <si>
+    <t>SMF</t>
+  </si>
+  <si>
+    <t>MMF</t>
+  </si>
+  <si>
+    <t>Tipo</t>
+  </si>
+  <si>
+    <t>Fibra Optica</t>
+  </si>
+  <si>
+    <t>Monomodo</t>
+  </si>
+  <si>
+    <t>Multimodo</t>
+  </si>
+  <si>
+    <t>Luz</t>
+  </si>
+  <si>
+    <t>Laser</t>
+  </si>
+  <si>
+    <t>LED</t>
+  </si>
+  <si>
+    <t>Nucleo</t>
+  </si>
+  <si>
+    <t>Ventaja</t>
+  </si>
+  <si>
+    <t>Desventaja</t>
+  </si>
+  <si>
+    <t>Electrica</t>
+  </si>
+  <si>
+    <t>Economica</t>
+  </si>
+  <si>
+    <t>Distancia</t>
+  </si>
+  <si>
+    <t>200KM</t>
+  </si>
+  <si>
+    <t>2KM</t>
+  </si>
+  <si>
+    <t>Capacidad</t>
+  </si>
+  <si>
+    <t>10Gbps</t>
+  </si>
+  <si>
+    <t>100Gbps</t>
+  </si>
+  <si>
+    <t>Amplitud Modulada</t>
+  </si>
+  <si>
+    <t>Frecuencia Modulada</t>
+  </si>
+  <si>
+    <t>Fase Modulada</t>
+  </si>
+  <si>
+    <t>Señal Portadora</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -149,8 +490,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="20">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -199,8 +548,63 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="mediumGray">
+        <bgColor theme="9" tint="0.39997558519241921"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="mediumGray"/>
+    </fill>
+    <fill>
+      <patternFill patternType="mediumGray">
+        <bgColor theme="5" tint="0.39997558519241921"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="mediumGray">
+        <bgColor theme="9" tint="-0.249977111117893"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="mediumGray">
+        <bgColor theme="5" tint="-0.249977111117893"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="mediumGray">
+        <bgColor theme="4" tint="-0.249977111117893"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="mediumGray">
+        <bgColor theme="4" tint="0.59999389629810485"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="mediumGray">
+        <bgColor theme="7" tint="-0.249977111117893"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="mediumGray">
+        <bgColor theme="5" tint="-0.499984740745262"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor theme="0" tint="-0.14999847407452621"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -208,11 +612,22 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color theme="1"/>
+      </top>
+      <bottom style="medium">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
@@ -241,35 +656,78 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="2">
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
@@ -287,6 +745,30 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F321914E-0C2E-47FE-BF79-09AC5FEEFF7F}" name="Tabla2" displayName="Tabla2" ref="A4:C16" totalsRowShown="0">
+  <autoFilter ref="A4:C16" xr:uid="{F321914E-0C2E-47FE-BF79-09AC5FEEFF7F}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{797A346D-8319-41F2-8DBC-7D2930CA155C}" name="Unidad"/>
+    <tableColumn id="2" xr3:uid="{751E5162-6CCC-4BF7-A322-C3D0B01B872E}" name="Equivalencia"/>
+    <tableColumn id="3" xr3:uid="{E9368A4C-90B3-42CD-BF1F-3B3243FFB6F3}" name="Representacion"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E67F0501-A712-4C6B-A2BE-C0A5C2B48E86}" name="Tabla1" displayName="Tabla1" ref="E1:G8" totalsRowShown="0">
+  <autoFilter ref="E1:G8" xr:uid="{E67F0501-A712-4C6B-A2BE-C0A5C2B48E86}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{99A52C0E-0AE6-45DD-A9FF-5EC9F1B724B4}" name="Fibra Optica"/>
+    <tableColumn id="2" xr3:uid="{4FF6295B-B9D9-48D5-82E6-24F404E4B4AF}" name="SMF" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{3993BD79-1B61-487B-861B-D2A4B1FF702B}" name="MMF" dataDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -588,8 +1070,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D21B985-BDEA-4240-9CE0-603BEAF2CA2A}">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5:B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -601,16 +1083,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="10" t="s">
         <v>1</v>
       </c>
     </row>
@@ -618,13 +1100,13 @@
       <c r="A2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="D2" s="26" t="s">
         <v>8</v>
       </c>
     </row>
@@ -632,17 +1114,17 @@
       <c r="A3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="11"/>
-      <c r="C3" s="13"/>
-      <c r="D3" s="11"/>
+      <c r="B3" s="26"/>
+      <c r="C3" s="27"/>
+      <c r="D3" s="26"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="11"/>
-      <c r="C4" s="13"/>
-      <c r="D4" s="11"/>
+      <c r="B4" s="26"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="26"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
@@ -651,7 +1133,7 @@
       <c r="B5" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="14" t="s">
+      <c r="C5" s="11" t="s">
         <v>22</v>
       </c>
       <c r="D5" s="5" t="s">
@@ -665,7 +1147,7 @@
       <c r="B6" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="15" t="s">
+      <c r="C6" s="12" t="s">
         <v>23</v>
       </c>
       <c r="D6" s="7" t="s">
@@ -679,10 +1161,10 @@
       <c r="B7" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="C7" s="16" t="s">
+      <c r="C7" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="D7" s="10" t="s">
+      <c r="D7" s="25" t="s">
         <v>9</v>
       </c>
     </row>
@@ -693,18 +1175,18 @@
       <c r="B8" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="C8" s="17" t="s">
+      <c r="C8" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="D8" s="10"/>
+      <c r="D8" s="25"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="12" t="s">
+      <c r="A9" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="12"/>
-      <c r="C9" s="12"/>
-      <c r="D9" s="12" t="s">
+      <c r="B9" s="10"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="10" t="s">
         <v>5</v>
       </c>
     </row>
@@ -718,4 +1200,549 @@
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A317765E-A281-4865-BE02-AFF0F3EC16DB}">
+  <dimension ref="A1:J16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.85546875" customWidth="1"/>
+    <col min="3" max="3" width="15.42578125" customWidth="1"/>
+    <col min="4" max="4" width="3" customWidth="1"/>
+    <col min="5" max="5" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="3.85546875" customWidth="1"/>
+    <col min="10" max="10" width="34.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="31" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" s="31"/>
+      <c r="C3" s="31"/>
+      <c r="E3" s="31" t="s">
+        <v>30</v>
+      </c>
+      <c r="F3" s="31"/>
+      <c r="G3" s="31"/>
+    </row>
+    <row r="4" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E4" s="28" t="s">
+        <v>32</v>
+      </c>
+      <c r="F4" s="28" t="s">
+        <v>33</v>
+      </c>
+      <c r="G4" s="28" t="s">
+        <v>34</v>
+      </c>
+      <c r="I4" s="28" t="s">
+        <v>98</v>
+      </c>
+      <c r="J4" s="28" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C5" t="s">
+        <v>35</v>
+      </c>
+      <c r="E5" s="29" t="s">
+        <v>76</v>
+      </c>
+      <c r="F5" s="29" t="s">
+        <v>75</v>
+      </c>
+      <c r="G5" s="29" t="s">
+        <v>35</v>
+      </c>
+      <c r="I5" s="29" t="s">
+        <v>93</v>
+      </c>
+      <c r="J5" s="29" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C6" t="s">
+        <v>40</v>
+      </c>
+      <c r="E6" s="30" t="s">
+        <v>71</v>
+      </c>
+      <c r="F6" s="30" t="s">
+        <v>77</v>
+      </c>
+      <c r="G6" s="30" t="s">
+        <v>40</v>
+      </c>
+      <c r="I6" s="30" t="s">
+        <v>94</v>
+      </c>
+      <c r="J6" s="30" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>51</v>
+      </c>
+      <c r="B7" t="s">
+        <v>52</v>
+      </c>
+      <c r="C7" t="s">
+        <v>41</v>
+      </c>
+      <c r="E7" s="29" t="s">
+        <v>72</v>
+      </c>
+      <c r="F7" s="29" t="s">
+        <v>78</v>
+      </c>
+      <c r="G7" s="29" t="s">
+        <v>41</v>
+      </c>
+      <c r="I7" s="29" t="s">
+        <v>95</v>
+      </c>
+      <c r="J7" s="29" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>53</v>
+      </c>
+      <c r="B8" t="s">
+        <v>54</v>
+      </c>
+      <c r="C8" t="s">
+        <v>42</v>
+      </c>
+      <c r="E8" s="30" t="s">
+        <v>73</v>
+      </c>
+      <c r="F8" s="30" t="s">
+        <v>79</v>
+      </c>
+      <c r="G8" s="30" t="s">
+        <v>42</v>
+      </c>
+      <c r="I8" s="30" t="s">
+        <v>96</v>
+      </c>
+      <c r="J8" s="30" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>55</v>
+      </c>
+      <c r="B9" t="s">
+        <v>56</v>
+      </c>
+      <c r="C9" t="s">
+        <v>43</v>
+      </c>
+      <c r="E9" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="F9" s="29" t="s">
+        <v>80</v>
+      </c>
+      <c r="G9" s="29" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>57</v>
+      </c>
+      <c r="B10" t="s">
+        <v>64</v>
+      </c>
+      <c r="C10" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>58</v>
+      </c>
+      <c r="B11" t="s">
+        <v>65</v>
+      </c>
+      <c r="C11" t="s">
+        <v>45</v>
+      </c>
+      <c r="E11" s="31" t="s">
+        <v>81</v>
+      </c>
+      <c r="F11" s="31"/>
+      <c r="G11" s="31"/>
+    </row>
+    <row r="12" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>59</v>
+      </c>
+      <c r="B12" t="s">
+        <v>66</v>
+      </c>
+      <c r="C12" t="s">
+        <v>46</v>
+      </c>
+      <c r="E12" s="28" t="s">
+        <v>32</v>
+      </c>
+      <c r="F12" s="28" t="s">
+        <v>33</v>
+      </c>
+      <c r="G12" s="28" t="s">
+        <v>34</v>
+      </c>
+      <c r="I12" s="28" t="s">
+        <v>97</v>
+      </c>
+      <c r="J12" s="28" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>60</v>
+      </c>
+      <c r="B13" t="s">
+        <v>67</v>
+      </c>
+      <c r="C13" t="s">
+        <v>47</v>
+      </c>
+      <c r="E13" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="F13" s="29" t="s">
+        <v>86</v>
+      </c>
+      <c r="G13" s="29" t="s">
+        <v>35</v>
+      </c>
+      <c r="I13" s="29" t="s">
+        <v>90</v>
+      </c>
+      <c r="J13" s="29" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>61</v>
+      </c>
+      <c r="B14" t="s">
+        <v>68</v>
+      </c>
+      <c r="C14" t="s">
+        <v>48</v>
+      </c>
+      <c r="E14" s="30" t="s">
+        <v>83</v>
+      </c>
+      <c r="F14" s="30" t="s">
+        <v>87</v>
+      </c>
+      <c r="G14" s="30" t="s">
+        <v>40</v>
+      </c>
+      <c r="I14" s="30" t="s">
+        <v>91</v>
+      </c>
+      <c r="J14" s="30" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>62</v>
+      </c>
+      <c r="B15" t="s">
+        <v>69</v>
+      </c>
+      <c r="C15" t="s">
+        <v>49</v>
+      </c>
+      <c r="E15" s="29" t="s">
+        <v>84</v>
+      </c>
+      <c r="F15" s="29" t="s">
+        <v>88</v>
+      </c>
+      <c r="G15" s="29" t="s">
+        <v>41</v>
+      </c>
+      <c r="I15" s="29" t="s">
+        <v>92</v>
+      </c>
+      <c r="J15" s="29" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>63</v>
+      </c>
+      <c r="B16" t="s">
+        <v>70</v>
+      </c>
+      <c r="C16" t="s">
+        <v>50</v>
+      </c>
+      <c r="E16" s="30" t="s">
+        <v>85</v>
+      </c>
+      <c r="F16" s="30" t="s">
+        <v>89</v>
+      </c>
+      <c r="G16" s="30" t="s">
+        <v>42</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="E3:G3"/>
+    <mergeCell ref="E11:G11"/>
+  </mergeCells>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4AD9C28E-3B49-45BF-BDC2-96A37C9CBD38}">
+  <dimension ref="A1:G9"/>
+  <sheetViews>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1:G8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="13.85546875" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" customWidth="1"/>
+    <col min="5" max="5" width="12.42578125" customWidth="1"/>
+    <col min="6" max="6" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C1" t="s">
+        <v>105</v>
+      </c>
+      <c r="E1" t="s">
+        <v>119</v>
+      </c>
+      <c r="F1" t="s">
+        <v>116</v>
+      </c>
+      <c r="G1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="B2" s="23" t="s">
+        <v>114</v>
+      </c>
+      <c r="C2" s="16" t="s">
+        <v>108</v>
+      </c>
+      <c r="E2" t="s">
+        <v>118</v>
+      </c>
+      <c r="F2" s="24" t="s">
+        <v>120</v>
+      </c>
+      <c r="G2" s="24" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="17" t="s">
+        <v>107</v>
+      </c>
+      <c r="B3" s="23" t="s">
+        <v>114</v>
+      </c>
+      <c r="C3" s="18" t="s">
+        <v>111</v>
+      </c>
+      <c r="E3" t="s">
+        <v>122</v>
+      </c>
+      <c r="F3" s="24" t="s">
+        <v>123</v>
+      </c>
+      <c r="G3" s="24" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="16" t="s">
+        <v>108</v>
+      </c>
+      <c r="B4" s="23" t="s">
+        <v>115</v>
+      </c>
+      <c r="C4" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="E4" t="s">
+        <v>125</v>
+      </c>
+      <c r="F4" s="24">
+        <v>9</v>
+      </c>
+      <c r="G4" s="24">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="19" t="s">
+        <v>109</v>
+      </c>
+      <c r="B5" s="23"/>
+      <c r="C5" s="19" t="s">
+        <v>109</v>
+      </c>
+      <c r="E5" t="s">
+        <v>126</v>
+      </c>
+      <c r="F5" s="24" t="s">
+        <v>128</v>
+      </c>
+      <c r="G5" s="24" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="20" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6" s="23"/>
+      <c r="C6" s="20" t="s">
+        <v>110</v>
+      </c>
+      <c r="E6" t="s">
+        <v>127</v>
+      </c>
+      <c r="F6" s="24" t="s">
+        <v>129</v>
+      </c>
+      <c r="G6" s="24" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="18" t="s">
+        <v>111</v>
+      </c>
+      <c r="B7" s="23" t="s">
+        <v>115</v>
+      </c>
+      <c r="C7" s="17" t="s">
+        <v>107</v>
+      </c>
+      <c r="E7" t="s">
+        <v>130</v>
+      </c>
+      <c r="F7" s="24" t="s">
+        <v>131</v>
+      </c>
+      <c r="G7" s="24" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="21" t="s">
+        <v>112</v>
+      </c>
+      <c r="B8" s="23"/>
+      <c r="C8" s="21" t="s">
+        <v>112</v>
+      </c>
+      <c r="E8" t="s">
+        <v>133</v>
+      </c>
+      <c r="F8" s="24" t="s">
+        <v>134</v>
+      </c>
+      <c r="G8" s="24" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="22" t="s">
+        <v>113</v>
+      </c>
+      <c r="B9" s="23"/>
+      <c r="C9" s="22" t="s">
+        <v>113</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
enrutamiento estatico y subneteo
</commit_message>
<xml_diff>
--- a/docs/protocol-suite.xlsx
+++ b/docs/protocol-suite.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EducacionIT\Documents\networks\CISCO\saves\ccna-lx08\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13763AEF-7B87-43F3-A456-1733A36368DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99848AE4-4109-429F-84F0-5C0A4B5EF6A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30" yWindow="30" windowWidth="20460" windowHeight="10770" activeTab="4" xr2:uid="{5C0FE7F9-9F0A-47A7-8741-1649DE5ACCD4}"/>
+    <workbookView xWindow="30" yWindow="30" windowWidth="20460" windowHeight="10770" activeTab="5" xr2:uid="{5C0FE7F9-9F0A-47A7-8741-1649DE5ACCD4}"/>
   </bookViews>
   <sheets>
     <sheet name="models" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,8 @@
     <sheet name="fisica" sheetId="3" r:id="rId3"/>
     <sheet name="Sist." sheetId="4" r:id="rId4"/>
     <sheet name="IPv4" sheetId="5" r:id="rId5"/>
+    <sheet name="Classic" sheetId="6" r:id="rId6"/>
+    <sheet name="VLSM" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="507" uniqueCount="326">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="719" uniqueCount="477">
   <si>
     <t>OSI de ISO</t>
   </si>
@@ -1646,6 +1648,1047 @@
   </si>
   <si>
     <t>192.168.54.255</t>
+  </si>
+  <si>
+    <t>Subnetting</t>
+  </si>
+  <si>
+    <t>Practica que permite la subdivision de una red en redes mas pequeñas, a nivel logico, tomando bits de la porcion de hosts</t>
+  </si>
+  <si>
+    <t>Solicitado</t>
+  </si>
+  <si>
+    <t>Subredes</t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
+  <si>
+    <t>2^N &gt;= s</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>Red</t>
+  </si>
+  <si>
+    <t>A - 10.0.0.0</t>
+  </si>
+  <si>
+    <t>Salto</t>
+  </si>
+  <si>
+    <t>mask + N</t>
+  </si>
+  <si>
+    <t>Hosts</t>
+  </si>
+  <si>
+    <t>2^H-2</t>
+  </si>
+  <si>
+    <t>32-cidr</t>
+  </si>
+  <si>
+    <t>RED</t>
+  </si>
+  <si>
+    <t>Primer IP</t>
+  </si>
+  <si>
+    <t>Ultima IP</t>
+  </si>
+  <si>
+    <t>BROADCAST</t>
+  </si>
+  <si>
+    <t>10.0.0.1</t>
+  </si>
+  <si>
+    <t>255.224.0.0</t>
+  </si>
+  <si>
+    <t>NUMERO</t>
+  </si>
+  <si>
+    <t>01000000</t>
+  </si>
+  <si>
+    <t>11100000</t>
+  </si>
+  <si>
+    <t>porcion H</t>
+  </si>
+  <si>
+    <t>256 / subred</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>000</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>00000</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>001</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>00000</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>010</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>00000</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>011</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>00000</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>100</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>00000</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>101</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>00000</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>110</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>00000</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>111</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>00000</t>
+    </r>
+  </si>
+  <si>
+    <t>10.31.255.254</t>
+  </si>
+  <si>
+    <t>10.31.255.255</t>
+  </si>
+  <si>
+    <t>10.63.255.255</t>
+  </si>
+  <si>
+    <t>10.63.255.254</t>
+  </si>
+  <si>
+    <t>10.32.0.1</t>
+  </si>
+  <si>
+    <t>10.64.0.1</t>
+  </si>
+  <si>
+    <t>10.96.0.1</t>
+  </si>
+  <si>
+    <t>10.128.0.1</t>
+  </si>
+  <si>
+    <t>10.160.0.1</t>
+  </si>
+  <si>
+    <t>10.192.0.1</t>
+  </si>
+  <si>
+    <t>10.224.0.1</t>
+  </si>
+  <si>
+    <t>00011000</t>
+  </si>
+  <si>
+    <t>00011111</t>
+  </si>
+  <si>
+    <t>10.95.255.255</t>
+  </si>
+  <si>
+    <t>10.95.255.254</t>
+  </si>
+  <si>
+    <t>B-172.20.0.0</t>
+  </si>
+  <si>
+    <t>172.20.0.1</t>
+  </si>
+  <si>
+    <r>
+      <t>10.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.0.0</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>10.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>32</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.0.0</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>10.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>64</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.0.0</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>10.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>96</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.0.0</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>10.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>128</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.0.0</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>10.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>160</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.0.0</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>10.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>192</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.0.0</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>10.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>224</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.0.0</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>00</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>000000</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>01</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>000000</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>10</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>000000</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>11</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>000000</t>
+    </r>
+  </si>
+  <si>
+    <t>172.20.63.255</t>
+  </si>
+  <si>
+    <t>172.20.63.254</t>
+  </si>
+  <si>
+    <r>
+      <t>172.20.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>192</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.0</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>172.20.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>128</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.0</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>172.20.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>64</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.0</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>172.20.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.0</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>172.20.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>64</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>172.20.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>128</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>172.20.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>192</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <t>172.20.127.255</t>
+  </si>
+  <si>
+    <t>172.20.127.254</t>
+  </si>
+  <si>
+    <t>172.20.191.255</t>
+  </si>
+  <si>
+    <t>172.20.191.254</t>
+  </si>
+  <si>
+    <t>172.20.255.254</t>
+  </si>
+  <si>
+    <t>c -192.168.0.0</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>255.255.192.0</t>
+  </si>
+  <si>
+    <t>192.168.0.1</t>
+  </si>
+  <si>
+    <t>192.168.0.16</t>
+  </si>
+  <si>
+    <t>192.168.0.14</t>
+  </si>
+  <si>
+    <t>192.168.0.15</t>
+  </si>
+  <si>
+    <t>192.168.0.32</t>
+  </si>
+  <si>
+    <t>192.168.0.48</t>
+  </si>
+  <si>
+    <t>192.168.0.64</t>
+  </si>
+  <si>
+    <t>192.168.0.80</t>
+  </si>
+  <si>
+    <t>192.168.0.96</t>
+  </si>
+  <si>
+    <t>192.168.0.112</t>
+  </si>
+  <si>
+    <t>192.168.0.128</t>
+  </si>
+  <si>
+    <t>192.168.0.144</t>
+  </si>
+  <si>
+    <t>192.168.0.160</t>
+  </si>
+  <si>
+    <t>192.168.0.176</t>
+  </si>
+  <si>
+    <t>192.168.0.192</t>
+  </si>
+  <si>
+    <t>192.168.0.208</t>
+  </si>
+  <si>
+    <t>192.168.0.224</t>
+  </si>
+  <si>
+    <t>192.168.0.240</t>
+  </si>
+  <si>
+    <t>192.168.0.17</t>
+  </si>
+  <si>
+    <t>192.168.0.33</t>
+  </si>
+  <si>
+    <t>192.168.0.49</t>
+  </si>
+  <si>
+    <t>192.168.0.65</t>
+  </si>
+  <si>
+    <t>192.168.0.81</t>
+  </si>
+  <si>
+    <t>192.168.0.97</t>
+  </si>
+  <si>
+    <t>192.168.0.113</t>
+  </si>
+  <si>
+    <t>192.168.0.129</t>
+  </si>
+  <si>
+    <t>192.168.0.145</t>
+  </si>
+  <si>
+    <t>192.168.0.161</t>
+  </si>
+  <si>
+    <t>192.168.0.177</t>
+  </si>
+  <si>
+    <t>192.168.0.193</t>
+  </si>
+  <si>
+    <t>192.168.0.209</t>
+  </si>
+  <si>
+    <t>192.168.0.225</t>
+  </si>
+  <si>
+    <t>192.168.0.241</t>
+  </si>
+  <si>
+    <t>192.168.0.175</t>
+  </si>
+  <si>
+    <t>192.168.0.31</t>
+  </si>
+  <si>
+    <t>192.168.0.30</t>
+  </si>
+  <si>
+    <t>192.168.0.46</t>
+  </si>
+  <si>
+    <t>192.168.0.62</t>
+  </si>
+  <si>
+    <t>192.168.0.78</t>
+  </si>
+  <si>
+    <t>192.168.0.94</t>
+  </si>
+  <si>
+    <t>192.168.0.110</t>
+  </si>
+  <si>
+    <t>192.168.0.126</t>
+  </si>
+  <si>
+    <t>192.168.0.142</t>
+  </si>
+  <si>
+    <t>192.168.0.158</t>
+  </si>
+  <si>
+    <t>192.168.0.174</t>
+  </si>
+  <si>
+    <t>192.168.0.190</t>
+  </si>
+  <si>
+    <t>192.168.0.206</t>
+  </si>
+  <si>
+    <t>192.168.0.222</t>
+  </si>
+  <si>
+    <t>192.168.0.238</t>
+  </si>
+  <si>
+    <t>192.168.0.254</t>
+  </si>
+  <si>
+    <t>192.168.0.47</t>
+  </si>
+  <si>
+    <t>192.168.0.63</t>
+  </si>
+  <si>
+    <t>192.168.0.79</t>
+  </si>
+  <si>
+    <t>192.168.0.95</t>
+  </si>
+  <si>
+    <t>192.168.0.111</t>
+  </si>
+  <si>
+    <t>192.168.0.127</t>
+  </si>
+  <si>
+    <t>192.168.0.143</t>
+  </si>
+  <si>
+    <t>192.168.0.159</t>
+  </si>
+  <si>
+    <t>192.168.0.191</t>
+  </si>
+  <si>
+    <t>192.168.0.207</t>
+  </si>
+  <si>
+    <t>192.168.0.223</t>
+  </si>
+  <si>
+    <t>192.168.0.239</t>
+  </si>
+  <si>
+    <t>192.168.0.255</t>
+  </si>
+  <si>
+    <t>PAR</t>
+  </si>
+  <si>
+    <t>IMPAR</t>
+  </si>
+  <si>
+    <t>HOP</t>
+  </si>
+  <si>
+    <t>LIMIT</t>
+  </si>
+  <si>
+    <t>172.16.0.1</t>
+  </si>
+  <si>
+    <t>172.16.31.255</t>
+  </si>
+  <si>
+    <t>172.16.32.0</t>
+  </si>
+  <si>
+    <t>255.255.224.0</t>
+  </si>
+  <si>
+    <t>172.16.31.254</t>
   </si>
 </sst>
 </file>
@@ -1656,7 +2699,14 @@
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2091,83 +3141,83 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="107">
+  <cellXfs count="120">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2221,10 +3271,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="19" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2281,13 +3331,13 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="18" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="5" fillId="18" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="4" fillId="18" borderId="20" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="5" fillId="18" borderId="20" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="19" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2362,50 +3412,83 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2911,7 +3994,7 @@
     <mergeCell ref="B2:B4"/>
     <mergeCell ref="C2:C4"/>
   </mergeCells>
-  <phoneticPr fontId="2" type="noConversion"/>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -3267,7 +4350,7 @@
     <mergeCell ref="E3:G3"/>
     <mergeCell ref="E11:G11"/>
   </mergeCells>
-  <phoneticPr fontId="2" type="noConversion"/>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
@@ -3526,7 +4609,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
@@ -3781,16 +4864,16 @@
       <c r="K5" s="45" t="s">
         <v>163</v>
       </c>
-      <c r="L5" s="103" t="s">
+      <c r="L5" s="98" t="s">
         <v>223</v>
       </c>
-      <c r="M5" s="104"/>
-      <c r="N5" s="104"/>
-      <c r="O5" s="104"/>
-      <c r="P5" s="104"/>
-      <c r="Q5" s="104"/>
-      <c r="R5" s="104"/>
-      <c r="S5" s="105"/>
+      <c r="M5" s="99"/>
+      <c r="N5" s="99"/>
+      <c r="O5" s="99"/>
+      <c r="P5" s="99"/>
+      <c r="Q5" s="99"/>
+      <c r="R5" s="99"/>
+      <c r="S5" s="100"/>
       <c r="T5" s="46" t="s">
         <v>162</v>
       </c>
@@ -3814,10 +4897,10 @@
       <c r="F6" s="33">
         <v>16</v>
       </c>
-      <c r="H6" s="98" t="s">
+      <c r="H6" s="105" t="s">
         <v>231</v>
       </c>
-      <c r="I6" s="98"/>
+      <c r="I6" s="105"/>
       <c r="K6" s="47">
         <v>192</v>
       </c>
@@ -3919,25 +5002,25 @@
       <c r="AE7" s="28" t="s">
         <v>163</v>
       </c>
-      <c r="AF7" s="102">
+      <c r="AF7" s="104">
         <f>SUM(AF10:AU10)</f>
         <v>5620</v>
       </c>
-      <c r="AG7" s="102"/>
-      <c r="AH7" s="102"/>
-      <c r="AI7" s="102"/>
-      <c r="AJ7" s="102"/>
-      <c r="AK7" s="102"/>
-      <c r="AL7" s="102"/>
-      <c r="AM7" s="102"/>
-      <c r="AN7" s="102"/>
-      <c r="AO7" s="102"/>
-      <c r="AP7" s="102"/>
-      <c r="AQ7" s="102"/>
-      <c r="AR7" s="102"/>
-      <c r="AS7" s="102"/>
-      <c r="AT7" s="102"/>
-      <c r="AU7" s="102"/>
+      <c r="AG7" s="104"/>
+      <c r="AH7" s="104"/>
+      <c r="AI7" s="104"/>
+      <c r="AJ7" s="104"/>
+      <c r="AK7" s="104"/>
+      <c r="AL7" s="104"/>
+      <c r="AM7" s="104"/>
+      <c r="AN7" s="104"/>
+      <c r="AO7" s="104"/>
+      <c r="AP7" s="104"/>
+      <c r="AQ7" s="104"/>
+      <c r="AR7" s="104"/>
+      <c r="AS7" s="104"/>
+      <c r="AT7" s="104"/>
+      <c r="AU7" s="104"/>
     </row>
     <row r="8" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A8" s="28">
@@ -4200,30 +5283,30 @@
       <c r="AE10" s="28" t="s">
         <v>163</v>
       </c>
-      <c r="AF10" s="99">
+      <c r="AF10" s="101">
         <v>4096</v>
       </c>
-      <c r="AG10" s="100"/>
-      <c r="AH10" s="100"/>
-      <c r="AI10" s="101"/>
-      <c r="AJ10" s="99">
+      <c r="AG10" s="102"/>
+      <c r="AH10" s="102"/>
+      <c r="AI10" s="103"/>
+      <c r="AJ10" s="101">
         <v>1280</v>
       </c>
-      <c r="AK10" s="100"/>
-      <c r="AL10" s="100"/>
-      <c r="AM10" s="101"/>
-      <c r="AN10" s="99">
+      <c r="AK10" s="102"/>
+      <c r="AL10" s="102"/>
+      <c r="AM10" s="103"/>
+      <c r="AN10" s="101">
         <v>240</v>
       </c>
-      <c r="AO10" s="100"/>
-      <c r="AP10" s="100"/>
-      <c r="AQ10" s="101"/>
-      <c r="AR10" s="99">
+      <c r="AO10" s="102"/>
+      <c r="AP10" s="102"/>
+      <c r="AQ10" s="103"/>
+      <c r="AR10" s="101">
         <v>4</v>
       </c>
-      <c r="AS10" s="100"/>
-      <c r="AT10" s="100"/>
-      <c r="AU10" s="101"/>
+      <c r="AS10" s="102"/>
+      <c r="AT10" s="102"/>
+      <c r="AU10" s="103"/>
     </row>
     <row r="11" spans="1:47" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="28">
@@ -4241,10 +5324,10 @@
       <c r="F11" s="30">
         <v>16</v>
       </c>
-      <c r="H11" s="98" t="s">
+      <c r="H11" s="105" t="s">
         <v>231</v>
       </c>
-      <c r="I11" s="98"/>
+      <c r="I11" s="105"/>
       <c r="K11" s="51">
         <v>48</v>
       </c>
@@ -4294,30 +5377,30 @@
       <c r="AE11" s="28" t="s">
         <v>162</v>
       </c>
-      <c r="AF11" s="99">
+      <c r="AF11" s="101">
         <v>1</v>
       </c>
-      <c r="AG11" s="100"/>
-      <c r="AH11" s="100"/>
-      <c r="AI11" s="101"/>
-      <c r="AJ11" s="99">
+      <c r="AG11" s="102"/>
+      <c r="AH11" s="102"/>
+      <c r="AI11" s="103"/>
+      <c r="AJ11" s="101">
         <v>5</v>
       </c>
-      <c r="AK11" s="100"/>
-      <c r="AL11" s="100"/>
-      <c r="AM11" s="101"/>
-      <c r="AN11" s="99" t="s">
+      <c r="AK11" s="102"/>
+      <c r="AL11" s="102"/>
+      <c r="AM11" s="103"/>
+      <c r="AN11" s="101" t="s">
         <v>238</v>
       </c>
-      <c r="AO11" s="100"/>
-      <c r="AP11" s="100"/>
-      <c r="AQ11" s="101"/>
-      <c r="AR11" s="99">
+      <c r="AO11" s="102"/>
+      <c r="AP11" s="102"/>
+      <c r="AQ11" s="103"/>
+      <c r="AR11" s="101">
         <v>4</v>
       </c>
-      <c r="AS11" s="100"/>
-      <c r="AT11" s="100"/>
-      <c r="AU11" s="101"/>
+      <c r="AS11" s="102"/>
+      <c r="AT11" s="102"/>
+      <c r="AU11" s="103"/>
     </row>
     <row r="12" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A12" s="28">
@@ -4570,10 +5653,10 @@
       <c r="F16" s="30">
         <v>16</v>
       </c>
-      <c r="H16" s="98" t="s">
+      <c r="H16" s="105" t="s">
         <v>231</v>
       </c>
-      <c r="I16" s="98"/>
+      <c r="I16" s="105"/>
       <c r="K16" s="57">
         <v>10</v>
       </c>
@@ -4709,10 +5792,10 @@
       <c r="F20" s="30">
         <v>16</v>
       </c>
-      <c r="H20" s="98" t="s">
+      <c r="H20" s="105" t="s">
         <v>231</v>
       </c>
-      <c r="I20" s="98"/>
+      <c r="I20" s="105"/>
       <c r="X20" s="32"/>
       <c r="Y20" s="36"/>
     </row>
@@ -4749,22 +5832,22 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="H16:I16"/>
+    <mergeCell ref="H20:I20"/>
+    <mergeCell ref="H11:I11"/>
+    <mergeCell ref="AF10:AI10"/>
+    <mergeCell ref="AF11:AI11"/>
+    <mergeCell ref="AJ11:AM11"/>
+    <mergeCell ref="AN11:AQ11"/>
+    <mergeCell ref="AR11:AU11"/>
+    <mergeCell ref="H6:I6"/>
     <mergeCell ref="L5:S5"/>
     <mergeCell ref="AJ10:AM10"/>
     <mergeCell ref="AN10:AQ10"/>
     <mergeCell ref="AR10:AU10"/>
     <mergeCell ref="AF7:AU7"/>
-    <mergeCell ref="AF11:AI11"/>
-    <mergeCell ref="AJ11:AM11"/>
-    <mergeCell ref="AN11:AQ11"/>
-    <mergeCell ref="AR11:AU11"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="H16:I16"/>
-    <mergeCell ref="H20:I20"/>
-    <mergeCell ref="H11:I11"/>
-    <mergeCell ref="AF10:AI10"/>
   </mergeCells>
-  <phoneticPr fontId="2" type="noConversion"/>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
@@ -4776,7 +5859,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8CBB112-D597-4FBD-BD71-E33EC2CA62E0}">
   <dimension ref="A1:N26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView topLeftCell="A11" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection activeCell="A13" sqref="A13"/>
       <selection pane="topRight" activeCell="L26" sqref="L26"/>
@@ -4803,24 +5886,24 @@
       <c r="A1" s="28" t="s">
         <v>239</v>
       </c>
-      <c r="B1" s="98" t="s">
+      <c r="B1" s="105" t="s">
         <v>243</v>
       </c>
-      <c r="C1" s="98"/>
-      <c r="D1" s="98"/>
-      <c r="E1" s="98"/>
-      <c r="F1" s="98" t="s">
+      <c r="C1" s="105"/>
+      <c r="D1" s="105"/>
+      <c r="E1" s="105"/>
+      <c r="F1" s="105" t="s">
         <v>244</v>
       </c>
-      <c r="G1" s="98"/>
-      <c r="H1" s="98"/>
-      <c r="I1" s="98"/>
-      <c r="J1" s="98" t="s">
+      <c r="G1" s="105"/>
+      <c r="H1" s="105"/>
+      <c r="I1" s="105"/>
+      <c r="J1" s="105" t="s">
         <v>275</v>
       </c>
-      <c r="K1" s="98"/>
-      <c r="L1" s="98"/>
-      <c r="M1" s="98"/>
+      <c r="K1" s="105"/>
+      <c r="L1" s="105"/>
+      <c r="M1" s="105"/>
     </row>
     <row r="2" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="45" t="s">
@@ -5599,4 +6682,1291 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DB791F0-092A-481B-B45B-741D866A422F}">
+  <dimension ref="A1:V65"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D51" sqref="D51"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="22" width="4.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:22" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="110" t="s">
+        <v>326</v>
+      </c>
+      <c r="B1" s="111" t="s">
+        <v>327</v>
+      </c>
+      <c r="C1" s="111"/>
+      <c r="D1" s="111"/>
+      <c r="E1" s="111"/>
+      <c r="F1" s="111"/>
+      <c r="G1" s="111"/>
+      <c r="H1" s="111"/>
+      <c r="O1">
+        <v>1</v>
+      </c>
+      <c r="P1">
+        <v>1</v>
+      </c>
+      <c r="Q1">
+        <v>1</v>
+      </c>
+      <c r="R1">
+        <v>1</v>
+      </c>
+      <c r="S1">
+        <v>1</v>
+      </c>
+      <c r="T1">
+        <v>1</v>
+      </c>
+      <c r="U1">
+        <v>1</v>
+      </c>
+      <c r="V1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>333</v>
+      </c>
+      <c r="B2" s="107" t="s">
+        <v>328</v>
+      </c>
+      <c r="C2" s="107" t="s">
+        <v>329</v>
+      </c>
+      <c r="D2" s="107" t="s">
+        <v>21</v>
+      </c>
+      <c r="E2" s="107" t="s">
+        <v>335</v>
+      </c>
+      <c r="F2" s="107" t="s">
+        <v>277</v>
+      </c>
+      <c r="G2" s="107" t="s">
+        <v>349</v>
+      </c>
+      <c r="H2" s="107" t="s">
+        <v>337</v>
+      </c>
+      <c r="N2" t="s">
+        <v>276</v>
+      </c>
+      <c r="O2">
+        <v>128</v>
+      </c>
+      <c r="P2">
+        <v>192</v>
+      </c>
+      <c r="Q2">
+        <v>224</v>
+      </c>
+      <c r="R2">
+        <v>240</v>
+      </c>
+      <c r="S2">
+        <v>248</v>
+      </c>
+      <c r="T2">
+        <v>252</v>
+      </c>
+      <c r="U2">
+        <v>254</v>
+      </c>
+      <c r="V2">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>240</v>
+      </c>
+      <c r="B3" s="107" t="s">
+        <v>330</v>
+      </c>
+      <c r="C3" s="107" t="s">
+        <v>331</v>
+      </c>
+      <c r="D3" s="107" t="s">
+        <v>332</v>
+      </c>
+      <c r="E3" s="107" t="s">
+        <v>350</v>
+      </c>
+      <c r="F3" s="107" t="s">
+        <v>336</v>
+      </c>
+      <c r="G3" s="107" t="s">
+        <v>339</v>
+      </c>
+      <c r="H3" s="107" t="s">
+        <v>338</v>
+      </c>
+      <c r="N3" t="s">
+        <v>470</v>
+      </c>
+      <c r="O3">
+        <v>128</v>
+      </c>
+      <c r="P3">
+        <v>64</v>
+      </c>
+      <c r="Q3">
+        <v>32</v>
+      </c>
+      <c r="R3">
+        <v>16</v>
+      </c>
+      <c r="S3">
+        <v>8</v>
+      </c>
+      <c r="T3">
+        <v>4</v>
+      </c>
+      <c r="U3">
+        <v>2</v>
+      </c>
+      <c r="V3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>334</v>
+      </c>
+      <c r="B4" s="107">
+        <v>5</v>
+      </c>
+      <c r="C4" s="107">
+        <v>8</v>
+      </c>
+      <c r="D4" s="107">
+        <v>3</v>
+      </c>
+      <c r="E4" s="107">
+        <v>32</v>
+      </c>
+      <c r="F4" s="107">
+        <v>11</v>
+      </c>
+      <c r="G4" s="107">
+        <v>21</v>
+      </c>
+      <c r="H4" s="108">
+        <f>2^21-2</f>
+        <v>2097150</v>
+      </c>
+      <c r="N4" t="s">
+        <v>471</v>
+      </c>
+      <c r="O4">
+        <v>0</v>
+      </c>
+      <c r="P4">
+        <v>0</v>
+      </c>
+      <c r="Q4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="O5">
+        <v>128</v>
+      </c>
+      <c r="P5">
+        <v>64</v>
+      </c>
+      <c r="Q5">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>346</v>
+      </c>
+      <c r="B6" t="s">
+        <v>223</v>
+      </c>
+      <c r="C6" t="s">
+        <v>340</v>
+      </c>
+      <c r="D6" t="s">
+        <v>341</v>
+      </c>
+      <c r="E6" t="s">
+        <v>342</v>
+      </c>
+      <c r="F6" t="s">
+        <v>343</v>
+      </c>
+      <c r="G6" t="s">
+        <v>276</v>
+      </c>
+      <c r="P6">
+        <v>128</v>
+      </c>
+      <c r="Q6">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>0</v>
+      </c>
+      <c r="B7" s="109" t="s">
+        <v>351</v>
+      </c>
+      <c r="C7" s="112" t="s">
+        <v>376</v>
+      </c>
+      <c r="D7" s="113" t="s">
+        <v>344</v>
+      </c>
+      <c r="E7" s="107" t="s">
+        <v>359</v>
+      </c>
+      <c r="F7" s="107" t="s">
+        <v>360</v>
+      </c>
+      <c r="G7" s="107" t="s">
+        <v>345</v>
+      </c>
+      <c r="I7" s="107" t="s">
+        <v>286</v>
+      </c>
+      <c r="J7" s="107" t="s">
+        <v>291</v>
+      </c>
+      <c r="K7" s="107" t="s">
+        <v>292</v>
+      </c>
+      <c r="L7" s="107" t="s">
+        <v>293</v>
+      </c>
+      <c r="M7" s="107" t="s">
+        <v>294</v>
+      </c>
+      <c r="P7">
+        <v>192</v>
+      </c>
+      <c r="Q7">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>1</v>
+      </c>
+      <c r="B8" s="109" t="s">
+        <v>352</v>
+      </c>
+      <c r="C8" s="112" t="s">
+        <v>377</v>
+      </c>
+      <c r="D8" s="112" t="s">
+        <v>363</v>
+      </c>
+      <c r="E8" s="107" t="s">
+        <v>362</v>
+      </c>
+      <c r="F8" s="107" t="s">
+        <v>361</v>
+      </c>
+      <c r="G8" s="107" t="s">
+        <v>345</v>
+      </c>
+      <c r="I8" t="s">
+        <v>287</v>
+      </c>
+      <c r="J8" s="114" t="s">
+        <v>177</v>
+      </c>
+      <c r="K8" s="114" t="s">
+        <v>370</v>
+      </c>
+      <c r="L8" s="114" t="s">
+        <v>347</v>
+      </c>
+      <c r="M8" s="114" t="s">
+        <v>183</v>
+      </c>
+      <c r="Q8">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>2</v>
+      </c>
+      <c r="B9" s="109" t="s">
+        <v>353</v>
+      </c>
+      <c r="C9" s="112" t="s">
+        <v>378</v>
+      </c>
+      <c r="D9" s="112" t="s">
+        <v>364</v>
+      </c>
+      <c r="E9" s="107" t="s">
+        <v>373</v>
+      </c>
+      <c r="F9" s="107" t="s">
+        <v>372</v>
+      </c>
+      <c r="G9" s="107" t="s">
+        <v>345</v>
+      </c>
+      <c r="I9" t="s">
+        <v>276</v>
+      </c>
+      <c r="J9" s="114">
+        <v>11111111</v>
+      </c>
+      <c r="K9" s="114" t="s">
+        <v>348</v>
+      </c>
+      <c r="L9" s="114" t="s">
+        <v>167</v>
+      </c>
+      <c r="M9" s="114" t="s">
+        <v>167</v>
+      </c>
+      <c r="Q9">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>3</v>
+      </c>
+      <c r="B10" s="109" t="s">
+        <v>354</v>
+      </c>
+      <c r="C10" s="112" t="s">
+        <v>379</v>
+      </c>
+      <c r="D10" s="112" t="s">
+        <v>365</v>
+      </c>
+      <c r="E10" s="115">
+        <v>10127255254</v>
+      </c>
+      <c r="F10" s="115">
+        <v>10127255255</v>
+      </c>
+      <c r="G10" s="107" t="s">
+        <v>345</v>
+      </c>
+      <c r="I10" t="s">
+        <v>289</v>
+      </c>
+      <c r="J10" s="114" t="s">
+        <v>177</v>
+      </c>
+      <c r="K10" s="114" t="s">
+        <v>167</v>
+      </c>
+      <c r="L10" s="114" t="s">
+        <v>167</v>
+      </c>
+      <c r="M10" s="114" t="s">
+        <v>167</v>
+      </c>
+      <c r="Q10">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>4</v>
+      </c>
+      <c r="B11" s="109" t="s">
+        <v>355</v>
+      </c>
+      <c r="C11" s="112" t="s">
+        <v>380</v>
+      </c>
+      <c r="D11" s="112" t="s">
+        <v>366</v>
+      </c>
+      <c r="E11" s="115">
+        <v>10159255254</v>
+      </c>
+      <c r="F11" s="115">
+        <v>10159255255</v>
+      </c>
+      <c r="G11" s="107" t="s">
+        <v>345</v>
+      </c>
+      <c r="I11" t="s">
+        <v>290</v>
+      </c>
+      <c r="J11" s="114" t="s">
+        <v>177</v>
+      </c>
+      <c r="K11" s="114" t="s">
+        <v>371</v>
+      </c>
+      <c r="L11" s="114">
+        <v>11111111</v>
+      </c>
+      <c r="M11" s="114">
+        <v>11111111</v>
+      </c>
+      <c r="Q11">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>5</v>
+      </c>
+      <c r="B12" s="109" t="s">
+        <v>356</v>
+      </c>
+      <c r="C12" s="112" t="s">
+        <v>381</v>
+      </c>
+      <c r="D12" s="112" t="s">
+        <v>367</v>
+      </c>
+      <c r="E12" s="115">
+        <v>10191255254</v>
+      </c>
+      <c r="F12" s="115">
+        <v>10191255255</v>
+      </c>
+      <c r="G12" s="107" t="s">
+        <v>345</v>
+      </c>
+      <c r="J12" s="109"/>
+      <c r="K12" s="109"/>
+      <c r="L12" s="109"/>
+      <c r="M12" s="109"/>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>6</v>
+      </c>
+      <c r="B13" s="109" t="s">
+        <v>357</v>
+      </c>
+      <c r="C13" s="112" t="s">
+        <v>382</v>
+      </c>
+      <c r="D13" s="112" t="s">
+        <v>368</v>
+      </c>
+      <c r="E13" s="115">
+        <v>10223255254</v>
+      </c>
+      <c r="F13" s="115">
+        <v>10223255255</v>
+      </c>
+      <c r="G13" s="107" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>7</v>
+      </c>
+      <c r="B14" s="109" t="s">
+        <v>358</v>
+      </c>
+      <c r="C14" s="112" t="s">
+        <v>383</v>
+      </c>
+      <c r="D14" s="112" t="s">
+        <v>369</v>
+      </c>
+      <c r="E14" s="116">
+        <v>10255255254</v>
+      </c>
+      <c r="F14" s="116">
+        <v>10255255255</v>
+      </c>
+      <c r="G14" s="107" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>374</v>
+      </c>
+      <c r="B16">
+        <v>3</v>
+      </c>
+      <c r="C16">
+        <v>4</v>
+      </c>
+      <c r="D16">
+        <v>2</v>
+      </c>
+      <c r="E16" s="115">
+        <v>64</v>
+      </c>
+      <c r="F16" s="115">
+        <v>18</v>
+      </c>
+      <c r="G16">
+        <v>14</v>
+      </c>
+      <c r="H16" s="117">
+        <f>2^14-2</f>
+        <v>16382</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>346</v>
+      </c>
+      <c r="B18" t="s">
+        <v>223</v>
+      </c>
+      <c r="C18" t="s">
+        <v>340</v>
+      </c>
+      <c r="D18" t="s">
+        <v>341</v>
+      </c>
+      <c r="E18" t="s">
+        <v>342</v>
+      </c>
+      <c r="F18" t="s">
+        <v>343</v>
+      </c>
+      <c r="G18" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>0</v>
+      </c>
+      <c r="B19" s="109" t="s">
+        <v>384</v>
+      </c>
+      <c r="C19" s="109" t="s">
+        <v>393</v>
+      </c>
+      <c r="D19" s="109" t="s">
+        <v>375</v>
+      </c>
+      <c r="E19" s="107" t="s">
+        <v>389</v>
+      </c>
+      <c r="F19" s="107" t="s">
+        <v>388</v>
+      </c>
+      <c r="G19" s="107" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>1</v>
+      </c>
+      <c r="B20" s="109" t="s">
+        <v>385</v>
+      </c>
+      <c r="C20" s="109" t="s">
+        <v>392</v>
+      </c>
+      <c r="D20" s="109" t="s">
+        <v>394</v>
+      </c>
+      <c r="E20" s="107" t="s">
+        <v>398</v>
+      </c>
+      <c r="F20" s="107" t="s">
+        <v>397</v>
+      </c>
+      <c r="G20" s="107" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>2</v>
+      </c>
+      <c r="B21" s="109" t="s">
+        <v>386</v>
+      </c>
+      <c r="C21" s="112" t="s">
+        <v>391</v>
+      </c>
+      <c r="D21" s="112" t="s">
+        <v>395</v>
+      </c>
+      <c r="E21" s="107" t="s">
+        <v>400</v>
+      </c>
+      <c r="F21" s="107" t="s">
+        <v>399</v>
+      </c>
+      <c r="G21" s="107" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>3</v>
+      </c>
+      <c r="B22" s="109" t="s">
+        <v>387</v>
+      </c>
+      <c r="C22" s="112" t="s">
+        <v>390</v>
+      </c>
+      <c r="D22" s="112" t="s">
+        <v>396</v>
+      </c>
+      <c r="E22" s="115" t="s">
+        <v>401</v>
+      </c>
+      <c r="F22" s="115" t="s">
+        <v>308</v>
+      </c>
+      <c r="G22" s="107" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B23" s="109"/>
+      <c r="C23" s="112"/>
+      <c r="D23" s="112"/>
+      <c r="E23" s="115"/>
+      <c r="F23" s="115"/>
+      <c r="G23" s="107"/>
+    </row>
+    <row r="24" spans="1:8" s="107" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="107" t="s">
+        <v>402</v>
+      </c>
+      <c r="B24" s="114" t="s">
+        <v>403</v>
+      </c>
+      <c r="C24" s="113">
+        <v>16</v>
+      </c>
+      <c r="D24" s="113">
+        <v>4</v>
+      </c>
+      <c r="E24" s="118">
+        <v>16</v>
+      </c>
+      <c r="F24" s="118">
+        <v>28</v>
+      </c>
+      <c r="G24" s="107">
+        <v>4</v>
+      </c>
+      <c r="H24" s="107">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B25" s="109"/>
+      <c r="C25" s="112" t="s">
+        <v>468</v>
+      </c>
+      <c r="D25" s="112" t="s">
+        <v>469</v>
+      </c>
+      <c r="E25" s="115" t="s">
+        <v>468</v>
+      </c>
+      <c r="F25" s="115" t="s">
+        <v>469</v>
+      </c>
+      <c r="G25" s="107"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>346</v>
+      </c>
+      <c r="B26" t="s">
+        <v>223</v>
+      </c>
+      <c r="C26" t="s">
+        <v>340</v>
+      </c>
+      <c r="D26" t="s">
+        <v>341</v>
+      </c>
+      <c r="E26" t="s">
+        <v>342</v>
+      </c>
+      <c r="F26" t="s">
+        <v>343</v>
+      </c>
+      <c r="G26" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>0</v>
+      </c>
+      <c r="B27" s="109"/>
+      <c r="C27" s="109" t="s">
+        <v>268</v>
+      </c>
+      <c r="D27" s="109" t="s">
+        <v>405</v>
+      </c>
+      <c r="E27" s="107" t="s">
+        <v>407</v>
+      </c>
+      <c r="F27" s="107" t="s">
+        <v>408</v>
+      </c>
+      <c r="G27" s="119">
+        <v>255255255240</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>1</v>
+      </c>
+      <c r="B28" s="109"/>
+      <c r="C28" s="109" t="s">
+        <v>406</v>
+      </c>
+      <c r="D28" s="109" t="s">
+        <v>423</v>
+      </c>
+      <c r="E28" s="107" t="s">
+        <v>440</v>
+      </c>
+      <c r="F28" s="107" t="s">
+        <v>439</v>
+      </c>
+      <c r="G28" s="119">
+        <v>255255255240</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>2</v>
+      </c>
+      <c r="B29" s="109"/>
+      <c r="C29" s="109" t="s">
+        <v>409</v>
+      </c>
+      <c r="D29" s="109" t="s">
+        <v>424</v>
+      </c>
+      <c r="E29" s="107" t="s">
+        <v>441</v>
+      </c>
+      <c r="F29" s="107" t="s">
+        <v>455</v>
+      </c>
+      <c r="G29" s="119">
+        <v>255255255240</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>3</v>
+      </c>
+      <c r="B30" s="109"/>
+      <c r="C30" s="109" t="s">
+        <v>410</v>
+      </c>
+      <c r="D30" s="109" t="s">
+        <v>425</v>
+      </c>
+      <c r="E30" s="107" t="s">
+        <v>442</v>
+      </c>
+      <c r="F30" s="107" t="s">
+        <v>456</v>
+      </c>
+      <c r="G30" s="119">
+        <v>255255255240</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>4</v>
+      </c>
+      <c r="C31" s="109" t="s">
+        <v>411</v>
+      </c>
+      <c r="D31" s="109" t="s">
+        <v>426</v>
+      </c>
+      <c r="E31" s="107" t="s">
+        <v>443</v>
+      </c>
+      <c r="F31" s="107" t="s">
+        <v>457</v>
+      </c>
+      <c r="G31" s="119">
+        <v>255255255240</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>5</v>
+      </c>
+      <c r="C32" s="109" t="s">
+        <v>412</v>
+      </c>
+      <c r="D32" s="109" t="s">
+        <v>427</v>
+      </c>
+      <c r="E32" s="107" t="s">
+        <v>444</v>
+      </c>
+      <c r="F32" s="107" t="s">
+        <v>458</v>
+      </c>
+      <c r="G32" s="119">
+        <v>255255255240</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>6</v>
+      </c>
+      <c r="C33" s="109" t="s">
+        <v>413</v>
+      </c>
+      <c r="D33" s="109" t="s">
+        <v>428</v>
+      </c>
+      <c r="E33" s="107" t="s">
+        <v>445</v>
+      </c>
+      <c r="F33" s="107" t="s">
+        <v>459</v>
+      </c>
+      <c r="G33" s="119">
+        <v>255255255240</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>7</v>
+      </c>
+      <c r="C34" s="109" t="s">
+        <v>414</v>
+      </c>
+      <c r="D34" s="109" t="s">
+        <v>429</v>
+      </c>
+      <c r="E34" s="107" t="s">
+        <v>446</v>
+      </c>
+      <c r="F34" s="107" t="s">
+        <v>460</v>
+      </c>
+      <c r="G34" s="119">
+        <v>255255255240</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>8</v>
+      </c>
+      <c r="C35" s="109" t="s">
+        <v>415</v>
+      </c>
+      <c r="D35" s="109" t="s">
+        <v>430</v>
+      </c>
+      <c r="E35" s="107" t="s">
+        <v>447</v>
+      </c>
+      <c r="F35" s="107" t="s">
+        <v>461</v>
+      </c>
+      <c r="G35" s="119">
+        <v>255255255240</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>9</v>
+      </c>
+      <c r="C36" s="109" t="s">
+        <v>416</v>
+      </c>
+      <c r="D36" s="109" t="s">
+        <v>431</v>
+      </c>
+      <c r="E36" s="107" t="s">
+        <v>448</v>
+      </c>
+      <c r="F36" s="107" t="s">
+        <v>462</v>
+      </c>
+      <c r="G36" s="119">
+        <v>255255255240</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>10</v>
+      </c>
+      <c r="C37" s="109" t="s">
+        <v>417</v>
+      </c>
+      <c r="D37" s="109" t="s">
+        <v>432</v>
+      </c>
+      <c r="E37" s="107" t="s">
+        <v>449</v>
+      </c>
+      <c r="F37" s="107" t="s">
+        <v>438</v>
+      </c>
+      <c r="G37" s="119">
+        <v>255255255240</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>11</v>
+      </c>
+      <c r="C38" s="109" t="s">
+        <v>418</v>
+      </c>
+      <c r="D38" s="109" t="s">
+        <v>433</v>
+      </c>
+      <c r="E38" s="107" t="s">
+        <v>450</v>
+      </c>
+      <c r="F38" s="107" t="s">
+        <v>463</v>
+      </c>
+      <c r="G38" s="119">
+        <v>255255255240</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>12</v>
+      </c>
+      <c r="C39" s="109" t="s">
+        <v>419</v>
+      </c>
+      <c r="D39" s="109" t="s">
+        <v>434</v>
+      </c>
+      <c r="E39" s="107" t="s">
+        <v>451</v>
+      </c>
+      <c r="F39" s="107" t="s">
+        <v>464</v>
+      </c>
+      <c r="G39" s="119">
+        <v>255255255240</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>13</v>
+      </c>
+      <c r="C40" s="109" t="s">
+        <v>420</v>
+      </c>
+      <c r="D40" s="109" t="s">
+        <v>435</v>
+      </c>
+      <c r="E40" s="107" t="s">
+        <v>452</v>
+      </c>
+      <c r="F40" s="107" t="s">
+        <v>465</v>
+      </c>
+      <c r="G40" s="119">
+        <v>255255255240</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>14</v>
+      </c>
+      <c r="C41" s="109" t="s">
+        <v>421</v>
+      </c>
+      <c r="D41" s="109" t="s">
+        <v>436</v>
+      </c>
+      <c r="E41" s="107" t="s">
+        <v>453</v>
+      </c>
+      <c r="F41" s="107" t="s">
+        <v>466</v>
+      </c>
+      <c r="G41" s="119">
+        <v>255255255240</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>15</v>
+      </c>
+      <c r="C42" s="109" t="s">
+        <v>422</v>
+      </c>
+      <c r="D42" s="109" t="s">
+        <v>437</v>
+      </c>
+      <c r="E42" s="107" t="s">
+        <v>454</v>
+      </c>
+      <c r="F42" s="107" t="s">
+        <v>467</v>
+      </c>
+      <c r="G42" s="119">
+        <v>255255255240</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>266</v>
+      </c>
+      <c r="B47">
+        <v>6</v>
+      </c>
+      <c r="C47">
+        <v>8</v>
+      </c>
+      <c r="D47">
+        <v>3</v>
+      </c>
+      <c r="E47">
+        <v>32</v>
+      </c>
+      <c r="F47">
+        <v>19</v>
+      </c>
+      <c r="G47">
+        <v>13</v>
+      </c>
+      <c r="H47">
+        <f>2^13-2</f>
+        <v>8190</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>346</v>
+      </c>
+      <c r="B49" t="s">
+        <v>223</v>
+      </c>
+      <c r="C49" t="s">
+        <v>340</v>
+      </c>
+      <c r="D49" t="s">
+        <v>341</v>
+      </c>
+      <c r="E49" t="s">
+        <v>342</v>
+      </c>
+      <c r="F49" t="s">
+        <v>343</v>
+      </c>
+      <c r="G49" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>0</v>
+      </c>
+      <c r="B50" s="109"/>
+      <c r="C50" s="109" t="s">
+        <v>266</v>
+      </c>
+      <c r="D50" s="109" t="s">
+        <v>472</v>
+      </c>
+      <c r="E50" s="107" t="s">
+        <v>476</v>
+      </c>
+      <c r="F50" s="107" t="s">
+        <v>473</v>
+      </c>
+      <c r="G50" s="119" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>1</v>
+      </c>
+      <c r="B51" s="109"/>
+      <c r="C51" s="109" t="s">
+        <v>474</v>
+      </c>
+      <c r="D51" s="109"/>
+      <c r="E51" s="107"/>
+      <c r="F51" s="107"/>
+      <c r="G51" s="119"/>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>2</v>
+      </c>
+      <c r="B52" s="109"/>
+      <c r="C52" s="109"/>
+      <c r="D52" s="109"/>
+      <c r="E52" s="107"/>
+      <c r="F52" s="107"/>
+      <c r="G52" s="119"/>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>3</v>
+      </c>
+      <c r="B53" s="109"/>
+      <c r="C53" s="109"/>
+      <c r="D53" s="109"/>
+      <c r="E53" s="107"/>
+      <c r="F53" s="107"/>
+      <c r="G53" s="119"/>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>4</v>
+      </c>
+      <c r="C54" s="109"/>
+      <c r="D54" s="109"/>
+      <c r="E54" s="107"/>
+      <c r="F54" s="107"/>
+      <c r="G54" s="119"/>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>5</v>
+      </c>
+      <c r="C55" s="109"/>
+      <c r="D55" s="109"/>
+      <c r="E55" s="107"/>
+      <c r="F55" s="107"/>
+      <c r="G55" s="119"/>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>6</v>
+      </c>
+      <c r="C56" s="109"/>
+      <c r="D56" s="109"/>
+      <c r="E56" s="107"/>
+      <c r="F56" s="107"/>
+      <c r="G56" s="119"/>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>7</v>
+      </c>
+      <c r="C57" s="109"/>
+      <c r="D57" s="109"/>
+      <c r="E57" s="107"/>
+      <c r="F57" s="107"/>
+      <c r="G57" s="119"/>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C58" s="109"/>
+      <c r="D58" s="109"/>
+      <c r="E58" s="107"/>
+      <c r="F58" s="107"/>
+      <c r="G58" s="119"/>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C59" s="109"/>
+      <c r="D59" s="109"/>
+      <c r="E59" s="107"/>
+      <c r="F59" s="107"/>
+      <c r="G59" s="119"/>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C60" s="109"/>
+      <c r="D60" s="109"/>
+      <c r="E60" s="107"/>
+      <c r="F60" s="107"/>
+      <c r="G60" s="119"/>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C61" s="109"/>
+      <c r="D61" s="109"/>
+      <c r="E61" s="107"/>
+      <c r="F61" s="107"/>
+      <c r="G61" s="119"/>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C62" s="109"/>
+      <c r="D62" s="109"/>
+      <c r="E62" s="107"/>
+      <c r="F62" s="107"/>
+      <c r="G62" s="119"/>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C63" s="109"/>
+      <c r="D63" s="109"/>
+      <c r="E63" s="107"/>
+      <c r="F63" s="107"/>
+      <c r="G63" s="119"/>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C64" s="109"/>
+      <c r="D64" s="109"/>
+      <c r="E64" s="107"/>
+      <c r="F64" s="107"/>
+      <c r="G64" s="119"/>
+    </row>
+    <row r="65" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C65" s="109"/>
+      <c r="D65" s="109"/>
+      <c r="E65" s="107"/>
+      <c r="F65" s="107"/>
+      <c r="G65" s="119"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:H1"/>
+  </mergeCells>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C11A5F22-AD4E-415C-B377-AE140E43FC65}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
configuracion topologia con IPV6
</commit_message>
<xml_diff>
--- a/docs/protocol-suite.xlsx
+++ b/docs/protocol-suite.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EducacionIT\Documents\networks\CISCO\saves\ccna-lx08\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B752FD5-7C94-4DC8-A578-6EC9CD14E7FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23A81CD2-52E5-43E4-9EF5-157A61E62772}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="8" xr2:uid="{5C0FE7F9-9F0A-47A7-8741-1649DE5ACCD4}"/>
+    <workbookView xWindow="30" yWindow="30" windowWidth="20460" windowHeight="10770" activeTab="8" xr2:uid="{5C0FE7F9-9F0A-47A7-8741-1649DE5ACCD4}"/>
   </bookViews>
   <sheets>
     <sheet name="models" sheetId="1" r:id="rId1"/>
@@ -22,6 +22,7 @@
     <sheet name="VLSM" sheetId="7" r:id="rId7"/>
     <sheet name="Routing" sheetId="8" r:id="rId8"/>
     <sheet name="IPv6" sheetId="9" r:id="rId9"/>
+    <sheet name="Hoja1" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1062" uniqueCount="655">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1138" uniqueCount="705">
   <si>
     <t>OSI de ISO</t>
   </si>
@@ -3253,16 +3254,280 @@
     <t>grupos 0</t>
   </si>
   <si>
-    <t>2</t>
-  </si>
-  <si>
     <t>::</t>
   </si>
   <si>
     <t>resultado</t>
   </si>
   <si>
-    <t>2001:DB6:ACAD:1::2</t>
+    <t>Direccion</t>
+  </si>
+  <si>
+    <t>Fin</t>
+  </si>
+  <si>
+    <t>Ini</t>
+  </si>
+  <si>
+    <t>Equiv.</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Global</t>
+  </si>
+  <si>
+    <t>Unique</t>
+  </si>
+  <si>
+    <t>Link-Local</t>
+  </si>
+  <si>
+    <t>2000::</t>
+  </si>
+  <si>
+    <t>3FFF::</t>
+  </si>
+  <si>
+    <t>IPv4 Publico</t>
+  </si>
+  <si>
+    <t>FC00::</t>
+  </si>
+  <si>
+    <t>FDFF::</t>
+  </si>
+  <si>
+    <t>IPv4 Privado</t>
+  </si>
+  <si>
+    <t>FE80::</t>
+  </si>
+  <si>
+    <t>FEBF::</t>
+  </si>
+  <si>
+    <t>IPv4 APIPA</t>
+  </si>
+  <si>
+    <t>FF00::</t>
+  </si>
+  <si>
+    <t>FFFF::</t>
+  </si>
+  <si>
+    <t>EUI-64</t>
+  </si>
+  <si>
+    <t>MAC</t>
+  </si>
+  <si>
+    <t>A64E</t>
+  </si>
+  <si>
+    <t>B5</t>
+  </si>
+  <si>
+    <t>16 Bits</t>
+  </si>
+  <si>
+    <t>!7bit</t>
+  </si>
+  <si>
+    <t>8130</t>
+  </si>
+  <si>
+    <t>00-01-c7-8d-14-b1</t>
+  </si>
+  <si>
+    <t>14B1</t>
+  </si>
+  <si>
+    <t>C7</t>
+  </si>
+  <si>
+    <t>8D</t>
+  </si>
+  <si>
+    <t>81</t>
+  </si>
+  <si>
+    <t>4E</t>
+  </si>
+  <si>
+    <t>FF</t>
+  </si>
+  <si>
+    <t>FE</t>
+  </si>
+  <si>
+    <t>A6</t>
+  </si>
+  <si>
+    <t>31</t>
+  </si>
+  <si>
+    <t>Extended Unique ID</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>B1</t>
+  </si>
+  <si>
+    <t>01</t>
+  </si>
+  <si>
+    <t>00</t>
+  </si>
+  <si>
+    <r>
+      <t>0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF800000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>A</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>4</t>
+    </r>
+  </si>
+  <si>
+    <t>.31</t>
+  </si>
+  <si>
+    <t>B5.</t>
+  </si>
+  <si>
+    <t>8D.</t>
+  </si>
+  <si>
+    <t>.C7</t>
+  </si>
+  <si>
+    <r>
+      <t>FE80::A</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF800000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>4</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>4E:31</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF800000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>FF:FE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>B5:8130</t>
+    </r>
+  </si>
+  <si>
+    <t>IPv6</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>FE80::</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF800000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>01:C7</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF800000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>FF:FE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>8D:14B1</t>
+    </r>
+  </si>
+  <si>
+    <t>IPv4 Clase D</t>
+  </si>
+  <si>
+    <t>2001:DB6:ACAD:1::1</t>
   </si>
 </sst>
 </file>
@@ -3273,7 +3538,7 @@
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3357,8 +3622,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="24">
+  <fills count="25">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3483,6 +3755,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3872,7 +4150,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="173">
+  <cellXfs count="211">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
@@ -4287,22 +4565,34 @@
     <xf numFmtId="0" fontId="0" fillId="21" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -4317,18 +4607,18 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="18" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -4353,27 +4643,105 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="18" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="19" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="10" fillId="19" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="19" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="19" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="19" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="10" fillId="19" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="19" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="19" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="19" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="18" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="4" fillId="18" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="7" fillId="19" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="7" fillId="19" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="19" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="7" fillId="19" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="19" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="8" fillId="19" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="7" fillId="19" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="19" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="19" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="18" borderId="20" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="19" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="19" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="19" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="19" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Millares" xfId="1" builtinId="3"/>
@@ -5636,13 +6004,13 @@
       <c r="A2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="151" t="s">
+      <c r="B2" s="155" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="152" t="s">
+      <c r="C2" s="156" t="s">
         <v>24</v>
       </c>
-      <c r="D2" s="151" t="s">
+      <c r="D2" s="155" t="s">
         <v>8</v>
       </c>
     </row>
@@ -5650,17 +6018,17 @@
       <c r="A3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="151"/>
-      <c r="C3" s="152"/>
-      <c r="D3" s="151"/>
+      <c r="B3" s="155"/>
+      <c r="C3" s="156"/>
+      <c r="D3" s="155"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="151"/>
-      <c r="C4" s="152"/>
-      <c r="D4" s="151"/>
+      <c r="B4" s="155"/>
+      <c r="C4" s="156"/>
+      <c r="D4" s="155"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
@@ -5700,7 +6068,7 @@
       <c r="C7" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="D7" s="150" t="s">
+      <c r="D7" s="154" t="s">
         <v>9</v>
       </c>
     </row>
@@ -5714,7 +6082,7 @@
       <c r="C8" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="D8" s="150"/>
+      <c r="D8" s="154"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
@@ -5734,6 +6102,20 @@
     <mergeCell ref="C2:C4"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE92A873-F0AF-4CAF-9520-2399455F7343}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H20" sqref="H20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -5771,16 +6153,16 @@
       </c>
     </row>
     <row r="3" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="153" t="s">
+      <c r="A3" s="157" t="s">
         <v>29</v>
       </c>
-      <c r="B3" s="153"/>
-      <c r="C3" s="153"/>
-      <c r="E3" s="153" t="s">
+      <c r="B3" s="157"/>
+      <c r="C3" s="157"/>
+      <c r="E3" s="157" t="s">
         <v>30</v>
       </c>
-      <c r="F3" s="153"/>
-      <c r="G3" s="153"/>
+      <c r="F3" s="157"/>
+      <c r="G3" s="157"/>
     </row>
     <row r="4" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
@@ -5953,11 +6335,11 @@
       <c r="C11" t="s">
         <v>45</v>
       </c>
-      <c r="E11" s="153" t="s">
+      <c r="E11" s="157" t="s">
         <v>81</v>
       </c>
-      <c r="F11" s="153"/>
-      <c r="G11" s="153"/>
+      <c r="F11" s="157"/>
+      <c r="G11" s="157"/>
     </row>
     <row r="12" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
@@ -6603,16 +6985,16 @@
       <c r="K5" s="45" t="s">
         <v>163</v>
       </c>
-      <c r="L5" s="158" t="s">
+      <c r="L5" s="162" t="s">
         <v>223</v>
       </c>
-      <c r="M5" s="159"/>
-      <c r="N5" s="159"/>
-      <c r="O5" s="159"/>
-      <c r="P5" s="159"/>
-      <c r="Q5" s="159"/>
-      <c r="R5" s="159"/>
-      <c r="S5" s="160"/>
+      <c r="M5" s="163"/>
+      <c r="N5" s="163"/>
+      <c r="O5" s="163"/>
+      <c r="P5" s="163"/>
+      <c r="Q5" s="163"/>
+      <c r="R5" s="163"/>
+      <c r="S5" s="164"/>
       <c r="T5" s="46" t="s">
         <v>162</v>
       </c>
@@ -6636,10 +7018,10 @@
       <c r="F6" s="33">
         <v>16</v>
       </c>
-      <c r="H6" s="154" t="s">
+      <c r="H6" s="161" t="s">
         <v>231</v>
       </c>
-      <c r="I6" s="154"/>
+      <c r="I6" s="161"/>
       <c r="K6" s="47">
         <v>192</v>
       </c>
@@ -6741,25 +7123,25 @@
       <c r="AE7" s="28" t="s">
         <v>163</v>
       </c>
-      <c r="AF7" s="161">
+      <c r="AF7" s="165">
         <f>SUM(AF10:AU10)</f>
         <v>5620</v>
       </c>
-      <c r="AG7" s="161"/>
-      <c r="AH7" s="161"/>
-      <c r="AI7" s="161"/>
-      <c r="AJ7" s="161"/>
-      <c r="AK7" s="161"/>
-      <c r="AL7" s="161"/>
-      <c r="AM7" s="161"/>
-      <c r="AN7" s="161"/>
-      <c r="AO7" s="161"/>
-      <c r="AP7" s="161"/>
-      <c r="AQ7" s="161"/>
-      <c r="AR7" s="161"/>
-      <c r="AS7" s="161"/>
-      <c r="AT7" s="161"/>
-      <c r="AU7" s="161"/>
+      <c r="AG7" s="165"/>
+      <c r="AH7" s="165"/>
+      <c r="AI7" s="165"/>
+      <c r="AJ7" s="165"/>
+      <c r="AK7" s="165"/>
+      <c r="AL7" s="165"/>
+      <c r="AM7" s="165"/>
+      <c r="AN7" s="165"/>
+      <c r="AO7" s="165"/>
+      <c r="AP7" s="165"/>
+      <c r="AQ7" s="165"/>
+      <c r="AR7" s="165"/>
+      <c r="AS7" s="165"/>
+      <c r="AT7" s="165"/>
+      <c r="AU7" s="165"/>
     </row>
     <row r="8" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A8" s="28">
@@ -7022,30 +7404,30 @@
       <c r="AE10" s="28" t="s">
         <v>163</v>
       </c>
-      <c r="AF10" s="155">
+      <c r="AF10" s="158">
         <v>4096</v>
       </c>
-      <c r="AG10" s="156"/>
-      <c r="AH10" s="156"/>
-      <c r="AI10" s="157"/>
-      <c r="AJ10" s="155">
+      <c r="AG10" s="159"/>
+      <c r="AH10" s="159"/>
+      <c r="AI10" s="160"/>
+      <c r="AJ10" s="158">
         <v>1280</v>
       </c>
-      <c r="AK10" s="156"/>
-      <c r="AL10" s="156"/>
-      <c r="AM10" s="157"/>
-      <c r="AN10" s="155">
+      <c r="AK10" s="159"/>
+      <c r="AL10" s="159"/>
+      <c r="AM10" s="160"/>
+      <c r="AN10" s="158">
         <v>240</v>
       </c>
-      <c r="AO10" s="156"/>
-      <c r="AP10" s="156"/>
-      <c r="AQ10" s="157"/>
-      <c r="AR10" s="155">
+      <c r="AO10" s="159"/>
+      <c r="AP10" s="159"/>
+      <c r="AQ10" s="160"/>
+      <c r="AR10" s="158">
         <v>4</v>
       </c>
-      <c r="AS10" s="156"/>
-      <c r="AT10" s="156"/>
-      <c r="AU10" s="157"/>
+      <c r="AS10" s="159"/>
+      <c r="AT10" s="159"/>
+      <c r="AU10" s="160"/>
     </row>
     <row r="11" spans="1:47" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="28">
@@ -7063,10 +7445,10 @@
       <c r="F11" s="30">
         <v>16</v>
       </c>
-      <c r="H11" s="154" t="s">
+      <c r="H11" s="161" t="s">
         <v>231</v>
       </c>
-      <c r="I11" s="154"/>
+      <c r="I11" s="161"/>
       <c r="K11" s="51">
         <v>48</v>
       </c>
@@ -7116,30 +7498,30 @@
       <c r="AE11" s="28" t="s">
         <v>162</v>
       </c>
-      <c r="AF11" s="155">
+      <c r="AF11" s="158">
         <v>1</v>
       </c>
-      <c r="AG11" s="156"/>
-      <c r="AH11" s="156"/>
-      <c r="AI11" s="157"/>
-      <c r="AJ11" s="155">
+      <c r="AG11" s="159"/>
+      <c r="AH11" s="159"/>
+      <c r="AI11" s="160"/>
+      <c r="AJ11" s="158">
         <v>5</v>
       </c>
-      <c r="AK11" s="156"/>
-      <c r="AL11" s="156"/>
-      <c r="AM11" s="157"/>
-      <c r="AN11" s="155" t="s">
+      <c r="AK11" s="159"/>
+      <c r="AL11" s="159"/>
+      <c r="AM11" s="160"/>
+      <c r="AN11" s="158" t="s">
         <v>238</v>
       </c>
-      <c r="AO11" s="156"/>
-      <c r="AP11" s="156"/>
-      <c r="AQ11" s="157"/>
-      <c r="AR11" s="155">
+      <c r="AO11" s="159"/>
+      <c r="AP11" s="159"/>
+      <c r="AQ11" s="160"/>
+      <c r="AR11" s="158">
         <v>4</v>
       </c>
-      <c r="AS11" s="156"/>
-      <c r="AT11" s="156"/>
-      <c r="AU11" s="157"/>
+      <c r="AS11" s="159"/>
+      <c r="AT11" s="159"/>
+      <c r="AU11" s="160"/>
     </row>
     <row r="12" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A12" s="28">
@@ -7392,10 +7774,10 @@
       <c r="F16" s="30">
         <v>16</v>
       </c>
-      <c r="H16" s="154" t="s">
+      <c r="H16" s="161" t="s">
         <v>231</v>
       </c>
-      <c r="I16" s="154"/>
+      <c r="I16" s="161"/>
       <c r="K16" s="57">
         <v>10</v>
       </c>
@@ -7531,10 +7913,10 @@
       <c r="F20" s="30">
         <v>16</v>
       </c>
-      <c r="H20" s="154" t="s">
+      <c r="H20" s="161" t="s">
         <v>231</v>
       </c>
-      <c r="I20" s="154"/>
+      <c r="I20" s="161"/>
       <c r="X20" s="32"/>
       <c r="Y20" s="36"/>
     </row>
@@ -7571,6 +7953,11 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="H16:I16"/>
+    <mergeCell ref="H20:I20"/>
+    <mergeCell ref="H11:I11"/>
+    <mergeCell ref="AF10:AI10"/>
+    <mergeCell ref="AF11:AI11"/>
     <mergeCell ref="AJ11:AM11"/>
     <mergeCell ref="AN11:AQ11"/>
     <mergeCell ref="AR11:AU11"/>
@@ -7580,11 +7967,6 @@
     <mergeCell ref="AN10:AQ10"/>
     <mergeCell ref="AR10:AU10"/>
     <mergeCell ref="AF7:AU7"/>
-    <mergeCell ref="H16:I16"/>
-    <mergeCell ref="H20:I20"/>
-    <mergeCell ref="H11:I11"/>
-    <mergeCell ref="AF10:AI10"/>
-    <mergeCell ref="AF11:AI11"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7598,10 +7980,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8CBB112-D597-4FBD-BD71-E33EC2CA62E0}">
   <dimension ref="A1:N26"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection activeCell="A13" sqref="A13"/>
-      <selection pane="topRight" activeCell="L26" sqref="L26"/>
+      <selection pane="topRight" activeCell="B8" sqref="B8:E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7625,24 +8007,24 @@
       <c r="A1" s="28" t="s">
         <v>239</v>
       </c>
-      <c r="B1" s="154" t="s">
+      <c r="B1" s="161" t="s">
         <v>243</v>
       </c>
-      <c r="C1" s="154"/>
-      <c r="D1" s="154"/>
-      <c r="E1" s="154"/>
-      <c r="F1" s="154" t="s">
+      <c r="C1" s="161"/>
+      <c r="D1" s="161"/>
+      <c r="E1" s="161"/>
+      <c r="F1" s="161" t="s">
         <v>244</v>
       </c>
-      <c r="G1" s="154"/>
-      <c r="H1" s="154"/>
-      <c r="I1" s="154"/>
-      <c r="J1" s="154" t="s">
+      <c r="G1" s="161"/>
+      <c r="H1" s="161"/>
+      <c r="I1" s="161"/>
+      <c r="J1" s="161" t="s">
         <v>275</v>
       </c>
-      <c r="K1" s="154"/>
-      <c r="L1" s="154"/>
-      <c r="M1" s="154"/>
+      <c r="K1" s="161"/>
+      <c r="L1" s="161"/>
+      <c r="M1" s="161"/>
     </row>
     <row r="2" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="45" t="s">
@@ -7870,13 +8252,13 @@
       <c r="A8" s="28" t="s">
         <v>249</v>
       </c>
-      <c r="B8" s="162">
+      <c r="B8" s="166">
         <f>2^32</f>
         <v>4294967296</v>
       </c>
-      <c r="C8" s="162"/>
-      <c r="D8" s="162"/>
-      <c r="E8" s="162"/>
+      <c r="C8" s="166"/>
+      <c r="D8" s="166"/>
+      <c r="E8" s="166"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="28" t="s">
@@ -8428,8 +8810,8 @@
   <dimension ref="A1:V58"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E3" sqref="E3"/>
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8449,15 +8831,15 @@
       <c r="A1" s="107" t="s">
         <v>326</v>
       </c>
-      <c r="B1" s="163" t="s">
+      <c r="B1" s="167" t="s">
         <v>500</v>
       </c>
-      <c r="C1" s="163"/>
-      <c r="D1" s="163"/>
-      <c r="E1" s="163"/>
-      <c r="F1" s="163"/>
-      <c r="G1" s="163"/>
-      <c r="H1" s="163"/>
+      <c r="C1" s="167"/>
+      <c r="D1" s="167"/>
+      <c r="E1" s="167"/>
+      <c r="F1" s="167"/>
+      <c r="G1" s="167"/>
+      <c r="H1" s="167"/>
       <c r="O1">
         <v>1</v>
       </c>
@@ -9930,15 +10312,15 @@
       <c r="A1" s="94" t="s">
         <v>518</v>
       </c>
-      <c r="B1" s="164" t="s">
+      <c r="B1" s="168" t="s">
         <v>525</v>
       </c>
-      <c r="C1" s="164"/>
-      <c r="D1" s="164"/>
-      <c r="E1" s="164"/>
-      <c r="F1" s="164"/>
-      <c r="G1" s="164"/>
-      <c r="H1" s="164"/>
+      <c r="C1" s="168"/>
+      <c r="D1" s="168"/>
+      <c r="E1" s="168"/>
+      <c r="F1" s="168"/>
+      <c r="G1" s="168"/>
+      <c r="H1" s="168"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -10779,7 +11161,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{168581C0-15D8-4648-ABAA-ECEC60EE4C1A}">
   <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
@@ -10794,7 +11176,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="145" t="s">
+      <c r="A1" s="144" t="s">
         <v>590</v>
       </c>
       <c r="B1" s="103" t="s">
@@ -10820,184 +11202,184 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="146" t="s">
+      <c r="A2" s="145" t="s">
         <v>591</v>
       </c>
-      <c r="B2" s="147" t="s">
+      <c r="B2" s="146" t="s">
         <v>265</v>
       </c>
-      <c r="C2" s="148" t="s">
+      <c r="C2" s="147" t="s">
         <v>596</v>
       </c>
-      <c r="D2" s="148" t="s">
+      <c r="D2" s="147" t="s">
         <v>597</v>
       </c>
-      <c r="E2" s="148" t="s">
+      <c r="E2" s="147" t="s">
         <v>604</v>
       </c>
-      <c r="F2" s="148" t="s">
+      <c r="F2" s="147" t="s">
         <v>598</v>
       </c>
-      <c r="G2" s="147" t="s">
+      <c r="G2" s="146" t="s">
         <v>598</v>
       </c>
-      <c r="H2" s="147" t="s">
+      <c r="H2" s="146" t="s">
         <v>591</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="146" t="s">
+      <c r="A3" s="145" t="s">
         <v>592</v>
       </c>
-      <c r="B3" s="147" t="s">
+      <c r="B3" s="146" t="s">
         <v>265</v>
       </c>
-      <c r="C3" s="148" t="s">
+      <c r="C3" s="147" t="s">
         <v>265</v>
       </c>
-      <c r="D3" s="148" t="s">
+      <c r="D3" s="147" t="s">
         <v>603</v>
       </c>
-      <c r="E3" s="148" t="s">
+      <c r="E3" s="147" t="s">
         <v>605</v>
       </c>
-      <c r="F3" s="148" t="s">
+      <c r="F3" s="147" t="s">
         <v>599</v>
       </c>
-      <c r="G3" s="147" t="s">
+      <c r="G3" s="146" t="s">
         <v>599</v>
       </c>
-      <c r="H3" s="147" t="s">
+      <c r="H3" s="146" t="s">
         <v>610</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="146" t="s">
+      <c r="A4" s="145" t="s">
         <v>589</v>
       </c>
-      <c r="B4" s="147" t="s">
+      <c r="B4" s="146" t="s">
         <v>265</v>
       </c>
-      <c r="C4" s="148" t="s">
+      <c r="C4" s="147" t="s">
         <v>265</v>
       </c>
-      <c r="D4" s="148" t="s">
+      <c r="D4" s="147" t="s">
         <v>265</v>
       </c>
-      <c r="E4" s="148" t="s">
+      <c r="E4" s="147" t="s">
         <v>606</v>
       </c>
-      <c r="F4" s="148" t="s">
+      <c r="F4" s="147" t="s">
         <v>600</v>
       </c>
-      <c r="G4" s="147" t="s">
+      <c r="G4" s="146" t="s">
         <v>607</v>
       </c>
-      <c r="H4" s="147" t="s">
+      <c r="H4" s="146" t="s">
         <v>589</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="146" t="s">
+      <c r="A5" s="145" t="s">
         <v>593</v>
       </c>
-      <c r="B5" s="147" t="s">
+      <c r="B5" s="146" t="s">
         <v>265</v>
       </c>
-      <c r="C5" s="148" t="s">
+      <c r="C5" s="147" t="s">
         <v>265</v>
       </c>
-      <c r="D5" s="148" t="s">
+      <c r="D5" s="147" t="s">
         <v>265</v>
       </c>
-      <c r="E5" s="148" t="s">
+      <c r="E5" s="147" t="s">
         <v>265</v>
       </c>
-      <c r="F5" s="148" t="s">
+      <c r="F5" s="147" t="s">
         <v>601</v>
       </c>
-      <c r="G5" s="147" t="s">
+      <c r="G5" s="146" t="s">
         <v>608</v>
       </c>
-      <c r="H5" s="147" t="s">
+      <c r="H5" s="146" t="s">
         <v>611</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="146" t="s">
+      <c r="A6" s="145" t="s">
         <v>595</v>
       </c>
-      <c r="B6" s="147" t="s">
+      <c r="B6" s="146" t="s">
         <v>265</v>
       </c>
-      <c r="C6" s="147" t="s">
+      <c r="C6" s="146" t="s">
         <v>265</v>
       </c>
-      <c r="D6" s="147" t="s">
+      <c r="D6" s="146" t="s">
         <v>265</v>
       </c>
-      <c r="E6" s="147" t="s">
+      <c r="E6" s="146" t="s">
         <v>265</v>
       </c>
-      <c r="F6" s="147" t="s">
+      <c r="F6" s="146" t="s">
         <v>265</v>
       </c>
-      <c r="G6" s="147" t="s">
+      <c r="G6" s="146" t="s">
         <v>609</v>
       </c>
-      <c r="H6" s="147" t="s">
+      <c r="H6" s="146" t="s">
         <v>612</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="146" t="s">
+      <c r="A7" s="145" t="s">
         <v>594</v>
       </c>
-      <c r="B7" s="147" t="s">
+      <c r="B7" s="146" t="s">
         <v>265</v>
       </c>
-      <c r="C7" s="147" t="s">
+      <c r="C7" s="146" t="s">
         <v>265</v>
       </c>
-      <c r="D7" s="147" t="s">
+      <c r="D7" s="146" t="s">
         <v>265</v>
       </c>
-      <c r="E7" s="147" t="s">
+      <c r="E7" s="146" t="s">
         <v>265</v>
       </c>
-      <c r="F7" s="147" t="s">
+      <c r="F7" s="146" t="s">
         <v>265</v>
       </c>
-      <c r="G7" s="147" t="s">
+      <c r="G7" s="146" t="s">
         <v>265</v>
       </c>
-      <c r="H7" s="147" t="s">
+      <c r="H7" s="146" t="s">
         <v>602</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="146" t="s">
+      <c r="A8" s="145" t="s">
         <v>343</v>
       </c>
-      <c r="B8" s="147" t="s">
+      <c r="B8" s="146" t="s">
         <v>265</v>
       </c>
-      <c r="C8" s="147" t="s">
+      <c r="C8" s="146" t="s">
         <v>265</v>
       </c>
-      <c r="D8" s="147" t="s">
+      <c r="D8" s="146" t="s">
         <v>265</v>
       </c>
-      <c r="E8" s="147" t="s">
+      <c r="E8" s="146" t="s">
         <v>265</v>
       </c>
-      <c r="F8" s="147" t="s">
+      <c r="F8" s="146" t="s">
         <v>265</v>
       </c>
-      <c r="G8" s="147" t="s">
+      <c r="G8" s="146" t="s">
         <v>265</v>
       </c>
-      <c r="H8" s="147" t="s">
+      <c r="H8" s="146" t="s">
         <v>265</v>
       </c>
     </row>
@@ -11005,31 +11387,31 @@
       <c r="A9" s="103" t="s">
         <v>336</v>
       </c>
-      <c r="B9" s="149">
+      <c r="B9" s="148">
         <f t="shared" ref="B9:H9" si="0">2^(32-B1)-2</f>
         <v>16777214</v>
       </c>
-      <c r="C9" s="149">
+      <c r="C9" s="148">
         <f t="shared" si="0"/>
         <v>4194302</v>
       </c>
-      <c r="D9" s="149">
+      <c r="D9" s="148">
         <f t="shared" si="0"/>
         <v>65534</v>
       </c>
-      <c r="E9" s="149">
+      <c r="E9" s="148">
         <f t="shared" si="0"/>
         <v>4094</v>
       </c>
-      <c r="F9" s="149">
+      <c r="F9" s="148">
         <f t="shared" si="0"/>
         <v>254</v>
       </c>
-      <c r="G9" s="149">
+      <c r="G9" s="148">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="H9" s="149">
+      <c r="H9" s="148">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
@@ -11038,12 +11420,12 @@
       <c r="A11" s="90" t="s">
         <v>622</v>
       </c>
-      <c r="B11" s="165" t="s">
+      <c r="B11" s="169" t="s">
         <v>628</v>
       </c>
-      <c r="C11" s="165"/>
-      <c r="D11" s="165"/>
-      <c r="E11" s="165"/>
+      <c r="C11" s="169"/>
+      <c r="D11" s="169"/>
+      <c r="E11" s="169"/>
       <c r="F11" s="61" t="s">
         <v>629</v>
       </c>
@@ -11054,12 +11436,12 @@
       <c r="A12" s="90" t="s">
         <v>621</v>
       </c>
-      <c r="B12" s="165" t="s">
+      <c r="B12" s="169" t="s">
         <v>620</v>
       </c>
-      <c r="C12" s="165"/>
-      <c r="D12" s="165"/>
-      <c r="E12" s="165"/>
+      <c r="C12" s="169"/>
+      <c r="D12" s="169"/>
+      <c r="E12" s="169"/>
       <c r="F12" s="61" t="s">
         <v>626</v>
       </c>
@@ -11070,12 +11452,12 @@
       <c r="A13" s="90" t="s">
         <v>623</v>
       </c>
-      <c r="B13" s="165" t="s">
+      <c r="B13" s="169" t="s">
         <v>627</v>
       </c>
-      <c r="C13" s="165"/>
-      <c r="D13" s="165"/>
-      <c r="E13" s="165"/>
+      <c r="C13" s="169"/>
+      <c r="D13" s="169"/>
+      <c r="E13" s="169"/>
       <c r="F13" s="90" t="s">
         <v>630</v>
       </c>
@@ -11084,12 +11466,12 @@
       <c r="A14" s="90" t="s">
         <v>624</v>
       </c>
-      <c r="B14" s="165" t="s">
+      <c r="B14" s="169" t="s">
         <v>625</v>
       </c>
-      <c r="C14" s="165"/>
-      <c r="D14" s="165"/>
-      <c r="E14" s="165"/>
+      <c r="C14" s="169"/>
+      <c r="D14" s="169"/>
+      <c r="E14" s="169"/>
       <c r="F14" s="90" t="s">
         <v>631</v>
       </c>
@@ -11111,163 +11493,502 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DDFA7A63-B76F-41E1-9D58-B82CFEA5C5F4}">
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:Z11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="R6" sqref="R6:Z6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="8" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.7109375" style="97" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="3.28515625" style="97" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="3" style="97" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="3.140625" style="97" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="3" style="97" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="3.28515625" style="97" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="3" style="97" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="3.140625" style="97" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="2.7109375" customWidth="1"/>
+    <col min="11" max="11" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6.28515625" style="149" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="6.42578125" style="149" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="4.28515625" style="149" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.85546875" style="150" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="2.5703125" customWidth="1"/>
+    <col min="17" max="17" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="6" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="21" max="24" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="6.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="171" t="s">
+        <v>672</v>
+      </c>
+      <c r="B1" s="185" t="s">
+        <v>689</v>
+      </c>
+      <c r="C1" s="185"/>
+      <c r="D1" s="185"/>
+      <c r="E1" s="185"/>
+      <c r="F1" s="185"/>
+      <c r="G1" s="185"/>
+      <c r="H1" s="185"/>
+      <c r="I1" s="185"/>
+      <c r="K1" s="171" t="s">
+        <v>653</v>
+      </c>
+      <c r="L1" s="185" t="s">
+        <v>655</v>
+      </c>
+      <c r="M1" s="185" t="s">
+        <v>654</v>
+      </c>
+      <c r="N1" s="65" t="s">
+        <v>21</v>
+      </c>
+      <c r="O1" s="186" t="s">
+        <v>656</v>
+      </c>
+      <c r="Q1" s="171" t="s">
         <v>649</v>
       </c>
-      <c r="B1" s="167" t="s">
+      <c r="R1" s="185" t="s">
         <v>633</v>
       </c>
-      <c r="C1" s="167"/>
-      <c r="D1" s="167"/>
-      <c r="E1" s="169" t="s">
+      <c r="S1" s="185"/>
+      <c r="T1" s="185"/>
+      <c r="U1" s="65" t="s">
         <v>641</v>
       </c>
-      <c r="F1" s="171" t="s">
+      <c r="V1" s="185" t="s">
         <v>640</v>
       </c>
-      <c r="G1" s="171"/>
-      <c r="H1" s="171"/>
-      <c r="I1" s="171"/>
-      <c r="J1" s="144" t="s">
+      <c r="W1" s="185"/>
+      <c r="X1" s="185"/>
+      <c r="Y1" s="185"/>
+      <c r="Z1" s="45" t="s">
         <v>642</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A2" s="187" t="s">
+        <v>673</v>
+      </c>
+      <c r="B2" s="188" t="s">
+        <v>674</v>
+      </c>
+      <c r="C2" s="188"/>
+      <c r="D2" s="196" t="s">
+        <v>696</v>
+      </c>
+      <c r="E2" s="196"/>
+      <c r="F2" s="195" t="s">
+        <v>697</v>
+      </c>
+      <c r="G2" s="195"/>
+      <c r="H2" s="188" t="s">
+        <v>678</v>
+      </c>
+      <c r="I2" s="188"/>
+      <c r="K2" s="172" t="s">
+        <v>658</v>
+      </c>
+      <c r="L2" s="173" t="s">
+        <v>661</v>
+      </c>
+      <c r="M2" s="173" t="s">
+        <v>662</v>
+      </c>
+      <c r="N2" s="203">
+        <v>3</v>
+      </c>
+      <c r="O2" s="200" t="s">
+        <v>663</v>
+      </c>
+      <c r="Q2" s="172" t="s">
         <v>632</v>
       </c>
-      <c r="B2" s="168" t="s">
+      <c r="R2" s="173" t="s">
         <v>634</v>
       </c>
-      <c r="C2" s="168" t="s">
+      <c r="S2" s="173" t="s">
         <v>636</v>
       </c>
-      <c r="D2" s="168" t="s">
+      <c r="T2" s="173" t="s">
         <v>635</v>
       </c>
-      <c r="E2" s="170" t="s">
+      <c r="U2" s="174" t="s">
         <v>637</v>
       </c>
-      <c r="F2" s="172" t="s">
+      <c r="V2" s="175" t="s">
         <v>638</v>
       </c>
-      <c r="G2" s="172" t="s">
+      <c r="W2" s="175" t="s">
         <v>638</v>
       </c>
-      <c r="H2" s="172" t="s">
+      <c r="X2" s="175" t="s">
         <v>638</v>
       </c>
-      <c r="I2" s="172" t="s">
+      <c r="Y2" s="175" t="s">
         <v>639</v>
       </c>
-      <c r="J2" s="29" t="s">
+      <c r="Z2" s="68" t="s">
         <v>643</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A3" s="189" t="s">
+        <v>676</v>
+      </c>
+      <c r="B3" s="190" t="s">
+        <v>687</v>
+      </c>
+      <c r="C3" s="190" t="s">
+        <v>684</v>
+      </c>
+      <c r="D3" s="190" t="s">
+        <v>688</v>
+      </c>
+      <c r="E3" s="152" t="s">
+        <v>685</v>
+      </c>
+      <c r="F3" s="152" t="s">
+        <v>686</v>
+      </c>
+      <c r="G3" s="190" t="s">
+        <v>675</v>
+      </c>
+      <c r="H3" s="190" t="s">
+        <v>683</v>
+      </c>
+      <c r="I3" s="190" t="s">
+        <v>619</v>
+      </c>
+      <c r="K3" s="176" t="s">
+        <v>659</v>
+      </c>
+      <c r="L3" s="151" t="s">
+        <v>664</v>
+      </c>
+      <c r="M3" s="151" t="s">
+        <v>665</v>
+      </c>
+      <c r="N3" s="204">
+        <v>7</v>
+      </c>
+      <c r="O3" s="170" t="s">
+        <v>666</v>
+      </c>
+      <c r="Q3" s="176" t="s">
         <v>644</v>
       </c>
-      <c r="B3" s="168" t="s">
+      <c r="R3" s="151" t="s">
         <v>634</v>
       </c>
-      <c r="C3" s="168" t="s">
+      <c r="S3" s="151" t="s">
         <v>648</v>
       </c>
-      <c r="D3" s="168" t="s">
+      <c r="T3" s="151" t="s">
         <v>635</v>
       </c>
-      <c r="E3" s="170" t="s">
+      <c r="U3" s="152" t="s">
         <v>645</v>
       </c>
-      <c r="F3" s="172" t="s">
+      <c r="V3" s="153" t="s">
         <v>646</v>
       </c>
-      <c r="G3" s="172" t="s">
+      <c r="W3" s="153" t="s">
         <v>646</v>
       </c>
-      <c r="H3" s="172" t="s">
+      <c r="X3" s="153" t="s">
         <v>646</v>
       </c>
-      <c r="I3" s="172" t="s">
+      <c r="Y3" s="153" t="s">
         <v>647</v>
       </c>
-      <c r="J3" s="172" t="s">
+      <c r="Z3" s="153" t="s">
         <v>643</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A4" s="191" t="s">
+        <v>677</v>
+      </c>
+      <c r="B4" s="192" t="s">
+        <v>695</v>
+      </c>
+      <c r="C4" s="192" t="s">
+        <v>684</v>
+      </c>
+      <c r="D4" s="192" t="s">
+        <v>688</v>
+      </c>
+      <c r="E4" s="179" t="s">
+        <v>685</v>
+      </c>
+      <c r="F4" s="194" t="s">
+        <v>686</v>
+      </c>
+      <c r="G4" s="193" t="s">
+        <v>675</v>
+      </c>
+      <c r="H4" s="193" t="s">
+        <v>683</v>
+      </c>
+      <c r="I4" s="192" t="s">
+        <v>619</v>
+      </c>
+      <c r="K4" s="177" t="s">
+        <v>660</v>
+      </c>
+      <c r="L4" s="178" t="s">
+        <v>667</v>
+      </c>
+      <c r="M4" s="178" t="s">
+        <v>668</v>
+      </c>
+      <c r="N4" s="205">
+        <v>10</v>
+      </c>
+      <c r="O4" s="201" t="s">
+        <v>669</v>
+      </c>
+      <c r="Q4" s="177" t="s">
         <v>650</v>
       </c>
-      <c r="B4" s="168" t="s">
+      <c r="R4" s="178" t="s">
         <v>634</v>
       </c>
-      <c r="C4" s="168" t="s">
+      <c r="S4" s="178" t="s">
         <v>648</v>
       </c>
-      <c r="D4" s="168" t="s">
+      <c r="T4" s="178" t="s">
         <v>635</v>
       </c>
-      <c r="E4" s="170" t="s">
+      <c r="U4" s="179" t="s">
         <v>645</v>
       </c>
-      <c r="F4" s="166" t="s">
+      <c r="V4" s="184" t="s">
+        <v>651</v>
+      </c>
+      <c r="W4" s="184"/>
+      <c r="X4" s="184"/>
+      <c r="Y4" s="180" t="s">
+        <v>647</v>
+      </c>
+      <c r="Z4" s="78" t="s">
+        <v>643</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="181" t="s">
+        <v>701</v>
+      </c>
+      <c r="B5" s="183" t="s">
+        <v>700</v>
+      </c>
+      <c r="C5" s="183"/>
+      <c r="D5" s="183"/>
+      <c r="E5" s="183"/>
+      <c r="F5" s="183"/>
+      <c r="G5" s="183"/>
+      <c r="H5" s="183"/>
+      <c r="I5" s="183"/>
+      <c r="K5" s="181" t="s">
+        <v>269</v>
+      </c>
+      <c r="L5" s="199" t="s">
+        <v>670</v>
+      </c>
+      <c r="M5" s="199" t="s">
+        <v>671</v>
+      </c>
+      <c r="N5" s="206">
+        <v>8</v>
+      </c>
+      <c r="O5" s="202" t="s">
+        <v>703</v>
+      </c>
+      <c r="Q5" s="181" t="s">
         <v>652</v>
       </c>
-      <c r="G4" s="166"/>
-      <c r="H4" s="166"/>
-      <c r="I4" s="172" t="s">
-        <v>651</v>
-      </c>
-      <c r="J4" s="29" t="s">
+      <c r="R5" s="183" t="s">
+        <v>704</v>
+      </c>
+      <c r="S5" s="183"/>
+      <c r="T5" s="183"/>
+      <c r="U5" s="183"/>
+      <c r="V5" s="183"/>
+      <c r="W5" s="183"/>
+      <c r="X5" s="183"/>
+      <c r="Y5" s="183"/>
+      <c r="Z5" s="182" t="s">
         <v>643</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>653</v>
-      </c>
-      <c r="B5" s="166" t="s">
-        <v>654</v>
-      </c>
-      <c r="C5" s="166"/>
-      <c r="D5" s="166"/>
-      <c r="E5" s="166"/>
-      <c r="F5" s="166"/>
-      <c r="G5" s="166"/>
-      <c r="H5" s="166"/>
-      <c r="I5" s="166"/>
-      <c r="J5" s="172" t="s">
-        <v>643</v>
-      </c>
+    <row r="6" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K6" s="207"/>
+      <c r="L6" s="208"/>
+      <c r="M6" s="209"/>
+      <c r="N6" s="209"/>
+      <c r="O6" s="209"/>
+      <c r="P6" s="209"/>
+      <c r="Q6" s="210" t="s">
+        <v>657</v>
+      </c>
+      <c r="R6" s="198">
+        <f>2^128</f>
+        <v>3.4028236692093846E+38</v>
+      </c>
+      <c r="S6" s="198"/>
+      <c r="T6" s="198"/>
+      <c r="U6" s="198"/>
+      <c r="V6" s="198"/>
+      <c r="W6" s="198"/>
+      <c r="X6" s="198"/>
+      <c r="Y6" s="198"/>
+      <c r="Z6" s="198"/>
+    </row>
+    <row r="7" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="171" t="s">
+        <v>672</v>
+      </c>
+      <c r="B7" s="185" t="s">
+        <v>679</v>
+      </c>
+      <c r="C7" s="185"/>
+      <c r="D7" s="185"/>
+      <c r="E7" s="185"/>
+      <c r="F7" s="185"/>
+      <c r="G7" s="185"/>
+      <c r="H7" s="185"/>
+      <c r="I7" s="185"/>
+    </row>
+    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A8" s="187" t="s">
+        <v>673</v>
+      </c>
+      <c r="B8" s="188" t="s">
+        <v>639</v>
+      </c>
+      <c r="C8" s="188"/>
+      <c r="D8" s="197" t="s">
+        <v>699</v>
+      </c>
+      <c r="E8" s="196"/>
+      <c r="F8" s="195" t="s">
+        <v>698</v>
+      </c>
+      <c r="G8" s="195"/>
+      <c r="H8" s="188" t="s">
+        <v>680</v>
+      </c>
+      <c r="I8" s="188"/>
+    </row>
+    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A9" s="189" t="s">
+        <v>676</v>
+      </c>
+      <c r="B9" s="190" t="s">
+        <v>693</v>
+      </c>
+      <c r="C9" s="190" t="s">
+        <v>692</v>
+      </c>
+      <c r="D9" s="190" t="s">
+        <v>681</v>
+      </c>
+      <c r="E9" s="152" t="s">
+        <v>685</v>
+      </c>
+      <c r="F9" s="152" t="s">
+        <v>686</v>
+      </c>
+      <c r="G9" s="190" t="s">
+        <v>682</v>
+      </c>
+      <c r="H9" s="190" t="s">
+        <v>690</v>
+      </c>
+      <c r="I9" s="190" t="s">
+        <v>691</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A10" s="191" t="s">
+        <v>677</v>
+      </c>
+      <c r="B10" s="192" t="s">
+        <v>694</v>
+      </c>
+      <c r="C10" s="192" t="s">
+        <v>692</v>
+      </c>
+      <c r="D10" s="192" t="s">
+        <v>681</v>
+      </c>
+      <c r="E10" s="179" t="s">
+        <v>685</v>
+      </c>
+      <c r="F10" s="194" t="s">
+        <v>686</v>
+      </c>
+      <c r="G10" s="193" t="s">
+        <v>682</v>
+      </c>
+      <c r="H10" s="193" t="s">
+        <v>690</v>
+      </c>
+      <c r="I10" s="192" t="s">
+        <v>691</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="181" t="s">
+        <v>701</v>
+      </c>
+      <c r="B11" s="183" t="s">
+        <v>702</v>
+      </c>
+      <c r="C11" s="183"/>
+      <c r="D11" s="183"/>
+      <c r="E11" s="183"/>
+      <c r="F11" s="183"/>
+      <c r="G11" s="183"/>
+      <c r="H11" s="183"/>
+      <c r="I11" s="183"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="F1:I1"/>
-    <mergeCell ref="F4:H4"/>
+  <mergeCells count="18">
+    <mergeCell ref="R6:Z6"/>
     <mergeCell ref="B5:I5"/>
+    <mergeCell ref="B11:I11"/>
+    <mergeCell ref="B7:I7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="B1:I1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="R1:T1"/>
+    <mergeCell ref="V1:Y1"/>
+    <mergeCell ref="V4:X4"/>
+    <mergeCell ref="R5:Y5"/>
+    <mergeCell ref="L1:M1"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="D3:D4 B8:C8 B9:C10 H9:H10" numberStoredAsText="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
comunicacion entre segmentos de red
</commit_message>
<xml_diff>
--- a/docs/protocol-suite.xlsx
+++ b/docs/protocol-suite.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EducacionIT\Documents\networks\CISCO\saves\ccna-lj20\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1648CE65-D9BB-4239-837D-F484C59411EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04BE2073-7D0A-4BEC-8682-3FEFD39946CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{078AB514-2E24-4AE3-970C-AD73C7910696}"/>
+    <workbookView xWindow="30" yWindow="30" windowWidth="20460" windowHeight="10770" activeTab="2" xr2:uid="{078AB514-2E24-4AE3-970C-AD73C7910696}"/>
   </bookViews>
   <sheets>
     <sheet name="suite" sheetId="1" r:id="rId1"/>
     <sheet name="unidades" sheetId="2" r:id="rId2"/>
+    <sheet name="fisica" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="96">
   <si>
     <t>OSI de ISO</t>
   </si>
@@ -118,9 +119,6 @@
     <t>100baseT - 100baseTX</t>
   </si>
   <si>
-    <t>binary digit</t>
-  </si>
-  <si>
     <t>Almacenamiento</t>
   </si>
   <si>
@@ -211,113 +209,128 @@
     <t>1000KB</t>
   </si>
   <si>
+    <t>1000MB</t>
+  </si>
+  <si>
+    <t>1000GB</t>
+  </si>
+  <si>
+    <t>1000TB</t>
+  </si>
+  <si>
+    <t>1000PB</t>
+  </si>
+  <si>
+    <t>1000XB</t>
+  </si>
+  <si>
+    <t>1000ZB</t>
+  </si>
+  <si>
+    <t>1000YB</t>
+  </si>
+  <si>
+    <t>1000BB</t>
+  </si>
+  <si>
+    <t>1000GeB</t>
+  </si>
+  <si>
+    <t>Potencia</t>
+  </si>
+  <si>
+    <t>Ancho de Banda</t>
+  </si>
+  <si>
+    <t>1000bps</t>
+  </si>
+  <si>
+    <t>bits/sec</t>
+  </si>
+  <si>
+    <t>Kilobits /sec</t>
+  </si>
+  <si>
+    <t>Megabits/sec</t>
+  </si>
+  <si>
+    <t>1000Kbps</t>
+  </si>
+  <si>
+    <t>Gigabits/sec</t>
+  </si>
+  <si>
+    <t>Terabits/sec</t>
+  </si>
+  <si>
+    <t>1000Gbps</t>
+  </si>
+  <si>
+    <t>1000Mbps</t>
+  </si>
+  <si>
+    <t>binary digits</t>
+  </si>
+  <si>
+    <t>Frecuencia</t>
+  </si>
+  <si>
+    <t>Hertz</t>
+  </si>
+  <si>
+    <t>KiloHertz</t>
+  </si>
+  <si>
+    <t>MegaHertz</t>
+  </si>
+  <si>
+    <t>GigaHertz</t>
+  </si>
+  <si>
+    <t>TeraHertz</t>
+  </si>
+  <si>
+    <t>1000Hz</t>
+  </si>
+  <si>
+    <t>1000KHz</t>
+  </si>
+  <si>
+    <t>1000MHz</t>
+  </si>
+  <si>
+    <t>1000GHz</t>
+  </si>
+  <si>
+    <t>1 ciclo/segundo</t>
+  </si>
+  <si>
+    <t>Binary Digit</t>
+  </si>
+  <si>
+    <t>bit</t>
+  </si>
+  <si>
+    <t>Minimo</t>
+  </si>
+  <si>
     <t>b</t>
   </si>
   <si>
-    <t>1000MB</t>
-  </si>
-  <si>
-    <t>1000GB</t>
-  </si>
-  <si>
-    <t>1000TB</t>
-  </si>
-  <si>
-    <t>1000PB</t>
-  </si>
-  <si>
-    <t>1000XB</t>
-  </si>
-  <si>
-    <t>1000ZB</t>
-  </si>
-  <si>
-    <t>1000YB</t>
-  </si>
-  <si>
-    <t>1000BB</t>
-  </si>
-  <si>
-    <t>1000GeB</t>
-  </si>
-  <si>
-    <t>Potencia</t>
-  </si>
-  <si>
-    <t>Ancho de Banda</t>
-  </si>
-  <si>
-    <t>1000bps</t>
-  </si>
-  <si>
-    <t>bits/sec</t>
-  </si>
-  <si>
-    <t>Kilobits /sec</t>
-  </si>
-  <si>
-    <t>Megabits/sec</t>
-  </si>
-  <si>
-    <t>1000Kbps</t>
-  </si>
-  <si>
-    <t>Gigabits/sec</t>
-  </si>
-  <si>
-    <t>Terabits/sec</t>
-  </si>
-  <si>
-    <t>1000Gbps</t>
-  </si>
-  <si>
-    <t>1000Mbps</t>
-  </si>
-  <si>
-    <t>binary digits</t>
-  </si>
-  <si>
-    <t>Frecuencia</t>
-  </si>
-  <si>
-    <t>Hertz</t>
-  </si>
-  <si>
-    <t>KiloHertz</t>
-  </si>
-  <si>
-    <t>MegaHertz</t>
-  </si>
-  <si>
-    <t>GigaHertz</t>
-  </si>
-  <si>
-    <t>TeraHertz</t>
-  </si>
-  <si>
-    <t>1000Hz</t>
-  </si>
-  <si>
-    <t>1000KHz</t>
-  </si>
-  <si>
-    <t>1000MHz</t>
-  </si>
-  <si>
-    <t>1000GHz</t>
-  </si>
-  <si>
-    <t>1 ciclo/segundo</t>
-  </si>
-  <si>
-    <t>minima u.</t>
+    <t>Representacion de dos posibles valores</t>
+  </si>
+  <si>
+    <t>TIA-568A</t>
+  </si>
+  <si>
+    <t>TIA-568B</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -338,8 +351,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -381,8 +402,20 @@
         <bgColor rgb="FFA50021"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor theme="0" tint="-0.14999847407452621"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -390,11 +423,22 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -448,6 +492,12 @@
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -945,305 +995,314 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A707C052-38DB-4245-83BC-3FDD2D63A656}">
   <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection sqref="A1:C1"/>
+    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1:G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" customWidth="1"/>
-    <col min="3" max="3" width="9.28515625" customWidth="1"/>
-    <col min="4" max="4" width="3" customWidth="1"/>
+    <col min="2" max="2" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="2.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.5703125" customWidth="1"/>
+    <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="19" t="s">
         <v>91</v>
       </c>
-      <c r="B1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C1" t="s">
-        <v>58</v>
-      </c>
+      <c r="B1" s="20" t="s">
+        <v>89</v>
+      </c>
+      <c r="C1" s="21" t="s">
+        <v>90</v>
+      </c>
+      <c r="D1" s="20" t="s">
+        <v>92</v>
+      </c>
+      <c r="E1" s="22" t="s">
+        <v>93</v>
+      </c>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B2" s="18"/>
       <c r="C2" s="18"/>
       <c r="E2" s="18" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F2" s="18"/>
       <c r="G2" s="18"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" t="s">
         <v>29</v>
       </c>
-      <c r="B3" t="s">
-        <v>30</v>
-      </c>
       <c r="C3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F3" t="s">
         <v>29</v>
       </c>
-      <c r="F3" t="s">
-        <v>30</v>
-      </c>
       <c r="G3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" t="s">
         <v>31</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>32</v>
       </c>
-      <c r="C4" t="s">
-        <v>33</v>
-      </c>
       <c r="E4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="F4" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="G4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E5" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F5" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="G5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E6" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F6" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="G6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B7" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E7" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F7" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="G7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B8" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E8" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F8" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="G8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B9" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E9" s="18" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="F9" s="18"/>
       <c r="G9" s="18"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B10" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E10" t="s">
+        <v>28</v>
+      </c>
+      <c r="F10" t="s">
         <v>29</v>
       </c>
-      <c r="F10" t="s">
-        <v>30</v>
-      </c>
       <c r="G10" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B11" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E11" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="F11" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="G11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B12" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E12" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="F12" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="G12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B13" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E13" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="F13" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="G13" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B14" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C14" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E14" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="F14" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="G14" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B15" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C15" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E15" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="F15" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="G15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="E2:G2"/>
     <mergeCell ref="E9:G9"/>
+    <mergeCell ref="E1:G1"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1253,4 +1312,33 @@
     <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3142012-29F0-4708-9A27-7709474E8C46}">
+  <dimension ref="B1:D1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="4.85546875" customWidth="1"/>
+    <col min="2" max="2" width="23" customWidth="1"/>
+    <col min="4" max="4" width="22.85546875" customWidth="1"/>
+    <col min="5" max="5" width="7.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
funcionamiento y protocolos capa fisica
</commit_message>
<xml_diff>
--- a/docs/protocol-suite.xlsx
+++ b/docs/protocol-suite.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EducacionIT\Documents\networks\CISCO\saves\ccna-lj20\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04BE2073-7D0A-4BEC-8682-3FEFD39946CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18177619-7524-45F1-8F41-6B0CBD280E6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="30" yWindow="30" windowWidth="20460" windowHeight="10770" activeTab="2" xr2:uid="{078AB514-2E24-4AE3-970C-AD73C7910696}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="180">
   <si>
     <t>OSI de ISO</t>
   </si>
@@ -324,6 +324,258 @@
   </si>
   <si>
     <t>TIA-568B</t>
+  </si>
+  <si>
+    <t>B.verde</t>
+  </si>
+  <si>
+    <t>Verde</t>
+  </si>
+  <si>
+    <t>B.Naranja</t>
+  </si>
+  <si>
+    <t>Azul</t>
+  </si>
+  <si>
+    <t>B.Azul</t>
+  </si>
+  <si>
+    <t>Naranja</t>
+  </si>
+  <si>
+    <t>B.Marron</t>
+  </si>
+  <si>
+    <t>Marron</t>
+  </si>
+  <si>
+    <t>Tx</t>
+  </si>
+  <si>
+    <t>Rx</t>
+  </si>
+  <si>
+    <t>Simplex</t>
+  </si>
+  <si>
+    <t>Half Duplex</t>
+  </si>
+  <si>
+    <t>Full Duplex</t>
+  </si>
+  <si>
+    <t>Full Full Duplex</t>
+  </si>
+  <si>
+    <t>Un host envia el otro solo recibe</t>
+  </si>
+  <si>
+    <t>Un host envia o recibe datos</t>
+  </si>
+  <si>
+    <t>Un host envia y recibe datos</t>
+  </si>
+  <si>
+    <t>Varios hosts envian y reciben</t>
+  </si>
+  <si>
+    <t>Tipo</t>
+  </si>
+  <si>
+    <t>Descripcion de la comunicación</t>
+  </si>
+  <si>
+    <t>Caracteristica</t>
+  </si>
+  <si>
+    <t>SMF</t>
+  </si>
+  <si>
+    <t>MMF</t>
+  </si>
+  <si>
+    <t>Monomodo</t>
+  </si>
+  <si>
+    <t>Multimodo</t>
+  </si>
+  <si>
+    <t>Luz</t>
+  </si>
+  <si>
+    <t>Laser</t>
+  </si>
+  <si>
+    <t>LED</t>
+  </si>
+  <si>
+    <t>Nucleo</t>
+  </si>
+  <si>
+    <t>9 micrones</t>
+  </si>
+  <si>
+    <t>60 micrones</t>
+  </si>
+  <si>
+    <t>Distancia</t>
+  </si>
+  <si>
+    <t>Capacidad</t>
+  </si>
+  <si>
+    <t>200km</t>
+  </si>
+  <si>
+    <t>2km</t>
+  </si>
+  <si>
+    <t>100gbps</t>
+  </si>
+  <si>
+    <t>10gbps</t>
+  </si>
+  <si>
+    <t>Ventaja</t>
+  </si>
+  <si>
+    <t>Desventaja</t>
+  </si>
+  <si>
+    <t>Economica</t>
+  </si>
+  <si>
+    <t>Electronica</t>
+  </si>
+  <si>
+    <t>Descripcion</t>
+  </si>
+  <si>
+    <t>Carrier</t>
+  </si>
+  <si>
+    <t>AM</t>
+  </si>
+  <si>
+    <t>FM</t>
+  </si>
+  <si>
+    <t>PM</t>
+  </si>
+  <si>
+    <t>Señalizacion</t>
+  </si>
+  <si>
+    <t>Señal portadora</t>
+  </si>
+  <si>
+    <t>Amplitud Modulada</t>
+  </si>
+  <si>
+    <t>Frecuencia Modulada</t>
+  </si>
+  <si>
+    <t>Fase Modulada</t>
+  </si>
+  <si>
+    <t>Problematicas</t>
+  </si>
+  <si>
+    <t>EMI</t>
+  </si>
+  <si>
+    <t>RFI</t>
+  </si>
+  <si>
+    <t>Crosstalk</t>
+  </si>
+  <si>
+    <t>Colision</t>
+  </si>
+  <si>
+    <t>Choque no intencional de datos</t>
+  </si>
+  <si>
+    <t>Interferencia Electromagnetica</t>
+  </si>
+  <si>
+    <t>Interferencia por Radiofrecuencia</t>
+  </si>
+  <si>
+    <t>Diafonia (Cruce de Señales)</t>
+  </si>
+  <si>
+    <t>Conectores</t>
+  </si>
+  <si>
+    <t>FC</t>
+  </si>
+  <si>
+    <t>ST</t>
+  </si>
+  <si>
+    <t>LC</t>
+  </si>
+  <si>
+    <t>SC</t>
+  </si>
+  <si>
+    <t>Ferrule Connector</t>
+  </si>
+  <si>
+    <t>Straight Tip</t>
+  </si>
+  <si>
+    <t>Lucent Connector</t>
+  </si>
+  <si>
+    <t>Suscriber Connector</t>
+  </si>
+  <si>
+    <t>Terminaciones</t>
+  </si>
+  <si>
+    <t>PC</t>
+  </si>
+  <si>
+    <t>UPC</t>
+  </si>
+  <si>
+    <t>APC</t>
+  </si>
+  <si>
+    <t>Physical Connector</t>
+  </si>
+  <si>
+    <t>Ultra Physical Connector</t>
+  </si>
+  <si>
+    <t>Angled Physical Connector</t>
+  </si>
+  <si>
+    <t>Empresarial</t>
+  </si>
+  <si>
+    <t>Hogareño</t>
+  </si>
+  <si>
+    <t>Uso</t>
+  </si>
+  <si>
+    <t>Onda Sinusoidal</t>
+  </si>
+  <si>
+    <t>Alteracion Eje Y</t>
+  </si>
+  <si>
+    <t>Alteracion Eje X</t>
+  </si>
+  <si>
+    <t>Combinacion de Ondas</t>
+  </si>
+  <si>
+    <t>Detalle</t>
   </si>
 </sst>
 </file>
@@ -360,7 +612,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="32">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -414,8 +666,121 @@
         <bgColor theme="0" tint="-0.14999847407452621"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="lightUp">
+        <bgColor theme="8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightUp">
+        <bgColor theme="4" tint="-0.249977111117893"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightUp">
+        <bgColor theme="9" tint="-0.249977111117893"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightUp">
+        <bgColor theme="5" tint="-0.249977111117893"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightUp">
+        <bgColor theme="0" tint="-0.34998626667073579"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightUp">
+        <bgColor theme="7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightUp">
+        <bgColor theme="4" tint="-0.499984740745262"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightUp">
+        <bgColor theme="5" tint="0.39997558519241921"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightUp">
+        <bgColor theme="9" tint="0.39997558519241921"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightUp">
+        <bgColor theme="4" tint="0.39997558519241921"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightUp">
+        <bgColor theme="9" tint="-0.499984740745262"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightUp">
+        <bgColor theme="7" tint="-0.249977111117893"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightUp">
+        <bgColor theme="5" tint="-0.499984740745262"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightUp">
+        <fgColor auto="1"/>
+        <bgColor theme="5" tint="0.39997558519241921"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightUp">
+        <fgColor auto="1"/>
+        <bgColor theme="5" tint="-0.249977111117893"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightUp">
+        <fgColor auto="1"/>
+        <bgColor theme="9" tint="0.39997558519241921"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightUp">
+        <fgColor auto="1"/>
+        <bgColor theme="4" tint="-0.499984740745262"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightUp">
+        <fgColor auto="1"/>
+        <bgColor theme="4" tint="0.39997558519241921"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightUp">
+        <fgColor auto="1"/>
+        <bgColor theme="9" tint="-0.499984740745262"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightUp">
+        <fgColor auto="1"/>
+        <bgColor theme="7" tint="-0.249977111117893"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightUp">
+        <fgColor auto="1"/>
+        <bgColor theme="5" tint="-0.499984740745262"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -434,11 +799,31 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color theme="1"/>
+      </top>
+      <bottom style="medium">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -482,24 +867,71 @@
     <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -889,13 +1321,13 @@
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="16" t="s">
+      <c r="C2" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="D2" s="15" t="s">
+      <c r="D2" s="20" t="s">
         <v>14</v>
       </c>
     </row>
@@ -903,17 +1335,17 @@
       <c r="A3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="15"/>
-      <c r="C3" s="16"/>
-      <c r="D3" s="15"/>
+      <c r="B3" s="20"/>
+      <c r="C3" s="21"/>
+      <c r="D3" s="20"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="15"/>
-      <c r="C4" s="16"/>
-      <c r="D4" s="15"/>
+      <c r="B4" s="20"/>
+      <c r="C4" s="21"/>
+      <c r="D4" s="20"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
@@ -953,7 +1385,7 @@
       <c r="C7" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="D7" s="17" t="s">
+      <c r="D7" s="22" t="s">
         <v>11</v>
       </c>
     </row>
@@ -967,7 +1399,7 @@
       <c r="C8" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="D8" s="17"/>
+      <c r="D8" s="22"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
@@ -996,7 +1428,7 @@
   <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:G1"/>
+      <selection activeCell="A3" sqref="A3:C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1011,35 +1443,35 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="16" t="s">
         <v>91</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="17" t="s">
         <v>89</v>
       </c>
-      <c r="C1" s="21" t="s">
+      <c r="C1" s="18" t="s">
         <v>90</v>
       </c>
-      <c r="D1" s="20" t="s">
+      <c r="D1" s="17" t="s">
         <v>92</v>
       </c>
-      <c r="E1" s="22" t="s">
+      <c r="E1" s="24" t="s">
         <v>93</v>
       </c>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="18"/>
-      <c r="C2" s="18"/>
-      <c r="E2" s="18" t="s">
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
+      <c r="E2" s="23" t="s">
         <v>67</v>
       </c>
-      <c r="F2" s="18"/>
-      <c r="G2" s="18"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -1171,11 +1603,11 @@
       <c r="C9" t="s">
         <v>48</v>
       </c>
-      <c r="E9" s="18" t="s">
+      <c r="E9" s="23" t="s">
         <v>78</v>
       </c>
-      <c r="F9" s="18"/>
-      <c r="G9" s="18"/>
+      <c r="F9" s="23"/>
+      <c r="G9" s="23"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -1316,29 +1748,373 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3142012-29F0-4708-9A27-7709474E8C46}">
-  <dimension ref="B1:D1"/>
+  <dimension ref="A1:J15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.85546875" customWidth="1"/>
-    <col min="2" max="2" width="23" customWidth="1"/>
-    <col min="4" max="4" width="22.85546875" customWidth="1"/>
-    <col min="5" max="5" width="7.140625" customWidth="1"/>
+    <col min="1" max="1" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="14.7109375" customWidth="1"/>
+    <col min="4" max="4" width="4.5703125" customWidth="1"/>
+    <col min="5" max="5" width="16.28515625" customWidth="1"/>
+    <col min="6" max="7" width="20.7109375" customWidth="1"/>
+    <col min="8" max="8" width="5" customWidth="1"/>
+    <col min="9" max="9" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="31.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B1" t="s">
+    <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
         <v>94</v>
       </c>
-      <c r="D1" t="s">
+      <c r="C1" t="s">
         <v>95</v>
       </c>
+      <c r="E1" s="25" t="s">
+        <v>116</v>
+      </c>
+      <c r="F1" s="25" t="s">
+        <v>117</v>
+      </c>
+      <c r="G1" s="25" t="s">
+        <v>118</v>
+      </c>
+      <c r="I1" s="28" t="s">
+        <v>156</v>
+      </c>
+      <c r="J1" s="28"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="38" t="s">
+        <v>96</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>104</v>
+      </c>
+      <c r="C2" s="44" t="s">
+        <v>98</v>
+      </c>
+      <c r="E2" s="26" t="s">
+        <v>114</v>
+      </c>
+      <c r="F2" s="26" t="s">
+        <v>119</v>
+      </c>
+      <c r="G2" s="26" t="s">
+        <v>120</v>
+      </c>
+      <c r="I2" s="29" t="s">
+        <v>157</v>
+      </c>
+      <c r="J2" s="29" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="41" t="s">
+        <v>97</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>104</v>
+      </c>
+      <c r="C3" s="45" t="s">
+        <v>101</v>
+      </c>
+      <c r="E3" s="27" t="s">
+        <v>121</v>
+      </c>
+      <c r="F3" s="27" t="s">
+        <v>122</v>
+      </c>
+      <c r="G3" s="27" t="s">
+        <v>123</v>
+      </c>
+      <c r="I3" s="30" t="s">
+        <v>158</v>
+      </c>
+      <c r="J3" s="30" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="36" t="s">
+        <v>98</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>105</v>
+      </c>
+      <c r="C4" s="46" t="s">
+        <v>96</v>
+      </c>
+      <c r="E4" s="26" t="s">
+        <v>124</v>
+      </c>
+      <c r="F4" s="26" t="s">
+        <v>125</v>
+      </c>
+      <c r="G4" s="26" t="s">
+        <v>126</v>
+      </c>
+      <c r="I4" s="31" t="s">
+        <v>159</v>
+      </c>
+      <c r="J4" s="31" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="39" t="s">
+        <v>99</v>
+      </c>
+      <c r="B5" s="15"/>
+      <c r="C5" s="47" t="s">
+        <v>99</v>
+      </c>
+      <c r="E5" s="27" t="s">
+        <v>127</v>
+      </c>
+      <c r="F5" s="27" t="s">
+        <v>129</v>
+      </c>
+      <c r="G5" s="27" t="s">
+        <v>130</v>
+      </c>
+      <c r="I5" s="32" t="s">
+        <v>160</v>
+      </c>
+      <c r="J5" s="32" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="40" t="s">
+        <v>100</v>
+      </c>
+      <c r="B6" s="15"/>
+      <c r="C6" s="48" t="s">
+        <v>100</v>
+      </c>
+      <c r="E6" s="26" t="s">
+        <v>128</v>
+      </c>
+      <c r="F6" s="26" t="s">
+        <v>132</v>
+      </c>
+      <c r="G6" s="26" t="s">
+        <v>131</v>
+      </c>
+      <c r="I6" s="28" t="s">
+        <v>165</v>
+      </c>
+      <c r="J6" s="28"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="37" t="s">
+        <v>101</v>
+      </c>
+      <c r="B7" s="15" t="s">
+        <v>105</v>
+      </c>
+      <c r="C7" s="49" t="s">
+        <v>97</v>
+      </c>
+      <c r="E7" s="27" t="s">
+        <v>133</v>
+      </c>
+      <c r="F7" s="27" t="s">
+        <v>136</v>
+      </c>
+      <c r="G7" s="27" t="s">
+        <v>135</v>
+      </c>
+      <c r="I7" s="33" t="s">
+        <v>166</v>
+      </c>
+      <c r="J7" s="33" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="42" t="s">
+        <v>102</v>
+      </c>
+      <c r="B8" s="15"/>
+      <c r="C8" s="50" t="s">
+        <v>102</v>
+      </c>
+      <c r="E8" s="26" t="s">
+        <v>134</v>
+      </c>
+      <c r="F8" s="26" t="s">
+        <v>135</v>
+      </c>
+      <c r="G8" s="26" t="s">
+        <v>136</v>
+      </c>
+      <c r="I8" s="34" t="s">
+        <v>167</v>
+      </c>
+      <c r="J8" s="34" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="43" t="s">
+        <v>103</v>
+      </c>
+      <c r="B9" s="15"/>
+      <c r="C9" s="51" t="s">
+        <v>103</v>
+      </c>
+      <c r="E9" s="27" t="s">
+        <v>174</v>
+      </c>
+      <c r="F9" s="27" t="s">
+        <v>172</v>
+      </c>
+      <c r="G9" s="27" t="s">
+        <v>173</v>
+      </c>
+      <c r="I9" s="35" t="s">
+        <v>168</v>
+      </c>
+      <c r="J9" s="35" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="11" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="25" t="s">
+        <v>114</v>
+      </c>
+      <c r="B11" s="25" t="s">
+        <v>115</v>
+      </c>
+      <c r="C11" s="25"/>
+      <c r="D11" s="19"/>
+      <c r="E11" s="25" t="s">
+        <v>142</v>
+      </c>
+      <c r="F11" s="25" t="s">
+        <v>137</v>
+      </c>
+      <c r="G11" s="25" t="s">
+        <v>179</v>
+      </c>
+      <c r="I11" s="25" t="s">
+        <v>147</v>
+      </c>
+      <c r="J11" s="25"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="26" t="s">
+        <v>106</v>
+      </c>
+      <c r="B12" s="26" t="s">
+        <v>110</v>
+      </c>
+      <c r="C12" s="26"/>
+      <c r="D12" s="19"/>
+      <c r="E12" s="26" t="s">
+        <v>138</v>
+      </c>
+      <c r="F12" s="26" t="s">
+        <v>143</v>
+      </c>
+      <c r="G12" s="26" t="s">
+        <v>175</v>
+      </c>
+      <c r="I12" s="26" t="s">
+        <v>148</v>
+      </c>
+      <c r="J12" s="26" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="27" t="s">
+        <v>107</v>
+      </c>
+      <c r="B13" s="27" t="s">
+        <v>111</v>
+      </c>
+      <c r="C13" s="27"/>
+      <c r="D13" s="19"/>
+      <c r="E13" s="27" t="s">
+        <v>139</v>
+      </c>
+      <c r="F13" s="27" t="s">
+        <v>144</v>
+      </c>
+      <c r="G13" s="27" t="s">
+        <v>176</v>
+      </c>
+      <c r="I13" s="27" t="s">
+        <v>149</v>
+      </c>
+      <c r="J13" s="27" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="26" t="s">
+        <v>108</v>
+      </c>
+      <c r="B14" s="26" t="s">
+        <v>112</v>
+      </c>
+      <c r="C14" s="26"/>
+      <c r="D14" s="19"/>
+      <c r="E14" s="26" t="s">
+        <v>140</v>
+      </c>
+      <c r="F14" s="26" t="s">
+        <v>145</v>
+      </c>
+      <c r="G14" s="26" t="s">
+        <v>177</v>
+      </c>
+      <c r="I14" s="26" t="s">
+        <v>150</v>
+      </c>
+      <c r="J14" s="26" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="27" t="s">
+        <v>109</v>
+      </c>
+      <c r="B15" s="27" t="s">
+        <v>113</v>
+      </c>
+      <c r="C15" s="27"/>
+      <c r="D15" s="19"/>
+      <c r="E15" s="27" t="s">
+        <v>141</v>
+      </c>
+      <c r="F15" s="27" t="s">
+        <v>146</v>
+      </c>
+      <c r="G15" s="27" t="s">
+        <v>178</v>
+      </c>
+      <c r="I15" s="27" t="s">
+        <v>151</v>
+      </c>
+      <c r="J15" s="27" t="s">
+        <v>152</v>
+      </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="I1:J1"/>
+    <mergeCell ref="I6:J6"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
protocolos ipv6 y ndp
</commit_message>
<xml_diff>
--- a/docs/protocol-suite.xlsx
+++ b/docs/protocol-suite.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EducacionIT\Documents\networks\CISCO\saves\ccna-lj20\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B83E1D0-233E-432D-833F-4FC83A1CBB88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE172A43-73BA-4C52-8904-D9F925C2F3D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="8" xr2:uid="{078AB514-2E24-4AE3-970C-AD73C7910696}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="953" uniqueCount="595">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1081" uniqueCount="676">
   <si>
     <t>OSI de ISO</t>
   </si>
@@ -2939,9 +2939,6 @@
     <t>DB6</t>
   </si>
   <si>
-    <t>bloques 0</t>
-  </si>
-  <si>
     <t>::</t>
   </si>
   <si>
@@ -2958,6 +2955,264 @@
   </si>
   <si>
     <t>simplif</t>
+  </si>
+  <si>
+    <t>grupos 0</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>INI</t>
+  </si>
+  <si>
+    <t>FIN</t>
+  </si>
+  <si>
+    <t>Global</t>
+  </si>
+  <si>
+    <t>3FFF</t>
+  </si>
+  <si>
+    <t>001</t>
+  </si>
+  <si>
+    <t>Funcion</t>
+  </si>
+  <si>
+    <t>IPv4 Publica</t>
+  </si>
+  <si>
+    <t>Equiv.</t>
+  </si>
+  <si>
+    <t>WAN Enrutable</t>
+  </si>
+  <si>
+    <t>Link-Local</t>
+  </si>
+  <si>
+    <t>Unique-Local</t>
+  </si>
+  <si>
+    <t>FC00</t>
+  </si>
+  <si>
+    <t>FE80</t>
+  </si>
+  <si>
+    <t>FDFF</t>
+  </si>
+  <si>
+    <t>1111.110</t>
+  </si>
+  <si>
+    <t>LAN Enrutable</t>
+  </si>
+  <si>
+    <t>IPv4 Privada</t>
+  </si>
+  <si>
+    <t>FEBF</t>
+  </si>
+  <si>
+    <t>1111.1110.10</t>
+  </si>
+  <si>
+    <t>Secuencia</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>Comunicación LAN</t>
+  </si>
+  <si>
+    <t>IPv4 APIPA</t>
+  </si>
+  <si>
+    <t>Multicast</t>
+  </si>
+  <si>
+    <t>IPv4 Multicast</t>
+  </si>
+  <si>
+    <t>FF00</t>
+  </si>
+  <si>
+    <t>FFFF</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>1111.1111</t>
+  </si>
+  <si>
+    <t>Grupos LAN</t>
+  </si>
+  <si>
+    <t>Anycast</t>
+  </si>
+  <si>
+    <t>En IPv6 los mensajes estan identificados por funcionamiento de Host</t>
+  </si>
+  <si>
+    <t>EUI-64</t>
+  </si>
+  <si>
+    <t>Extended Unique Identifier 64</t>
+  </si>
+  <si>
+    <t>MAC</t>
+  </si>
+  <si>
+    <t>00</t>
+  </si>
+  <si>
+    <t>90</t>
+  </si>
+  <si>
+    <t>2b</t>
+  </si>
+  <si>
+    <t>19</t>
+  </si>
+  <si>
+    <t>99</t>
+  </si>
+  <si>
+    <t>a4</t>
+  </si>
+  <si>
+    <t>16 bits</t>
+  </si>
+  <si>
+    <t>FE</t>
+  </si>
+  <si>
+    <t>! bit 7</t>
+  </si>
+  <si>
+    <t>02</t>
+  </si>
+  <si>
+    <t>2B</t>
+  </si>
+  <si>
+    <t>A4</t>
+  </si>
+  <si>
+    <r>
+      <t>0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFA50021"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2</t>
+    </r>
+  </si>
+  <si>
+    <t>FE80::290:2BFF:FE19:99A4/64</t>
+  </si>
+  <si>
+    <t>0090</t>
+  </si>
+  <si>
+    <t>99A4</t>
+  </si>
+  <si>
+    <t>0004.9a24.01ad</t>
+  </si>
+  <si>
+    <t>0030.f2c4.3002</t>
+  </si>
+  <si>
+    <t>000a.41ce.0d53</t>
+  </si>
+  <si>
+    <t>0090.2b19.99a4</t>
+  </si>
+  <si>
+    <t>0090.0c75.c41a</t>
+  </si>
+  <si>
+    <t>0060.3e86.8deb</t>
+  </si>
+  <si>
+    <t>mac</t>
+  </si>
+  <si>
+    <t>address</t>
+  </si>
+  <si>
+    <t>9a</t>
+  </si>
+  <si>
+    <t>01ad</t>
+  </si>
+  <si>
+    <t>0004</t>
+  </si>
+  <si>
+    <t>04</t>
+  </si>
+  <si>
+    <t>ff</t>
+  </si>
+  <si>
+    <t>fe</t>
+  </si>
+  <si>
+    <t>24</t>
+  </si>
+  <si>
+    <t>0a</t>
+  </si>
+  <si>
+    <t>01</t>
+  </si>
+  <si>
+    <t>ad</t>
+  </si>
+  <si>
+    <t>fe80::204:9aff:fe24:1ad/64</t>
+  </si>
+  <si>
+    <t>FE80::20A:41FF:FECE:D53/64</t>
+  </si>
+  <si>
+    <t>41</t>
+  </si>
+  <si>
+    <t>ce</t>
+  </si>
+  <si>
+    <t>0d</t>
+  </si>
+  <si>
+    <t>53</t>
+  </si>
+  <si>
+    <t>000A</t>
+  </si>
+  <si>
+    <t>Ce</t>
+  </si>
+  <si>
+    <t>0D53</t>
   </si>
 </sst>
 </file>
@@ -2968,7 +3223,7 @@
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3026,14 +3281,38 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="4" tint="-0.249977111117893"/>
+      <color theme="9" tint="-0.499984740745262"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="9" tint="-0.249977111117893"/>
+      <color theme="4" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="9" tint="0.59999389629810485"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="8" tint="0.79998168889431442"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="5" tint="0.79998168889431442"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -3384,7 +3663,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="176">
+  <cellXfs count="202">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3762,46 +4041,126 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="10" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="9" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="10" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="10" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="5" fillId="10" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="9" fillId="10" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="9" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="7" fillId="10" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="10" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="10" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="10" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="10" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="10" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="10" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -9572,168 +9931,686 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D32392E-F434-412B-A6BA-FD626CD67179}">
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:R24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="H21" sqref="B21:I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="10" width="5.85546875" customWidth="1"/>
+    <col min="1" max="1" width="9.28515625" style="59" bestFit="1" customWidth="1"/>
+    <col min="2" max="10" width="6" style="59" customWidth="1"/>
     <col min="11" max="11" width="2.85546875" customWidth="1"/>
+    <col min="12" max="12" width="12.5703125" style="59" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.7109375" style="59" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="13.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="168" t="s">
         <v>578</v>
       </c>
-      <c r="B1" s="162" t="s">
+      <c r="B1" s="184" t="s">
         <v>579</v>
       </c>
-      <c r="C1" s="162"/>
-      <c r="D1" s="162"/>
-      <c r="E1" s="166" t="s">
+      <c r="C1" s="184"/>
+      <c r="D1" s="184"/>
+      <c r="E1" s="182" t="s">
         <v>580</v>
       </c>
-      <c r="F1" s="170" t="s">
+      <c r="F1" s="185" t="s">
         <v>581</v>
       </c>
-      <c r="G1" s="170"/>
-      <c r="H1" s="170"/>
-      <c r="I1" s="170"/>
-      <c r="J1" s="161" t="s">
+      <c r="G1" s="185"/>
+      <c r="H1" s="185"/>
+      <c r="I1" s="185"/>
+      <c r="J1" s="168" t="s">
+        <v>590</v>
+      </c>
+      <c r="L1" s="163" t="s">
+        <v>595</v>
+      </c>
+      <c r="M1" s="188" t="s">
+        <v>596</v>
+      </c>
+      <c r="N1" s="188" t="s">
+        <v>597</v>
+      </c>
+      <c r="O1" s="188" t="s">
+        <v>21</v>
+      </c>
+      <c r="P1" s="163" t="s">
+        <v>615</v>
+      </c>
+      <c r="Q1" s="188" t="s">
+        <v>601</v>
+      </c>
+      <c r="R1" s="188" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A2" s="169" t="s">
+        <v>593</v>
+      </c>
+      <c r="B2" s="179">
+        <v>2001</v>
+      </c>
+      <c r="C2" s="179" t="s">
+        <v>582</v>
+      </c>
+      <c r="D2" s="179" t="s">
+        <v>583</v>
+      </c>
+      <c r="E2" s="176" t="s">
+        <v>584</v>
+      </c>
+      <c r="F2" s="173" t="s">
+        <v>585</v>
+      </c>
+      <c r="G2" s="173" t="s">
+        <v>585</v>
+      </c>
+      <c r="H2" s="173" t="s">
+        <v>585</v>
+      </c>
+      <c r="I2" s="173" t="s">
+        <v>584</v>
+      </c>
+      <c r="J2" s="164" t="s">
         <v>591</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="L2" s="189" t="s">
+        <v>598</v>
+      </c>
+      <c r="M2" s="190">
+        <v>2000</v>
+      </c>
+      <c r="N2" s="190" t="s">
+        <v>599</v>
+      </c>
+      <c r="O2" s="190" t="s">
+        <v>616</v>
+      </c>
+      <c r="P2" s="191" t="s">
+        <v>600</v>
+      </c>
+      <c r="Q2" s="191" t="s">
+        <v>604</v>
+      </c>
+      <c r="R2" s="191" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A3" s="170" t="s">
+        <v>586</v>
+      </c>
+      <c r="B3" s="180">
+        <v>2001</v>
+      </c>
+      <c r="C3" s="180" t="s">
+        <v>587</v>
+      </c>
+      <c r="D3" s="180" t="s">
+        <v>583</v>
+      </c>
+      <c r="E3" s="177">
+        <v>1</v>
+      </c>
+      <c r="F3" s="174">
+        <v>0</v>
+      </c>
+      <c r="G3" s="174">
+        <v>0</v>
+      </c>
+      <c r="H3" s="174">
+        <v>0</v>
+      </c>
+      <c r="I3" s="174">
+        <v>1</v>
+      </c>
+      <c r="J3" s="165" t="s">
+        <v>591</v>
+      </c>
+      <c r="L3" s="186" t="s">
+        <v>606</v>
+      </c>
+      <c r="M3" s="187" t="s">
+        <v>607</v>
+      </c>
+      <c r="N3" s="187" t="s">
+        <v>609</v>
+      </c>
+      <c r="O3" s="187" t="s">
+        <v>617</v>
+      </c>
+      <c r="P3" s="186" t="s">
+        <v>610</v>
+      </c>
+      <c r="Q3" s="186" t="s">
+        <v>611</v>
+      </c>
+      <c r="R3" s="186" t="s">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A4" s="171" t="s">
         <v>594</v>
       </c>
-      <c r="B2" s="163">
+      <c r="B4" s="181">
         <v>2001</v>
       </c>
-      <c r="C2" s="163" t="s">
-        <v>582</v>
-      </c>
-      <c r="D2" s="163" t="s">
+      <c r="C4" s="181" t="s">
+        <v>587</v>
+      </c>
+      <c r="D4" s="181" t="s">
         <v>583</v>
       </c>
-      <c r="E2" s="167" t="s">
-        <v>584</v>
-      </c>
-      <c r="F2" s="171" t="s">
-        <v>585</v>
-      </c>
-      <c r="G2" s="171" t="s">
-        <v>585</v>
-      </c>
-      <c r="H2" s="171" t="s">
-        <v>585</v>
-      </c>
-      <c r="I2" s="171" t="s">
-        <v>584</v>
-      </c>
-      <c r="J2" s="47" t="s">
+      <c r="E4" s="178">
+        <v>1</v>
+      </c>
+      <c r="F4" s="183" t="s">
+        <v>588</v>
+      </c>
+      <c r="G4" s="183"/>
+      <c r="H4" s="183"/>
+      <c r="I4" s="175">
+        <v>1</v>
+      </c>
+      <c r="J4" s="166" t="s">
+        <v>591</v>
+      </c>
+      <c r="L4" s="192" t="s">
+        <v>605</v>
+      </c>
+      <c r="M4" s="193" t="s">
+        <v>608</v>
+      </c>
+      <c r="N4" s="193" t="s">
+        <v>613</v>
+      </c>
+      <c r="O4" s="193" t="s">
+        <v>618</v>
+      </c>
+      <c r="P4" s="192" t="s">
+        <v>614</v>
+      </c>
+      <c r="Q4" s="192" t="s">
+        <v>619</v>
+      </c>
+      <c r="R4" s="192" t="s">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A5" s="170" t="s">
+        <v>589</v>
+      </c>
+      <c r="B5" s="161" t="s">
         <v>592</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>586</v>
-      </c>
-      <c r="B3" s="164">
-        <v>2001</v>
-      </c>
-      <c r="C3" s="164" t="s">
-        <v>587</v>
-      </c>
-      <c r="D3" s="164" t="s">
-        <v>583</v>
-      </c>
-      <c r="E3" s="168">
-        <v>1</v>
-      </c>
-      <c r="F3" s="172">
-        <v>0</v>
-      </c>
-      <c r="G3" s="172">
-        <v>0</v>
-      </c>
-      <c r="H3" s="172">
-        <v>0</v>
-      </c>
-      <c r="I3" s="172">
-        <v>1</v>
-      </c>
-      <c r="J3" s="47" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>588</v>
-      </c>
-      <c r="B4" s="165">
-        <v>2001</v>
-      </c>
-      <c r="C4" s="165" t="s">
-        <v>587</v>
-      </c>
-      <c r="D4" s="165" t="s">
-        <v>583</v>
-      </c>
-      <c r="E4" s="169">
-        <v>1</v>
-      </c>
-      <c r="F4" s="173" t="s">
-        <v>589</v>
-      </c>
-      <c r="G4" s="173"/>
-      <c r="H4" s="173"/>
-      <c r="I4" s="174">
-        <v>1</v>
-      </c>
-      <c r="J4" s="47" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>590</v>
-      </c>
-      <c r="B5" s="152" t="s">
-        <v>593</v>
-      </c>
-      <c r="C5" s="152"/>
-      <c r="D5" s="152"/>
-      <c r="E5" s="152"/>
-      <c r="F5" s="152"/>
-      <c r="G5" s="152"/>
-      <c r="H5" s="152"/>
-      <c r="I5" s="152"/>
-      <c r="J5" s="152"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="C5" s="161"/>
+      <c r="D5" s="161"/>
+      <c r="E5" s="161"/>
+      <c r="F5" s="161"/>
+      <c r="G5" s="161"/>
+      <c r="H5" s="161"/>
+      <c r="I5" s="161"/>
+      <c r="J5" s="161"/>
+      <c r="L5" s="186" t="s">
+        <v>621</v>
+      </c>
+      <c r="M5" s="187" t="s">
+        <v>623</v>
+      </c>
+      <c r="N5" s="187" t="s">
+        <v>624</v>
+      </c>
+      <c r="O5" s="187" t="s">
+        <v>625</v>
+      </c>
+      <c r="P5" s="186" t="s">
+        <v>626</v>
+      </c>
+      <c r="Q5" s="186" t="s">
+        <v>627</v>
+      </c>
+      <c r="R5" s="186" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="172" t="s">
         <v>280</v>
       </c>
-      <c r="B6" s="175">
+      <c r="B6" s="162">
         <f>2^128</f>
         <v>3.4028236692093846E+38</v>
       </c>
-      <c r="C6" s="175"/>
-      <c r="D6" s="175"/>
-      <c r="E6" s="175"/>
-      <c r="F6" s="175"/>
-      <c r="G6" s="175"/>
-      <c r="H6" s="175"/>
-      <c r="I6" s="175"/>
-      <c r="J6" s="175"/>
+      <c r="C6" s="162"/>
+      <c r="D6" s="162"/>
+      <c r="E6" s="162"/>
+      <c r="F6" s="162"/>
+      <c r="G6" s="162"/>
+      <c r="H6" s="162"/>
+      <c r="I6" s="162"/>
+      <c r="J6" s="162"/>
+      <c r="L6" s="194" t="s">
+        <v>628</v>
+      </c>
+      <c r="M6" s="195" t="s">
+        <v>629</v>
+      </c>
+      <c r="N6" s="195"/>
+      <c r="O6" s="195"/>
+      <c r="P6" s="195"/>
+      <c r="Q6" s="195"/>
+      <c r="R6" s="195"/>
+    </row>
+    <row r="7" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="8" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="167" t="s">
+        <v>630</v>
+      </c>
+      <c r="B8" s="154" t="s">
+        <v>631</v>
+      </c>
+      <c r="C8" s="154"/>
+      <c r="D8" s="154"/>
+      <c r="E8" s="154"/>
+      <c r="F8" s="154"/>
+      <c r="G8" s="154"/>
+      <c r="H8" s="154"/>
+      <c r="I8" s="154"/>
+      <c r="J8" s="167" t="s">
+        <v>590</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A9" s="169" t="s">
+        <v>632</v>
+      </c>
+      <c r="B9" s="201" t="s">
+        <v>647</v>
+      </c>
+      <c r="C9" s="201"/>
+      <c r="D9" s="201" t="s">
+        <v>635</v>
+      </c>
+      <c r="E9" s="201"/>
+      <c r="F9" s="200" t="s">
+        <v>636</v>
+      </c>
+      <c r="G9" s="200"/>
+      <c r="H9" s="200" t="s">
+        <v>648</v>
+      </c>
+      <c r="I9" s="200"/>
+      <c r="J9" s="62" t="s">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A10" s="170" t="s">
+        <v>639</v>
+      </c>
+      <c r="B10" s="102" t="s">
+        <v>633</v>
+      </c>
+      <c r="C10" s="102" t="s">
+        <v>634</v>
+      </c>
+      <c r="D10" s="102" t="s">
+        <v>635</v>
+      </c>
+      <c r="E10" s="196" t="s">
+        <v>233</v>
+      </c>
+      <c r="F10" s="196" t="s">
+        <v>640</v>
+      </c>
+      <c r="G10" s="102" t="s">
+        <v>636</v>
+      </c>
+      <c r="H10" s="102" t="s">
+        <v>637</v>
+      </c>
+      <c r="I10" s="197" t="s">
+        <v>638</v>
+      </c>
+      <c r="J10" s="126" t="s">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A11" s="171" t="s">
+        <v>641</v>
+      </c>
+      <c r="B11" s="105" t="s">
+        <v>645</v>
+      </c>
+      <c r="C11" s="105" t="s">
+        <v>634</v>
+      </c>
+      <c r="D11" s="105" t="s">
+        <v>643</v>
+      </c>
+      <c r="E11" s="105" t="s">
+        <v>233</v>
+      </c>
+      <c r="F11" s="105" t="s">
+        <v>640</v>
+      </c>
+      <c r="G11" s="105" t="s">
+        <v>636</v>
+      </c>
+      <c r="H11" s="105" t="s">
+        <v>637</v>
+      </c>
+      <c r="I11" s="105" t="s">
+        <v>644</v>
+      </c>
+      <c r="J11" s="127" t="s">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="198" t="s">
+        <v>595</v>
+      </c>
+      <c r="B12" s="199" t="s">
+        <v>646</v>
+      </c>
+      <c r="C12" s="199"/>
+      <c r="D12" s="199"/>
+      <c r="E12" s="199"/>
+      <c r="F12" s="199"/>
+      <c r="G12" s="199"/>
+      <c r="H12" s="199"/>
+      <c r="I12" s="199"/>
+      <c r="J12" s="199"/>
+    </row>
+    <row r="13" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="14" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="167"/>
+      <c r="B14" s="154"/>
+      <c r="C14" s="154"/>
+      <c r="D14" s="154"/>
+      <c r="E14" s="154"/>
+      <c r="F14" s="154"/>
+      <c r="G14" s="154"/>
+      <c r="H14" s="154"/>
+      <c r="I14" s="154"/>
+      <c r="J14" s="167"/>
+      <c r="L14" t="s">
+        <v>649</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A15" s="169" t="s">
+        <v>655</v>
+      </c>
+      <c r="B15" s="201" t="s">
+        <v>659</v>
+      </c>
+      <c r="C15" s="201"/>
+      <c r="D15" s="201" t="s">
+        <v>657</v>
+      </c>
+      <c r="E15" s="201"/>
+      <c r="F15" s="200">
+        <v>24</v>
+      </c>
+      <c r="G15" s="200"/>
+      <c r="H15" s="200" t="s">
+        <v>658</v>
+      </c>
+      <c r="I15" s="200"/>
+      <c r="J15" s="62" t="s">
+        <v>591</v>
+      </c>
+      <c r="L15" t="s">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A16" s="170" t="s">
+        <v>639</v>
+      </c>
+      <c r="B16" s="102" t="s">
+        <v>633</v>
+      </c>
+      <c r="C16" s="102" t="s">
+        <v>660</v>
+      </c>
+      <c r="D16" s="102" t="s">
+        <v>657</v>
+      </c>
+      <c r="E16" s="196" t="s">
+        <v>661</v>
+      </c>
+      <c r="F16" s="196" t="s">
+        <v>662</v>
+      </c>
+      <c r="G16" s="102" t="s">
+        <v>663</v>
+      </c>
+      <c r="H16" s="102" t="s">
+        <v>665</v>
+      </c>
+      <c r="I16" s="197" t="s">
+        <v>666</v>
+      </c>
+      <c r="J16" s="126" t="s">
+        <v>591</v>
+      </c>
+      <c r="L16" t="s">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17" s="171" t="s">
+        <v>641</v>
+      </c>
+      <c r="B17" s="105" t="s">
+        <v>642</v>
+      </c>
+      <c r="C17" s="105" t="s">
+        <v>660</v>
+      </c>
+      <c r="D17" s="105" t="s">
+        <v>657</v>
+      </c>
+      <c r="E17" s="105" t="s">
+        <v>661</v>
+      </c>
+      <c r="F17" s="105" t="s">
+        <v>662</v>
+      </c>
+      <c r="G17" s="105" t="s">
+        <v>663</v>
+      </c>
+      <c r="H17" s="105" t="s">
+        <v>665</v>
+      </c>
+      <c r="I17" s="105" t="s">
+        <v>666</v>
+      </c>
+      <c r="J17" s="127" t="s">
+        <v>591</v>
+      </c>
+      <c r="L17" t="s">
+        <v>654</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="198" t="s">
+        <v>656</v>
+      </c>
+      <c r="B18" s="199" t="s">
+        <v>667</v>
+      </c>
+      <c r="C18" s="199"/>
+      <c r="D18" s="199"/>
+      <c r="E18" s="199"/>
+      <c r="F18" s="199"/>
+      <c r="G18" s="199"/>
+      <c r="H18" s="199"/>
+      <c r="I18" s="199"/>
+      <c r="J18" s="199"/>
+      <c r="L18" t="s">
+        <v>653</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L19" t="s">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="167"/>
+      <c r="B20" s="154"/>
+      <c r="C20" s="154"/>
+      <c r="D20" s="154"/>
+      <c r="E20" s="154"/>
+      <c r="F20" s="154"/>
+      <c r="G20" s="154"/>
+      <c r="H20" s="154"/>
+      <c r="I20" s="154"/>
+      <c r="J20" s="167"/>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A21" s="169" t="s">
+        <v>632</v>
+      </c>
+      <c r="B21" s="201" t="s">
+        <v>673</v>
+      </c>
+      <c r="C21" s="201"/>
+      <c r="D21" s="201" t="s">
+        <v>669</v>
+      </c>
+      <c r="E21" s="201"/>
+      <c r="F21" s="200" t="s">
+        <v>674</v>
+      </c>
+      <c r="G21" s="200"/>
+      <c r="H21" s="200" t="s">
+        <v>675</v>
+      </c>
+      <c r="I21" s="200"/>
+      <c r="J21" s="62" t="s">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A22" s="170" t="s">
+        <v>639</v>
+      </c>
+      <c r="B22" s="102" t="s">
+        <v>633</v>
+      </c>
+      <c r="C22" s="102" t="s">
+        <v>664</v>
+      </c>
+      <c r="D22" s="102" t="s">
+        <v>669</v>
+      </c>
+      <c r="E22" s="196" t="s">
+        <v>661</v>
+      </c>
+      <c r="F22" s="196" t="s">
+        <v>662</v>
+      </c>
+      <c r="G22" s="102" t="s">
+        <v>670</v>
+      </c>
+      <c r="H22" s="102" t="s">
+        <v>671</v>
+      </c>
+      <c r="I22" s="197" t="s">
+        <v>672</v>
+      </c>
+      <c r="J22" s="126" t="s">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A23" s="171" t="s">
+        <v>641</v>
+      </c>
+      <c r="B23" s="105" t="s">
+        <v>642</v>
+      </c>
+      <c r="C23" s="105" t="s">
+        <v>664</v>
+      </c>
+      <c r="D23" s="105" t="s">
+        <v>669</v>
+      </c>
+      <c r="E23" s="105" t="s">
+        <v>661</v>
+      </c>
+      <c r="F23" s="105" t="s">
+        <v>662</v>
+      </c>
+      <c r="G23" s="105" t="s">
+        <v>670</v>
+      </c>
+      <c r="H23" s="105" t="s">
+        <v>671</v>
+      </c>
+      <c r="I23" s="105" t="s">
+        <v>672</v>
+      </c>
+      <c r="J23" s="127" t="s">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="198" t="s">
+        <v>656</v>
+      </c>
+      <c r="B24" s="199" t="s">
+        <v>668</v>
+      </c>
+      <c r="C24" s="199"/>
+      <c r="D24" s="199"/>
+      <c r="E24" s="199"/>
+      <c r="F24" s="199"/>
+      <c r="G24" s="199"/>
+      <c r="H24" s="199"/>
+      <c r="I24" s="199"/>
+      <c r="J24" s="199"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="24">
+    <mergeCell ref="B24:J24"/>
+    <mergeCell ref="B18:J18"/>
+    <mergeCell ref="B14:I14"/>
+    <mergeCell ref="B20:I20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="H21:I21"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="B12:J12"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="M6:R6"/>
+    <mergeCell ref="B8:I8"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="F9:G9"/>
     <mergeCell ref="B6:J6"/>
     <mergeCell ref="B5:J5"/>
     <mergeCell ref="B1:D1"/>

</xml_diff>

<commit_message>
topologia con dominios de difusion y colision
</commit_message>
<xml_diff>
--- a/docs/protocol-suite.xlsx
+++ b/docs/protocol-suite.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EducacionIT\Documents\networks\CISCO\saves\ccna-m17\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B437438D-C152-46E5-BD9E-C964F7B0E6D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E878AD41-6941-45A4-96EA-3C5877D00EA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30" yWindow="30" windowWidth="20460" windowHeight="10770" activeTab="2" xr2:uid="{3B0E3487-A348-4FC2-ABFB-0BDF97959D6D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="3" xr2:uid="{3B0E3487-A348-4FC2-ABFB-0BDF97959D6D}"/>
   </bookViews>
   <sheets>
     <sheet name="suite" sheetId="1" r:id="rId1"/>
     <sheet name="unidades" sheetId="2" r:id="rId2"/>
     <sheet name="fisica" sheetId="3" r:id="rId3"/>
+    <sheet name="enlace" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="226">
   <si>
     <t>TCP/IP de IETF</t>
   </si>
@@ -519,6 +520,201 @@
   </si>
   <si>
     <t>Columna1</t>
+  </si>
+  <si>
+    <t>Conector</t>
+  </si>
+  <si>
+    <t>FC</t>
+  </si>
+  <si>
+    <t>SC</t>
+  </si>
+  <si>
+    <t>ST</t>
+  </si>
+  <si>
+    <t>LC</t>
+  </si>
+  <si>
+    <t>Ferrule Connector</t>
+  </si>
+  <si>
+    <t>Suscriber Connector</t>
+  </si>
+  <si>
+    <t>Lucent Connector</t>
+  </si>
+  <si>
+    <t>Pulido</t>
+  </si>
+  <si>
+    <t>PC</t>
+  </si>
+  <si>
+    <t>UPC</t>
+  </si>
+  <si>
+    <t>APC</t>
+  </si>
+  <si>
+    <t>Physical Contact</t>
+  </si>
+  <si>
+    <t>Ultra Physical Contact</t>
+  </si>
+  <si>
+    <t>Angled Physical Contact</t>
+  </si>
+  <si>
+    <t>Straigth Tip</t>
+  </si>
+  <si>
+    <t>FIBRA OPTICA</t>
+  </si>
+  <si>
+    <t>Problemas</t>
+  </si>
+  <si>
+    <t>EMI</t>
+  </si>
+  <si>
+    <t>RFI</t>
+  </si>
+  <si>
+    <t>Crosstalk</t>
+  </si>
+  <si>
+    <t>Colision</t>
+  </si>
+  <si>
+    <t>Interf. ElectroMagnetica</t>
+  </si>
+  <si>
+    <t>Interf. Radiofrecuencia</t>
+  </si>
+  <si>
+    <t>Diafonia</t>
+  </si>
+  <si>
+    <t>Cruce de señales no intencional</t>
+  </si>
+  <si>
+    <t>Concepto</t>
+  </si>
+  <si>
+    <t>UTP</t>
+  </si>
+  <si>
+    <t>MDIX</t>
+  </si>
+  <si>
+    <t>auto</t>
+  </si>
+  <si>
+    <t>DUPLEX</t>
+  </si>
+  <si>
+    <t>half</t>
+  </si>
+  <si>
+    <t>full</t>
+  </si>
+  <si>
+    <t>Media Detection Interface Cross</t>
+  </si>
+  <si>
+    <t>host envia o recibe tramas</t>
+  </si>
+  <si>
+    <t>host envia y recibe tramas</t>
+  </si>
+  <si>
+    <t>Subcapas</t>
+  </si>
+  <si>
+    <t>MAC</t>
+  </si>
+  <si>
+    <t>LLC</t>
+  </si>
+  <si>
+    <t>Media Access Control</t>
+  </si>
+  <si>
+    <t>Link Layer Control</t>
+  </si>
+  <si>
+    <t>Detalle</t>
+  </si>
+  <si>
+    <t>Dominios</t>
+  </si>
+  <si>
+    <t>Difusion</t>
+  </si>
+  <si>
+    <t>Tramas de datos</t>
+  </si>
+  <si>
+    <t>Choque de tramas</t>
+  </si>
+  <si>
+    <t>Alcance de la topologia</t>
+  </si>
+  <si>
+    <t>Tramas</t>
+  </si>
+  <si>
+    <t>Runt</t>
+  </si>
+  <si>
+    <t>Giant</t>
+  </si>
+  <si>
+    <t>Throttle</t>
+  </si>
+  <si>
+    <t>CRC</t>
+  </si>
+  <si>
+    <t>Detalles</t>
+  </si>
+  <si>
+    <t>Menores a 64 Bytes</t>
+  </si>
+  <si>
+    <t>Mayores a 1500 Bytes</t>
+  </si>
+  <si>
+    <t>Desbordamiento buffer</t>
+  </si>
+  <si>
+    <t>Errores de comprobacion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Metodos </t>
+  </si>
+  <si>
+    <t>Tipo de Reenvio</t>
+  </si>
+  <si>
+    <t>Cut Through</t>
+  </si>
+  <si>
+    <t>Store N Forward</t>
+  </si>
+  <si>
+    <t>Fragment Free</t>
+  </si>
+  <si>
+    <t>Almacena y verifica la trama antes de reenviar</t>
+  </si>
+  <si>
+    <t>Identifica la mac de destino y reenvia la trama</t>
+  </si>
+  <si>
+    <t>Almacena los primeros 64Bytes y reenvia la trama</t>
   </si>
 </sst>
 </file>
@@ -730,7 +926,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="72">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -862,24 +1058,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
@@ -910,6 +1088,27 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -923,13 +1122,25 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="9">
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -1201,13 +1412,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0BC87975-7230-475B-8262-181204CAE7B1}" name="Tabla1" displayName="Tabla1" ref="A4:D16" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0BC87975-7230-475B-8262-181204CAE7B1}" name="Tabla1" displayName="Tabla1" ref="A4:D16" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
   <autoFilter ref="A4:D16" xr:uid="{0BC87975-7230-475B-8262-181204CAE7B1}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{AA838185-0FBE-48A6-BD26-7791BD1B49F4}" name="Unidad" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{5E2AB38B-2656-45B7-BF1A-B4A8EB5C4B39}" name="Equivalencia" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{2FD161C7-1944-4097-893A-2891B8231278}" name="Exponente" dataDxfId="1"/>
-    <tableColumn id="4" xr3:uid="{7ABC2AC5-E028-4519-9DE2-86A5D25EEC89}" name="Real" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{AA838185-0FBE-48A6-BD26-7791BD1B49F4}" name="Unidad" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{5E2AB38B-2656-45B7-BF1A-B4A8EB5C4B39}" name="Equivalencia" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{2FD161C7-1944-4097-893A-2891B8231278}" name="Exponente" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{7ABC2AC5-E028-4519-9DE2-86A5D25EEC89}" name="Real" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1220,6 +1431,72 @@
     <tableColumn id="1" xr3:uid="{597EFBCC-9525-4E46-BD43-4C40D876E4A0}" name="Fibra"/>
     <tableColumn id="2" xr3:uid="{23E356F1-AC07-4B0B-A872-ACADFB65D65C}" name="SMF"/>
     <tableColumn id="3" xr3:uid="{FC10F880-4024-4C8E-83C3-BF20CB90E6CE}" name="MMF"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{0DAD3A51-191C-4DA7-94CC-E291B3EB197E}" name="Tabla3" displayName="Tabla3" ref="A9:B13" totalsRowShown="0">
+  <autoFilter ref="A9:B13" xr:uid="{0DAD3A51-191C-4DA7-94CC-E291B3EB197E}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{BD79D12C-A00D-4344-A172-72C97BCF4C59}" name="Tramas"/>
+    <tableColumn id="2" xr3:uid="{356F9C6D-29CC-41E7-ABA4-A917B56A7A28}" name="Detalles"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{8DD5D4F9-F883-4EC0-8F15-88859F17FEBA}" name="Tabla4" displayName="Tabla4" ref="A5:B7" totalsRowShown="0">
+  <autoFilter ref="A5:B7" xr:uid="{8DD5D4F9-F883-4EC0-8F15-88859F17FEBA}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{A54D1158-3CAD-4BA1-AC14-41AEF6D072B0}" name="Dominios"/>
+    <tableColumn id="2" xr3:uid="{7EB6BED5-3CE5-4521-B470-69C2144B8D49}" name="Alcance de la topologia"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{BB5466ED-D1C0-44DC-A21A-556814D732C8}" name="Tabla5" displayName="Tabla5" ref="A1:B3" totalsRowShown="0">
+  <autoFilter ref="A1:B3" xr:uid="{BB5466ED-D1C0-44DC-A21A-556814D732C8}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{9FF6D522-EAAD-429F-A7AF-863BB79E5892}" name="Subcapas"/>
+    <tableColumn id="2" xr3:uid="{EC87B701-89EC-4709-9254-122C601E96E6}" name="Detalle"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{130D6413-83DD-440F-AE43-F16E3162D9FA}" name="Tabla6" displayName="Tabla6" ref="D9:E12" totalsRowShown="0">
+  <autoFilter ref="D9:E12" xr:uid="{130D6413-83DD-440F-AE43-F16E3162D9FA}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{FF33D1A9-3826-4709-84BA-D340C054E22E}" name="Metodos " dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{61E2EBF1-2F1F-4C51-9B75-6130CE37B41C}" name="Tipo de Reenvio"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{17465A86-035D-4585-9581-996B21581188}" name="Tabla7" displayName="Tabla7" ref="D1:E3" totalsRowShown="0">
+  <autoFilter ref="D1:E3" xr:uid="{17465A86-035D-4585-9581-996B21581188}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{76CBC02F-7A2C-4C92-8579-1054339DAA7C}" name="DUPLEX" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{3E135D84-9C8B-4998-94D5-18F64E0E4A8F}" name="Descripcion"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{B6666A7A-E263-4068-B2EE-C47CE1A234BD}" name="Tabla8" displayName="Tabla8" ref="D5:E6" totalsRowShown="0">
+  <autoFilter ref="D5:E6" xr:uid="{B6666A7A-E263-4068-B2EE-C47CE1A234BD}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{A84FF7C8-8351-4D78-8C0F-B152D69E936E}" name="MDIX" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{0508C805-7645-4664-B7CC-58EC5B5CE1CD}" name="Descripcion"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1554,13 +1831,13 @@
       <c r="A2" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="46" t="s">
+      <c r="B2" s="59" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="47" t="s">
+      <c r="C2" s="60" t="s">
         <v>22</v>
       </c>
-      <c r="D2" s="46" t="s">
+      <c r="D2" s="59" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1568,17 +1845,17 @@
       <c r="A3" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="46"/>
-      <c r="C3" s="47"/>
-      <c r="D3" s="46"/>
+      <c r="B3" s="59"/>
+      <c r="C3" s="60"/>
+      <c r="D3" s="59"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="46"/>
-      <c r="C4" s="47"/>
-      <c r="D4" s="46"/>
+      <c r="B4" s="59"/>
+      <c r="C4" s="60"/>
+      <c r="D4" s="59"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
@@ -1618,7 +1895,7 @@
       <c r="C7" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="D7" s="48" t="s">
+      <c r="D7" s="61" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1632,16 +1909,16 @@
       <c r="C8" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="D8" s="48"/>
+      <c r="D8" s="61"/>
     </row>
     <row r="9" spans="1:4" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B9" s="49" t="s">
+      <c r="B9" s="62" t="s">
         <v>27</v>
       </c>
-      <c r="C9" s="49"/>
+      <c r="C9" s="62"/>
       <c r="D9" s="4" t="s">
         <v>3</v>
       </c>
@@ -1702,17 +1979,17 @@
       <c r="I1" s="18"/>
     </row>
     <row r="3" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="50" t="s">
+      <c r="A3" s="63" t="s">
         <v>30</v>
       </c>
-      <c r="B3" s="50"/>
-      <c r="C3" s="50"/>
-      <c r="D3" s="50"/>
-      <c r="F3" s="51" t="s">
+      <c r="B3" s="63"/>
+      <c r="C3" s="63"/>
+      <c r="D3" s="63"/>
+      <c r="F3" s="64" t="s">
         <v>31</v>
       </c>
-      <c r="G3" s="51"/>
-      <c r="H3" s="51"/>
+      <c r="G3" s="64"/>
+      <c r="H3" s="64"/>
     </row>
     <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="20" t="s">
@@ -1879,11 +2156,11 @@
       <c r="D11" s="23" t="s">
         <v>82</v>
       </c>
-      <c r="F11" s="51" t="s">
+      <c r="F11" s="64" t="s">
         <v>32</v>
       </c>
-      <c r="G11" s="51"/>
-      <c r="H11" s="51"/>
+      <c r="G11" s="64"/>
+      <c r="H11" s="64"/>
     </row>
     <row r="12" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="24" t="s">
@@ -2016,10 +2293,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F405CE0-0F74-437F-B302-F6ED29D5D8DD}">
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:J15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView topLeftCell="D8" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2030,25 +2307,39 @@
     <col min="6" max="6" width="11.85546875" customWidth="1"/>
     <col min="7" max="7" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="2.85546875" customWidth="1"/>
-    <col min="9" max="13" width="11.85546875" customWidth="1"/>
+    <col min="9" max="9" width="11" customWidth="1"/>
+    <col min="10" max="10" width="29.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="13" width="11.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>107</v>
       </c>
+      <c r="B1" s="19" t="s">
+        <v>188</v>
+      </c>
       <c r="C1" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="52" t="s">
+      <c r="E1" s="63" t="s">
+        <v>177</v>
+      </c>
+      <c r="F1" s="63"/>
+      <c r="G1" s="63"/>
+      <c r="I1" s="65" t="s">
+        <v>161</v>
+      </c>
+      <c r="J1" s="65"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="46" t="s">
         <v>109</v>
       </c>
       <c r="B2" s="19" t="s">
         <v>117</v>
       </c>
-      <c r="C2" s="54" t="s">
+      <c r="C2" s="48" t="s">
         <v>111</v>
       </c>
       <c r="E2" t="s">
@@ -2060,15 +2351,21 @@
       <c r="G2" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="53" t="s">
+      <c r="I2" s="58" t="s">
+        <v>162</v>
+      </c>
+      <c r="J2" s="58" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="47" t="s">
         <v>110</v>
       </c>
       <c r="B3" s="19" t="s">
         <v>117</v>
       </c>
-      <c r="C3" s="57" t="s">
+      <c r="C3" s="51" t="s">
         <v>114</v>
       </c>
       <c r="E3" t="s">
@@ -2080,15 +2377,21 @@
       <c r="G3" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="54" t="s">
+      <c r="I3" s="55" t="s">
+        <v>163</v>
+      </c>
+      <c r="J3" s="55" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="48" t="s">
         <v>111</v>
       </c>
       <c r="B4" s="19" t="s">
         <v>118</v>
       </c>
-      <c r="C4" s="52" t="s">
+      <c r="C4" s="46" t="s">
         <v>109</v>
       </c>
       <c r="E4" t="s">
@@ -2100,13 +2403,19 @@
       <c r="G4" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="55" t="s">
+      <c r="I4" s="54" t="s">
+        <v>164</v>
+      </c>
+      <c r="J4" s="54" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="49" t="s">
         <v>112</v>
       </c>
       <c r="B5" s="19"/>
-      <c r="C5" s="55" t="s">
+      <c r="C5" s="49" t="s">
         <v>112</v>
       </c>
       <c r="E5" t="s">
@@ -2118,13 +2427,19 @@
       <c r="G5" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="56" t="s">
+      <c r="I5" s="56" t="s">
+        <v>165</v>
+      </c>
+      <c r="J5" s="56" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="50" t="s">
         <v>113</v>
       </c>
       <c r="B6" s="19"/>
-      <c r="C6" s="56" t="s">
+      <c r="C6" s="50" t="s">
         <v>113</v>
       </c>
       <c r="E6" t="s">
@@ -2136,15 +2451,19 @@
       <c r="G6" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="57" t="s">
+      <c r="I6" s="65" t="s">
+        <v>169</v>
+      </c>
+      <c r="J6" s="65"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="51" t="s">
         <v>114</v>
       </c>
       <c r="B7" s="19" t="s">
         <v>118</v>
       </c>
-      <c r="C7" s="53" t="s">
+      <c r="C7" s="47" t="s">
         <v>110</v>
       </c>
       <c r="E7" t="s">
@@ -2156,13 +2475,19 @@
       <c r="G7" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="58" t="s">
+      <c r="I7" s="55" t="s">
+        <v>170</v>
+      </c>
+      <c r="J7" s="55" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="52" t="s">
         <v>115</v>
       </c>
       <c r="B8" s="19"/>
-      <c r="C8" s="58" t="s">
+      <c r="C8" s="52" t="s">
         <v>115</v>
       </c>
       <c r="E8" t="s">
@@ -2174,13 +2499,19 @@
       <c r="G8" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="59" t="s">
+      <c r="I8" s="54" t="s">
+        <v>171</v>
+      </c>
+      <c r="J8" s="54" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="53" t="s">
         <v>116</v>
       </c>
       <c r="B9" s="19"/>
-      <c r="C9" s="59" t="s">
+      <c r="C9" s="53" t="s">
         <v>116</v>
       </c>
       <c r="E9" t="s">
@@ -2192,94 +2523,128 @@
       <c r="G9" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="11" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="63" t="s">
+      <c r="I9" s="56" t="s">
+        <v>172</v>
+      </c>
+      <c r="J9" s="56" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="11" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="57" t="s">
         <v>119</v>
       </c>
-      <c r="B11" s="69" t="s">
+      <c r="B11" s="70" t="s">
         <v>120</v>
       </c>
-      <c r="C11" s="69"/>
-      <c r="E11" s="63" t="s">
+      <c r="C11" s="70"/>
+      <c r="E11" s="57" t="s">
         <v>129</v>
       </c>
-      <c r="F11" s="69" t="s">
-        <v>120</v>
-      </c>
-      <c r="G11" s="69" t="s">
+      <c r="F11" s="70" t="s">
+        <v>187</v>
+      </c>
+      <c r="G11" s="70" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="64" t="s">
+      <c r="I11" s="57" t="s">
+        <v>178</v>
+      </c>
+      <c r="J11" s="57" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="58" t="s">
         <v>121</v>
       </c>
-      <c r="B12" s="65" t="s">
+      <c r="B12" s="66" t="s">
         <v>128</v>
       </c>
-      <c r="C12" s="65"/>
-      <c r="E12" s="64" t="s">
+      <c r="C12" s="66"/>
+      <c r="E12" s="58" t="s">
         <v>130</v>
       </c>
-      <c r="F12" s="65" t="s">
+      <c r="F12" s="66" t="s">
         <v>131</v>
       </c>
-      <c r="G12" s="65"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="61" t="s">
+      <c r="G12" s="66"/>
+      <c r="I12" s="58" t="s">
+        <v>179</v>
+      </c>
+      <c r="J12" s="58" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="55" t="s">
         <v>122</v>
       </c>
-      <c r="B13" s="66" t="s">
+      <c r="B13" s="67" t="s">
         <v>125</v>
       </c>
-      <c r="C13" s="66"/>
-      <c r="E13" s="61" t="s">
+      <c r="C13" s="67"/>
+      <c r="E13" s="55" t="s">
         <v>132</v>
       </c>
-      <c r="F13" s="66" t="s">
+      <c r="F13" s="67" t="s">
         <v>135</v>
       </c>
-      <c r="G13" s="66"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="60" t="s">
+      <c r="G13" s="67"/>
+      <c r="I13" s="55" t="s">
+        <v>180</v>
+      </c>
+      <c r="J13" s="55" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="54" t="s">
         <v>123</v>
       </c>
-      <c r="B14" s="67" t="s">
+      <c r="B14" s="68" t="s">
         <v>126</v>
       </c>
-      <c r="C14" s="67"/>
-      <c r="E14" s="60" t="s">
+      <c r="C14" s="68"/>
+      <c r="E14" s="54" t="s">
         <v>133</v>
       </c>
-      <c r="F14" s="67" t="s">
+      <c r="F14" s="68" t="s">
         <v>136</v>
       </c>
-      <c r="G14" s="67"/>
-    </row>
-    <row r="15" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="62" t="s">
+      <c r="G14" s="68"/>
+      <c r="I14" s="54" t="s">
+        <v>181</v>
+      </c>
+      <c r="J14" s="54" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="56" t="s">
         <v>124</v>
       </c>
-      <c r="B15" s="68" t="s">
+      <c r="B15" s="69" t="s">
         <v>127</v>
       </c>
-      <c r="C15" s="68"/>
-      <c r="E15" s="62" t="s">
+      <c r="C15" s="69"/>
+      <c r="E15" s="56" t="s">
         <v>134</v>
       </c>
-      <c r="F15" s="68" t="s">
+      <c r="F15" s="69" t="s">
         <v>137</v>
       </c>
-      <c r="G15" s="68"/>
+      <c r="G15" s="69"/>
+      <c r="I15" s="56" t="s">
+        <v>182</v>
+      </c>
+      <c r="J15" s="56" t="s">
+        <v>186</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="10">
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="F13:G13"/>
+  <mergeCells count="13">
     <mergeCell ref="F14:G14"/>
     <mergeCell ref="F15:G15"/>
     <mergeCell ref="F11:G11"/>
@@ -2288,6 +2653,11 @@
     <mergeCell ref="B13:C13"/>
     <mergeCell ref="B14:C14"/>
     <mergeCell ref="B15:C15"/>
+    <mergeCell ref="I1:J1"/>
+    <mergeCell ref="I6:J6"/>
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="F13:G13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -2295,4 +2665,183 @@
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B26DD20-43D5-45C3-8DFE-6E0DFA1B2623}">
+  <dimension ref="A1:E13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10" style="71" customWidth="1"/>
+    <col min="2" max="2" width="28.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="2.85546875" customWidth="1"/>
+    <col min="4" max="4" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="45.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="2.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>197</v>
+      </c>
+      <c r="B1" t="s">
+        <v>202</v>
+      </c>
+      <c r="D1" s="71" t="s">
+        <v>191</v>
+      </c>
+      <c r="E1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>198</v>
+      </c>
+      <c r="B2" t="s">
+        <v>200</v>
+      </c>
+      <c r="D2" s="71" t="s">
+        <v>192</v>
+      </c>
+      <c r="E2" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>199</v>
+      </c>
+      <c r="B3" t="s">
+        <v>201</v>
+      </c>
+      <c r="D3" s="71" t="s">
+        <v>193</v>
+      </c>
+      <c r="E3" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>203</v>
+      </c>
+      <c r="B5" t="s">
+        <v>207</v>
+      </c>
+      <c r="D5" s="71" t="s">
+        <v>189</v>
+      </c>
+      <c r="E5" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>204</v>
+      </c>
+      <c r="B6" t="s">
+        <v>205</v>
+      </c>
+      <c r="D6" s="71" t="s">
+        <v>190</v>
+      </c>
+      <c r="E6" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>182</v>
+      </c>
+      <c r="B7" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>208</v>
+      </c>
+      <c r="B9" t="s">
+        <v>213</v>
+      </c>
+      <c r="D9" s="71" t="s">
+        <v>218</v>
+      </c>
+      <c r="E9" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>209</v>
+      </c>
+      <c r="B10" t="s">
+        <v>214</v>
+      </c>
+      <c r="D10" s="71" t="s">
+        <v>220</v>
+      </c>
+      <c r="E10" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>210</v>
+      </c>
+      <c r="B11" t="s">
+        <v>215</v>
+      </c>
+      <c r="D11" s="71" t="s">
+        <v>221</v>
+      </c>
+      <c r="E11" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="71" t="s">
+        <v>211</v>
+      </c>
+      <c r="B12" t="s">
+        <v>216</v>
+      </c>
+      <c r="D12" s="71" t="s">
+        <v>222</v>
+      </c>
+      <c r="E12" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="71" t="s">
+        <v>212</v>
+      </c>
+      <c r="B13" t="s">
+        <v>217</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="6">
+    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
+    <tablePart r:id="rId5"/>
+    <tablePart r:id="rId6"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
dominios de colision y difusion
</commit_message>
<xml_diff>
--- a/docs/protocol-suite.xlsx
+++ b/docs/protocol-suite.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EducacionIT\Documents\networks\CISCO\saves\ccna-m17\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CA94368-AA50-44A0-8862-860BE631F787}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4890C386-2B89-4350-A8F3-E889DB281A4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="3" xr2:uid="{3B0E3487-A348-4FC2-ABFB-0BDF97959D6D}"/>
   </bookViews>
@@ -2671,7 +2671,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B26DD20-43D5-45C3-8DFE-6E0DFA1B2623}">
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
enrutamiento estatico con rutas sumarizadas
</commit_message>
<xml_diff>
--- a/docs/protocol-suite.xlsx
+++ b/docs/protocol-suite.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EducacionIT\Documents\networks\CISCO\saves\ccna-m17\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DED09E9-B791-41D9-9680-E23573D85329}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F09B427-E17C-4CD5-94C4-3DDA0C580527}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="8" xr2:uid="{3B0E3487-A348-4FC2-ABFB-0BDF97959D6D}"/>
   </bookViews>
@@ -7056,8 +7056,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="4258214" y="963490"/>
-          <a:ext cx="353039" cy="728929"/>
+          <a:off x="4254953" y="963490"/>
+          <a:ext cx="352768" cy="728371"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -7071,13 +7071,13 @@
                 <a:pt x="0" y="0"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="240026" y="0"/>
+                <a:pt x="239843" y="0"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="240026" y="728929"/>
+                <a:pt x="239843" y="728371"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="353039" y="728929"/>
+                <a:pt x="352768" y="728371"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -7118,8 +7118,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="4258214" y="963490"/>
-          <a:ext cx="353039" cy="242976"/>
+          <a:off x="4254953" y="963490"/>
+          <a:ext cx="352768" cy="242790"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -7133,13 +7133,13 @@
                 <a:pt x="0" y="0"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="240026" y="0"/>
+                <a:pt x="239843" y="0"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="240026" y="242976"/>
+                <a:pt x="239843" y="242790"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="353039" y="242976"/>
+                <a:pt x="352768" y="242790"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -7180,8 +7180,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="4258214" y="720513"/>
-          <a:ext cx="353039" cy="242976"/>
+          <a:off x="4254953" y="720699"/>
+          <a:ext cx="352768" cy="242790"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -7192,16 +7192,16 @@
           <a:pathLst>
             <a:path>
               <a:moveTo>
-                <a:pt x="0" y="242976"/>
+                <a:pt x="0" y="242790"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="240026" y="242976"/>
+                <a:pt x="239843" y="242790"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="240026" y="0"/>
+                <a:pt x="239843" y="0"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="353039" y="0"/>
+                <a:pt x="352768" y="0"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -7242,8 +7242,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="4258214" y="234560"/>
-          <a:ext cx="353039" cy="728929"/>
+          <a:off x="4254953" y="235118"/>
+          <a:ext cx="352768" cy="728371"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -7254,16 +7254,16 @@
           <a:pathLst>
             <a:path>
               <a:moveTo>
-                <a:pt x="0" y="728929"/>
+                <a:pt x="0" y="728371"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="240026" y="728929"/>
+                <a:pt x="239843" y="728371"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="240026" y="0"/>
+                <a:pt x="239843" y="0"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="353039" y="0"/>
+                <a:pt x="352768" y="0"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -7304,8 +7304,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="3380311" y="917770"/>
-          <a:ext cx="155651" cy="91440"/>
+          <a:off x="3377723" y="917769"/>
+          <a:ext cx="155532" cy="91440"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -7319,7 +7319,7 @@
                 <a:pt x="0" y="45720"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="155651" y="45720"/>
+                <a:pt x="155532" y="45720"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -7360,8 +7360,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="2071120" y="917770"/>
-          <a:ext cx="179068" cy="91440"/>
+          <a:off x="2069534" y="917769"/>
+          <a:ext cx="178930" cy="91440"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -7375,7 +7375,7 @@
                 <a:pt x="0" y="45720"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="179068" y="45720"/>
+                <a:pt x="178930" y="45720"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -7416,8 +7416,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="1130417" y="917770"/>
-          <a:ext cx="216633" cy="91440"/>
+          <a:off x="1129551" y="917769"/>
+          <a:ext cx="216467" cy="91440"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -7431,7 +7431,7 @@
                 <a:pt x="0" y="45720"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="216633" y="45720"/>
+                <a:pt x="216467" y="45720"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -7472,8 +7472,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="293" y="791146"/>
-          <a:ext cx="1130123" cy="344687"/>
+          <a:off x="293" y="791278"/>
+          <a:ext cx="1129258" cy="344423"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -7539,8 +7539,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="293" y="791146"/>
-        <a:ext cx="1130123" cy="344687"/>
+        <a:off x="293" y="791278"/>
+        <a:ext cx="1129258" cy="344423"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{F0031F58-C3EF-4FE5-9CA2-259F62269C2D}">
@@ -7550,8 +7550,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="1347050" y="601457"/>
-          <a:ext cx="724070" cy="724064"/>
+          <a:off x="1346019" y="601734"/>
+          <a:ext cx="723515" cy="723510"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
           <a:avLst/>
@@ -7617,8 +7617,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="1453088" y="707494"/>
-        <a:ext cx="511994" cy="511990"/>
+        <a:off x="1451975" y="707690"/>
+        <a:ext cx="511603" cy="511598"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{0A4D0610-D733-4901-9EDE-3CFD8851320E}">
@@ -7628,8 +7628,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="2250188" y="791146"/>
-          <a:ext cx="1130123" cy="344687"/>
+          <a:off x="2248465" y="791278"/>
+          <a:ext cx="1129258" cy="344423"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -7695,8 +7695,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="2250188" y="791146"/>
-        <a:ext cx="1130123" cy="344687"/>
+        <a:off x="2248465" y="791278"/>
+        <a:ext cx="1129258" cy="344423"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{14A42A52-0C40-47A4-928E-3C72C1AA182E}">
@@ -7706,8 +7706,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="3535963" y="602367"/>
-          <a:ext cx="722250" cy="722244"/>
+          <a:off x="3533256" y="602644"/>
+          <a:ext cx="721697" cy="721691"/>
         </a:xfrm>
         <a:prstGeom prst="flowChartConnector">
           <a:avLst/>
@@ -7773,8 +7773,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="3641734" y="708137"/>
-        <a:ext cx="510708" cy="510704"/>
+        <a:off x="3638946" y="708333"/>
+        <a:ext cx="510317" cy="510313"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{ED39B4D4-C882-4F96-8813-186B1B392815}">
@@ -7784,8 +7784,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="4611253" y="62216"/>
-          <a:ext cx="1130123" cy="344687"/>
+          <a:off x="4607722" y="62906"/>
+          <a:ext cx="1129258" cy="344423"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -7851,8 +7851,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="4611253" y="62216"/>
-        <a:ext cx="1130123" cy="344687"/>
+        <a:off x="4607722" y="62906"/>
+        <a:ext cx="1129258" cy="344423"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{13D2BC7E-B9A8-430E-8574-A57A85597C80}">
@@ -7862,8 +7862,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="4611253" y="548169"/>
-          <a:ext cx="1130123" cy="344687"/>
+          <a:off x="4607722" y="548487"/>
+          <a:ext cx="1129258" cy="344423"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -7929,8 +7929,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="4611253" y="548169"/>
-        <a:ext cx="1130123" cy="344687"/>
+        <a:off x="4607722" y="548487"/>
+        <a:ext cx="1129258" cy="344423"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{B57558C7-CC91-4E8E-ADA7-69F72314096E}">
@@ -7940,8 +7940,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="4611253" y="1034122"/>
-          <a:ext cx="1130123" cy="344687"/>
+          <a:off x="4607722" y="1034068"/>
+          <a:ext cx="1129258" cy="344423"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -8007,8 +8007,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="4611253" y="1034122"/>
-        <a:ext cx="1130123" cy="344687"/>
+        <a:off x="4607722" y="1034068"/>
+        <a:ext cx="1129258" cy="344423"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{ED5BC5F9-93FD-4F76-B2B3-B0975F037838}">
@@ -8018,8 +8018,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="4611253" y="1520075"/>
-          <a:ext cx="1130123" cy="344687"/>
+          <a:off x="4607722" y="1519649"/>
+          <a:ext cx="1129258" cy="344423"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -8085,8 +8085,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="4611253" y="1520075"/>
-        <a:ext cx="1130123" cy="344687"/>
+        <a:off x="4607722" y="1519649"/>
+        <a:ext cx="1129258" cy="344423"/>
       </dsp:txXfrm>
     </dsp:sp>
   </dsp:spTree>
@@ -14468,20 +14468,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C517D60C-B106-4EB5-A3AA-123C6DFD220C}">
   <dimension ref="A1:I43"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+    <sheetView topLeftCell="A3" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A3" sqref="A3"/>
-      <selection pane="bottomLeft" activeCell="G4" sqref="G4"/>
+      <selection pane="bottomLeft" activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="7.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -15478,7 +15478,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C4CBB4D-C973-4D68-8A35-032D87F031CE}">
   <dimension ref="A1:S31"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+    <sheetView topLeftCell="A3" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A3" sqref="A3"/>
       <selection pane="bottomLeft" activeCell="D5" sqref="D5"/>
@@ -16325,8 +16325,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FAC4EC1-B914-4487-811E-91ED6BC7F9D2}">
   <dimension ref="A1:N14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
enrutamiento ipv6 dual stack
</commit_message>
<xml_diff>
--- a/docs/protocol-suite.xlsx
+++ b/docs/protocol-suite.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EducacionIT\Documents\networks\CISCO\saves\ccna-m17\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F610168-6299-4B34-B164-C1128B2C118D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C88A9E2-4B7F-4746-9CCB-D808E1B66A40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="9" xr2:uid="{3B0E3487-A348-4FC2-ABFB-0BDF97959D6D}"/>
   </bookViews>
@@ -4433,7 +4433,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="264">
+  <cellXfs count="266">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -4968,114 +4968,6 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="10" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -5107,49 +4999,159 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="17" fillId="10" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="10" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="17" fillId="10" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
+    <xf numFmtId="49" fontId="4" fillId="10" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="10" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="17" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="10" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="17" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="10" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="4" fillId="10" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="10" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Millares" xfId="1" builtinId="3"/>
@@ -11735,13 +11737,13 @@
       <c r="A2" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="200" t="s">
+      <c r="B2" s="222" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="201" t="s">
+      <c r="C2" s="223" t="s">
         <v>22</v>
       </c>
-      <c r="D2" s="200" t="s">
+      <c r="D2" s="222" t="s">
         <v>4</v>
       </c>
     </row>
@@ -11749,17 +11751,17 @@
       <c r="A3" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="200"/>
-      <c r="C3" s="201"/>
-      <c r="D3" s="200"/>
+      <c r="B3" s="222"/>
+      <c r="C3" s="223"/>
+      <c r="D3" s="222"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="200"/>
-      <c r="C4" s="201"/>
-      <c r="D4" s="200"/>
+      <c r="B4" s="222"/>
+      <c r="C4" s="223"/>
+      <c r="D4" s="222"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
@@ -11799,7 +11801,7 @@
       <c r="C7" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="D7" s="202" t="s">
+      <c r="D7" s="224" t="s">
         <v>7</v>
       </c>
     </row>
@@ -11813,16 +11815,16 @@
       <c r="C8" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="D8" s="202"/>
+      <c r="D8" s="224"/>
     </row>
     <row r="9" spans="1:4" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B9" s="203" t="s">
+      <c r="B9" s="225" t="s">
         <v>27</v>
       </c>
-      <c r="C9" s="203"/>
+      <c r="C9" s="225"/>
       <c r="D9" s="4" t="s">
         <v>3</v>
       </c>
@@ -11845,7 +11847,7 @@
   <dimension ref="A1:Z29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="L26" sqref="L26"/>
+      <selection activeCell="P11" sqref="P11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11866,20 +11868,20 @@
       <c r="A1" s="66" t="s">
         <v>719</v>
       </c>
-      <c r="B1" s="250" t="s">
+      <c r="B1" s="259" t="s">
         <v>714</v>
       </c>
-      <c r="C1" s="250"/>
-      <c r="D1" s="250"/>
+      <c r="C1" s="259"/>
+      <c r="D1" s="259"/>
       <c r="E1" s="79" t="s">
         <v>715</v>
       </c>
-      <c r="F1" s="250" t="s">
+      <c r="F1" s="259" t="s">
         <v>716</v>
       </c>
-      <c r="G1" s="250"/>
-      <c r="H1" s="250"/>
-      <c r="I1" s="250"/>
+      <c r="G1" s="259"/>
+      <c r="H1" s="259"/>
+      <c r="I1" s="259"/>
       <c r="J1" s="199" t="s">
         <v>717</v>
       </c>
@@ -11906,34 +11908,34 @@
       <c r="A2" s="173" t="s">
         <v>718</v>
       </c>
-      <c r="B2" s="240">
+      <c r="B2" s="204">
         <v>2001</v>
       </c>
-      <c r="C2" s="240" t="s">
+      <c r="C2" s="204" t="s">
         <v>709</v>
       </c>
-      <c r="D2" s="240" t="s">
+      <c r="D2" s="204" t="s">
         <v>710</v>
       </c>
-      <c r="E2" s="241" t="s">
+      <c r="E2" s="205" t="s">
         <v>711</v>
       </c>
-      <c r="F2" s="242" t="s">
+      <c r="F2" s="206" t="s">
         <v>712</v>
       </c>
-      <c r="G2" s="242" t="s">
+      <c r="G2" s="206" t="s">
         <v>712</v>
       </c>
-      <c r="H2" s="242" t="s">
+      <c r="H2" s="206" t="s">
         <v>712</v>
       </c>
-      <c r="I2" s="242" t="s">
+      <c r="I2" s="206" t="s">
         <v>711</v>
       </c>
-      <c r="J2" s="243" t="s">
+      <c r="J2" s="207" t="s">
         <v>713</v>
       </c>
-      <c r="L2" s="251" t="s">
+      <c r="L2" s="213" t="s">
         <v>735</v>
       </c>
       <c r="M2" s="58" t="s">
@@ -11956,34 +11958,34 @@
       <c r="A3" s="174" t="s">
         <v>720</v>
       </c>
-      <c r="B3" s="237" t="s">
+      <c r="B3" s="201" t="s">
         <v>721</v>
       </c>
-      <c r="C3" s="237" t="s">
+      <c r="C3" s="201" t="s">
         <v>709</v>
       </c>
-      <c r="D3" s="237" t="s">
+      <c r="D3" s="201" t="s">
         <v>722</v>
       </c>
-      <c r="E3" s="238" t="s">
+      <c r="E3" s="202" t="s">
         <v>290</v>
       </c>
-      <c r="F3" s="239" t="s">
+      <c r="F3" s="203" t="s">
         <v>723</v>
       </c>
-      <c r="G3" s="239" t="s">
+      <c r="G3" s="203" t="s">
         <v>723</v>
       </c>
-      <c r="H3" s="239" t="s">
+      <c r="H3" s="203" t="s">
         <v>723</v>
       </c>
-      <c r="I3" s="239" t="s">
+      <c r="I3" s="203" t="s">
         <v>290</v>
       </c>
-      <c r="J3" s="244" t="s">
+      <c r="J3" s="208" t="s">
         <v>713</v>
       </c>
-      <c r="L3" s="252" t="s">
+      <c r="L3" s="214" t="s">
         <v>740</v>
       </c>
       <c r="M3" s="55" t="s">
@@ -12006,30 +12008,30 @@
       <c r="A4" s="175" t="s">
         <v>724</v>
       </c>
-      <c r="B4" s="245" t="s">
+      <c r="B4" s="209" t="s">
         <v>721</v>
       </c>
-      <c r="C4" s="245" t="s">
+      <c r="C4" s="209" t="s">
         <v>709</v>
       </c>
-      <c r="D4" s="245" t="s">
+      <c r="D4" s="209" t="s">
         <v>722</v>
       </c>
-      <c r="E4" s="246" t="s">
+      <c r="E4" s="210" t="s">
         <v>290</v>
       </c>
-      <c r="F4" s="257" t="s">
+      <c r="F4" s="262" t="s">
         <v>725</v>
       </c>
-      <c r="G4" s="257"/>
-      <c r="H4" s="257"/>
-      <c r="I4" s="247" t="s">
+      <c r="G4" s="262"/>
+      <c r="H4" s="262"/>
+      <c r="I4" s="211" t="s">
         <v>290</v>
       </c>
-      <c r="J4" s="248" t="s">
+      <c r="J4" s="212" t="s">
         <v>713</v>
       </c>
-      <c r="L4" s="253" t="s">
+      <c r="L4" s="215" t="s">
         <v>741</v>
       </c>
       <c r="M4" s="54" t="s">
@@ -12052,18 +12054,18 @@
       <c r="A5" s="176" t="s">
         <v>301</v>
       </c>
-      <c r="B5" s="249" t="s">
+      <c r="B5" s="258" t="s">
         <v>726</v>
       </c>
-      <c r="C5" s="249"/>
-      <c r="D5" s="249"/>
-      <c r="E5" s="249"/>
-      <c r="F5" s="249"/>
-      <c r="G5" s="249"/>
-      <c r="H5" s="249"/>
-      <c r="I5" s="249"/>
-      <c r="J5" s="249"/>
-      <c r="L5" s="252" t="s">
+      <c r="C5" s="258"/>
+      <c r="D5" s="258"/>
+      <c r="E5" s="258"/>
+      <c r="F5" s="258"/>
+      <c r="G5" s="258"/>
+      <c r="H5" s="258"/>
+      <c r="I5" s="258"/>
+      <c r="J5" s="258"/>
+      <c r="L5" s="214" t="s">
         <v>337</v>
       </c>
       <c r="M5" s="55" t="s">
@@ -12083,100 +12085,110 @@
       </c>
     </row>
     <row r="6" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="236"/>
-      <c r="C6" s="236"/>
-      <c r="D6" s="236"/>
-      <c r="E6" s="236"/>
-      <c r="F6" s="236"/>
-      <c r="G6" s="236"/>
-      <c r="L6" s="254" t="s">
+      <c r="B6" s="200"/>
+      <c r="C6" s="200"/>
+      <c r="D6" s="200"/>
+      <c r="E6" s="200"/>
+      <c r="F6" s="200"/>
+      <c r="G6" s="200"/>
+      <c r="L6" s="216" t="s">
         <v>750</v>
       </c>
-      <c r="M6" s="255">
+      <c r="M6" s="263">
         <f>2^128</f>
         <v>3.4028236692093846E+38</v>
       </c>
-      <c r="N6" s="255"/>
-      <c r="O6" s="255"/>
-      <c r="P6" s="255"/>
-      <c r="Q6" s="255"/>
+      <c r="N6" s="263"/>
+      <c r="O6" s="263"/>
+      <c r="P6" s="263"/>
+      <c r="Q6" s="263"/>
     </row>
     <row r="7" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="66" t="s">
         <v>760</v>
       </c>
-      <c r="B7" s="250" t="s">
+      <c r="B7" s="259" t="s">
         <v>767</v>
       </c>
-      <c r="C7" s="250"/>
-      <c r="D7" s="250"/>
-      <c r="E7" s="250"/>
-      <c r="F7" s="250"/>
-      <c r="G7" s="250"/>
-      <c r="H7" s="250"/>
-      <c r="I7" s="250"/>
+      <c r="C7" s="259"/>
+      <c r="D7" s="259"/>
+      <c r="E7" s="259"/>
+      <c r="F7" s="259"/>
+      <c r="G7" s="259"/>
+      <c r="H7" s="259"/>
+      <c r="I7" s="259"/>
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A8" s="173" t="s">
         <v>198</v>
       </c>
-      <c r="B8" s="258" t="s">
+      <c r="B8" s="218" t="s">
         <v>761</v>
       </c>
-      <c r="C8" s="258" t="s">
+      <c r="C8" s="218" t="s">
         <v>762</v>
       </c>
-      <c r="D8" s="263" t="s">
+      <c r="D8" s="260" t="s">
         <v>763</v>
       </c>
-      <c r="E8" s="263"/>
-      <c r="F8" s="262" t="s">
+      <c r="E8" s="260"/>
+      <c r="F8" s="261" t="s">
         <v>764</v>
       </c>
-      <c r="G8" s="262"/>
-      <c r="H8" s="258" t="s">
+      <c r="G8" s="261"/>
+      <c r="H8" s="218" t="s">
         <v>765</v>
       </c>
-      <c r="I8" s="258" t="s">
+      <c r="I8" s="218" t="s">
         <v>766</v>
       </c>
+      <c r="L8" s="264"/>
+      <c r="M8" s="264"/>
+      <c r="N8" s="264"/>
+      <c r="O8" s="264"/>
+      <c r="P8" s="264"/>
     </row>
     <row r="9" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A9" s="174" t="s">
         <v>768</v>
       </c>
-      <c r="B9" s="259" t="s">
+      <c r="B9" s="219" t="s">
         <v>761</v>
       </c>
-      <c r="C9" s="259" t="s">
+      <c r="C9" s="219" t="s">
         <v>762</v>
       </c>
-      <c r="D9" s="259" t="s">
+      <c r="D9" s="219" t="s">
         <v>763</v>
       </c>
-      <c r="E9" s="238" t="s">
+      <c r="E9" s="202" t="s">
         <v>769</v>
       </c>
-      <c r="F9" s="238" t="s">
+      <c r="F9" s="202" t="s">
         <v>770</v>
       </c>
-      <c r="G9" s="259" t="s">
+      <c r="G9" s="219" t="s">
         <v>764</v>
       </c>
-      <c r="H9" s="259" t="s">
+      <c r="H9" s="219" t="s">
         <v>765</v>
       </c>
-      <c r="I9" s="259" t="s">
+      <c r="I9" s="219" t="s">
         <v>766</v>
       </c>
       <c r="J9" s="62"/>
+      <c r="L9" s="265"/>
+      <c r="M9" s="265"/>
+      <c r="N9" s="265"/>
+      <c r="O9" s="265"/>
+      <c r="P9" s="265"/>
       <c r="V9" t="s">
         <v>776</v>
       </c>
       <c r="W9" t="s">
         <v>754</v>
       </c>
-      <c r="X9" s="236" t="s">
+      <c r="X9" s="200" t="s">
         <v>758</v>
       </c>
       <c r="Y9" t="str">
@@ -12192,28 +12204,28 @@
       <c r="A10" s="175" t="s">
         <v>771</v>
       </c>
-      <c r="B10" s="260" t="s">
+      <c r="B10" s="220" t="s">
         <v>775</v>
       </c>
-      <c r="C10" s="260" t="s">
+      <c r="C10" s="220" t="s">
         <v>762</v>
       </c>
-      <c r="D10" s="260" t="s">
+      <c r="D10" s="220" t="s">
         <v>763</v>
       </c>
-      <c r="E10" s="260" t="s">
+      <c r="E10" s="220" t="s">
         <v>769</v>
       </c>
-      <c r="F10" s="261" t="s">
+      <c r="F10" s="221" t="s">
         <v>770</v>
       </c>
-      <c r="G10" s="261" t="s">
+      <c r="G10" s="221" t="s">
         <v>764</v>
       </c>
-      <c r="H10" s="261" t="s">
+      <c r="H10" s="221" t="s">
         <v>765</v>
       </c>
-      <c r="I10" s="260" t="s">
+      <c r="I10" s="220" t="s">
         <v>766</v>
       </c>
       <c r="V10" t="s">
@@ -12222,7 +12234,7 @@
       <c r="W10" t="s">
         <v>755</v>
       </c>
-      <c r="X10" s="256" t="s">
+      <c r="X10" s="217" t="s">
         <v>759</v>
       </c>
       <c r="Y10" t="str">
@@ -12238,23 +12250,23 @@
       <c r="A11" s="176" t="s">
         <v>773</v>
       </c>
-      <c r="B11" s="249" t="s">
+      <c r="B11" s="258" t="s">
         <v>774</v>
       </c>
-      <c r="C11" s="249"/>
-      <c r="D11" s="249"/>
-      <c r="E11" s="249"/>
-      <c r="F11" s="249"/>
-      <c r="G11" s="249"/>
-      <c r="H11" s="249"/>
-      <c r="I11" s="249"/>
+      <c r="C11" s="258"/>
+      <c r="D11" s="258"/>
+      <c r="E11" s="258"/>
+      <c r="F11" s="258"/>
+      <c r="G11" s="258"/>
+      <c r="H11" s="258"/>
+      <c r="I11" s="258"/>
       <c r="V11" t="s">
         <v>779</v>
       </c>
       <c r="W11" t="s">
         <v>753</v>
       </c>
-      <c r="X11" s="236" t="s">
+      <c r="X11" s="200" t="s">
         <v>757</v>
       </c>
       <c r="Y11" t="str">
@@ -12273,7 +12285,7 @@
       <c r="W12" t="s">
         <v>752</v>
       </c>
-      <c r="X12" s="236" t="s">
+      <c r="X12" s="200" t="s">
         <v>756</v>
       </c>
       <c r="Y12" t="str">
@@ -12289,39 +12301,39 @@
       <c r="A13" s="66" t="s">
         <v>760</v>
       </c>
-      <c r="B13" s="250" t="s">
+      <c r="B13" s="259" t="s">
         <v>780</v>
       </c>
-      <c r="C13" s="250"/>
-      <c r="D13" s="250"/>
-      <c r="E13" s="250"/>
-      <c r="F13" s="250"/>
-      <c r="G13" s="250"/>
-      <c r="H13" s="250"/>
-      <c r="I13" s="250"/>
+      <c r="C13" s="259"/>
+      <c r="D13" s="259"/>
+      <c r="E13" s="259"/>
+      <c r="F13" s="259"/>
+      <c r="G13" s="259"/>
+      <c r="H13" s="259"/>
+      <c r="I13" s="259"/>
     </row>
     <row r="14" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A14" s="173" t="s">
         <v>198</v>
       </c>
-      <c r="B14" s="258" t="s">
+      <c r="B14" s="218" t="s">
         <v>761</v>
       </c>
-      <c r="C14" s="258" t="s">
+      <c r="C14" s="218" t="s">
         <v>761</v>
       </c>
-      <c r="D14" s="263" t="s">
+      <c r="D14" s="260" t="s">
         <v>783</v>
       </c>
-      <c r="E14" s="263"/>
-      <c r="F14" s="262" t="s">
+      <c r="E14" s="260"/>
+      <c r="F14" s="261" t="s">
         <v>784</v>
       </c>
-      <c r="G14" s="262"/>
-      <c r="H14" s="258" t="s">
+      <c r="G14" s="261"/>
+      <c r="H14" s="218" t="s">
         <v>785</v>
       </c>
-      <c r="I14" s="258" t="s">
+      <c r="I14" s="218" t="s">
         <v>786</v>
       </c>
     </row>
@@ -12329,28 +12341,28 @@
       <c r="A15" s="174" t="s">
         <v>768</v>
       </c>
-      <c r="B15" s="259" t="s">
+      <c r="B15" s="219" t="s">
         <v>761</v>
       </c>
-      <c r="C15" s="259" t="s">
+      <c r="C15" s="219" t="s">
         <v>761</v>
       </c>
-      <c r="D15" s="259" t="s">
+      <c r="D15" s="219" t="s">
         <v>783</v>
       </c>
-      <c r="E15" s="238" t="s">
+      <c r="E15" s="202" t="s">
         <v>769</v>
       </c>
-      <c r="F15" s="238" t="s">
+      <c r="F15" s="202" t="s">
         <v>770</v>
       </c>
-      <c r="G15" s="259" t="s">
+      <c r="G15" s="219" t="s">
         <v>784</v>
       </c>
-      <c r="H15" s="259" t="s">
+      <c r="H15" s="219" t="s">
         <v>785</v>
       </c>
-      <c r="I15" s="259" t="s">
+      <c r="I15" s="219" t="s">
         <v>786</v>
       </c>
     </row>
@@ -12358,290 +12370,312 @@
       <c r="A16" s="175" t="s">
         <v>771</v>
       </c>
-      <c r="B16" s="260" t="s">
+      <c r="B16" s="220" t="s">
         <v>772</v>
       </c>
-      <c r="C16" s="260" t="s">
+      <c r="C16" s="220" t="s">
         <v>761</v>
       </c>
-      <c r="D16" s="260" t="s">
+      <c r="D16" s="220" t="s">
         <v>783</v>
       </c>
-      <c r="E16" s="260" t="s">
+      <c r="E16" s="220" t="s">
         <v>769</v>
       </c>
-      <c r="F16" s="260" t="s">
+      <c r="F16" s="220" t="s">
         <v>770</v>
       </c>
-      <c r="G16" s="260" t="s">
+      <c r="G16" s="220" t="s">
         <v>784</v>
       </c>
-      <c r="H16" s="260" t="s">
+      <c r="H16" s="220" t="s">
         <v>785</v>
       </c>
-      <c r="I16" s="260" t="s">
+      <c r="I16" s="220" t="s">
         <v>786</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="176" t="s">
         <v>773</v>
       </c>
-      <c r="B17" s="249" t="s">
+      <c r="B17" s="258" t="s">
         <v>787</v>
       </c>
-      <c r="C17" s="249"/>
-      <c r="D17" s="249"/>
-      <c r="E17" s="249"/>
-      <c r="F17" s="249"/>
-      <c r="G17" s="249"/>
-      <c r="H17" s="249"/>
-      <c r="I17" s="249"/>
-    </row>
-    <row r="18" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="19" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C17" s="258"/>
+      <c r="D17" s="258"/>
+      <c r="E17" s="258"/>
+      <c r="F17" s="258"/>
+      <c r="G17" s="258"/>
+      <c r="H17" s="258"/>
+      <c r="I17" s="258"/>
+    </row>
+    <row r="18" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="19" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="66" t="s">
         <v>760</v>
       </c>
-      <c r="B19" s="250" t="s">
+      <c r="B19" s="259" t="s">
         <v>782</v>
       </c>
-      <c r="C19" s="250"/>
-      <c r="D19" s="250"/>
-      <c r="E19" s="250"/>
-      <c r="F19" s="250"/>
-      <c r="G19" s="250"/>
-      <c r="H19" s="250"/>
-      <c r="I19" s="250"/>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C19" s="259"/>
+      <c r="D19" s="259"/>
+      <c r="E19" s="259"/>
+      <c r="F19" s="259"/>
+      <c r="G19" s="259"/>
+      <c r="H19" s="259"/>
+      <c r="I19" s="259"/>
+      <c r="L19" s="264"/>
+      <c r="M19" s="264"/>
+      <c r="N19" s="264"/>
+      <c r="O19" s="264"/>
+      <c r="P19" s="264"/>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" s="173" t="s">
         <v>198</v>
       </c>
-      <c r="B20" s="258" t="s">
+      <c r="B20" s="218" t="s">
         <v>761</v>
       </c>
-      <c r="C20" s="258" t="s">
+      <c r="C20" s="218" t="s">
         <v>762</v>
       </c>
-      <c r="D20" s="263" t="s">
+      <c r="D20" s="260" t="s">
         <v>788</v>
       </c>
-      <c r="E20" s="263"/>
-      <c r="F20" s="262" t="s">
+      <c r="E20" s="260"/>
+      <c r="F20" s="261" t="s">
         <v>789</v>
       </c>
-      <c r="G20" s="262"/>
-      <c r="H20" s="258" t="s">
+      <c r="G20" s="261"/>
+      <c r="H20" s="218" t="s">
         <v>790</v>
       </c>
-      <c r="I20" s="258" t="s">
+      <c r="I20" s="218" t="s">
         <v>791</v>
       </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L20" s="264"/>
+      <c r="M20" s="264"/>
+      <c r="N20" s="264"/>
+      <c r="O20" s="264"/>
+      <c r="P20" s="264"/>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" s="174" t="s">
         <v>768</v>
       </c>
-      <c r="B21" s="259" t="s">
+      <c r="B21" s="219" t="s">
         <v>761</v>
       </c>
-      <c r="C21" s="259" t="s">
+      <c r="C21" s="219" t="s">
         <v>762</v>
       </c>
-      <c r="D21" s="259" t="s">
+      <c r="D21" s="219" t="s">
         <v>788</v>
       </c>
-      <c r="E21" s="238" t="s">
+      <c r="E21" s="202" t="s">
         <v>769</v>
       </c>
-      <c r="F21" s="238" t="s">
+      <c r="F21" s="202" t="s">
         <v>770</v>
       </c>
-      <c r="G21" s="259" t="s">
+      <c r="G21" s="219" t="s">
         <v>792</v>
       </c>
-      <c r="H21" s="259" t="s">
+      <c r="H21" s="219" t="s">
         <v>790</v>
       </c>
-      <c r="I21" s="259" t="s">
+      <c r="I21" s="219" t="s">
         <v>791</v>
       </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L21" s="264"/>
+      <c r="M21" s="264"/>
+      <c r="N21" s="264"/>
+      <c r="O21" s="264"/>
+      <c r="P21" s="264"/>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" s="175" t="s">
         <v>771</v>
       </c>
-      <c r="B22" s="260" t="s">
+      <c r="B22" s="220" t="s">
         <v>772</v>
       </c>
-      <c r="C22" s="260" t="s">
+      <c r="C22" s="220" t="s">
         <v>762</v>
       </c>
-      <c r="D22" s="260" t="s">
+      <c r="D22" s="220" t="s">
         <v>788</v>
       </c>
-      <c r="E22" s="260" t="s">
+      <c r="E22" s="220" t="s">
         <v>769</v>
       </c>
-      <c r="F22" s="261" t="s">
+      <c r="F22" s="221" t="s">
         <v>770</v>
       </c>
-      <c r="G22" s="261" t="s">
+      <c r="G22" s="221" t="s">
         <v>792</v>
       </c>
-      <c r="H22" s="261" t="s">
+      <c r="H22" s="221" t="s">
         <v>790</v>
       </c>
-      <c r="I22" s="260" t="s">
+      <c r="I22" s="220" t="s">
         <v>791</v>
       </c>
-    </row>
-    <row r="23" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L22" s="264"/>
+      <c r="M22" s="264"/>
+      <c r="N22" s="264"/>
+      <c r="O22" s="264"/>
+      <c r="P22" s="264"/>
+    </row>
+    <row r="23" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="176" t="s">
         <v>773</v>
       </c>
-      <c r="B23" s="249" t="s">
+      <c r="B23" s="258" t="s">
         <v>793</v>
       </c>
-      <c r="C23" s="249"/>
-      <c r="D23" s="249"/>
-      <c r="E23" s="249"/>
-      <c r="F23" s="249"/>
-      <c r="G23" s="249"/>
-      <c r="H23" s="249"/>
-      <c r="I23" s="249"/>
-    </row>
-    <row r="24" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="25" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C23" s="258"/>
+      <c r="D23" s="258"/>
+      <c r="E23" s="258"/>
+      <c r="F23" s="258"/>
+      <c r="G23" s="258"/>
+      <c r="H23" s="258"/>
+      <c r="I23" s="258"/>
+      <c r="L23" s="264"/>
+      <c r="M23" s="264"/>
+      <c r="N23" s="264"/>
+      <c r="O23" s="264"/>
+      <c r="P23" s="264"/>
+    </row>
+    <row r="24" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L24" s="264"/>
+      <c r="M24" s="264"/>
+      <c r="N24" s="264"/>
+      <c r="O24" s="264"/>
+      <c r="P24" s="264"/>
+    </row>
+    <row r="25" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="66" t="s">
         <v>760</v>
       </c>
-      <c r="B25" s="250" t="s">
+      <c r="B25" s="259" t="s">
         <v>781</v>
       </c>
-      <c r="C25" s="250"/>
-      <c r="D25" s="250"/>
-      <c r="E25" s="250"/>
-      <c r="F25" s="250"/>
-      <c r="G25" s="250"/>
-      <c r="H25" s="250"/>
-      <c r="I25" s="250"/>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C25" s="259"/>
+      <c r="D25" s="259"/>
+      <c r="E25" s="259"/>
+      <c r="F25" s="259"/>
+      <c r="G25" s="259"/>
+      <c r="H25" s="259"/>
+      <c r="I25" s="259"/>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" s="173" t="s">
         <v>198</v>
       </c>
-      <c r="B26" s="258" t="s">
+      <c r="B26" s="218" t="s">
         <v>761</v>
       </c>
-      <c r="C26" s="258" t="s">
+      <c r="C26" s="218" t="s">
         <v>794</v>
       </c>
-      <c r="D26" s="263" t="s">
+      <c r="D26" s="260" t="s">
         <v>795</v>
       </c>
-      <c r="E26" s="263"/>
-      <c r="F26" s="262" t="s">
+      <c r="E26" s="260"/>
+      <c r="F26" s="261" t="s">
         <v>796</v>
       </c>
-      <c r="G26" s="262"/>
-      <c r="H26" s="258" t="s">
+      <c r="G26" s="261"/>
+      <c r="H26" s="218" t="s">
         <v>797</v>
       </c>
-      <c r="I26" s="258" t="s">
+      <c r="I26" s="218" t="s">
         <v>798</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" s="174" t="s">
         <v>768</v>
       </c>
-      <c r="B27" s="259" t="s">
+      <c r="B27" s="219" t="s">
         <v>761</v>
       </c>
-      <c r="C27" s="259" t="s">
+      <c r="C27" s="219" t="s">
         <v>794</v>
       </c>
-      <c r="D27" s="259" t="s">
+      <c r="D27" s="219" t="s">
         <v>795</v>
       </c>
-      <c r="E27" s="238" t="s">
+      <c r="E27" s="202" t="s">
         <v>769</v>
       </c>
-      <c r="F27" s="238" t="s">
+      <c r="F27" s="202" t="s">
         <v>770</v>
       </c>
-      <c r="G27" s="259" t="s">
+      <c r="G27" s="219" t="s">
         <v>796</v>
       </c>
-      <c r="H27" s="259" t="s">
+      <c r="H27" s="219" t="s">
         <v>797</v>
       </c>
-      <c r="I27" s="259" t="s">
+      <c r="I27" s="219" t="s">
         <v>798</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28" s="175" t="s">
         <v>771</v>
       </c>
-      <c r="B28" s="260" t="s">
+      <c r="B28" s="220" t="s">
         <v>775</v>
       </c>
-      <c r="C28" s="260" t="s">
+      <c r="C28" s="220" t="s">
         <v>794</v>
       </c>
-      <c r="D28" s="260" t="s">
+      <c r="D28" s="220" t="s">
         <v>795</v>
       </c>
-      <c r="E28" s="260" t="s">
+      <c r="E28" s="220" t="s">
         <v>769</v>
       </c>
-      <c r="F28" s="261" t="s">
+      <c r="F28" s="221" t="s">
         <v>770</v>
       </c>
-      <c r="G28" s="261" t="s">
+      <c r="G28" s="221" t="s">
         <v>796</v>
       </c>
-      <c r="H28" s="261" t="s">
+      <c r="H28" s="221" t="s">
         <v>797</v>
       </c>
-      <c r="I28" s="260" t="s">
+      <c r="I28" s="220" t="s">
         <v>798</v>
       </c>
     </row>
-    <row r="29" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="176" t="s">
         <v>773</v>
       </c>
-      <c r="B29" s="249" t="s">
+      <c r="B29" s="258" t="s">
         <v>799</v>
       </c>
-      <c r="C29" s="249"/>
-      <c r="D29" s="249"/>
-      <c r="E29" s="249"/>
-      <c r="F29" s="249"/>
-      <c r="G29" s="249"/>
-      <c r="H29" s="249"/>
-      <c r="I29" s="249"/>
+      <c r="C29" s="258"/>
+      <c r="D29" s="258"/>
+      <c r="E29" s="258"/>
+      <c r="F29" s="258"/>
+      <c r="G29" s="258"/>
+      <c r="H29" s="258"/>
+      <c r="I29" s="258"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="M13:O16">
     <sortCondition ref="M13:M16"/>
   </sortState>
   <mergeCells count="21">
-    <mergeCell ref="B23:I23"/>
-    <mergeCell ref="B25:I25"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="F26:G26"/>
-    <mergeCell ref="B29:I29"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="B17:I17"/>
-    <mergeCell ref="B19:I19"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="F1:I1"/>
     <mergeCell ref="F4:H4"/>
     <mergeCell ref="B11:I11"/>
     <mergeCell ref="B13:I13"/>
@@ -12650,8 +12684,17 @@
     <mergeCell ref="B7:I7"/>
     <mergeCell ref="D8:E8"/>
     <mergeCell ref="F8:G8"/>
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="F1:I1"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="B17:I17"/>
+    <mergeCell ref="B19:I19"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="B23:I23"/>
+    <mergeCell ref="B25:I25"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="F26:G26"/>
+    <mergeCell ref="B29:I29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -12700,17 +12743,17 @@
       <c r="I1" s="18"/>
     </row>
     <row r="3" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="204" t="s">
+      <c r="A3" s="226" t="s">
         <v>30</v>
       </c>
-      <c r="B3" s="204"/>
-      <c r="C3" s="204"/>
-      <c r="D3" s="204"/>
-      <c r="F3" s="205" t="s">
+      <c r="B3" s="226"/>
+      <c r="C3" s="226"/>
+      <c r="D3" s="226"/>
+      <c r="F3" s="227" t="s">
         <v>31</v>
       </c>
-      <c r="G3" s="205"/>
-      <c r="H3" s="205"/>
+      <c r="G3" s="227"/>
+      <c r="H3" s="227"/>
     </row>
     <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="20" t="s">
@@ -12877,11 +12920,11 @@
       <c r="D11" s="23" t="s">
         <v>82</v>
       </c>
-      <c r="F11" s="205" t="s">
+      <c r="F11" s="227" t="s">
         <v>32</v>
       </c>
-      <c r="G11" s="205"/>
-      <c r="H11" s="205"/>
+      <c r="G11" s="227"/>
+      <c r="H11" s="227"/>
     </row>
     <row r="12" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="24" t="s">
@@ -13043,15 +13086,15 @@
       <c r="C1" t="s">
         <v>108</v>
       </c>
-      <c r="E1" s="204" t="s">
+      <c r="E1" s="226" t="s">
         <v>177</v>
       </c>
-      <c r="F1" s="204"/>
-      <c r="G1" s="204"/>
-      <c r="I1" s="211" t="s">
+      <c r="F1" s="226"/>
+      <c r="G1" s="226"/>
+      <c r="I1" s="228" t="s">
         <v>161</v>
       </c>
-      <c r="J1" s="211"/>
+      <c r="J1" s="228"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="46" t="s">
@@ -13172,10 +13215,10 @@
       <c r="G6" t="s">
         <v>155</v>
       </c>
-      <c r="I6" s="211" t="s">
+      <c r="I6" s="228" t="s">
         <v>169</v>
       </c>
-      <c r="J6" s="211"/>
+      <c r="J6" s="228"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="51" t="s">
@@ -13256,17 +13299,17 @@
       <c r="A11" s="57" t="s">
         <v>119</v>
       </c>
-      <c r="B11" s="208" t="s">
+      <c r="B11" s="233" t="s">
         <v>120</v>
       </c>
-      <c r="C11" s="208"/>
+      <c r="C11" s="233"/>
       <c r="E11" s="57" t="s">
         <v>129</v>
       </c>
-      <c r="F11" s="208" t="s">
+      <c r="F11" s="233" t="s">
         <v>187</v>
       </c>
-      <c r="G11" s="208" t="s">
+      <c r="G11" s="233" t="s">
         <v>160</v>
       </c>
       <c r="I11" s="57" t="s">
@@ -13280,17 +13323,17 @@
       <c r="A12" s="58" t="s">
         <v>121</v>
       </c>
-      <c r="B12" s="209" t="s">
+      <c r="B12" s="229" t="s">
         <v>128</v>
       </c>
-      <c r="C12" s="209"/>
+      <c r="C12" s="229"/>
       <c r="E12" s="58" t="s">
         <v>130</v>
       </c>
-      <c r="F12" s="209" t="s">
+      <c r="F12" s="229" t="s">
         <v>131</v>
       </c>
-      <c r="G12" s="209"/>
+      <c r="G12" s="229"/>
       <c r="I12" s="58" t="s">
         <v>179</v>
       </c>
@@ -13302,17 +13345,17 @@
       <c r="A13" s="55" t="s">
         <v>122</v>
       </c>
-      <c r="B13" s="210" t="s">
+      <c r="B13" s="230" t="s">
         <v>125</v>
       </c>
-      <c r="C13" s="210"/>
+      <c r="C13" s="230"/>
       <c r="E13" s="55" t="s">
         <v>132</v>
       </c>
-      <c r="F13" s="210" t="s">
+      <c r="F13" s="230" t="s">
         <v>135</v>
       </c>
-      <c r="G13" s="210"/>
+      <c r="G13" s="230"/>
       <c r="I13" s="55" t="s">
         <v>180</v>
       </c>
@@ -13324,17 +13367,17 @@
       <c r="A14" s="54" t="s">
         <v>123</v>
       </c>
-      <c r="B14" s="206" t="s">
+      <c r="B14" s="231" t="s">
         <v>126</v>
       </c>
-      <c r="C14" s="206"/>
+      <c r="C14" s="231"/>
       <c r="E14" s="54" t="s">
         <v>133</v>
       </c>
-      <c r="F14" s="206" t="s">
+      <c r="F14" s="231" t="s">
         <v>136</v>
       </c>
-      <c r="G14" s="206"/>
+      <c r="G14" s="231"/>
       <c r="I14" s="54" t="s">
         <v>181</v>
       </c>
@@ -13346,17 +13389,17 @@
       <c r="A15" s="56" t="s">
         <v>124</v>
       </c>
-      <c r="B15" s="207" t="s">
+      <c r="B15" s="232" t="s">
         <v>127</v>
       </c>
-      <c r="C15" s="207"/>
+      <c r="C15" s="232"/>
       <c r="E15" s="56" t="s">
         <v>134</v>
       </c>
-      <c r="F15" s="207" t="s">
+      <c r="F15" s="232" t="s">
         <v>137</v>
       </c>
-      <c r="G15" s="207"/>
+      <c r="G15" s="232"/>
       <c r="I15" s="56" t="s">
         <v>182</v>
       </c>
@@ -13366,11 +13409,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="I1:J1"/>
-    <mergeCell ref="I6:J6"/>
-    <mergeCell ref="E1:G1"/>
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="F13:G13"/>
     <mergeCell ref="F14:G14"/>
     <mergeCell ref="F15:G15"/>
     <mergeCell ref="F11:G11"/>
@@ -13379,6 +13417,11 @@
     <mergeCell ref="B13:C13"/>
     <mergeCell ref="B14:C14"/>
     <mergeCell ref="B15:C15"/>
+    <mergeCell ref="I1:J1"/>
+    <mergeCell ref="I6:J6"/>
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="F13:G13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -13798,16 +13841,16 @@
       <c r="K5" s="72" t="s">
         <v>226</v>
       </c>
-      <c r="L5" s="213" t="s">
+      <c r="L5" s="235" t="s">
         <v>300</v>
       </c>
-      <c r="M5" s="213"/>
-      <c r="N5" s="213"/>
-      <c r="O5" s="213"/>
-      <c r="P5" s="213"/>
-      <c r="Q5" s="213"/>
-      <c r="R5" s="213"/>
-      <c r="S5" s="213"/>
+      <c r="M5" s="235"/>
+      <c r="N5" s="235"/>
+      <c r="O5" s="235"/>
+      <c r="P5" s="235"/>
+      <c r="Q5" s="235"/>
+      <c r="R5" s="235"/>
+      <c r="S5" s="235"/>
     </row>
     <row r="6" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A6" s="30">
@@ -14040,10 +14083,10 @@
       <c r="F10">
         <v>10</v>
       </c>
-      <c r="H10" s="204" t="s">
+      <c r="H10" s="226" t="s">
         <v>302</v>
       </c>
-      <c r="I10" s="204"/>
+      <c r="I10" s="226"/>
       <c r="K10" s="71">
         <v>127</v>
       </c>
@@ -14161,10 +14204,10 @@
       <c r="F12">
         <v>16</v>
       </c>
-      <c r="H12" s="204" t="s">
+      <c r="H12" s="226" t="s">
         <v>301</v>
       </c>
-      <c r="I12" s="204"/>
+      <c r="I12" s="226"/>
       <c r="K12" s="71">
         <v>68</v>
       </c>
@@ -14226,10 +14269,10 @@
       <c r="F13">
         <v>4</v>
       </c>
-      <c r="H13" s="204" t="s">
+      <c r="H13" s="226" t="s">
         <v>303</v>
       </c>
-      <c r="I13" s="204"/>
+      <c r="I13" s="226"/>
       <c r="K13" s="71">
         <v>180</v>
       </c>
@@ -14394,10 +14437,10 @@
       <c r="F15">
         <v>16</v>
       </c>
-      <c r="H15" s="204" t="s">
+      <c r="H15" s="226" t="s">
         <v>301</v>
       </c>
-      <c r="I15" s="204"/>
+      <c r="I15" s="226"/>
       <c r="K15" s="71">
         <v>63</v>
       </c>
@@ -14511,10 +14554,10 @@
       <c r="F16">
         <v>3</v>
       </c>
-      <c r="H16" s="204" t="s">
+      <c r="H16" s="226" t="s">
         <v>307</v>
       </c>
-      <c r="I16" s="204"/>
+      <c r="I16" s="226"/>
       <c r="K16" s="71">
         <v>224</v>
       </c>
@@ -14665,30 +14708,30 @@
       <c r="AA17" s="82"/>
       <c r="AB17" s="69"/>
       <c r="AC17" s="68"/>
-      <c r="AE17" s="212" t="s">
+      <c r="AE17" s="234" t="s">
         <v>83</v>
       </c>
-      <c r="AF17" s="212"/>
-      <c r="AG17" s="212"/>
-      <c r="AH17" s="212"/>
-      <c r="AI17" s="212">
+      <c r="AF17" s="234"/>
+      <c r="AG17" s="234"/>
+      <c r="AH17" s="234"/>
+      <c r="AI17" s="234">
         <v>4</v>
       </c>
-      <c r="AJ17" s="212"/>
-      <c r="AK17" s="212"/>
-      <c r="AL17" s="212"/>
-      <c r="AM17" s="212" t="s">
+      <c r="AJ17" s="234"/>
+      <c r="AK17" s="234"/>
+      <c r="AL17" s="234"/>
+      <c r="AM17" s="234" t="s">
         <v>324</v>
       </c>
-      <c r="AN17" s="212"/>
-      <c r="AO17" s="212"/>
-      <c r="AP17" s="212"/>
-      <c r="AQ17" s="212">
+      <c r="AN17" s="234"/>
+      <c r="AO17" s="234"/>
+      <c r="AP17" s="234"/>
+      <c r="AQ17" s="234">
         <v>6</v>
       </c>
-      <c r="AR17" s="212"/>
-      <c r="AS17" s="212"/>
-      <c r="AT17" s="212"/>
+      <c r="AR17" s="234"/>
+      <c r="AS17" s="234"/>
+      <c r="AT17" s="234"/>
     </row>
     <row r="18" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A18" s="59">
@@ -14918,16 +14961,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="H16:I16"/>
+    <mergeCell ref="H15:I15"/>
     <mergeCell ref="AE17:AH17"/>
     <mergeCell ref="AI17:AL17"/>
     <mergeCell ref="AM17:AP17"/>
     <mergeCell ref="AQ17:AT17"/>
     <mergeCell ref="L5:S5"/>
-    <mergeCell ref="H10:I10"/>
-    <mergeCell ref="H13:I13"/>
-    <mergeCell ref="H12:I12"/>
-    <mergeCell ref="H16:I16"/>
-    <mergeCell ref="H15:I15"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -14972,24 +15015,24 @@
       <c r="A1" s="105" t="s">
         <v>325</v>
       </c>
-      <c r="B1" s="223" t="s">
+      <c r="B1" s="245" t="s">
         <v>329</v>
       </c>
-      <c r="C1" s="224"/>
-      <c r="D1" s="224"/>
-      <c r="E1" s="225"/>
-      <c r="F1" s="223" t="s">
+      <c r="C1" s="246"/>
+      <c r="D1" s="246"/>
+      <c r="E1" s="247"/>
+      <c r="F1" s="245" t="s">
         <v>330</v>
       </c>
-      <c r="G1" s="224"/>
-      <c r="H1" s="224"/>
-      <c r="I1" s="225"/>
-      <c r="J1" s="220" t="s">
+      <c r="G1" s="246"/>
+      <c r="H1" s="246"/>
+      <c r="I1" s="247"/>
+      <c r="J1" s="242" t="s">
         <v>347</v>
       </c>
-      <c r="K1" s="221"/>
-      <c r="L1" s="221"/>
-      <c r="M1" s="222"/>
+      <c r="K1" s="243"/>
+      <c r="L1" s="243"/>
+      <c r="M1" s="244"/>
     </row>
     <row r="2" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="106" t="s">
@@ -15174,18 +15217,18 @@
       <c r="E6" s="115" t="s">
         <v>400</v>
       </c>
-      <c r="F6" s="214" t="s">
+      <c r="F6" s="236" t="s">
         <v>337</v>
       </c>
-      <c r="G6" s="215"/>
-      <c r="H6" s="215"/>
-      <c r="I6" s="216"/>
-      <c r="J6" s="214" t="s">
+      <c r="G6" s="237"/>
+      <c r="H6" s="237"/>
+      <c r="I6" s="238"/>
+      <c r="J6" s="236" t="s">
         <v>337</v>
       </c>
-      <c r="K6" s="215"/>
-      <c r="L6" s="215"/>
-      <c r="M6" s="216"/>
+      <c r="K6" s="237"/>
+      <c r="L6" s="237"/>
+      <c r="M6" s="238"/>
     </row>
     <row r="7" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="123" t="s">
@@ -15203,18 +15246,18 @@
       <c r="E7" s="125" t="s">
         <v>402</v>
       </c>
-      <c r="F7" s="217" t="s">
+      <c r="F7" s="239" t="s">
         <v>338</v>
       </c>
-      <c r="G7" s="218"/>
-      <c r="H7" s="218"/>
-      <c r="I7" s="219"/>
-      <c r="J7" s="217" t="s">
+      <c r="G7" s="240"/>
+      <c r="H7" s="240"/>
+      <c r="I7" s="241"/>
+      <c r="J7" s="239" t="s">
         <v>338</v>
       </c>
-      <c r="K7" s="218"/>
-      <c r="L7" s="218"/>
-      <c r="M7" s="219"/>
+      <c r="K7" s="240"/>
+      <c r="L7" s="240"/>
+      <c r="M7" s="241"/>
     </row>
     <row r="8" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="9" spans="1:13" s="101" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -15839,15 +15882,15 @@
       <c r="A1" s="100" t="s">
         <v>391</v>
       </c>
-      <c r="B1" s="226" t="s">
+      <c r="B1" s="248" t="s">
         <v>392</v>
       </c>
-      <c r="C1" s="226"/>
-      <c r="D1" s="226"/>
-      <c r="E1" s="226"/>
-      <c r="F1" s="226"/>
-      <c r="G1" s="226"/>
-      <c r="H1" s="226"/>
+      <c r="C1" s="248"/>
+      <c r="D1" s="248"/>
+      <c r="E1" s="248"/>
+      <c r="F1" s="248"/>
+      <c r="G1" s="248"/>
+      <c r="H1" s="248"/>
     </row>
     <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:9" s="99" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -16854,14 +16897,14 @@
       <c r="A1" s="100" t="s">
         <v>573</v>
       </c>
-      <c r="B1" s="227" t="s">
+      <c r="B1" s="249" t="s">
         <v>574</v>
       </c>
-      <c r="C1" s="227"/>
-      <c r="D1" s="227"/>
-      <c r="E1" s="227"/>
-      <c r="F1" s="227"/>
-      <c r="G1" s="227"/>
+      <c r="C1" s="249"/>
+      <c r="D1" s="249"/>
+      <c r="E1" s="249"/>
+      <c r="F1" s="249"/>
+      <c r="G1" s="249"/>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="99" t="s">
@@ -17700,16 +17743,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="228" t="s">
+      <c r="A1" s="250" t="s">
         <v>690</v>
       </c>
-      <c r="B1" s="228"/>
-      <c r="C1" s="228"/>
-      <c r="E1" s="228" t="s">
+      <c r="B1" s="250"/>
+      <c r="C1" s="250"/>
+      <c r="E1" s="250" t="s">
         <v>689</v>
       </c>
-      <c r="F1" s="228"/>
-      <c r="G1" s="228"/>
+      <c r="F1" s="250"/>
+      <c r="G1" s="250"/>
       <c r="I1" s="57" t="s">
         <v>688</v>
       </c>
@@ -17778,7 +17821,7 @@
       <c r="M2" s="195" t="s">
         <v>368</v>
       </c>
-      <c r="N2" s="227" t="s">
+      <c r="N2" s="249" t="s">
         <v>681</v>
       </c>
       <c r="P2" t="s">
@@ -17831,7 +17874,7 @@
       <c r="M3" s="183" t="s">
         <v>645</v>
       </c>
-      <c r="N3" s="227"/>
+      <c r="N3" s="249"/>
       <c r="P3" t="s">
         <v>696</v>
       </c>
@@ -17882,7 +17925,7 @@
       <c r="M4" s="188" t="s">
         <v>656</v>
       </c>
-      <c r="N4" s="230"/>
+      <c r="N4" s="252"/>
       <c r="P4" t="s">
         <v>697</v>
       </c>
@@ -17933,7 +17976,7 @@
       <c r="M5" s="192" t="s">
         <v>667</v>
       </c>
-      <c r="N5" s="231" t="s">
+      <c r="N5" s="253" t="s">
         <v>666</v>
       </c>
       <c r="P5" t="s">
@@ -17986,7 +18029,7 @@
       <c r="M6" s="188" t="s">
         <v>660</v>
       </c>
-      <c r="N6" s="232"/>
+      <c r="N6" s="254"/>
       <c r="P6" t="s">
         <v>699</v>
       </c>
@@ -18037,7 +18080,7 @@
       <c r="M7" s="183" t="s">
         <v>656</v>
       </c>
-      <c r="N7" s="233"/>
+      <c r="N7" s="255"/>
       <c r="P7" t="s">
         <v>700</v>
       </c>
@@ -18089,7 +18132,7 @@
       <c r="M8" s="184" t="s">
         <v>650</v>
       </c>
-      <c r="N8" s="234" t="s">
+      <c r="N8" s="256" t="s">
         <v>649</v>
       </c>
       <c r="P8" t="s">
@@ -18133,7 +18176,7 @@
       <c r="M9" s="183" t="s">
         <v>645</v>
       </c>
-      <c r="N9" s="229"/>
+      <c r="N9" s="251"/>
       <c r="P9" t="s">
         <v>701</v>
       </c>
@@ -18151,11 +18194,11 @@
       </c>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A10" s="229" t="s">
+      <c r="A10" s="251" t="s">
         <v>644</v>
       </c>
-      <c r="B10" s="229"/>
-      <c r="C10" s="229"/>
+      <c r="B10" s="251"/>
+      <c r="C10" s="251"/>
       <c r="E10" t="s">
         <v>637</v>
       </c>
@@ -18180,7 +18223,7 @@
       <c r="M10" s="179" t="s">
         <v>639</v>
       </c>
-      <c r="N10" s="235"/>
+      <c r="N10" s="257"/>
       <c r="P10" t="s">
         <v>703</v>
       </c>
@@ -18198,9 +18241,9 @@
       </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A11" s="229"/>
-      <c r="B11" s="229"/>
-      <c r="C11" s="229"/>
+      <c r="A11" s="251"/>
+      <c r="B11" s="251"/>
+      <c r="C11" s="251"/>
       <c r="E11" t="s">
         <v>249</v>
       </c>
@@ -18227,9 +18270,9 @@
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A12" s="229"/>
-      <c r="B12" s="229"/>
-      <c r="C12" s="229"/>
+      <c r="A12" s="251"/>
+      <c r="B12" s="251"/>
+      <c r="C12" s="251"/>
       <c r="E12" t="s">
         <v>637</v>
       </c>
@@ -18256,9 +18299,9 @@
       </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A13" s="229"/>
-      <c r="B13" s="229"/>
-      <c r="C13" s="229"/>
+      <c r="A13" s="251"/>
+      <c r="B13" s="251"/>
+      <c r="C13" s="251"/>
       <c r="E13" t="s">
         <v>417</v>
       </c>

</xml_diff>